<commit_message>
converted from desktop app to a web app
</commit_message>
<xml_diff>
--- a/cockpit_template.xlsx
+++ b/cockpit_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Roi.Dital/roid_playground/paamonim/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA44CAAA-BD1E-C74B-8B0B-93DDDEFD3413}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{396250F9-7E74-214F-B58F-7A8F37B3D5B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="19440" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="19440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="רציונל" sheetId="3" r:id="rId1"/>
@@ -840,6 +840,90 @@
     <xf numFmtId="0" fontId="15" fillId="12" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -923,90 +1007,6 @@
     </xf>
     <xf numFmtId="0" fontId="17" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1998,24 +1998,24 @@
   <sheetData>
     <row r="1" spans="6:21" ht="20" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F2" s="92" t="s">
+      <c r="F2" s="48" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="92"/>
-      <c r="H2" s="92"/>
-      <c r="I2" s="92"/>
-      <c r="J2" s="92"/>
-      <c r="K2" s="92"/>
-      <c r="L2" s="92"/>
-      <c r="M2" s="92"/>
-      <c r="N2" s="92"/>
-      <c r="O2" s="92"/>
-      <c r="P2" s="92"/>
-      <c r="Q2" s="92"/>
-      <c r="R2" s="92"/>
-      <c r="S2" s="92"/>
-      <c r="T2" s="92"/>
-      <c r="U2" s="92"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="48"/>
+      <c r="J2" s="48"/>
+      <c r="K2" s="48"/>
+      <c r="L2" s="48"/>
+      <c r="M2" s="48"/>
+      <c r="N2" s="48"/>
+      <c r="O2" s="48"/>
+      <c r="P2" s="48"/>
+      <c r="Q2" s="48"/>
+      <c r="R2" s="48"/>
+      <c r="S2" s="48"/>
+      <c r="T2" s="48"/>
+      <c r="U2" s="48"/>
     </row>
     <row r="3" spans="6:21" x14ac:dyDescent="0.2">
       <c r="F3" s="30"/>
@@ -2036,68 +2036,68 @@
       <c r="U3" s="30"/>
     </row>
     <row r="4" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F4" s="87" t="s">
+      <c r="F4" s="56" t="s">
         <v>23</v>
       </c>
-      <c r="G4" s="88"/>
-      <c r="H4" s="88"/>
-      <c r="I4" s="88"/>
-      <c r="J4" s="88"/>
-      <c r="K4" s="88"/>
-      <c r="L4" s="88"/>
-      <c r="M4" s="88"/>
-      <c r="N4" s="88"/>
-      <c r="O4" s="88"/>
-      <c r="P4" s="88"/>
-      <c r="Q4" s="88"/>
-      <c r="R4" s="88"/>
-      <c r="S4" s="88"/>
-      <c r="T4" s="88"/>
-      <c r="U4" s="89"/>
+      <c r="G4" s="57"/>
+      <c r="H4" s="57"/>
+      <c r="I4" s="57"/>
+      <c r="J4" s="57"/>
+      <c r="K4" s="57"/>
+      <c r="L4" s="57"/>
+      <c r="M4" s="57"/>
+      <c r="N4" s="57"/>
+      <c r="O4" s="57"/>
+      <c r="P4" s="57"/>
+      <c r="Q4" s="57"/>
+      <c r="R4" s="57"/>
+      <c r="S4" s="57"/>
+      <c r="T4" s="57"/>
+      <c r="U4" s="58"/>
     </row>
     <row r="5" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F5" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="G5" s="72" t="s">
+      <c r="G5" s="59" t="s">
         <v>40</v>
       </c>
-      <c r="H5" s="72"/>
-      <c r="I5" s="72"/>
-      <c r="J5" s="72"/>
-      <c r="K5" s="72"/>
-      <c r="L5" s="72"/>
-      <c r="M5" s="72"/>
-      <c r="N5" s="72"/>
-      <c r="O5" s="72"/>
-      <c r="P5" s="72"/>
-      <c r="Q5" s="72"/>
-      <c r="R5" s="72"/>
-      <c r="S5" s="72"/>
-      <c r="T5" s="72"/>
-      <c r="U5" s="73"/>
+      <c r="H5" s="59"/>
+      <c r="I5" s="59"/>
+      <c r="J5" s="59"/>
+      <c r="K5" s="59"/>
+      <c r="L5" s="59"/>
+      <c r="M5" s="59"/>
+      <c r="N5" s="59"/>
+      <c r="O5" s="59"/>
+      <c r="P5" s="59"/>
+      <c r="Q5" s="59"/>
+      <c r="R5" s="59"/>
+      <c r="S5" s="59"/>
+      <c r="T5" s="59"/>
+      <c r="U5" s="60"/>
     </row>
     <row r="6" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F6" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="90" t="s">
+      <c r="G6" s="44" t="s">
         <v>42</v>
       </c>
-      <c r="H6" s="90"/>
-      <c r="I6" s="90"/>
-      <c r="J6" s="90"/>
-      <c r="K6" s="90"/>
-      <c r="L6" s="90"/>
-      <c r="M6" s="90"/>
-      <c r="N6" s="90"/>
-      <c r="O6" s="90"/>
-      <c r="P6" s="90"/>
-      <c r="Q6" s="90"/>
-      <c r="R6" s="90"/>
-      <c r="S6" s="90"/>
-      <c r="T6" s="90"/>
-      <c r="U6" s="91"/>
+      <c r="H6" s="44"/>
+      <c r="I6" s="44"/>
+      <c r="J6" s="44"/>
+      <c r="K6" s="44"/>
+      <c r="L6" s="44"/>
+      <c r="M6" s="44"/>
+      <c r="N6" s="44"/>
+      <c r="O6" s="44"/>
+      <c r="P6" s="44"/>
+      <c r="Q6" s="44"/>
+      <c r="R6" s="44"/>
+      <c r="S6" s="44"/>
+      <c r="T6" s="44"/>
+      <c r="U6" s="45"/>
     </row>
     <row r="7" spans="6:21" x14ac:dyDescent="0.2">
       <c r="F7" s="31"/>
@@ -2118,46 +2118,46 @@
       <c r="U7" s="31"/>
     </row>
     <row r="8" spans="6:21" ht="26" x14ac:dyDescent="0.2">
-      <c r="F8" s="93" t="s">
+      <c r="F8" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="G8" s="94"/>
-      <c r="H8" s="94"/>
-      <c r="I8" s="94"/>
-      <c r="J8" s="94"/>
-      <c r="K8" s="94"/>
-      <c r="L8" s="94"/>
-      <c r="M8" s="94"/>
-      <c r="N8" s="94"/>
-      <c r="O8" s="94"/>
-      <c r="P8" s="94"/>
-      <c r="Q8" s="94"/>
-      <c r="R8" s="94"/>
-      <c r="S8" s="94"/>
-      <c r="T8" s="94"/>
-      <c r="U8" s="95"/>
+      <c r="G8" s="50"/>
+      <c r="H8" s="50"/>
+      <c r="I8" s="50"/>
+      <c r="J8" s="50"/>
+      <c r="K8" s="50"/>
+      <c r="L8" s="50"/>
+      <c r="M8" s="50"/>
+      <c r="N8" s="50"/>
+      <c r="O8" s="50"/>
+      <c r="P8" s="50"/>
+      <c r="Q8" s="50"/>
+      <c r="R8" s="50"/>
+      <c r="S8" s="50"/>
+      <c r="T8" s="50"/>
+      <c r="U8" s="51"/>
     </row>
     <row r="9" spans="6:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F9" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="G9" s="96" t="s">
+      <c r="G9" s="52" t="s">
         <v>60</v>
       </c>
-      <c r="H9" s="96"/>
-      <c r="I9" s="96"/>
-      <c r="J9" s="96"/>
-      <c r="K9" s="96"/>
-      <c r="L9" s="96"/>
-      <c r="M9" s="96"/>
-      <c r="N9" s="96"/>
-      <c r="O9" s="96"/>
-      <c r="P9" s="96"/>
-      <c r="Q9" s="96"/>
-      <c r="R9" s="96"/>
-      <c r="S9" s="96"/>
-      <c r="T9" s="96"/>
-      <c r="U9" s="97"/>
+      <c r="H9" s="52"/>
+      <c r="I9" s="52"/>
+      <c r="J9" s="52"/>
+      <c r="K9" s="52"/>
+      <c r="L9" s="52"/>
+      <c r="M9" s="52"/>
+      <c r="N9" s="52"/>
+      <c r="O9" s="52"/>
+      <c r="P9" s="52"/>
+      <c r="Q9" s="52"/>
+      <c r="R9" s="52"/>
+      <c r="S9" s="52"/>
+      <c r="T9" s="52"/>
+      <c r="U9" s="53"/>
     </row>
     <row r="10" spans="6:21" x14ac:dyDescent="0.2">
       <c r="F10" s="32"/>
@@ -2196,68 +2196,68 @@
       <c r="U12" s="32"/>
     </row>
     <row r="13" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F13" s="87" t="s">
+      <c r="F13" s="56" t="s">
         <v>58</v>
       </c>
-      <c r="G13" s="88"/>
-      <c r="H13" s="88"/>
-      <c r="I13" s="88"/>
-      <c r="J13" s="88"/>
-      <c r="K13" s="88"/>
-      <c r="L13" s="88"/>
-      <c r="M13" s="88"/>
-      <c r="N13" s="88"/>
-      <c r="O13" s="88"/>
-      <c r="P13" s="88"/>
-      <c r="Q13" s="88"/>
-      <c r="R13" s="88"/>
-      <c r="S13" s="88"/>
-      <c r="T13" s="88"/>
-      <c r="U13" s="89"/>
+      <c r="G13" s="57"/>
+      <c r="H13" s="57"/>
+      <c r="I13" s="57"/>
+      <c r="J13" s="57"/>
+      <c r="K13" s="57"/>
+      <c r="L13" s="57"/>
+      <c r="M13" s="57"/>
+      <c r="N13" s="57"/>
+      <c r="O13" s="57"/>
+      <c r="P13" s="57"/>
+      <c r="Q13" s="57"/>
+      <c r="R13" s="57"/>
+      <c r="S13" s="57"/>
+      <c r="T13" s="57"/>
+      <c r="U13" s="58"/>
     </row>
     <row r="14" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F14" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="G14" s="98" t="s">
+      <c r="G14" s="54" t="s">
         <v>44</v>
       </c>
-      <c r="H14" s="98"/>
-      <c r="I14" s="98"/>
-      <c r="J14" s="98"/>
-      <c r="K14" s="98"/>
-      <c r="L14" s="98"/>
-      <c r="M14" s="98"/>
-      <c r="N14" s="98"/>
-      <c r="O14" s="98"/>
-      <c r="P14" s="98"/>
-      <c r="Q14" s="98"/>
-      <c r="R14" s="98"/>
-      <c r="S14" s="98"/>
-      <c r="T14" s="98"/>
-      <c r="U14" s="99"/>
+      <c r="H14" s="54"/>
+      <c r="I14" s="54"/>
+      <c r="J14" s="54"/>
+      <c r="K14" s="54"/>
+      <c r="L14" s="54"/>
+      <c r="M14" s="54"/>
+      <c r="N14" s="54"/>
+      <c r="O14" s="54"/>
+      <c r="P14" s="54"/>
+      <c r="Q14" s="54"/>
+      <c r="R14" s="54"/>
+      <c r="S14" s="54"/>
+      <c r="T14" s="54"/>
+      <c r="U14" s="55"/>
     </row>
     <row r="15" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F15" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="G15" s="98" t="s">
+      <c r="G15" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="H15" s="98"/>
-      <c r="I15" s="98"/>
-      <c r="J15" s="98"/>
-      <c r="K15" s="98"/>
-      <c r="L15" s="98"/>
-      <c r="M15" s="98"/>
-      <c r="N15" s="98"/>
-      <c r="O15" s="98"/>
-      <c r="P15" s="98"/>
-      <c r="Q15" s="98"/>
-      <c r="R15" s="98"/>
-      <c r="S15" s="98"/>
-      <c r="T15" s="98"/>
-      <c r="U15" s="99"/>
+      <c r="H15" s="54"/>
+      <c r="I15" s="54"/>
+      <c r="J15" s="54"/>
+      <c r="K15" s="54"/>
+      <c r="L15" s="54"/>
+      <c r="M15" s="54"/>
+      <c r="N15" s="54"/>
+      <c r="O15" s="54"/>
+      <c r="P15" s="54"/>
+      <c r="Q15" s="54"/>
+      <c r="R15" s="54"/>
+      <c r="S15" s="54"/>
+      <c r="T15" s="54"/>
+      <c r="U15" s="55"/>
     </row>
     <row r="16" spans="6:21" x14ac:dyDescent="0.2">
       <c r="F16" s="36"/>
@@ -2278,46 +2278,46 @@
       <c r="U16" s="37"/>
     </row>
     <row r="17" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F17" s="81" t="s">
+      <c r="F17" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="G17" s="82"/>
-      <c r="H17" s="82"/>
-      <c r="I17" s="82"/>
-      <c r="J17" s="82"/>
-      <c r="K17" s="82"/>
-      <c r="L17" s="82"/>
-      <c r="M17" s="82"/>
-      <c r="N17" s="82"/>
-      <c r="O17" s="82"/>
-      <c r="P17" s="82"/>
-      <c r="Q17" s="82"/>
-      <c r="R17" s="82"/>
-      <c r="S17" s="82"/>
-      <c r="T17" s="82"/>
-      <c r="U17" s="83"/>
+      <c r="G17" s="62"/>
+      <c r="H17" s="62"/>
+      <c r="I17" s="62"/>
+      <c r="J17" s="62"/>
+      <c r="K17" s="62"/>
+      <c r="L17" s="62"/>
+      <c r="M17" s="62"/>
+      <c r="N17" s="62"/>
+      <c r="O17" s="62"/>
+      <c r="P17" s="62"/>
+      <c r="Q17" s="62"/>
+      <c r="R17" s="62"/>
+      <c r="S17" s="62"/>
+      <c r="T17" s="62"/>
+      <c r="U17" s="63"/>
     </row>
     <row r="18" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F18" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="G18" s="98" t="s">
+      <c r="G18" s="54" t="s">
         <v>48</v>
       </c>
-      <c r="H18" s="98"/>
-      <c r="I18" s="98"/>
-      <c r="J18" s="98"/>
-      <c r="K18" s="98"/>
-      <c r="L18" s="98"/>
-      <c r="M18" s="98"/>
-      <c r="N18" s="98"/>
-      <c r="O18" s="98"/>
-      <c r="P18" s="98"/>
-      <c r="Q18" s="98"/>
-      <c r="R18" s="98"/>
-      <c r="S18" s="98"/>
-      <c r="T18" s="98"/>
-      <c r="U18" s="99"/>
+      <c r="H18" s="54"/>
+      <c r="I18" s="54"/>
+      <c r="J18" s="54"/>
+      <c r="K18" s="54"/>
+      <c r="L18" s="54"/>
+      <c r="M18" s="54"/>
+      <c r="N18" s="54"/>
+      <c r="O18" s="54"/>
+      <c r="P18" s="54"/>
+      <c r="Q18" s="54"/>
+      <c r="R18" s="54"/>
+      <c r="S18" s="54"/>
+      <c r="T18" s="54"/>
+      <c r="U18" s="55"/>
     </row>
     <row r="19" spans="6:21" x14ac:dyDescent="0.2">
       <c r="F19" s="36"/>
@@ -2338,46 +2338,46 @@
       <c r="U19" s="37"/>
     </row>
     <row r="20" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F20" s="81" t="s">
+      <c r="F20" s="61" t="s">
         <v>45</v>
       </c>
-      <c r="G20" s="82"/>
-      <c r="H20" s="82"/>
-      <c r="I20" s="82"/>
-      <c r="J20" s="82"/>
-      <c r="K20" s="82"/>
-      <c r="L20" s="82"/>
-      <c r="M20" s="82"/>
-      <c r="N20" s="82"/>
-      <c r="O20" s="82"/>
-      <c r="P20" s="82"/>
-      <c r="Q20" s="82"/>
-      <c r="R20" s="82"/>
-      <c r="S20" s="82"/>
-      <c r="T20" s="82"/>
-      <c r="U20" s="83"/>
+      <c r="G20" s="62"/>
+      <c r="H20" s="62"/>
+      <c r="I20" s="62"/>
+      <c r="J20" s="62"/>
+      <c r="K20" s="62"/>
+      <c r="L20" s="62"/>
+      <c r="M20" s="62"/>
+      <c r="N20" s="62"/>
+      <c r="O20" s="62"/>
+      <c r="P20" s="62"/>
+      <c r="Q20" s="62"/>
+      <c r="R20" s="62"/>
+      <c r="S20" s="62"/>
+      <c r="T20" s="62"/>
+      <c r="U20" s="63"/>
     </row>
     <row r="21" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F21" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="G21" s="98" t="s">
+      <c r="G21" s="54" t="s">
         <v>59</v>
       </c>
-      <c r="H21" s="98"/>
-      <c r="I21" s="98"/>
-      <c r="J21" s="98"/>
-      <c r="K21" s="98"/>
-      <c r="L21" s="98"/>
-      <c r="M21" s="98"/>
-      <c r="N21" s="98"/>
-      <c r="O21" s="98"/>
-      <c r="P21" s="98"/>
-      <c r="Q21" s="98"/>
-      <c r="R21" s="98"/>
-      <c r="S21" s="98"/>
-      <c r="T21" s="98"/>
-      <c r="U21" s="99"/>
+      <c r="H21" s="54"/>
+      <c r="I21" s="54"/>
+      <c r="J21" s="54"/>
+      <c r="K21" s="54"/>
+      <c r="L21" s="54"/>
+      <c r="M21" s="54"/>
+      <c r="N21" s="54"/>
+      <c r="O21" s="54"/>
+      <c r="P21" s="54"/>
+      <c r="Q21" s="54"/>
+      <c r="R21" s="54"/>
+      <c r="S21" s="54"/>
+      <c r="T21" s="54"/>
+      <c r="U21" s="55"/>
     </row>
     <row r="22" spans="6:21" x14ac:dyDescent="0.2">
       <c r="F22" s="36"/>
@@ -2398,46 +2398,46 @@
       <c r="U22" s="37"/>
     </row>
     <row r="23" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F23" s="81" t="s">
+      <c r="F23" s="61" t="s">
         <v>46</v>
       </c>
-      <c r="G23" s="82"/>
-      <c r="H23" s="82"/>
-      <c r="I23" s="82"/>
-      <c r="J23" s="82"/>
-      <c r="K23" s="82"/>
-      <c r="L23" s="82"/>
-      <c r="M23" s="82"/>
-      <c r="N23" s="82"/>
-      <c r="O23" s="82"/>
-      <c r="P23" s="82"/>
-      <c r="Q23" s="82"/>
-      <c r="R23" s="82"/>
-      <c r="S23" s="82"/>
-      <c r="T23" s="82"/>
-      <c r="U23" s="83"/>
+      <c r="G23" s="62"/>
+      <c r="H23" s="62"/>
+      <c r="I23" s="62"/>
+      <c r="J23" s="62"/>
+      <c r="K23" s="62"/>
+      <c r="L23" s="62"/>
+      <c r="M23" s="62"/>
+      <c r="N23" s="62"/>
+      <c r="O23" s="62"/>
+      <c r="P23" s="62"/>
+      <c r="Q23" s="62"/>
+      <c r="R23" s="62"/>
+      <c r="S23" s="62"/>
+      <c r="T23" s="62"/>
+      <c r="U23" s="63"/>
     </row>
     <row r="24" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F24" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="G24" s="78" t="s">
+      <c r="G24" s="64" t="s">
         <v>47</v>
       </c>
-      <c r="H24" s="78"/>
-      <c r="I24" s="78"/>
-      <c r="J24" s="78"/>
-      <c r="K24" s="78"/>
-      <c r="L24" s="78"/>
-      <c r="M24" s="78"/>
-      <c r="N24" s="78"/>
-      <c r="O24" s="78"/>
-      <c r="P24" s="78"/>
-      <c r="Q24" s="78"/>
-      <c r="R24" s="78"/>
-      <c r="S24" s="78"/>
-      <c r="T24" s="78"/>
-      <c r="U24" s="79"/>
+      <c r="H24" s="64"/>
+      <c r="I24" s="64"/>
+      <c r="J24" s="64"/>
+      <c r="K24" s="64"/>
+      <c r="L24" s="64"/>
+      <c r="M24" s="64"/>
+      <c r="N24" s="64"/>
+      <c r="O24" s="64"/>
+      <c r="P24" s="64"/>
+      <c r="Q24" s="64"/>
+      <c r="R24" s="64"/>
+      <c r="S24" s="64"/>
+      <c r="T24" s="64"/>
+      <c r="U24" s="65"/>
     </row>
     <row r="25" spans="6:21" x14ac:dyDescent="0.2">
       <c r="F25" s="32"/>
@@ -2494,174 +2494,174 @@
       <c r="U27" s="32"/>
     </row>
     <row r="28" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F28" s="84" t="s">
+      <c r="F28" s="67" t="s">
         <v>17</v>
       </c>
-      <c r="G28" s="85"/>
-      <c r="H28" s="85"/>
-      <c r="I28" s="85"/>
-      <c r="J28" s="85"/>
-      <c r="K28" s="85"/>
-      <c r="L28" s="85"/>
-      <c r="M28" s="85"/>
-      <c r="N28" s="85"/>
-      <c r="O28" s="85"/>
-      <c r="P28" s="85"/>
-      <c r="Q28" s="85"/>
-      <c r="R28" s="85"/>
-      <c r="S28" s="85"/>
-      <c r="T28" s="85"/>
-      <c r="U28" s="86"/>
+      <c r="G28" s="68"/>
+      <c r="H28" s="68"/>
+      <c r="I28" s="68"/>
+      <c r="J28" s="68"/>
+      <c r="K28" s="68"/>
+      <c r="L28" s="68"/>
+      <c r="M28" s="68"/>
+      <c r="N28" s="68"/>
+      <c r="O28" s="68"/>
+      <c r="P28" s="68"/>
+      <c r="Q28" s="68"/>
+      <c r="R28" s="68"/>
+      <c r="S28" s="68"/>
+      <c r="T28" s="68"/>
+      <c r="U28" s="69"/>
     </row>
     <row r="29" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F29" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="G29" s="74" t="s">
+      <c r="G29" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="H29" s="74"/>
-      <c r="I29" s="74"/>
-      <c r="J29" s="74"/>
-      <c r="K29" s="74"/>
-      <c r="L29" s="74"/>
-      <c r="M29" s="74"/>
-      <c r="N29" s="74"/>
-      <c r="O29" s="74"/>
-      <c r="P29" s="74"/>
-      <c r="Q29" s="74"/>
-      <c r="R29" s="74"/>
-      <c r="S29" s="74"/>
-      <c r="T29" s="74"/>
-      <c r="U29" s="75"/>
+      <c r="H29" s="46"/>
+      <c r="I29" s="46"/>
+      <c r="J29" s="46"/>
+      <c r="K29" s="46"/>
+      <c r="L29" s="46"/>
+      <c r="M29" s="46"/>
+      <c r="N29" s="46"/>
+      <c r="O29" s="46"/>
+      <c r="P29" s="46"/>
+      <c r="Q29" s="46"/>
+      <c r="R29" s="46"/>
+      <c r="S29" s="46"/>
+      <c r="T29" s="46"/>
+      <c r="U29" s="47"/>
     </row>
     <row r="30" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F30" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="G30" s="74" t="s">
+      <c r="G30" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="H30" s="74"/>
-      <c r="I30" s="74"/>
-      <c r="J30" s="74"/>
-      <c r="K30" s="74"/>
-      <c r="L30" s="74"/>
-      <c r="M30" s="74"/>
-      <c r="N30" s="74"/>
-      <c r="O30" s="74"/>
-      <c r="P30" s="74"/>
-      <c r="Q30" s="74"/>
-      <c r="R30" s="74"/>
-      <c r="S30" s="74"/>
-      <c r="T30" s="74"/>
-      <c r="U30" s="75"/>
+      <c r="H30" s="46"/>
+      <c r="I30" s="46"/>
+      <c r="J30" s="46"/>
+      <c r="K30" s="46"/>
+      <c r="L30" s="46"/>
+      <c r="M30" s="46"/>
+      <c r="N30" s="46"/>
+      <c r="O30" s="46"/>
+      <c r="P30" s="46"/>
+      <c r="Q30" s="46"/>
+      <c r="R30" s="46"/>
+      <c r="S30" s="46"/>
+      <c r="T30" s="46"/>
+      <c r="U30" s="47"/>
     </row>
     <row r="31" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F31" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="G31" s="74" t="s">
+      <c r="G31" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="H31" s="74"/>
-      <c r="I31" s="74"/>
-      <c r="J31" s="74"/>
-      <c r="K31" s="74"/>
-      <c r="L31" s="74"/>
-      <c r="M31" s="74"/>
-      <c r="N31" s="74"/>
-      <c r="O31" s="74"/>
-      <c r="P31" s="74"/>
-      <c r="Q31" s="74"/>
-      <c r="R31" s="74"/>
-      <c r="S31" s="74"/>
-      <c r="T31" s="74"/>
-      <c r="U31" s="75"/>
+      <c r="H31" s="46"/>
+      <c r="I31" s="46"/>
+      <c r="J31" s="46"/>
+      <c r="K31" s="46"/>
+      <c r="L31" s="46"/>
+      <c r="M31" s="46"/>
+      <c r="N31" s="46"/>
+      <c r="O31" s="46"/>
+      <c r="P31" s="46"/>
+      <c r="Q31" s="46"/>
+      <c r="R31" s="46"/>
+      <c r="S31" s="46"/>
+      <c r="T31" s="46"/>
+      <c r="U31" s="47"/>
     </row>
     <row r="32" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F32" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="G32" s="74" t="s">
+      <c r="G32" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="H32" s="74"/>
-      <c r="I32" s="74"/>
-      <c r="J32" s="74"/>
-      <c r="K32" s="74"/>
-      <c r="L32" s="74"/>
-      <c r="M32" s="74"/>
-      <c r="N32" s="74"/>
-      <c r="O32" s="74"/>
-      <c r="P32" s="74"/>
-      <c r="Q32" s="74"/>
-      <c r="R32" s="74"/>
-      <c r="S32" s="74"/>
-      <c r="T32" s="74"/>
-      <c r="U32" s="75"/>
+      <c r="H32" s="46"/>
+      <c r="I32" s="46"/>
+      <c r="J32" s="46"/>
+      <c r="K32" s="46"/>
+      <c r="L32" s="46"/>
+      <c r="M32" s="46"/>
+      <c r="N32" s="46"/>
+      <c r="O32" s="46"/>
+      <c r="P32" s="46"/>
+      <c r="Q32" s="46"/>
+      <c r="R32" s="46"/>
+      <c r="S32" s="46"/>
+      <c r="T32" s="46"/>
+      <c r="U32" s="47"/>
     </row>
     <row r="33" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F33" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="G33" s="74" t="s">
+      <c r="G33" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="H33" s="74"/>
-      <c r="I33" s="74"/>
-      <c r="J33" s="74"/>
-      <c r="K33" s="74"/>
-      <c r="L33" s="74"/>
-      <c r="M33" s="74"/>
-      <c r="N33" s="74"/>
-      <c r="O33" s="74"/>
-      <c r="P33" s="74"/>
-      <c r="Q33" s="74"/>
-      <c r="R33" s="74"/>
-      <c r="S33" s="74"/>
-      <c r="T33" s="74"/>
-      <c r="U33" s="75"/>
+      <c r="H33" s="46"/>
+      <c r="I33" s="46"/>
+      <c r="J33" s="46"/>
+      <c r="K33" s="46"/>
+      <c r="L33" s="46"/>
+      <c r="M33" s="46"/>
+      <c r="N33" s="46"/>
+      <c r="O33" s="46"/>
+      <c r="P33" s="46"/>
+      <c r="Q33" s="46"/>
+      <c r="R33" s="46"/>
+      <c r="S33" s="46"/>
+      <c r="T33" s="46"/>
+      <c r="U33" s="47"/>
     </row>
     <row r="34" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F34" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="G34" s="76" t="s">
+      <c r="G34" s="70" t="s">
         <v>31</v>
       </c>
-      <c r="H34" s="76"/>
-      <c r="I34" s="76"/>
-      <c r="J34" s="76"/>
-      <c r="K34" s="76"/>
-      <c r="L34" s="76"/>
-      <c r="M34" s="76"/>
-      <c r="N34" s="76"/>
-      <c r="O34" s="76"/>
-      <c r="P34" s="76"/>
-      <c r="Q34" s="76"/>
-      <c r="R34" s="76"/>
-      <c r="S34" s="76"/>
-      <c r="T34" s="76"/>
-      <c r="U34" s="77"/>
+      <c r="H34" s="70"/>
+      <c r="I34" s="70"/>
+      <c r="J34" s="70"/>
+      <c r="K34" s="70"/>
+      <c r="L34" s="70"/>
+      <c r="M34" s="70"/>
+      <c r="N34" s="70"/>
+      <c r="O34" s="70"/>
+      <c r="P34" s="70"/>
+      <c r="Q34" s="70"/>
+      <c r="R34" s="70"/>
+      <c r="S34" s="70"/>
+      <c r="T34" s="70"/>
+      <c r="U34" s="71"/>
     </row>
     <row r="35" spans="6:21" x14ac:dyDescent="0.2">
       <c r="F35" s="32"/>
-      <c r="G35" s="80"/>
-      <c r="H35" s="80"/>
-      <c r="I35" s="80"/>
-      <c r="J35" s="80"/>
-      <c r="K35" s="80"/>
-      <c r="L35" s="80"/>
-      <c r="M35" s="80"/>
-      <c r="N35" s="80"/>
-      <c r="O35" s="80"/>
-      <c r="P35" s="80"/>
-      <c r="Q35" s="80"/>
-      <c r="R35" s="80"/>
-      <c r="S35" s="80"/>
-      <c r="T35" s="80"/>
-      <c r="U35" s="80"/>
+      <c r="G35" s="66"/>
+      <c r="H35" s="66"/>
+      <c r="I35" s="66"/>
+      <c r="J35" s="66"/>
+      <c r="K35" s="66"/>
+      <c r="L35" s="66"/>
+      <c r="M35" s="66"/>
+      <c r="N35" s="66"/>
+      <c r="O35" s="66"/>
+      <c r="P35" s="66"/>
+      <c r="Q35" s="66"/>
+      <c r="R35" s="66"/>
+      <c r="S35" s="66"/>
+      <c r="T35" s="66"/>
+      <c r="U35" s="66"/>
     </row>
     <row r="37" spans="6:21" x14ac:dyDescent="0.2">
       <c r="F37" s="32"/>
@@ -2682,68 +2682,68 @@
       <c r="U37" s="32"/>
     </row>
     <row r="38" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F38" s="87" t="s">
+      <c r="F38" s="56" t="s">
         <v>21</v>
       </c>
-      <c r="G38" s="88"/>
-      <c r="H38" s="88"/>
-      <c r="I38" s="88"/>
-      <c r="J38" s="88"/>
-      <c r="K38" s="88"/>
-      <c r="L38" s="88"/>
-      <c r="M38" s="88"/>
-      <c r="N38" s="88"/>
-      <c r="O38" s="88"/>
-      <c r="P38" s="88"/>
-      <c r="Q38" s="88"/>
-      <c r="R38" s="88"/>
-      <c r="S38" s="88"/>
-      <c r="T38" s="88"/>
-      <c r="U38" s="89"/>
+      <c r="G38" s="57"/>
+      <c r="H38" s="57"/>
+      <c r="I38" s="57"/>
+      <c r="J38" s="57"/>
+      <c r="K38" s="57"/>
+      <c r="L38" s="57"/>
+      <c r="M38" s="57"/>
+      <c r="N38" s="57"/>
+      <c r="O38" s="57"/>
+      <c r="P38" s="57"/>
+      <c r="Q38" s="57"/>
+      <c r="R38" s="57"/>
+      <c r="S38" s="57"/>
+      <c r="T38" s="57"/>
+      <c r="U38" s="58"/>
     </row>
     <row r="39" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F39" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="G39" s="72" t="s">
+      <c r="G39" s="59" t="s">
         <v>41</v>
       </c>
-      <c r="H39" s="72"/>
-      <c r="I39" s="72"/>
-      <c r="J39" s="72"/>
-      <c r="K39" s="72"/>
-      <c r="L39" s="72"/>
-      <c r="M39" s="72"/>
-      <c r="N39" s="72"/>
-      <c r="O39" s="72"/>
-      <c r="P39" s="72"/>
-      <c r="Q39" s="72"/>
-      <c r="R39" s="72"/>
-      <c r="S39" s="72"/>
-      <c r="T39" s="72"/>
-      <c r="U39" s="73"/>
+      <c r="H39" s="59"/>
+      <c r="I39" s="59"/>
+      <c r="J39" s="59"/>
+      <c r="K39" s="59"/>
+      <c r="L39" s="59"/>
+      <c r="M39" s="59"/>
+      <c r="N39" s="59"/>
+      <c r="O39" s="59"/>
+      <c r="P39" s="59"/>
+      <c r="Q39" s="59"/>
+      <c r="R39" s="59"/>
+      <c r="S39" s="59"/>
+      <c r="T39" s="59"/>
+      <c r="U39" s="60"/>
     </row>
     <row r="40" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F40" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="G40" s="72" t="s">
+      <c r="G40" s="59" t="s">
         <v>32</v>
       </c>
-      <c r="H40" s="72"/>
-      <c r="I40" s="72"/>
-      <c r="J40" s="72"/>
-      <c r="K40" s="72"/>
-      <c r="L40" s="72"/>
-      <c r="M40" s="72"/>
-      <c r="N40" s="72"/>
-      <c r="O40" s="72"/>
-      <c r="P40" s="72"/>
-      <c r="Q40" s="72"/>
-      <c r="R40" s="72"/>
-      <c r="S40" s="72"/>
-      <c r="T40" s="72"/>
-      <c r="U40" s="73"/>
+      <c r="H40" s="59"/>
+      <c r="I40" s="59"/>
+      <c r="J40" s="59"/>
+      <c r="K40" s="59"/>
+      <c r="L40" s="59"/>
+      <c r="M40" s="59"/>
+      <c r="N40" s="59"/>
+      <c r="O40" s="59"/>
+      <c r="P40" s="59"/>
+      <c r="Q40" s="59"/>
+      <c r="R40" s="59"/>
+      <c r="S40" s="59"/>
+      <c r="T40" s="59"/>
+      <c r="U40" s="60"/>
     </row>
     <row r="41" spans="6:21" x14ac:dyDescent="0.2">
       <c r="F41" s="41"/>
@@ -2767,189 +2767,216 @@
       <c r="F42" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="G42" s="72" t="s">
+      <c r="G42" s="59" t="s">
         <v>30</v>
       </c>
-      <c r="H42" s="72"/>
-      <c r="I42" s="72"/>
-      <c r="J42" s="72"/>
-      <c r="K42" s="72"/>
-      <c r="L42" s="72"/>
-      <c r="M42" s="72"/>
-      <c r="N42" s="72"/>
-      <c r="O42" s="72"/>
-      <c r="P42" s="72"/>
-      <c r="Q42" s="72"/>
-      <c r="R42" s="72"/>
-      <c r="S42" s="72"/>
-      <c r="T42" s="72"/>
-      <c r="U42" s="73"/>
+      <c r="H42" s="59"/>
+      <c r="I42" s="59"/>
+      <c r="J42" s="59"/>
+      <c r="K42" s="59"/>
+      <c r="L42" s="59"/>
+      <c r="M42" s="59"/>
+      <c r="N42" s="59"/>
+      <c r="O42" s="59"/>
+      <c r="P42" s="59"/>
+      <c r="Q42" s="59"/>
+      <c r="R42" s="59"/>
+      <c r="S42" s="59"/>
+      <c r="T42" s="59"/>
+      <c r="U42" s="60"/>
     </row>
     <row r="43" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F43" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="G43" s="90" t="s">
+      <c r="G43" s="44" t="s">
         <v>43</v>
       </c>
-      <c r="H43" s="90"/>
-      <c r="I43" s="90"/>
-      <c r="J43" s="90"/>
-      <c r="K43" s="90"/>
-      <c r="L43" s="90"/>
-      <c r="M43" s="90"/>
-      <c r="N43" s="90"/>
-      <c r="O43" s="90"/>
-      <c r="P43" s="90"/>
-      <c r="Q43" s="90"/>
-      <c r="R43" s="90"/>
-      <c r="S43" s="90"/>
-      <c r="T43" s="90"/>
-      <c r="U43" s="91"/>
+      <c r="H43" s="44"/>
+      <c r="I43" s="44"/>
+      <c r="J43" s="44"/>
+      <c r="K43" s="44"/>
+      <c r="L43" s="44"/>
+      <c r="M43" s="44"/>
+      <c r="N43" s="44"/>
+      <c r="O43" s="44"/>
+      <c r="P43" s="44"/>
+      <c r="Q43" s="44"/>
+      <c r="R43" s="44"/>
+      <c r="S43" s="44"/>
+      <c r="T43" s="44"/>
+      <c r="U43" s="45"/>
     </row>
     <row r="49" spans="5:25" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="M49" s="65" t="s">
+      <c r="M49" s="93" t="s">
         <v>50</v>
       </c>
-      <c r="N49" s="65"/>
-      <c r="O49" s="65"/>
+      <c r="N49" s="93"/>
+      <c r="O49" s="93"/>
     </row>
     <row r="51" spans="5:25" x14ac:dyDescent="0.2">
-      <c r="G51" s="56" t="s">
+      <c r="G51" s="84" t="s">
         <v>51</v>
       </c>
-      <c r="H51" s="57"/>
-      <c r="I51" s="58"/>
-      <c r="K51" s="56" t="s">
+      <c r="H51" s="85"/>
+      <c r="I51" s="86"/>
+      <c r="K51" s="84" t="s">
         <v>52</v>
       </c>
-      <c r="L51" s="57"/>
-      <c r="M51" s="58"/>
-      <c r="O51" s="56" t="s">
+      <c r="L51" s="85"/>
+      <c r="M51" s="86"/>
+      <c r="O51" s="84" t="s">
         <v>53</v>
       </c>
-      <c r="P51" s="57"/>
-      <c r="Q51" s="58"/>
-      <c r="S51" s="56" t="s">
+      <c r="P51" s="85"/>
+      <c r="Q51" s="86"/>
+      <c r="S51" s="84" t="s">
         <v>54</v>
       </c>
-      <c r="T51" s="57"/>
-      <c r="U51" s="58"/>
+      <c r="T51" s="85"/>
+      <c r="U51" s="86"/>
     </row>
     <row r="52" spans="5:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G52" s="59"/>
-      <c r="H52" s="60"/>
-      <c r="I52" s="61"/>
-      <c r="K52" s="59"/>
-      <c r="L52" s="60"/>
-      <c r="M52" s="61"/>
-      <c r="O52" s="59"/>
-      <c r="P52" s="60"/>
-      <c r="Q52" s="61"/>
-      <c r="S52" s="59"/>
-      <c r="T52" s="60"/>
-      <c r="U52" s="61"/>
+      <c r="G52" s="87"/>
+      <c r="H52" s="88"/>
+      <c r="I52" s="89"/>
+      <c r="K52" s="87"/>
+      <c r="L52" s="88"/>
+      <c r="M52" s="89"/>
+      <c r="O52" s="87"/>
+      <c r="P52" s="88"/>
+      <c r="Q52" s="89"/>
+      <c r="S52" s="87"/>
+      <c r="T52" s="88"/>
+      <c r="U52" s="89"/>
     </row>
     <row r="53" spans="5:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G53" s="62"/>
-      <c r="H53" s="63"/>
-      <c r="I53" s="64"/>
-      <c r="K53" s="62"/>
-      <c r="L53" s="63"/>
-      <c r="M53" s="64"/>
-      <c r="O53" s="62"/>
-      <c r="P53" s="63"/>
-      <c r="Q53" s="64"/>
-      <c r="S53" s="62"/>
-      <c r="T53" s="63"/>
-      <c r="U53" s="64"/>
+      <c r="G53" s="90"/>
+      <c r="H53" s="91"/>
+      <c r="I53" s="92"/>
+      <c r="K53" s="90"/>
+      <c r="L53" s="91"/>
+      <c r="M53" s="92"/>
+      <c r="O53" s="90"/>
+      <c r="P53" s="91"/>
+      <c r="Q53" s="92"/>
+      <c r="S53" s="90"/>
+      <c r="T53" s="91"/>
+      <c r="U53" s="92"/>
     </row>
     <row r="62" spans="5:25" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E62" s="65" t="s">
+      <c r="E62" s="93" t="s">
         <v>61</v>
       </c>
-      <c r="F62" s="65"/>
-      <c r="G62" s="65"/>
-      <c r="H62" s="65"/>
-      <c r="P62" s="65" t="s">
+      <c r="F62" s="93"/>
+      <c r="G62" s="93"/>
+      <c r="H62" s="93"/>
+      <c r="P62" s="93" t="s">
         <v>62</v>
       </c>
-      <c r="Q62" s="65"/>
-      <c r="R62" s="65"/>
-      <c r="S62" s="65"/>
-      <c r="V62" s="65" t="s">
+      <c r="Q62" s="93"/>
+      <c r="R62" s="93"/>
+      <c r="S62" s="93"/>
+      <c r="V62" s="93" t="s">
         <v>63</v>
       </c>
-      <c r="W62" s="65"/>
-      <c r="X62" s="65"/>
-      <c r="Y62" s="65"/>
+      <c r="W62" s="93"/>
+      <c r="X62" s="93"/>
+      <c r="Y62" s="93"/>
     </row>
     <row r="63" spans="5:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="66" spans="3:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C66" s="66" t="s">
+      <c r="C66" s="94" t="s">
         <v>57</v>
       </c>
-      <c r="D66" s="67"/>
-      <c r="F66" s="66" t="s">
+      <c r="D66" s="95"/>
+      <c r="F66" s="94" t="s">
         <v>57</v>
       </c>
-      <c r="G66" s="67"/>
-      <c r="I66" s="66" t="s">
+      <c r="G66" s="95"/>
+      <c r="I66" s="94" t="s">
         <v>57</v>
       </c>
-      <c r="J66" s="67"/>
-      <c r="N66" s="44" t="s">
+      <c r="J66" s="95"/>
+      <c r="N66" s="72" t="s">
         <v>57</v>
       </c>
-      <c r="O66" s="45"/>
-      <c r="Q66" s="44" t="s">
+      <c r="O66" s="73"/>
+      <c r="Q66" s="72" t="s">
         <v>57</v>
       </c>
-      <c r="R66" s="45"/>
-      <c r="T66" s="44" t="s">
+      <c r="R66" s="73"/>
+      <c r="T66" s="72" t="s">
         <v>56</v>
       </c>
-      <c r="U66" s="45"/>
-      <c r="W66" s="50" t="s">
+      <c r="U66" s="73"/>
+      <c r="W66" s="78" t="s">
         <v>55</v>
       </c>
-      <c r="X66" s="51"/>
+      <c r="X66" s="79"/>
     </row>
     <row r="67" spans="3:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C67" s="68"/>
-      <c r="D67" s="69"/>
-      <c r="F67" s="68"/>
-      <c r="G67" s="69"/>
-      <c r="I67" s="68"/>
-      <c r="J67" s="69"/>
-      <c r="N67" s="46"/>
-      <c r="O67" s="47"/>
-      <c r="Q67" s="46"/>
-      <c r="R67" s="47"/>
-      <c r="T67" s="46"/>
-      <c r="U67" s="47"/>
-      <c r="W67" s="52"/>
-      <c r="X67" s="53"/>
+      <c r="C67" s="96"/>
+      <c r="D67" s="97"/>
+      <c r="F67" s="96"/>
+      <c r="G67" s="97"/>
+      <c r="I67" s="96"/>
+      <c r="J67" s="97"/>
+      <c r="N67" s="74"/>
+      <c r="O67" s="75"/>
+      <c r="Q67" s="74"/>
+      <c r="R67" s="75"/>
+      <c r="T67" s="74"/>
+      <c r="U67" s="75"/>
+      <c r="W67" s="80"/>
+      <c r="X67" s="81"/>
     </row>
     <row r="68" spans="3:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C68" s="70"/>
-      <c r="D68" s="71"/>
-      <c r="F68" s="70"/>
-      <c r="G68" s="71"/>
-      <c r="I68" s="70"/>
-      <c r="J68" s="71"/>
-      <c r="N68" s="48"/>
-      <c r="O68" s="49"/>
-      <c r="Q68" s="48"/>
-      <c r="R68" s="49"/>
-      <c r="T68" s="48"/>
-      <c r="U68" s="49"/>
-      <c r="W68" s="54"/>
-      <c r="X68" s="55"/>
+      <c r="C68" s="98"/>
+      <c r="D68" s="99"/>
+      <c r="F68" s="98"/>
+      <c r="G68" s="99"/>
+      <c r="I68" s="98"/>
+      <c r="J68" s="99"/>
+      <c r="N68" s="76"/>
+      <c r="O68" s="77"/>
+      <c r="Q68" s="76"/>
+      <c r="R68" s="77"/>
+      <c r="T68" s="76"/>
+      <c r="U68" s="77"/>
+      <c r="W68" s="82"/>
+      <c r="X68" s="83"/>
     </row>
     <row r="69" spans="3:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="43">
+    <mergeCell ref="T66:U68"/>
+    <mergeCell ref="W66:X68"/>
+    <mergeCell ref="S51:U53"/>
+    <mergeCell ref="M49:O49"/>
+    <mergeCell ref="C66:D68"/>
+    <mergeCell ref="F66:G68"/>
+    <mergeCell ref="I66:J68"/>
+    <mergeCell ref="N66:O68"/>
+    <mergeCell ref="Q66:R68"/>
+    <mergeCell ref="G51:I53"/>
+    <mergeCell ref="K51:M53"/>
+    <mergeCell ref="O51:Q53"/>
+    <mergeCell ref="E62:H62"/>
+    <mergeCell ref="P62:S62"/>
+    <mergeCell ref="V62:Y62"/>
+    <mergeCell ref="G39:U39"/>
+    <mergeCell ref="G40:U40"/>
+    <mergeCell ref="G30:U30"/>
+    <mergeCell ref="G31:U31"/>
+    <mergeCell ref="G32:U32"/>
+    <mergeCell ref="G33:U33"/>
+    <mergeCell ref="G34:U34"/>
+    <mergeCell ref="G24:U24"/>
+    <mergeCell ref="G35:U35"/>
+    <mergeCell ref="F17:U17"/>
+    <mergeCell ref="F28:U28"/>
+    <mergeCell ref="F38:U38"/>
     <mergeCell ref="G43:U43"/>
     <mergeCell ref="G29:U29"/>
     <mergeCell ref="F2:U2"/>
@@ -2966,33 +2993,6 @@
     <mergeCell ref="G15:U15"/>
     <mergeCell ref="G42:U42"/>
     <mergeCell ref="F23:U23"/>
-    <mergeCell ref="G24:U24"/>
-    <mergeCell ref="G35:U35"/>
-    <mergeCell ref="F17:U17"/>
-    <mergeCell ref="F28:U28"/>
-    <mergeCell ref="F38:U38"/>
-    <mergeCell ref="G39:U39"/>
-    <mergeCell ref="G40:U40"/>
-    <mergeCell ref="G30:U30"/>
-    <mergeCell ref="G31:U31"/>
-    <mergeCell ref="G32:U32"/>
-    <mergeCell ref="G33:U33"/>
-    <mergeCell ref="G34:U34"/>
-    <mergeCell ref="T66:U68"/>
-    <mergeCell ref="W66:X68"/>
-    <mergeCell ref="S51:U53"/>
-    <mergeCell ref="M49:O49"/>
-    <mergeCell ref="C66:D68"/>
-    <mergeCell ref="F66:G68"/>
-    <mergeCell ref="I66:J68"/>
-    <mergeCell ref="N66:O68"/>
-    <mergeCell ref="Q66:R68"/>
-    <mergeCell ref="G51:I53"/>
-    <mergeCell ref="K51:M53"/>
-    <mergeCell ref="O51:Q53"/>
-    <mergeCell ref="E62:H62"/>
-    <mergeCell ref="P62:S62"/>
-    <mergeCell ref="V62:Y62"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3587,7 +3587,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="F1:S21"/>
   <sheetViews>
-    <sheetView rightToLeft="1" topLeftCell="B1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="B1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="S3" sqref="S3"/>
     </sheetView>
@@ -3687,7 +3687,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="E2:M20"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView rightToLeft="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
@@ -3940,6 +3940,14 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="F15:H15"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="F18:H18"/>
     <mergeCell ref="F12:H12"/>
     <mergeCell ref="E2:M2"/>
     <mergeCell ref="E4:E5"/>
@@ -3952,14 +3960,6 @@
     <mergeCell ref="F9:H9"/>
     <mergeCell ref="F10:H10"/>
     <mergeCell ref="F11:H11"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="F14:H14"/>
-    <mergeCell ref="F15:H15"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="F18:H18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="53" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
fix escorts totals bug, add families totals
</commit_message>
<xml_diff>
--- a/cockpit_template.xlsx
+++ b/cockpit_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Roi.Dital/roid_playground/paamonim/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{396250F9-7E74-214F-B58F-7A8F37B3D5B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D0E34EE-9AFE-024C-9268-CAD46F4E0205}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="19440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="19440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="רציונל" sheetId="3" r:id="rId1"/>
@@ -22,7 +22,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="2">מלווים!$D$2:$I$47</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="4">מסרים!$E$1:$M$49</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">ראשי!$E$1:$N$63</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">ראשי!$E$1:$M$63</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="73">
   <si>
     <t>#</t>
   </si>
@@ -69,9 +69,6 @@
   </si>
   <si>
     <t>סטטוס</t>
-  </si>
-  <si>
-    <t>הסתיים</t>
   </si>
   <si>
     <t>רש"צים</t>
@@ -840,18 +837,150 @@
     <xf numFmtId="0" fontId="15" fillId="12" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="2"/>
     </xf>
@@ -875,138 +1004,6 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1998,24 +1995,24 @@
   <sheetData>
     <row r="1" spans="6:21" ht="20" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F2" s="48" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" s="48"/>
-      <c r="H2" s="48"/>
-      <c r="I2" s="48"/>
-      <c r="J2" s="48"/>
-      <c r="K2" s="48"/>
-      <c r="L2" s="48"/>
-      <c r="M2" s="48"/>
-      <c r="N2" s="48"/>
-      <c r="O2" s="48"/>
-      <c r="P2" s="48"/>
-      <c r="Q2" s="48"/>
-      <c r="R2" s="48"/>
-      <c r="S2" s="48"/>
-      <c r="T2" s="48"/>
-      <c r="U2" s="48"/>
+      <c r="F2" s="92" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="92"/>
+      <c r="H2" s="92"/>
+      <c r="I2" s="92"/>
+      <c r="J2" s="92"/>
+      <c r="K2" s="92"/>
+      <c r="L2" s="92"/>
+      <c r="M2" s="92"/>
+      <c r="N2" s="92"/>
+      <c r="O2" s="92"/>
+      <c r="P2" s="92"/>
+      <c r="Q2" s="92"/>
+      <c r="R2" s="92"/>
+      <c r="S2" s="92"/>
+      <c r="T2" s="92"/>
+      <c r="U2" s="92"/>
     </row>
     <row r="3" spans="6:21" x14ac:dyDescent="0.2">
       <c r="F3" s="30"/>
@@ -2036,68 +2033,68 @@
       <c r="U3" s="30"/>
     </row>
     <row r="4" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F4" s="56" t="s">
-        <v>23</v>
-      </c>
-      <c r="G4" s="57"/>
-      <c r="H4" s="57"/>
-      <c r="I4" s="57"/>
-      <c r="J4" s="57"/>
-      <c r="K4" s="57"/>
-      <c r="L4" s="57"/>
-      <c r="M4" s="57"/>
-      <c r="N4" s="57"/>
-      <c r="O4" s="57"/>
-      <c r="P4" s="57"/>
-      <c r="Q4" s="57"/>
-      <c r="R4" s="57"/>
-      <c r="S4" s="57"/>
-      <c r="T4" s="57"/>
-      <c r="U4" s="58"/>
+      <c r="F4" s="87" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="88"/>
+      <c r="H4" s="88"/>
+      <c r="I4" s="88"/>
+      <c r="J4" s="88"/>
+      <c r="K4" s="88"/>
+      <c r="L4" s="88"/>
+      <c r="M4" s="88"/>
+      <c r="N4" s="88"/>
+      <c r="O4" s="88"/>
+      <c r="P4" s="88"/>
+      <c r="Q4" s="88"/>
+      <c r="R4" s="88"/>
+      <c r="S4" s="88"/>
+      <c r="T4" s="88"/>
+      <c r="U4" s="89"/>
     </row>
     <row r="5" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F5" s="35" t="s">
-        <v>20</v>
-      </c>
-      <c r="G5" s="59" t="s">
-        <v>40</v>
-      </c>
-      <c r="H5" s="59"/>
-      <c r="I5" s="59"/>
-      <c r="J5" s="59"/>
-      <c r="K5" s="59"/>
-      <c r="L5" s="59"/>
-      <c r="M5" s="59"/>
-      <c r="N5" s="59"/>
-      <c r="O5" s="59"/>
-      <c r="P5" s="59"/>
-      <c r="Q5" s="59"/>
-      <c r="R5" s="59"/>
-      <c r="S5" s="59"/>
-      <c r="T5" s="59"/>
-      <c r="U5" s="60"/>
+        <v>19</v>
+      </c>
+      <c r="G5" s="72" t="s">
+        <v>39</v>
+      </c>
+      <c r="H5" s="72"/>
+      <c r="I5" s="72"/>
+      <c r="J5" s="72"/>
+      <c r="K5" s="72"/>
+      <c r="L5" s="72"/>
+      <c r="M5" s="72"/>
+      <c r="N5" s="72"/>
+      <c r="O5" s="72"/>
+      <c r="P5" s="72"/>
+      <c r="Q5" s="72"/>
+      <c r="R5" s="72"/>
+      <c r="S5" s="72"/>
+      <c r="T5" s="72"/>
+      <c r="U5" s="73"/>
     </row>
     <row r="6" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F6" s="38" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" s="44" t="s">
-        <v>42</v>
-      </c>
-      <c r="H6" s="44"/>
-      <c r="I6" s="44"/>
-      <c r="J6" s="44"/>
-      <c r="K6" s="44"/>
-      <c r="L6" s="44"/>
-      <c r="M6" s="44"/>
-      <c r="N6" s="44"/>
-      <c r="O6" s="44"/>
-      <c r="P6" s="44"/>
-      <c r="Q6" s="44"/>
-      <c r="R6" s="44"/>
-      <c r="S6" s="44"/>
-      <c r="T6" s="44"/>
-      <c r="U6" s="45"/>
+        <v>19</v>
+      </c>
+      <c r="G6" s="90" t="s">
+        <v>41</v>
+      </c>
+      <c r="H6" s="90"/>
+      <c r="I6" s="90"/>
+      <c r="J6" s="90"/>
+      <c r="K6" s="90"/>
+      <c r="L6" s="90"/>
+      <c r="M6" s="90"/>
+      <c r="N6" s="90"/>
+      <c r="O6" s="90"/>
+      <c r="P6" s="90"/>
+      <c r="Q6" s="90"/>
+      <c r="R6" s="90"/>
+      <c r="S6" s="90"/>
+      <c r="T6" s="90"/>
+      <c r="U6" s="91"/>
     </row>
     <row r="7" spans="6:21" x14ac:dyDescent="0.2">
       <c r="F7" s="31"/>
@@ -2118,46 +2115,46 @@
       <c r="U7" s="31"/>
     </row>
     <row r="8" spans="6:21" ht="26" x14ac:dyDescent="0.2">
-      <c r="F8" s="49" t="s">
-        <v>19</v>
-      </c>
-      <c r="G8" s="50"/>
-      <c r="H8" s="50"/>
-      <c r="I8" s="50"/>
-      <c r="J8" s="50"/>
-      <c r="K8" s="50"/>
-      <c r="L8" s="50"/>
-      <c r="M8" s="50"/>
-      <c r="N8" s="50"/>
-      <c r="O8" s="50"/>
-      <c r="P8" s="50"/>
-      <c r="Q8" s="50"/>
-      <c r="R8" s="50"/>
-      <c r="S8" s="50"/>
-      <c r="T8" s="50"/>
-      <c r="U8" s="51"/>
+      <c r="F8" s="93" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" s="94"/>
+      <c r="H8" s="94"/>
+      <c r="I8" s="94"/>
+      <c r="J8" s="94"/>
+      <c r="K8" s="94"/>
+      <c r="L8" s="94"/>
+      <c r="M8" s="94"/>
+      <c r="N8" s="94"/>
+      <c r="O8" s="94"/>
+      <c r="P8" s="94"/>
+      <c r="Q8" s="94"/>
+      <c r="R8" s="94"/>
+      <c r="S8" s="94"/>
+      <c r="T8" s="94"/>
+      <c r="U8" s="95"/>
     </row>
     <row r="9" spans="6:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F9" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="G9" s="52" t="s">
-        <v>60</v>
-      </c>
-      <c r="H9" s="52"/>
-      <c r="I9" s="52"/>
-      <c r="J9" s="52"/>
-      <c r="K9" s="52"/>
-      <c r="L9" s="52"/>
-      <c r="M9" s="52"/>
-      <c r="N9" s="52"/>
-      <c r="O9" s="52"/>
-      <c r="P9" s="52"/>
-      <c r="Q9" s="52"/>
-      <c r="R9" s="52"/>
-      <c r="S9" s="52"/>
-      <c r="T9" s="52"/>
-      <c r="U9" s="53"/>
+        <v>19</v>
+      </c>
+      <c r="G9" s="96" t="s">
+        <v>59</v>
+      </c>
+      <c r="H9" s="96"/>
+      <c r="I9" s="96"/>
+      <c r="J9" s="96"/>
+      <c r="K9" s="96"/>
+      <c r="L9" s="96"/>
+      <c r="M9" s="96"/>
+      <c r="N9" s="96"/>
+      <c r="O9" s="96"/>
+      <c r="P9" s="96"/>
+      <c r="Q9" s="96"/>
+      <c r="R9" s="96"/>
+      <c r="S9" s="96"/>
+      <c r="T9" s="96"/>
+      <c r="U9" s="97"/>
     </row>
     <row r="10" spans="6:21" x14ac:dyDescent="0.2">
       <c r="F10" s="32"/>
@@ -2196,68 +2193,68 @@
       <c r="U12" s="32"/>
     </row>
     <row r="13" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F13" s="56" t="s">
-        <v>58</v>
-      </c>
-      <c r="G13" s="57"/>
-      <c r="H13" s="57"/>
-      <c r="I13" s="57"/>
-      <c r="J13" s="57"/>
-      <c r="K13" s="57"/>
-      <c r="L13" s="57"/>
-      <c r="M13" s="57"/>
-      <c r="N13" s="57"/>
-      <c r="O13" s="57"/>
-      <c r="P13" s="57"/>
-      <c r="Q13" s="57"/>
-      <c r="R13" s="57"/>
-      <c r="S13" s="57"/>
-      <c r="T13" s="57"/>
-      <c r="U13" s="58"/>
+      <c r="F13" s="87" t="s">
+        <v>57</v>
+      </c>
+      <c r="G13" s="88"/>
+      <c r="H13" s="88"/>
+      <c r="I13" s="88"/>
+      <c r="J13" s="88"/>
+      <c r="K13" s="88"/>
+      <c r="L13" s="88"/>
+      <c r="M13" s="88"/>
+      <c r="N13" s="88"/>
+      <c r="O13" s="88"/>
+      <c r="P13" s="88"/>
+      <c r="Q13" s="88"/>
+      <c r="R13" s="88"/>
+      <c r="S13" s="88"/>
+      <c r="T13" s="88"/>
+      <c r="U13" s="89"/>
     </row>
     <row r="14" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F14" s="35" t="s">
-        <v>20</v>
-      </c>
-      <c r="G14" s="54" t="s">
-        <v>44</v>
-      </c>
-      <c r="H14" s="54"/>
-      <c r="I14" s="54"/>
-      <c r="J14" s="54"/>
-      <c r="K14" s="54"/>
-      <c r="L14" s="54"/>
-      <c r="M14" s="54"/>
-      <c r="N14" s="54"/>
-      <c r="O14" s="54"/>
-      <c r="P14" s="54"/>
-      <c r="Q14" s="54"/>
-      <c r="R14" s="54"/>
-      <c r="S14" s="54"/>
-      <c r="T14" s="54"/>
-      <c r="U14" s="55"/>
+        <v>19</v>
+      </c>
+      <c r="G14" s="98" t="s">
+        <v>43</v>
+      </c>
+      <c r="H14" s="98"/>
+      <c r="I14" s="98"/>
+      <c r="J14" s="98"/>
+      <c r="K14" s="98"/>
+      <c r="L14" s="98"/>
+      <c r="M14" s="98"/>
+      <c r="N14" s="98"/>
+      <c r="O14" s="98"/>
+      <c r="P14" s="98"/>
+      <c r="Q14" s="98"/>
+      <c r="R14" s="98"/>
+      <c r="S14" s="98"/>
+      <c r="T14" s="98"/>
+      <c r="U14" s="99"/>
     </row>
     <row r="15" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F15" s="35" t="s">
-        <v>20</v>
-      </c>
-      <c r="G15" s="54" t="s">
-        <v>49</v>
-      </c>
-      <c r="H15" s="54"/>
-      <c r="I15" s="54"/>
-      <c r="J15" s="54"/>
-      <c r="K15" s="54"/>
-      <c r="L15" s="54"/>
-      <c r="M15" s="54"/>
-      <c r="N15" s="54"/>
-      <c r="O15" s="54"/>
-      <c r="P15" s="54"/>
-      <c r="Q15" s="54"/>
-      <c r="R15" s="54"/>
-      <c r="S15" s="54"/>
-      <c r="T15" s="54"/>
-      <c r="U15" s="55"/>
+        <v>19</v>
+      </c>
+      <c r="G15" s="98" t="s">
+        <v>48</v>
+      </c>
+      <c r="H15" s="98"/>
+      <c r="I15" s="98"/>
+      <c r="J15" s="98"/>
+      <c r="K15" s="98"/>
+      <c r="L15" s="98"/>
+      <c r="M15" s="98"/>
+      <c r="N15" s="98"/>
+      <c r="O15" s="98"/>
+      <c r="P15" s="98"/>
+      <c r="Q15" s="98"/>
+      <c r="R15" s="98"/>
+      <c r="S15" s="98"/>
+      <c r="T15" s="98"/>
+      <c r="U15" s="99"/>
     </row>
     <row r="16" spans="6:21" x14ac:dyDescent="0.2">
       <c r="F16" s="36"/>
@@ -2278,46 +2275,46 @@
       <c r="U16" s="37"/>
     </row>
     <row r="17" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F17" s="61" t="s">
-        <v>16</v>
-      </c>
-      <c r="G17" s="62"/>
-      <c r="H17" s="62"/>
-      <c r="I17" s="62"/>
-      <c r="J17" s="62"/>
-      <c r="K17" s="62"/>
-      <c r="L17" s="62"/>
-      <c r="M17" s="62"/>
-      <c r="N17" s="62"/>
-      <c r="O17" s="62"/>
-      <c r="P17" s="62"/>
-      <c r="Q17" s="62"/>
-      <c r="R17" s="62"/>
-      <c r="S17" s="62"/>
-      <c r="T17" s="62"/>
-      <c r="U17" s="63"/>
+      <c r="F17" s="81" t="s">
+        <v>15</v>
+      </c>
+      <c r="G17" s="82"/>
+      <c r="H17" s="82"/>
+      <c r="I17" s="82"/>
+      <c r="J17" s="82"/>
+      <c r="K17" s="82"/>
+      <c r="L17" s="82"/>
+      <c r="M17" s="82"/>
+      <c r="N17" s="82"/>
+      <c r="O17" s="82"/>
+      <c r="P17" s="82"/>
+      <c r="Q17" s="82"/>
+      <c r="R17" s="82"/>
+      <c r="S17" s="82"/>
+      <c r="T17" s="82"/>
+      <c r="U17" s="83"/>
     </row>
     <row r="18" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F18" s="35" t="s">
-        <v>20</v>
-      </c>
-      <c r="G18" s="54" t="s">
-        <v>48</v>
-      </c>
-      <c r="H18" s="54"/>
-      <c r="I18" s="54"/>
-      <c r="J18" s="54"/>
-      <c r="K18" s="54"/>
-      <c r="L18" s="54"/>
-      <c r="M18" s="54"/>
-      <c r="N18" s="54"/>
-      <c r="O18" s="54"/>
-      <c r="P18" s="54"/>
-      <c r="Q18" s="54"/>
-      <c r="R18" s="54"/>
-      <c r="S18" s="54"/>
-      <c r="T18" s="54"/>
-      <c r="U18" s="55"/>
+        <v>19</v>
+      </c>
+      <c r="G18" s="98" t="s">
+        <v>47</v>
+      </c>
+      <c r="H18" s="98"/>
+      <c r="I18" s="98"/>
+      <c r="J18" s="98"/>
+      <c r="K18" s="98"/>
+      <c r="L18" s="98"/>
+      <c r="M18" s="98"/>
+      <c r="N18" s="98"/>
+      <c r="O18" s="98"/>
+      <c r="P18" s="98"/>
+      <c r="Q18" s="98"/>
+      <c r="R18" s="98"/>
+      <c r="S18" s="98"/>
+      <c r="T18" s="98"/>
+      <c r="U18" s="99"/>
     </row>
     <row r="19" spans="6:21" x14ac:dyDescent="0.2">
       <c r="F19" s="36"/>
@@ -2338,46 +2335,46 @@
       <c r="U19" s="37"/>
     </row>
     <row r="20" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F20" s="61" t="s">
-        <v>45</v>
-      </c>
-      <c r="G20" s="62"/>
-      <c r="H20" s="62"/>
-      <c r="I20" s="62"/>
-      <c r="J20" s="62"/>
-      <c r="K20" s="62"/>
-      <c r="L20" s="62"/>
-      <c r="M20" s="62"/>
-      <c r="N20" s="62"/>
-      <c r="O20" s="62"/>
-      <c r="P20" s="62"/>
-      <c r="Q20" s="62"/>
-      <c r="R20" s="62"/>
-      <c r="S20" s="62"/>
-      <c r="T20" s="62"/>
-      <c r="U20" s="63"/>
+      <c r="F20" s="81" t="s">
+        <v>44</v>
+      </c>
+      <c r="G20" s="82"/>
+      <c r="H20" s="82"/>
+      <c r="I20" s="82"/>
+      <c r="J20" s="82"/>
+      <c r="K20" s="82"/>
+      <c r="L20" s="82"/>
+      <c r="M20" s="82"/>
+      <c r="N20" s="82"/>
+      <c r="O20" s="82"/>
+      <c r="P20" s="82"/>
+      <c r="Q20" s="82"/>
+      <c r="R20" s="82"/>
+      <c r="S20" s="82"/>
+      <c r="T20" s="82"/>
+      <c r="U20" s="83"/>
     </row>
     <row r="21" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F21" s="35" t="s">
-        <v>20</v>
-      </c>
-      <c r="G21" s="54" t="s">
-        <v>59</v>
-      </c>
-      <c r="H21" s="54"/>
-      <c r="I21" s="54"/>
-      <c r="J21" s="54"/>
-      <c r="K21" s="54"/>
-      <c r="L21" s="54"/>
-      <c r="M21" s="54"/>
-      <c r="N21" s="54"/>
-      <c r="O21" s="54"/>
-      <c r="P21" s="54"/>
-      <c r="Q21" s="54"/>
-      <c r="R21" s="54"/>
-      <c r="S21" s="54"/>
-      <c r="T21" s="54"/>
-      <c r="U21" s="55"/>
+        <v>19</v>
+      </c>
+      <c r="G21" s="98" t="s">
+        <v>58</v>
+      </c>
+      <c r="H21" s="98"/>
+      <c r="I21" s="98"/>
+      <c r="J21" s="98"/>
+      <c r="K21" s="98"/>
+      <c r="L21" s="98"/>
+      <c r="M21" s="98"/>
+      <c r="N21" s="98"/>
+      <c r="O21" s="98"/>
+      <c r="P21" s="98"/>
+      <c r="Q21" s="98"/>
+      <c r="R21" s="98"/>
+      <c r="S21" s="98"/>
+      <c r="T21" s="98"/>
+      <c r="U21" s="99"/>
     </row>
     <row r="22" spans="6:21" x14ac:dyDescent="0.2">
       <c r="F22" s="36"/>
@@ -2398,46 +2395,46 @@
       <c r="U22" s="37"/>
     </row>
     <row r="23" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F23" s="61" t="s">
-        <v>46</v>
-      </c>
-      <c r="G23" s="62"/>
-      <c r="H23" s="62"/>
-      <c r="I23" s="62"/>
-      <c r="J23" s="62"/>
-      <c r="K23" s="62"/>
-      <c r="L23" s="62"/>
-      <c r="M23" s="62"/>
-      <c r="N23" s="62"/>
-      <c r="O23" s="62"/>
-      <c r="P23" s="62"/>
-      <c r="Q23" s="62"/>
-      <c r="R23" s="62"/>
-      <c r="S23" s="62"/>
-      <c r="T23" s="62"/>
-      <c r="U23" s="63"/>
+      <c r="F23" s="81" t="s">
+        <v>45</v>
+      </c>
+      <c r="G23" s="82"/>
+      <c r="H23" s="82"/>
+      <c r="I23" s="82"/>
+      <c r="J23" s="82"/>
+      <c r="K23" s="82"/>
+      <c r="L23" s="82"/>
+      <c r="M23" s="82"/>
+      <c r="N23" s="82"/>
+      <c r="O23" s="82"/>
+      <c r="P23" s="82"/>
+      <c r="Q23" s="82"/>
+      <c r="R23" s="82"/>
+      <c r="S23" s="82"/>
+      <c r="T23" s="82"/>
+      <c r="U23" s="83"/>
     </row>
     <row r="24" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F24" s="38" t="s">
-        <v>20</v>
-      </c>
-      <c r="G24" s="64" t="s">
-        <v>47</v>
-      </c>
-      <c r="H24" s="64"/>
-      <c r="I24" s="64"/>
-      <c r="J24" s="64"/>
-      <c r="K24" s="64"/>
-      <c r="L24" s="64"/>
-      <c r="M24" s="64"/>
-      <c r="N24" s="64"/>
-      <c r="O24" s="64"/>
-      <c r="P24" s="64"/>
-      <c r="Q24" s="64"/>
-      <c r="R24" s="64"/>
-      <c r="S24" s="64"/>
-      <c r="T24" s="64"/>
-      <c r="U24" s="65"/>
+        <v>19</v>
+      </c>
+      <c r="G24" s="78" t="s">
+        <v>46</v>
+      </c>
+      <c r="H24" s="78"/>
+      <c r="I24" s="78"/>
+      <c r="J24" s="78"/>
+      <c r="K24" s="78"/>
+      <c r="L24" s="78"/>
+      <c r="M24" s="78"/>
+      <c r="N24" s="78"/>
+      <c r="O24" s="78"/>
+      <c r="P24" s="78"/>
+      <c r="Q24" s="78"/>
+      <c r="R24" s="78"/>
+      <c r="S24" s="78"/>
+      <c r="T24" s="78"/>
+      <c r="U24" s="79"/>
     </row>
     <row r="25" spans="6:21" x14ac:dyDescent="0.2">
       <c r="F25" s="32"/>
@@ -2494,174 +2491,174 @@
       <c r="U27" s="32"/>
     </row>
     <row r="28" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F28" s="67" t="s">
-        <v>17</v>
-      </c>
-      <c r="G28" s="68"/>
-      <c r="H28" s="68"/>
-      <c r="I28" s="68"/>
-      <c r="J28" s="68"/>
-      <c r="K28" s="68"/>
-      <c r="L28" s="68"/>
-      <c r="M28" s="68"/>
-      <c r="N28" s="68"/>
-      <c r="O28" s="68"/>
-      <c r="P28" s="68"/>
-      <c r="Q28" s="68"/>
-      <c r="R28" s="68"/>
-      <c r="S28" s="68"/>
-      <c r="T28" s="68"/>
-      <c r="U28" s="69"/>
+      <c r="F28" s="84" t="s">
+        <v>16</v>
+      </c>
+      <c r="G28" s="85"/>
+      <c r="H28" s="85"/>
+      <c r="I28" s="85"/>
+      <c r="J28" s="85"/>
+      <c r="K28" s="85"/>
+      <c r="L28" s="85"/>
+      <c r="M28" s="85"/>
+      <c r="N28" s="85"/>
+      <c r="O28" s="85"/>
+      <c r="P28" s="85"/>
+      <c r="Q28" s="85"/>
+      <c r="R28" s="85"/>
+      <c r="S28" s="85"/>
+      <c r="T28" s="85"/>
+      <c r="U28" s="86"/>
     </row>
     <row r="29" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F29" s="39" t="s">
-        <v>20</v>
-      </c>
-      <c r="G29" s="46" t="s">
-        <v>26</v>
-      </c>
-      <c r="H29" s="46"/>
-      <c r="I29" s="46"/>
-      <c r="J29" s="46"/>
-      <c r="K29" s="46"/>
-      <c r="L29" s="46"/>
-      <c r="M29" s="46"/>
-      <c r="N29" s="46"/>
-      <c r="O29" s="46"/>
-      <c r="P29" s="46"/>
-      <c r="Q29" s="46"/>
-      <c r="R29" s="46"/>
-      <c r="S29" s="46"/>
-      <c r="T29" s="46"/>
-      <c r="U29" s="47"/>
+        <v>19</v>
+      </c>
+      <c r="G29" s="74" t="s">
+        <v>25</v>
+      </c>
+      <c r="H29" s="74"/>
+      <c r="I29" s="74"/>
+      <c r="J29" s="74"/>
+      <c r="K29" s="74"/>
+      <c r="L29" s="74"/>
+      <c r="M29" s="74"/>
+      <c r="N29" s="74"/>
+      <c r="O29" s="74"/>
+      <c r="P29" s="74"/>
+      <c r="Q29" s="74"/>
+      <c r="R29" s="74"/>
+      <c r="S29" s="74"/>
+      <c r="T29" s="74"/>
+      <c r="U29" s="75"/>
     </row>
     <row r="30" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F30" s="39" t="s">
-        <v>20</v>
-      </c>
-      <c r="G30" s="46" t="s">
-        <v>22</v>
-      </c>
-      <c r="H30" s="46"/>
-      <c r="I30" s="46"/>
-      <c r="J30" s="46"/>
-      <c r="K30" s="46"/>
-      <c r="L30" s="46"/>
-      <c r="M30" s="46"/>
-      <c r="N30" s="46"/>
-      <c r="O30" s="46"/>
-      <c r="P30" s="46"/>
-      <c r="Q30" s="46"/>
-      <c r="R30" s="46"/>
-      <c r="S30" s="46"/>
-      <c r="T30" s="46"/>
-      <c r="U30" s="47"/>
+        <v>19</v>
+      </c>
+      <c r="G30" s="74" t="s">
+        <v>21</v>
+      </c>
+      <c r="H30" s="74"/>
+      <c r="I30" s="74"/>
+      <c r="J30" s="74"/>
+      <c r="K30" s="74"/>
+      <c r="L30" s="74"/>
+      <c r="M30" s="74"/>
+      <c r="N30" s="74"/>
+      <c r="O30" s="74"/>
+      <c r="P30" s="74"/>
+      <c r="Q30" s="74"/>
+      <c r="R30" s="74"/>
+      <c r="S30" s="74"/>
+      <c r="T30" s="74"/>
+      <c r="U30" s="75"/>
     </row>
     <row r="31" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F31" s="39" t="s">
-        <v>20</v>
-      </c>
-      <c r="G31" s="46" t="s">
-        <v>27</v>
-      </c>
-      <c r="H31" s="46"/>
-      <c r="I31" s="46"/>
-      <c r="J31" s="46"/>
-      <c r="K31" s="46"/>
-      <c r="L31" s="46"/>
-      <c r="M31" s="46"/>
-      <c r="N31" s="46"/>
-      <c r="O31" s="46"/>
-      <c r="P31" s="46"/>
-      <c r="Q31" s="46"/>
-      <c r="R31" s="46"/>
-      <c r="S31" s="46"/>
-      <c r="T31" s="46"/>
-      <c r="U31" s="47"/>
+        <v>19</v>
+      </c>
+      <c r="G31" s="74" t="s">
+        <v>26</v>
+      </c>
+      <c r="H31" s="74"/>
+      <c r="I31" s="74"/>
+      <c r="J31" s="74"/>
+      <c r="K31" s="74"/>
+      <c r="L31" s="74"/>
+      <c r="M31" s="74"/>
+      <c r="N31" s="74"/>
+      <c r="O31" s="74"/>
+      <c r="P31" s="74"/>
+      <c r="Q31" s="74"/>
+      <c r="R31" s="74"/>
+      <c r="S31" s="74"/>
+      <c r="T31" s="74"/>
+      <c r="U31" s="75"/>
     </row>
     <row r="32" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F32" s="39" t="s">
-        <v>20</v>
-      </c>
-      <c r="G32" s="46" t="s">
-        <v>29</v>
-      </c>
-      <c r="H32" s="46"/>
-      <c r="I32" s="46"/>
-      <c r="J32" s="46"/>
-      <c r="K32" s="46"/>
-      <c r="L32" s="46"/>
-      <c r="M32" s="46"/>
-      <c r="N32" s="46"/>
-      <c r="O32" s="46"/>
-      <c r="P32" s="46"/>
-      <c r="Q32" s="46"/>
-      <c r="R32" s="46"/>
-      <c r="S32" s="46"/>
-      <c r="T32" s="46"/>
-      <c r="U32" s="47"/>
+        <v>19</v>
+      </c>
+      <c r="G32" s="74" t="s">
+        <v>28</v>
+      </c>
+      <c r="H32" s="74"/>
+      <c r="I32" s="74"/>
+      <c r="J32" s="74"/>
+      <c r="K32" s="74"/>
+      <c r="L32" s="74"/>
+      <c r="M32" s="74"/>
+      <c r="N32" s="74"/>
+      <c r="O32" s="74"/>
+      <c r="P32" s="74"/>
+      <c r="Q32" s="74"/>
+      <c r="R32" s="74"/>
+      <c r="S32" s="74"/>
+      <c r="T32" s="74"/>
+      <c r="U32" s="75"/>
     </row>
     <row r="33" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F33" s="39" t="s">
-        <v>20</v>
-      </c>
-      <c r="G33" s="46" t="s">
-        <v>28</v>
-      </c>
-      <c r="H33" s="46"/>
-      <c r="I33" s="46"/>
-      <c r="J33" s="46"/>
-      <c r="K33" s="46"/>
-      <c r="L33" s="46"/>
-      <c r="M33" s="46"/>
-      <c r="N33" s="46"/>
-      <c r="O33" s="46"/>
-      <c r="P33" s="46"/>
-      <c r="Q33" s="46"/>
-      <c r="R33" s="46"/>
-      <c r="S33" s="46"/>
-      <c r="T33" s="46"/>
-      <c r="U33" s="47"/>
+        <v>19</v>
+      </c>
+      <c r="G33" s="74" t="s">
+        <v>27</v>
+      </c>
+      <c r="H33" s="74"/>
+      <c r="I33" s="74"/>
+      <c r="J33" s="74"/>
+      <c r="K33" s="74"/>
+      <c r="L33" s="74"/>
+      <c r="M33" s="74"/>
+      <c r="N33" s="74"/>
+      <c r="O33" s="74"/>
+      <c r="P33" s="74"/>
+      <c r="Q33" s="74"/>
+      <c r="R33" s="74"/>
+      <c r="S33" s="74"/>
+      <c r="T33" s="74"/>
+      <c r="U33" s="75"/>
     </row>
     <row r="34" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F34" s="40" t="s">
-        <v>20</v>
-      </c>
-      <c r="G34" s="70" t="s">
-        <v>31</v>
-      </c>
-      <c r="H34" s="70"/>
-      <c r="I34" s="70"/>
-      <c r="J34" s="70"/>
-      <c r="K34" s="70"/>
-      <c r="L34" s="70"/>
-      <c r="M34" s="70"/>
-      <c r="N34" s="70"/>
-      <c r="O34" s="70"/>
-      <c r="P34" s="70"/>
-      <c r="Q34" s="70"/>
-      <c r="R34" s="70"/>
-      <c r="S34" s="70"/>
-      <c r="T34" s="70"/>
-      <c r="U34" s="71"/>
+        <v>19</v>
+      </c>
+      <c r="G34" s="76" t="s">
+        <v>30</v>
+      </c>
+      <c r="H34" s="76"/>
+      <c r="I34" s="76"/>
+      <c r="J34" s="76"/>
+      <c r="K34" s="76"/>
+      <c r="L34" s="76"/>
+      <c r="M34" s="76"/>
+      <c r="N34" s="76"/>
+      <c r="O34" s="76"/>
+      <c r="P34" s="76"/>
+      <c r="Q34" s="76"/>
+      <c r="R34" s="76"/>
+      <c r="S34" s="76"/>
+      <c r="T34" s="76"/>
+      <c r="U34" s="77"/>
     </row>
     <row r="35" spans="6:21" x14ac:dyDescent="0.2">
       <c r="F35" s="32"/>
-      <c r="G35" s="66"/>
-      <c r="H35" s="66"/>
-      <c r="I35" s="66"/>
-      <c r="J35" s="66"/>
-      <c r="K35" s="66"/>
-      <c r="L35" s="66"/>
-      <c r="M35" s="66"/>
-      <c r="N35" s="66"/>
-      <c r="O35" s="66"/>
-      <c r="P35" s="66"/>
-      <c r="Q35" s="66"/>
-      <c r="R35" s="66"/>
-      <c r="S35" s="66"/>
-      <c r="T35" s="66"/>
-      <c r="U35" s="66"/>
+      <c r="G35" s="80"/>
+      <c r="H35" s="80"/>
+      <c r="I35" s="80"/>
+      <c r="J35" s="80"/>
+      <c r="K35" s="80"/>
+      <c r="L35" s="80"/>
+      <c r="M35" s="80"/>
+      <c r="N35" s="80"/>
+      <c r="O35" s="80"/>
+      <c r="P35" s="80"/>
+      <c r="Q35" s="80"/>
+      <c r="R35" s="80"/>
+      <c r="S35" s="80"/>
+      <c r="T35" s="80"/>
+      <c r="U35" s="80"/>
     </row>
     <row r="37" spans="6:21" x14ac:dyDescent="0.2">
       <c r="F37" s="32"/>
@@ -2682,68 +2679,68 @@
       <c r="U37" s="32"/>
     </row>
     <row r="38" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F38" s="56" t="s">
-        <v>21</v>
-      </c>
-      <c r="G38" s="57"/>
-      <c r="H38" s="57"/>
-      <c r="I38" s="57"/>
-      <c r="J38" s="57"/>
-      <c r="K38" s="57"/>
-      <c r="L38" s="57"/>
-      <c r="M38" s="57"/>
-      <c r="N38" s="57"/>
-      <c r="O38" s="57"/>
-      <c r="P38" s="57"/>
-      <c r="Q38" s="57"/>
-      <c r="R38" s="57"/>
-      <c r="S38" s="57"/>
-      <c r="T38" s="57"/>
-      <c r="U38" s="58"/>
+      <c r="F38" s="87" t="s">
+        <v>20</v>
+      </c>
+      <c r="G38" s="88"/>
+      <c r="H38" s="88"/>
+      <c r="I38" s="88"/>
+      <c r="J38" s="88"/>
+      <c r="K38" s="88"/>
+      <c r="L38" s="88"/>
+      <c r="M38" s="88"/>
+      <c r="N38" s="88"/>
+      <c r="O38" s="88"/>
+      <c r="P38" s="88"/>
+      <c r="Q38" s="88"/>
+      <c r="R38" s="88"/>
+      <c r="S38" s="88"/>
+      <c r="T38" s="88"/>
+      <c r="U38" s="89"/>
     </row>
     <row r="39" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F39" s="35" t="s">
-        <v>20</v>
-      </c>
-      <c r="G39" s="59" t="s">
-        <v>41</v>
-      </c>
-      <c r="H39" s="59"/>
-      <c r="I39" s="59"/>
-      <c r="J39" s="59"/>
-      <c r="K39" s="59"/>
-      <c r="L39" s="59"/>
-      <c r="M39" s="59"/>
-      <c r="N39" s="59"/>
-      <c r="O39" s="59"/>
-      <c r="P39" s="59"/>
-      <c r="Q39" s="59"/>
-      <c r="R39" s="59"/>
-      <c r="S39" s="59"/>
-      <c r="T39" s="59"/>
-      <c r="U39" s="60"/>
+        <v>19</v>
+      </c>
+      <c r="G39" s="72" t="s">
+        <v>40</v>
+      </c>
+      <c r="H39" s="72"/>
+      <c r="I39" s="72"/>
+      <c r="J39" s="72"/>
+      <c r="K39" s="72"/>
+      <c r="L39" s="72"/>
+      <c r="M39" s="72"/>
+      <c r="N39" s="72"/>
+      <c r="O39" s="72"/>
+      <c r="P39" s="72"/>
+      <c r="Q39" s="72"/>
+      <c r="R39" s="72"/>
+      <c r="S39" s="72"/>
+      <c r="T39" s="72"/>
+      <c r="U39" s="73"/>
     </row>
     <row r="40" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F40" s="35" t="s">
-        <v>20</v>
-      </c>
-      <c r="G40" s="59" t="s">
-        <v>32</v>
-      </c>
-      <c r="H40" s="59"/>
-      <c r="I40" s="59"/>
-      <c r="J40" s="59"/>
-      <c r="K40" s="59"/>
-      <c r="L40" s="59"/>
-      <c r="M40" s="59"/>
-      <c r="N40" s="59"/>
-      <c r="O40" s="59"/>
-      <c r="P40" s="59"/>
-      <c r="Q40" s="59"/>
-      <c r="R40" s="59"/>
-      <c r="S40" s="59"/>
-      <c r="T40" s="59"/>
-      <c r="U40" s="60"/>
+        <v>19</v>
+      </c>
+      <c r="G40" s="72" t="s">
+        <v>31</v>
+      </c>
+      <c r="H40" s="72"/>
+      <c r="I40" s="72"/>
+      <c r="J40" s="72"/>
+      <c r="K40" s="72"/>
+      <c r="L40" s="72"/>
+      <c r="M40" s="72"/>
+      <c r="N40" s="72"/>
+      <c r="O40" s="72"/>
+      <c r="P40" s="72"/>
+      <c r="Q40" s="72"/>
+      <c r="R40" s="72"/>
+      <c r="S40" s="72"/>
+      <c r="T40" s="72"/>
+      <c r="U40" s="73"/>
     </row>
     <row r="41" spans="6:21" x14ac:dyDescent="0.2">
       <c r="F41" s="41"/>
@@ -2765,218 +2762,191 @@
     </row>
     <row r="42" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F42" s="35" t="s">
-        <v>20</v>
-      </c>
-      <c r="G42" s="59" t="s">
-        <v>30</v>
-      </c>
-      <c r="H42" s="59"/>
-      <c r="I42" s="59"/>
-      <c r="J42" s="59"/>
-      <c r="K42" s="59"/>
-      <c r="L42" s="59"/>
-      <c r="M42" s="59"/>
-      <c r="N42" s="59"/>
-      <c r="O42" s="59"/>
-      <c r="P42" s="59"/>
-      <c r="Q42" s="59"/>
-      <c r="R42" s="59"/>
-      <c r="S42" s="59"/>
-      <c r="T42" s="59"/>
-      <c r="U42" s="60"/>
+        <v>19</v>
+      </c>
+      <c r="G42" s="72" t="s">
+        <v>29</v>
+      </c>
+      <c r="H42" s="72"/>
+      <c r="I42" s="72"/>
+      <c r="J42" s="72"/>
+      <c r="K42" s="72"/>
+      <c r="L42" s="72"/>
+      <c r="M42" s="72"/>
+      <c r="N42" s="72"/>
+      <c r="O42" s="72"/>
+      <c r="P42" s="72"/>
+      <c r="Q42" s="72"/>
+      <c r="R42" s="72"/>
+      <c r="S42" s="72"/>
+      <c r="T42" s="72"/>
+      <c r="U42" s="73"/>
     </row>
     <row r="43" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F43" s="38" t="s">
-        <v>20</v>
-      </c>
-      <c r="G43" s="44" t="s">
-        <v>43</v>
-      </c>
-      <c r="H43" s="44"/>
-      <c r="I43" s="44"/>
-      <c r="J43" s="44"/>
-      <c r="K43" s="44"/>
-      <c r="L43" s="44"/>
-      <c r="M43" s="44"/>
-      <c r="N43" s="44"/>
-      <c r="O43" s="44"/>
-      <c r="P43" s="44"/>
-      <c r="Q43" s="44"/>
-      <c r="R43" s="44"/>
-      <c r="S43" s="44"/>
-      <c r="T43" s="44"/>
-      <c r="U43" s="45"/>
+        <v>19</v>
+      </c>
+      <c r="G43" s="90" t="s">
+        <v>42</v>
+      </c>
+      <c r="H43" s="90"/>
+      <c r="I43" s="90"/>
+      <c r="J43" s="90"/>
+      <c r="K43" s="90"/>
+      <c r="L43" s="90"/>
+      <c r="M43" s="90"/>
+      <c r="N43" s="90"/>
+      <c r="O43" s="90"/>
+      <c r="P43" s="90"/>
+      <c r="Q43" s="90"/>
+      <c r="R43" s="90"/>
+      <c r="S43" s="90"/>
+      <c r="T43" s="90"/>
+      <c r="U43" s="91"/>
     </row>
     <row r="49" spans="5:25" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="M49" s="93" t="s">
+      <c r="M49" s="65" t="s">
+        <v>49</v>
+      </c>
+      <c r="N49" s="65"/>
+      <c r="O49" s="65"/>
+    </row>
+    <row r="51" spans="5:25" x14ac:dyDescent="0.2">
+      <c r="G51" s="56" t="s">
         <v>50</v>
       </c>
-      <c r="N49" s="93"/>
-      <c r="O49" s="93"/>
-    </row>
-    <row r="51" spans="5:25" x14ac:dyDescent="0.2">
-      <c r="G51" s="84" t="s">
+      <c r="H51" s="57"/>
+      <c r="I51" s="58"/>
+      <c r="K51" s="56" t="s">
         <v>51</v>
       </c>
-      <c r="H51" s="85"/>
-      <c r="I51" s="86"/>
-      <c r="K51" s="84" t="s">
+      <c r="L51" s="57"/>
+      <c r="M51" s="58"/>
+      <c r="O51" s="56" t="s">
         <v>52</v>
       </c>
-      <c r="L51" s="85"/>
-      <c r="M51" s="86"/>
-      <c r="O51" s="84" t="s">
+      <c r="P51" s="57"/>
+      <c r="Q51" s="58"/>
+      <c r="S51" s="56" t="s">
         <v>53</v>
       </c>
-      <c r="P51" s="85"/>
-      <c r="Q51" s="86"/>
-      <c r="S51" s="84" t="s">
-        <v>54</v>
-      </c>
-      <c r="T51" s="85"/>
-      <c r="U51" s="86"/>
+      <c r="T51" s="57"/>
+      <c r="U51" s="58"/>
     </row>
     <row r="52" spans="5:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G52" s="87"/>
-      <c r="H52" s="88"/>
-      <c r="I52" s="89"/>
-      <c r="K52" s="87"/>
-      <c r="L52" s="88"/>
-      <c r="M52" s="89"/>
-      <c r="O52" s="87"/>
-      <c r="P52" s="88"/>
-      <c r="Q52" s="89"/>
-      <c r="S52" s="87"/>
-      <c r="T52" s="88"/>
-      <c r="U52" s="89"/>
+      <c r="G52" s="59"/>
+      <c r="H52" s="60"/>
+      <c r="I52" s="61"/>
+      <c r="K52" s="59"/>
+      <c r="L52" s="60"/>
+      <c r="M52" s="61"/>
+      <c r="O52" s="59"/>
+      <c r="P52" s="60"/>
+      <c r="Q52" s="61"/>
+      <c r="S52" s="59"/>
+      <c r="T52" s="60"/>
+      <c r="U52" s="61"/>
     </row>
     <row r="53" spans="5:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G53" s="90"/>
-      <c r="H53" s="91"/>
-      <c r="I53" s="92"/>
-      <c r="K53" s="90"/>
-      <c r="L53" s="91"/>
-      <c r="M53" s="92"/>
-      <c r="O53" s="90"/>
-      <c r="P53" s="91"/>
-      <c r="Q53" s="92"/>
-      <c r="S53" s="90"/>
-      <c r="T53" s="91"/>
-      <c r="U53" s="92"/>
+      <c r="G53" s="62"/>
+      <c r="H53" s="63"/>
+      <c r="I53" s="64"/>
+      <c r="K53" s="62"/>
+      <c r="L53" s="63"/>
+      <c r="M53" s="64"/>
+      <c r="O53" s="62"/>
+      <c r="P53" s="63"/>
+      <c r="Q53" s="64"/>
+      <c r="S53" s="62"/>
+      <c r="T53" s="63"/>
+      <c r="U53" s="64"/>
     </row>
     <row r="62" spans="5:25" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E62" s="93" t="s">
+      <c r="E62" s="65" t="s">
+        <v>60</v>
+      </c>
+      <c r="F62" s="65"/>
+      <c r="G62" s="65"/>
+      <c r="H62" s="65"/>
+      <c r="P62" s="65" t="s">
         <v>61</v>
       </c>
-      <c r="F62" s="93"/>
-      <c r="G62" s="93"/>
-      <c r="H62" s="93"/>
-      <c r="P62" s="93" t="s">
+      <c r="Q62" s="65"/>
+      <c r="R62" s="65"/>
+      <c r="S62" s="65"/>
+      <c r="V62" s="65" t="s">
         <v>62</v>
       </c>
-      <c r="Q62" s="93"/>
-      <c r="R62" s="93"/>
-      <c r="S62" s="93"/>
-      <c r="V62" s="93" t="s">
-        <v>63</v>
-      </c>
-      <c r="W62" s="93"/>
-      <c r="X62" s="93"/>
-      <c r="Y62" s="93"/>
+      <c r="W62" s="65"/>
+      <c r="X62" s="65"/>
+      <c r="Y62" s="65"/>
     </row>
     <row r="63" spans="5:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="66" spans="3:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C66" s="94" t="s">
-        <v>57</v>
-      </c>
-      <c r="D66" s="95"/>
-      <c r="F66" s="94" t="s">
-        <v>57</v>
-      </c>
-      <c r="G66" s="95"/>
-      <c r="I66" s="94" t="s">
-        <v>57</v>
-      </c>
-      <c r="J66" s="95"/>
-      <c r="N66" s="72" t="s">
-        <v>57</v>
-      </c>
-      <c r="O66" s="73"/>
-      <c r="Q66" s="72" t="s">
-        <v>57</v>
-      </c>
-      <c r="R66" s="73"/>
-      <c r="T66" s="72" t="s">
+      <c r="C66" s="66" t="s">
         <v>56</v>
       </c>
-      <c r="U66" s="73"/>
-      <c r="W66" s="78" t="s">
+      <c r="D66" s="67"/>
+      <c r="F66" s="66" t="s">
+        <v>56</v>
+      </c>
+      <c r="G66" s="67"/>
+      <c r="I66" s="66" t="s">
+        <v>56</v>
+      </c>
+      <c r="J66" s="67"/>
+      <c r="N66" s="44" t="s">
+        <v>56</v>
+      </c>
+      <c r="O66" s="45"/>
+      <c r="Q66" s="44" t="s">
+        <v>56</v>
+      </c>
+      <c r="R66" s="45"/>
+      <c r="T66" s="44" t="s">
         <v>55</v>
       </c>
-      <c r="X66" s="79"/>
+      <c r="U66" s="45"/>
+      <c r="W66" s="50" t="s">
+        <v>54</v>
+      </c>
+      <c r="X66" s="51"/>
     </row>
     <row r="67" spans="3:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C67" s="96"/>
-      <c r="D67" s="97"/>
-      <c r="F67" s="96"/>
-      <c r="G67" s="97"/>
-      <c r="I67" s="96"/>
-      <c r="J67" s="97"/>
-      <c r="N67" s="74"/>
-      <c r="O67" s="75"/>
-      <c r="Q67" s="74"/>
-      <c r="R67" s="75"/>
-      <c r="T67" s="74"/>
-      <c r="U67" s="75"/>
-      <c r="W67" s="80"/>
-      <c r="X67" s="81"/>
+      <c r="C67" s="68"/>
+      <c r="D67" s="69"/>
+      <c r="F67" s="68"/>
+      <c r="G67" s="69"/>
+      <c r="I67" s="68"/>
+      <c r="J67" s="69"/>
+      <c r="N67" s="46"/>
+      <c r="O67" s="47"/>
+      <c r="Q67" s="46"/>
+      <c r="R67" s="47"/>
+      <c r="T67" s="46"/>
+      <c r="U67" s="47"/>
+      <c r="W67" s="52"/>
+      <c r="X67" s="53"/>
     </row>
     <row r="68" spans="3:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C68" s="98"/>
-      <c r="D68" s="99"/>
-      <c r="F68" s="98"/>
-      <c r="G68" s="99"/>
-      <c r="I68" s="98"/>
-      <c r="J68" s="99"/>
-      <c r="N68" s="76"/>
-      <c r="O68" s="77"/>
-      <c r="Q68" s="76"/>
-      <c r="R68" s="77"/>
-      <c r="T68" s="76"/>
-      <c r="U68" s="77"/>
-      <c r="W68" s="82"/>
-      <c r="X68" s="83"/>
+      <c r="C68" s="70"/>
+      <c r="D68" s="71"/>
+      <c r="F68" s="70"/>
+      <c r="G68" s="71"/>
+      <c r="I68" s="70"/>
+      <c r="J68" s="71"/>
+      <c r="N68" s="48"/>
+      <c r="O68" s="49"/>
+      <c r="Q68" s="48"/>
+      <c r="R68" s="49"/>
+      <c r="T68" s="48"/>
+      <c r="U68" s="49"/>
+      <c r="W68" s="54"/>
+      <c r="X68" s="55"/>
     </row>
     <row r="69" spans="3:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="43">
-    <mergeCell ref="T66:U68"/>
-    <mergeCell ref="W66:X68"/>
-    <mergeCell ref="S51:U53"/>
-    <mergeCell ref="M49:O49"/>
-    <mergeCell ref="C66:D68"/>
-    <mergeCell ref="F66:G68"/>
-    <mergeCell ref="I66:J68"/>
-    <mergeCell ref="N66:O68"/>
-    <mergeCell ref="Q66:R68"/>
-    <mergeCell ref="G51:I53"/>
-    <mergeCell ref="K51:M53"/>
-    <mergeCell ref="O51:Q53"/>
-    <mergeCell ref="E62:H62"/>
-    <mergeCell ref="P62:S62"/>
-    <mergeCell ref="V62:Y62"/>
-    <mergeCell ref="G39:U39"/>
-    <mergeCell ref="G40:U40"/>
-    <mergeCell ref="G30:U30"/>
-    <mergeCell ref="G31:U31"/>
-    <mergeCell ref="G32:U32"/>
-    <mergeCell ref="G33:U33"/>
-    <mergeCell ref="G34:U34"/>
-    <mergeCell ref="G24:U24"/>
-    <mergeCell ref="G35:U35"/>
-    <mergeCell ref="F17:U17"/>
-    <mergeCell ref="F28:U28"/>
-    <mergeCell ref="F38:U38"/>
     <mergeCell ref="G43:U43"/>
     <mergeCell ref="G29:U29"/>
     <mergeCell ref="F2:U2"/>
@@ -2993,6 +2963,33 @@
     <mergeCell ref="G15:U15"/>
     <mergeCell ref="G42:U42"/>
     <mergeCell ref="F23:U23"/>
+    <mergeCell ref="G24:U24"/>
+    <mergeCell ref="G35:U35"/>
+    <mergeCell ref="F17:U17"/>
+    <mergeCell ref="F28:U28"/>
+    <mergeCell ref="F38:U38"/>
+    <mergeCell ref="G39:U39"/>
+    <mergeCell ref="G40:U40"/>
+    <mergeCell ref="G30:U30"/>
+    <mergeCell ref="G31:U31"/>
+    <mergeCell ref="G32:U32"/>
+    <mergeCell ref="G33:U33"/>
+    <mergeCell ref="G34:U34"/>
+    <mergeCell ref="T66:U68"/>
+    <mergeCell ref="W66:X68"/>
+    <mergeCell ref="S51:U53"/>
+    <mergeCell ref="M49:O49"/>
+    <mergeCell ref="C66:D68"/>
+    <mergeCell ref="F66:G68"/>
+    <mergeCell ref="I66:J68"/>
+    <mergeCell ref="N66:O68"/>
+    <mergeCell ref="Q66:R68"/>
+    <mergeCell ref="G51:I53"/>
+    <mergeCell ref="K51:M53"/>
+    <mergeCell ref="O51:Q53"/>
+    <mergeCell ref="E62:H62"/>
+    <mergeCell ref="P62:S62"/>
+    <mergeCell ref="V62:Y62"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3002,11 +2999,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="E1:N48"/>
+  <dimension ref="E1:M48"/>
   <sheetViews>
-    <sheetView rightToLeft="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView rightToLeft="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K15" sqref="K15"/>
+      <selection pane="bottomLeft" activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3014,18 +3011,18 @@
     <col min="5" max="5" width="7.83203125" style="1" customWidth="1"/>
     <col min="6" max="6" width="21.1640625" customWidth="1"/>
     <col min="7" max="8" width="9.6640625" customWidth="1"/>
-    <col min="9" max="13" width="12.6640625" customWidth="1"/>
-    <col min="14" max="14" width="50.6640625" customWidth="1"/>
+    <col min="9" max="12" width="12.6640625" customWidth="1"/>
+    <col min="13" max="13" width="50.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="5:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="5:13" x14ac:dyDescent="0.2">
       <c r="E1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="5:14" ht="26" x14ac:dyDescent="0.2">
+    <row r="2" spans="5:13" ht="26" x14ac:dyDescent="0.2">
       <c r="E2" s="102" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F2" s="102"/>
       <c r="G2" s="102"/>
@@ -3035,9 +3032,8 @@
       <c r="K2" s="102"/>
       <c r="L2" s="102"/>
       <c r="M2" s="102"/>
-      <c r="N2" s="102"/>
-    </row>
-    <row r="4" spans="5:14" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="5:13" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E4"/>
       <c r="F4" s="104" t="s">
         <v>6</v>
@@ -3045,20 +3041,19 @@
       <c r="G4" s="105"/>
       <c r="H4" s="106"/>
       <c r="I4" s="103" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J4" s="103"/>
       <c r="K4" s="103"/>
       <c r="L4" s="103"/>
-      <c r="M4" s="103"/>
-      <c r="N4" s="100" t="s">
+      <c r="M4" s="100" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="5:14" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="5:13" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E5"/>
       <c r="F5" s="26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G5" s="26" t="s">
         <v>1</v>
@@ -3074,42 +3069,39 @@
         <v>1</v>
       </c>
       <c r="L5" s="103"/>
-      <c r="M5" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="N5" s="101"/>
-    </row>
-    <row r="6" spans="5:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M5" s="101"/>
+    </row>
+    <row r="6" spans="5:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E6"/>
     </row>
-    <row r="7" spans="5:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="5:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E7"/>
     </row>
-    <row r="8" spans="5:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="5:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E8"/>
     </row>
-    <row r="9" spans="5:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="5:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E9"/>
     </row>
-    <row r="10" spans="5:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="5:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E10"/>
     </row>
-    <row r="11" spans="5:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="5:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E11"/>
     </row>
-    <row r="12" spans="5:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="5:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E12"/>
     </row>
-    <row r="13" spans="5:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="5:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E13"/>
     </row>
-    <row r="14" spans="5:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="5:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E14"/>
     </row>
-    <row r="15" spans="5:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="5:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E15"/>
     </row>
-    <row r="16" spans="5:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="5:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E16"/>
     </row>
     <row r="17" spans="5:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -3210,10 +3202,10 @@
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="N4:N5"/>
-    <mergeCell ref="E2:N2"/>
+    <mergeCell ref="M4:M5"/>
+    <mergeCell ref="E2:M2"/>
     <mergeCell ref="K5:L5"/>
-    <mergeCell ref="I4:M4"/>
+    <mergeCell ref="I4:L4"/>
     <mergeCell ref="F4:H4"/>
     <mergeCell ref="I5:J5"/>
   </mergeCells>
@@ -3242,7 +3234,7 @@
   <sheetData>
     <row r="3" spans="4:9" s="13" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D3" s="109" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E3" s="109"/>
       <c r="F3" s="109"/>
@@ -3252,22 +3244,22 @@
     </row>
     <row r="5" spans="4:9" s="8" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D5" s="27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E5" s="27" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F5" s="27" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G5" s="27" t="s">
         <v>7</v>
       </c>
       <c r="H5" s="27" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I5" s="27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="4:9" s="8" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3587,7 +3579,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="F1:S21"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="B1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+    <sheetView rightToLeft="1" topLeftCell="B1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="S3" sqref="S3"/>
     </sheetView>
@@ -3611,7 +3603,7 @@
   <sheetData>
     <row r="1" spans="6:19" ht="21" x14ac:dyDescent="0.2">
       <c r="F1" s="110" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G1" s="110"/>
       <c r="H1" s="110"/>
@@ -3629,46 +3621,46 @@
     </row>
     <row r="2" spans="6:19" ht="68" x14ac:dyDescent="0.2">
       <c r="F2" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="G2" s="33" t="s">
+      <c r="H2" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="H2" s="33" t="s">
+      <c r="I2" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="I2" s="33" t="s">
+      <c r="J2" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="J2" s="33" t="s">
-        <v>37</v>
-      </c>
       <c r="K2" s="33" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L2" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="M2" s="33" t="s">
         <v>66</v>
       </c>
-      <c r="M2" s="33" t="s">
+      <c r="N2" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="N2" s="33" t="s">
+      <c r="O2" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="P2" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q2" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="O2" s="33" t="s">
-        <v>71</v>
-      </c>
-      <c r="P2" s="33" t="s">
+      <c r="R2" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="S2" s="43" t="s">
         <v>72</v>
-      </c>
-      <c r="Q2" s="33" t="s">
-        <v>69</v>
-      </c>
-      <c r="R2" s="33" t="s">
-        <v>70</v>
-      </c>
-      <c r="S2" s="43" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="8" spans="6:19" s="34" customFormat="1" x14ac:dyDescent="0.2"/>
@@ -3702,7 +3694,7 @@
   <sheetData>
     <row r="2" spans="5:13" ht="26" x14ac:dyDescent="0.2">
       <c r="E2" s="102" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F2" s="102"/>
       <c r="G2" s="102"/>
@@ -3718,12 +3710,12 @@
         <v>0</v>
       </c>
       <c r="F4" s="114" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G4" s="115"/>
       <c r="H4" s="116"/>
       <c r="I4" s="107" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J4" s="120"/>
       <c r="K4" s="120"/>
@@ -3940,14 +3932,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="F14:H14"/>
-    <mergeCell ref="F15:H15"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="F18:H18"/>
     <mergeCell ref="F12:H12"/>
     <mergeCell ref="E2:M2"/>
     <mergeCell ref="E4:E5"/>
@@ -3960,6 +3944,14 @@
     <mergeCell ref="F9:H9"/>
     <mergeCell ref="F10:H10"/>
     <mergeCell ref="F11:H11"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="F15:H15"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="F18:H18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="53" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
1st milestone - reorganize code, seperate into smaller files and more
</commit_message>
<xml_diff>
--- a/cockpit_template.xlsx
+++ b/cockpit_template.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Roi.Dital/roid_playground/paamonim/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D0E34EE-9AFE-024C-9268-CAD46F4E0205}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE3B73D5-58F7-1847-803C-B5B9DF2AC5D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="19440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="רציונל" sheetId="3" r:id="rId1"/>
-    <sheet name="ראשי" sheetId="1" r:id="rId2"/>
+    <sheet name="צוותים" sheetId="1" r:id="rId2"/>
     <sheet name="מלווים" sheetId="2" r:id="rId3"/>
     <sheet name="דוח משפחות" sheetId="6" r:id="rId4"/>
     <sheet name="מסרים" sheetId="4" r:id="rId5"/>
@@ -22,7 +22,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="2">מלווים!$D$2:$I$47</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="4">מסרים!$E$1:$M$49</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">ראשי!$E$1:$M$63</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">צוותים!$E$1:$M$63</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -837,6 +837,90 @@
     <xf numFmtId="0" fontId="15" fillId="12" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -920,90 +1004,6 @@
     </xf>
     <xf numFmtId="0" fontId="17" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1995,24 +1995,24 @@
   <sheetData>
     <row r="1" spans="6:21" ht="20" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F2" s="92" t="s">
+      <c r="F2" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="92"/>
-      <c r="H2" s="92"/>
-      <c r="I2" s="92"/>
-      <c r="J2" s="92"/>
-      <c r="K2" s="92"/>
-      <c r="L2" s="92"/>
-      <c r="M2" s="92"/>
-      <c r="N2" s="92"/>
-      <c r="O2" s="92"/>
-      <c r="P2" s="92"/>
-      <c r="Q2" s="92"/>
-      <c r="R2" s="92"/>
-      <c r="S2" s="92"/>
-      <c r="T2" s="92"/>
-      <c r="U2" s="92"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="48"/>
+      <c r="J2" s="48"/>
+      <c r="K2" s="48"/>
+      <c r="L2" s="48"/>
+      <c r="M2" s="48"/>
+      <c r="N2" s="48"/>
+      <c r="O2" s="48"/>
+      <c r="P2" s="48"/>
+      <c r="Q2" s="48"/>
+      <c r="R2" s="48"/>
+      <c r="S2" s="48"/>
+      <c r="T2" s="48"/>
+      <c r="U2" s="48"/>
     </row>
     <row r="3" spans="6:21" x14ac:dyDescent="0.2">
       <c r="F3" s="30"/>
@@ -2033,68 +2033,68 @@
       <c r="U3" s="30"/>
     </row>
     <row r="4" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F4" s="87" t="s">
+      <c r="F4" s="56" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="88"/>
-      <c r="H4" s="88"/>
-      <c r="I4" s="88"/>
-      <c r="J4" s="88"/>
-      <c r="K4" s="88"/>
-      <c r="L4" s="88"/>
-      <c r="M4" s="88"/>
-      <c r="N4" s="88"/>
-      <c r="O4" s="88"/>
-      <c r="P4" s="88"/>
-      <c r="Q4" s="88"/>
-      <c r="R4" s="88"/>
-      <c r="S4" s="88"/>
-      <c r="T4" s="88"/>
-      <c r="U4" s="89"/>
+      <c r="G4" s="57"/>
+      <c r="H4" s="57"/>
+      <c r="I4" s="57"/>
+      <c r="J4" s="57"/>
+      <c r="K4" s="57"/>
+      <c r="L4" s="57"/>
+      <c r="M4" s="57"/>
+      <c r="N4" s="57"/>
+      <c r="O4" s="57"/>
+      <c r="P4" s="57"/>
+      <c r="Q4" s="57"/>
+      <c r="R4" s="57"/>
+      <c r="S4" s="57"/>
+      <c r="T4" s="57"/>
+      <c r="U4" s="58"/>
     </row>
     <row r="5" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F5" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="72" t="s">
+      <c r="G5" s="59" t="s">
         <v>39</v>
       </c>
-      <c r="H5" s="72"/>
-      <c r="I5" s="72"/>
-      <c r="J5" s="72"/>
-      <c r="K5" s="72"/>
-      <c r="L5" s="72"/>
-      <c r="M5" s="72"/>
-      <c r="N5" s="72"/>
-      <c r="O5" s="72"/>
-      <c r="P5" s="72"/>
-      <c r="Q5" s="72"/>
-      <c r="R5" s="72"/>
-      <c r="S5" s="72"/>
-      <c r="T5" s="72"/>
-      <c r="U5" s="73"/>
+      <c r="H5" s="59"/>
+      <c r="I5" s="59"/>
+      <c r="J5" s="59"/>
+      <c r="K5" s="59"/>
+      <c r="L5" s="59"/>
+      <c r="M5" s="59"/>
+      <c r="N5" s="59"/>
+      <c r="O5" s="59"/>
+      <c r="P5" s="59"/>
+      <c r="Q5" s="59"/>
+      <c r="R5" s="59"/>
+      <c r="S5" s="59"/>
+      <c r="T5" s="59"/>
+      <c r="U5" s="60"/>
     </row>
     <row r="6" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F6" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="90" t="s">
+      <c r="G6" s="44" t="s">
         <v>41</v>
       </c>
-      <c r="H6" s="90"/>
-      <c r="I6" s="90"/>
-      <c r="J6" s="90"/>
-      <c r="K6" s="90"/>
-      <c r="L6" s="90"/>
-      <c r="M6" s="90"/>
-      <c r="N6" s="90"/>
-      <c r="O6" s="90"/>
-      <c r="P6" s="90"/>
-      <c r="Q6" s="90"/>
-      <c r="R6" s="90"/>
-      <c r="S6" s="90"/>
-      <c r="T6" s="90"/>
-      <c r="U6" s="91"/>
+      <c r="H6" s="44"/>
+      <c r="I6" s="44"/>
+      <c r="J6" s="44"/>
+      <c r="K6" s="44"/>
+      <c r="L6" s="44"/>
+      <c r="M6" s="44"/>
+      <c r="N6" s="44"/>
+      <c r="O6" s="44"/>
+      <c r="P6" s="44"/>
+      <c r="Q6" s="44"/>
+      <c r="R6" s="44"/>
+      <c r="S6" s="44"/>
+      <c r="T6" s="44"/>
+      <c r="U6" s="45"/>
     </row>
     <row r="7" spans="6:21" x14ac:dyDescent="0.2">
       <c r="F7" s="31"/>
@@ -2115,46 +2115,46 @@
       <c r="U7" s="31"/>
     </row>
     <row r="8" spans="6:21" ht="26" x14ac:dyDescent="0.2">
-      <c r="F8" s="93" t="s">
+      <c r="F8" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="G8" s="94"/>
-      <c r="H8" s="94"/>
-      <c r="I8" s="94"/>
-      <c r="J8" s="94"/>
-      <c r="K8" s="94"/>
-      <c r="L8" s="94"/>
-      <c r="M8" s="94"/>
-      <c r="N8" s="94"/>
-      <c r="O8" s="94"/>
-      <c r="P8" s="94"/>
-      <c r="Q8" s="94"/>
-      <c r="R8" s="94"/>
-      <c r="S8" s="94"/>
-      <c r="T8" s="94"/>
-      <c r="U8" s="95"/>
+      <c r="G8" s="50"/>
+      <c r="H8" s="50"/>
+      <c r="I8" s="50"/>
+      <c r="J8" s="50"/>
+      <c r="K8" s="50"/>
+      <c r="L8" s="50"/>
+      <c r="M8" s="50"/>
+      <c r="N8" s="50"/>
+      <c r="O8" s="50"/>
+      <c r="P8" s="50"/>
+      <c r="Q8" s="50"/>
+      <c r="R8" s="50"/>
+      <c r="S8" s="50"/>
+      <c r="T8" s="50"/>
+      <c r="U8" s="51"/>
     </row>
     <row r="9" spans="6:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F9" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="G9" s="96" t="s">
+      <c r="G9" s="52" t="s">
         <v>59</v>
       </c>
-      <c r="H9" s="96"/>
-      <c r="I9" s="96"/>
-      <c r="J9" s="96"/>
-      <c r="K9" s="96"/>
-      <c r="L9" s="96"/>
-      <c r="M9" s="96"/>
-      <c r="N9" s="96"/>
-      <c r="O9" s="96"/>
-      <c r="P9" s="96"/>
-      <c r="Q9" s="96"/>
-      <c r="R9" s="96"/>
-      <c r="S9" s="96"/>
-      <c r="T9" s="96"/>
-      <c r="U9" s="97"/>
+      <c r="H9" s="52"/>
+      <c r="I9" s="52"/>
+      <c r="J9" s="52"/>
+      <c r="K9" s="52"/>
+      <c r="L9" s="52"/>
+      <c r="M9" s="52"/>
+      <c r="N9" s="52"/>
+      <c r="O9" s="52"/>
+      <c r="P9" s="52"/>
+      <c r="Q9" s="52"/>
+      <c r="R9" s="52"/>
+      <c r="S9" s="52"/>
+      <c r="T9" s="52"/>
+      <c r="U9" s="53"/>
     </row>
     <row r="10" spans="6:21" x14ac:dyDescent="0.2">
       <c r="F10" s="32"/>
@@ -2193,68 +2193,68 @@
       <c r="U12" s="32"/>
     </row>
     <row r="13" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F13" s="87" t="s">
+      <c r="F13" s="56" t="s">
         <v>57</v>
       </c>
-      <c r="G13" s="88"/>
-      <c r="H13" s="88"/>
-      <c r="I13" s="88"/>
-      <c r="J13" s="88"/>
-      <c r="K13" s="88"/>
-      <c r="L13" s="88"/>
-      <c r="M13" s="88"/>
-      <c r="N13" s="88"/>
-      <c r="O13" s="88"/>
-      <c r="P13" s="88"/>
-      <c r="Q13" s="88"/>
-      <c r="R13" s="88"/>
-      <c r="S13" s="88"/>
-      <c r="T13" s="88"/>
-      <c r="U13" s="89"/>
+      <c r="G13" s="57"/>
+      <c r="H13" s="57"/>
+      <c r="I13" s="57"/>
+      <c r="J13" s="57"/>
+      <c r="K13" s="57"/>
+      <c r="L13" s="57"/>
+      <c r="M13" s="57"/>
+      <c r="N13" s="57"/>
+      <c r="O13" s="57"/>
+      <c r="P13" s="57"/>
+      <c r="Q13" s="57"/>
+      <c r="R13" s="57"/>
+      <c r="S13" s="57"/>
+      <c r="T13" s="57"/>
+      <c r="U13" s="58"/>
     </row>
     <row r="14" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F14" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="G14" s="98" t="s">
+      <c r="G14" s="54" t="s">
         <v>43</v>
       </c>
-      <c r="H14" s="98"/>
-      <c r="I14" s="98"/>
-      <c r="J14" s="98"/>
-      <c r="K14" s="98"/>
-      <c r="L14" s="98"/>
-      <c r="M14" s="98"/>
-      <c r="N14" s="98"/>
-      <c r="O14" s="98"/>
-      <c r="P14" s="98"/>
-      <c r="Q14" s="98"/>
-      <c r="R14" s="98"/>
-      <c r="S14" s="98"/>
-      <c r="T14" s="98"/>
-      <c r="U14" s="99"/>
+      <c r="H14" s="54"/>
+      <c r="I14" s="54"/>
+      <c r="J14" s="54"/>
+      <c r="K14" s="54"/>
+      <c r="L14" s="54"/>
+      <c r="M14" s="54"/>
+      <c r="N14" s="54"/>
+      <c r="O14" s="54"/>
+      <c r="P14" s="54"/>
+      <c r="Q14" s="54"/>
+      <c r="R14" s="54"/>
+      <c r="S14" s="54"/>
+      <c r="T14" s="54"/>
+      <c r="U14" s="55"/>
     </row>
     <row r="15" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F15" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="G15" s="98" t="s">
+      <c r="G15" s="54" t="s">
         <v>48</v>
       </c>
-      <c r="H15" s="98"/>
-      <c r="I15" s="98"/>
-      <c r="J15" s="98"/>
-      <c r="K15" s="98"/>
-      <c r="L15" s="98"/>
-      <c r="M15" s="98"/>
-      <c r="N15" s="98"/>
-      <c r="O15" s="98"/>
-      <c r="P15" s="98"/>
-      <c r="Q15" s="98"/>
-      <c r="R15" s="98"/>
-      <c r="S15" s="98"/>
-      <c r="T15" s="98"/>
-      <c r="U15" s="99"/>
+      <c r="H15" s="54"/>
+      <c r="I15" s="54"/>
+      <c r="J15" s="54"/>
+      <c r="K15" s="54"/>
+      <c r="L15" s="54"/>
+      <c r="M15" s="54"/>
+      <c r="N15" s="54"/>
+      <c r="O15" s="54"/>
+      <c r="P15" s="54"/>
+      <c r="Q15" s="54"/>
+      <c r="R15" s="54"/>
+      <c r="S15" s="54"/>
+      <c r="T15" s="54"/>
+      <c r="U15" s="55"/>
     </row>
     <row r="16" spans="6:21" x14ac:dyDescent="0.2">
       <c r="F16" s="36"/>
@@ -2275,46 +2275,46 @@
       <c r="U16" s="37"/>
     </row>
     <row r="17" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F17" s="81" t="s">
+      <c r="F17" s="61" t="s">
         <v>15</v>
       </c>
-      <c r="G17" s="82"/>
-      <c r="H17" s="82"/>
-      <c r="I17" s="82"/>
-      <c r="J17" s="82"/>
-      <c r="K17" s="82"/>
-      <c r="L17" s="82"/>
-      <c r="M17" s="82"/>
-      <c r="N17" s="82"/>
-      <c r="O17" s="82"/>
-      <c r="P17" s="82"/>
-      <c r="Q17" s="82"/>
-      <c r="R17" s="82"/>
-      <c r="S17" s="82"/>
-      <c r="T17" s="82"/>
-      <c r="U17" s="83"/>
+      <c r="G17" s="62"/>
+      <c r="H17" s="62"/>
+      <c r="I17" s="62"/>
+      <c r="J17" s="62"/>
+      <c r="K17" s="62"/>
+      <c r="L17" s="62"/>
+      <c r="M17" s="62"/>
+      <c r="N17" s="62"/>
+      <c r="O17" s="62"/>
+      <c r="P17" s="62"/>
+      <c r="Q17" s="62"/>
+      <c r="R17" s="62"/>
+      <c r="S17" s="62"/>
+      <c r="T17" s="62"/>
+      <c r="U17" s="63"/>
     </row>
     <row r="18" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F18" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="G18" s="98" t="s">
+      <c r="G18" s="54" t="s">
         <v>47</v>
       </c>
-      <c r="H18" s="98"/>
-      <c r="I18" s="98"/>
-      <c r="J18" s="98"/>
-      <c r="K18" s="98"/>
-      <c r="L18" s="98"/>
-      <c r="M18" s="98"/>
-      <c r="N18" s="98"/>
-      <c r="O18" s="98"/>
-      <c r="P18" s="98"/>
-      <c r="Q18" s="98"/>
-      <c r="R18" s="98"/>
-      <c r="S18" s="98"/>
-      <c r="T18" s="98"/>
-      <c r="U18" s="99"/>
+      <c r="H18" s="54"/>
+      <c r="I18" s="54"/>
+      <c r="J18" s="54"/>
+      <c r="K18" s="54"/>
+      <c r="L18" s="54"/>
+      <c r="M18" s="54"/>
+      <c r="N18" s="54"/>
+      <c r="O18" s="54"/>
+      <c r="P18" s="54"/>
+      <c r="Q18" s="54"/>
+      <c r="R18" s="54"/>
+      <c r="S18" s="54"/>
+      <c r="T18" s="54"/>
+      <c r="U18" s="55"/>
     </row>
     <row r="19" spans="6:21" x14ac:dyDescent="0.2">
       <c r="F19" s="36"/>
@@ -2335,46 +2335,46 @@
       <c r="U19" s="37"/>
     </row>
     <row r="20" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F20" s="81" t="s">
+      <c r="F20" s="61" t="s">
         <v>44</v>
       </c>
-      <c r="G20" s="82"/>
-      <c r="H20" s="82"/>
-      <c r="I20" s="82"/>
-      <c r="J20" s="82"/>
-      <c r="K20" s="82"/>
-      <c r="L20" s="82"/>
-      <c r="M20" s="82"/>
-      <c r="N20" s="82"/>
-      <c r="O20" s="82"/>
-      <c r="P20" s="82"/>
-      <c r="Q20" s="82"/>
-      <c r="R20" s="82"/>
-      <c r="S20" s="82"/>
-      <c r="T20" s="82"/>
-      <c r="U20" s="83"/>
+      <c r="G20" s="62"/>
+      <c r="H20" s="62"/>
+      <c r="I20" s="62"/>
+      <c r="J20" s="62"/>
+      <c r="K20" s="62"/>
+      <c r="L20" s="62"/>
+      <c r="M20" s="62"/>
+      <c r="N20" s="62"/>
+      <c r="O20" s="62"/>
+      <c r="P20" s="62"/>
+      <c r="Q20" s="62"/>
+      <c r="R20" s="62"/>
+      <c r="S20" s="62"/>
+      <c r="T20" s="62"/>
+      <c r="U20" s="63"/>
     </row>
     <row r="21" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F21" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="G21" s="98" t="s">
+      <c r="G21" s="54" t="s">
         <v>58</v>
       </c>
-      <c r="H21" s="98"/>
-      <c r="I21" s="98"/>
-      <c r="J21" s="98"/>
-      <c r="K21" s="98"/>
-      <c r="L21" s="98"/>
-      <c r="M21" s="98"/>
-      <c r="N21" s="98"/>
-      <c r="O21" s="98"/>
-      <c r="P21" s="98"/>
-      <c r="Q21" s="98"/>
-      <c r="R21" s="98"/>
-      <c r="S21" s="98"/>
-      <c r="T21" s="98"/>
-      <c r="U21" s="99"/>
+      <c r="H21" s="54"/>
+      <c r="I21" s="54"/>
+      <c r="J21" s="54"/>
+      <c r="K21" s="54"/>
+      <c r="L21" s="54"/>
+      <c r="M21" s="54"/>
+      <c r="N21" s="54"/>
+      <c r="O21" s="54"/>
+      <c r="P21" s="54"/>
+      <c r="Q21" s="54"/>
+      <c r="R21" s="54"/>
+      <c r="S21" s="54"/>
+      <c r="T21" s="54"/>
+      <c r="U21" s="55"/>
     </row>
     <row r="22" spans="6:21" x14ac:dyDescent="0.2">
       <c r="F22" s="36"/>
@@ -2395,46 +2395,46 @@
       <c r="U22" s="37"/>
     </row>
     <row r="23" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F23" s="81" t="s">
+      <c r="F23" s="61" t="s">
         <v>45</v>
       </c>
-      <c r="G23" s="82"/>
-      <c r="H23" s="82"/>
-      <c r="I23" s="82"/>
-      <c r="J23" s="82"/>
-      <c r="K23" s="82"/>
-      <c r="L23" s="82"/>
-      <c r="M23" s="82"/>
-      <c r="N23" s="82"/>
-      <c r="O23" s="82"/>
-      <c r="P23" s="82"/>
-      <c r="Q23" s="82"/>
-      <c r="R23" s="82"/>
-      <c r="S23" s="82"/>
-      <c r="T23" s="82"/>
-      <c r="U23" s="83"/>
+      <c r="G23" s="62"/>
+      <c r="H23" s="62"/>
+      <c r="I23" s="62"/>
+      <c r="J23" s="62"/>
+      <c r="K23" s="62"/>
+      <c r="L23" s="62"/>
+      <c r="M23" s="62"/>
+      <c r="N23" s="62"/>
+      <c r="O23" s="62"/>
+      <c r="P23" s="62"/>
+      <c r="Q23" s="62"/>
+      <c r="R23" s="62"/>
+      <c r="S23" s="62"/>
+      <c r="T23" s="62"/>
+      <c r="U23" s="63"/>
     </row>
     <row r="24" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F24" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="G24" s="78" t="s">
+      <c r="G24" s="64" t="s">
         <v>46</v>
       </c>
-      <c r="H24" s="78"/>
-      <c r="I24" s="78"/>
-      <c r="J24" s="78"/>
-      <c r="K24" s="78"/>
-      <c r="L24" s="78"/>
-      <c r="M24" s="78"/>
-      <c r="N24" s="78"/>
-      <c r="O24" s="78"/>
-      <c r="P24" s="78"/>
-      <c r="Q24" s="78"/>
-      <c r="R24" s="78"/>
-      <c r="S24" s="78"/>
-      <c r="T24" s="78"/>
-      <c r="U24" s="79"/>
+      <c r="H24" s="64"/>
+      <c r="I24" s="64"/>
+      <c r="J24" s="64"/>
+      <c r="K24" s="64"/>
+      <c r="L24" s="64"/>
+      <c r="M24" s="64"/>
+      <c r="N24" s="64"/>
+      <c r="O24" s="64"/>
+      <c r="P24" s="64"/>
+      <c r="Q24" s="64"/>
+      <c r="R24" s="64"/>
+      <c r="S24" s="64"/>
+      <c r="T24" s="64"/>
+      <c r="U24" s="65"/>
     </row>
     <row r="25" spans="6:21" x14ac:dyDescent="0.2">
       <c r="F25" s="32"/>
@@ -2491,174 +2491,174 @@
       <c r="U27" s="32"/>
     </row>
     <row r="28" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F28" s="84" t="s">
+      <c r="F28" s="67" t="s">
         <v>16</v>
       </c>
-      <c r="G28" s="85"/>
-      <c r="H28" s="85"/>
-      <c r="I28" s="85"/>
-      <c r="J28" s="85"/>
-      <c r="K28" s="85"/>
-      <c r="L28" s="85"/>
-      <c r="M28" s="85"/>
-      <c r="N28" s="85"/>
-      <c r="O28" s="85"/>
-      <c r="P28" s="85"/>
-      <c r="Q28" s="85"/>
-      <c r="R28" s="85"/>
-      <c r="S28" s="85"/>
-      <c r="T28" s="85"/>
-      <c r="U28" s="86"/>
+      <c r="G28" s="68"/>
+      <c r="H28" s="68"/>
+      <c r="I28" s="68"/>
+      <c r="J28" s="68"/>
+      <c r="K28" s="68"/>
+      <c r="L28" s="68"/>
+      <c r="M28" s="68"/>
+      <c r="N28" s="68"/>
+      <c r="O28" s="68"/>
+      <c r="P28" s="68"/>
+      <c r="Q28" s="68"/>
+      <c r="R28" s="68"/>
+      <c r="S28" s="68"/>
+      <c r="T28" s="68"/>
+      <c r="U28" s="69"/>
     </row>
     <row r="29" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F29" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="G29" s="74" t="s">
+      <c r="G29" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="H29" s="74"/>
-      <c r="I29" s="74"/>
-      <c r="J29" s="74"/>
-      <c r="K29" s="74"/>
-      <c r="L29" s="74"/>
-      <c r="M29" s="74"/>
-      <c r="N29" s="74"/>
-      <c r="O29" s="74"/>
-      <c r="P29" s="74"/>
-      <c r="Q29" s="74"/>
-      <c r="R29" s="74"/>
-      <c r="S29" s="74"/>
-      <c r="T29" s="74"/>
-      <c r="U29" s="75"/>
+      <c r="H29" s="46"/>
+      <c r="I29" s="46"/>
+      <c r="J29" s="46"/>
+      <c r="K29" s="46"/>
+      <c r="L29" s="46"/>
+      <c r="M29" s="46"/>
+      <c r="N29" s="46"/>
+      <c r="O29" s="46"/>
+      <c r="P29" s="46"/>
+      <c r="Q29" s="46"/>
+      <c r="R29" s="46"/>
+      <c r="S29" s="46"/>
+      <c r="T29" s="46"/>
+      <c r="U29" s="47"/>
     </row>
     <row r="30" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F30" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="G30" s="74" t="s">
+      <c r="G30" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="H30" s="74"/>
-      <c r="I30" s="74"/>
-      <c r="J30" s="74"/>
-      <c r="K30" s="74"/>
-      <c r="L30" s="74"/>
-      <c r="M30" s="74"/>
-      <c r="N30" s="74"/>
-      <c r="O30" s="74"/>
-      <c r="P30" s="74"/>
-      <c r="Q30" s="74"/>
-      <c r="R30" s="74"/>
-      <c r="S30" s="74"/>
-      <c r="T30" s="74"/>
-      <c r="U30" s="75"/>
+      <c r="H30" s="46"/>
+      <c r="I30" s="46"/>
+      <c r="J30" s="46"/>
+      <c r="K30" s="46"/>
+      <c r="L30" s="46"/>
+      <c r="M30" s="46"/>
+      <c r="N30" s="46"/>
+      <c r="O30" s="46"/>
+      <c r="P30" s="46"/>
+      <c r="Q30" s="46"/>
+      <c r="R30" s="46"/>
+      <c r="S30" s="46"/>
+      <c r="T30" s="46"/>
+      <c r="U30" s="47"/>
     </row>
     <row r="31" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F31" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="G31" s="74" t="s">
+      <c r="G31" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="H31" s="74"/>
-      <c r="I31" s="74"/>
-      <c r="J31" s="74"/>
-      <c r="K31" s="74"/>
-      <c r="L31" s="74"/>
-      <c r="M31" s="74"/>
-      <c r="N31" s="74"/>
-      <c r="O31" s="74"/>
-      <c r="P31" s="74"/>
-      <c r="Q31" s="74"/>
-      <c r="R31" s="74"/>
-      <c r="S31" s="74"/>
-      <c r="T31" s="74"/>
-      <c r="U31" s="75"/>
+      <c r="H31" s="46"/>
+      <c r="I31" s="46"/>
+      <c r="J31" s="46"/>
+      <c r="K31" s="46"/>
+      <c r="L31" s="46"/>
+      <c r="M31" s="46"/>
+      <c r="N31" s="46"/>
+      <c r="O31" s="46"/>
+      <c r="P31" s="46"/>
+      <c r="Q31" s="46"/>
+      <c r="R31" s="46"/>
+      <c r="S31" s="46"/>
+      <c r="T31" s="46"/>
+      <c r="U31" s="47"/>
     </row>
     <row r="32" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F32" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="G32" s="74" t="s">
+      <c r="G32" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="H32" s="74"/>
-      <c r="I32" s="74"/>
-      <c r="J32" s="74"/>
-      <c r="K32" s="74"/>
-      <c r="L32" s="74"/>
-      <c r="M32" s="74"/>
-      <c r="N32" s="74"/>
-      <c r="O32" s="74"/>
-      <c r="P32" s="74"/>
-      <c r="Q32" s="74"/>
-      <c r="R32" s="74"/>
-      <c r="S32" s="74"/>
-      <c r="T32" s="74"/>
-      <c r="U32" s="75"/>
+      <c r="H32" s="46"/>
+      <c r="I32" s="46"/>
+      <c r="J32" s="46"/>
+      <c r="K32" s="46"/>
+      <c r="L32" s="46"/>
+      <c r="M32" s="46"/>
+      <c r="N32" s="46"/>
+      <c r="O32" s="46"/>
+      <c r="P32" s="46"/>
+      <c r="Q32" s="46"/>
+      <c r="R32" s="46"/>
+      <c r="S32" s="46"/>
+      <c r="T32" s="46"/>
+      <c r="U32" s="47"/>
     </row>
     <row r="33" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F33" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="G33" s="74" t="s">
+      <c r="G33" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="H33" s="74"/>
-      <c r="I33" s="74"/>
-      <c r="J33" s="74"/>
-      <c r="K33" s="74"/>
-      <c r="L33" s="74"/>
-      <c r="M33" s="74"/>
-      <c r="N33" s="74"/>
-      <c r="O33" s="74"/>
-      <c r="P33" s="74"/>
-      <c r="Q33" s="74"/>
-      <c r="R33" s="74"/>
-      <c r="S33" s="74"/>
-      <c r="T33" s="74"/>
-      <c r="U33" s="75"/>
+      <c r="H33" s="46"/>
+      <c r="I33" s="46"/>
+      <c r="J33" s="46"/>
+      <c r="K33" s="46"/>
+      <c r="L33" s="46"/>
+      <c r="M33" s="46"/>
+      <c r="N33" s="46"/>
+      <c r="O33" s="46"/>
+      <c r="P33" s="46"/>
+      <c r="Q33" s="46"/>
+      <c r="R33" s="46"/>
+      <c r="S33" s="46"/>
+      <c r="T33" s="46"/>
+      <c r="U33" s="47"/>
     </row>
     <row r="34" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F34" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="G34" s="76" t="s">
+      <c r="G34" s="70" t="s">
         <v>30</v>
       </c>
-      <c r="H34" s="76"/>
-      <c r="I34" s="76"/>
-      <c r="J34" s="76"/>
-      <c r="K34" s="76"/>
-      <c r="L34" s="76"/>
-      <c r="M34" s="76"/>
-      <c r="N34" s="76"/>
-      <c r="O34" s="76"/>
-      <c r="P34" s="76"/>
-      <c r="Q34" s="76"/>
-      <c r="R34" s="76"/>
-      <c r="S34" s="76"/>
-      <c r="T34" s="76"/>
-      <c r="U34" s="77"/>
+      <c r="H34" s="70"/>
+      <c r="I34" s="70"/>
+      <c r="J34" s="70"/>
+      <c r="K34" s="70"/>
+      <c r="L34" s="70"/>
+      <c r="M34" s="70"/>
+      <c r="N34" s="70"/>
+      <c r="O34" s="70"/>
+      <c r="P34" s="70"/>
+      <c r="Q34" s="70"/>
+      <c r="R34" s="70"/>
+      <c r="S34" s="70"/>
+      <c r="T34" s="70"/>
+      <c r="U34" s="71"/>
     </row>
     <row r="35" spans="6:21" x14ac:dyDescent="0.2">
       <c r="F35" s="32"/>
-      <c r="G35" s="80"/>
-      <c r="H35" s="80"/>
-      <c r="I35" s="80"/>
-      <c r="J35" s="80"/>
-      <c r="K35" s="80"/>
-      <c r="L35" s="80"/>
-      <c r="M35" s="80"/>
-      <c r="N35" s="80"/>
-      <c r="O35" s="80"/>
-      <c r="P35" s="80"/>
-      <c r="Q35" s="80"/>
-      <c r="R35" s="80"/>
-      <c r="S35" s="80"/>
-      <c r="T35" s="80"/>
-      <c r="U35" s="80"/>
+      <c r="G35" s="66"/>
+      <c r="H35" s="66"/>
+      <c r="I35" s="66"/>
+      <c r="J35" s="66"/>
+      <c r="K35" s="66"/>
+      <c r="L35" s="66"/>
+      <c r="M35" s="66"/>
+      <c r="N35" s="66"/>
+      <c r="O35" s="66"/>
+      <c r="P35" s="66"/>
+      <c r="Q35" s="66"/>
+      <c r="R35" s="66"/>
+      <c r="S35" s="66"/>
+      <c r="T35" s="66"/>
+      <c r="U35" s="66"/>
     </row>
     <row r="37" spans="6:21" x14ac:dyDescent="0.2">
       <c r="F37" s="32"/>
@@ -2679,68 +2679,68 @@
       <c r="U37" s="32"/>
     </row>
     <row r="38" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F38" s="87" t="s">
+      <c r="F38" s="56" t="s">
         <v>20</v>
       </c>
-      <c r="G38" s="88"/>
-      <c r="H38" s="88"/>
-      <c r="I38" s="88"/>
-      <c r="J38" s="88"/>
-      <c r="K38" s="88"/>
-      <c r="L38" s="88"/>
-      <c r="M38" s="88"/>
-      <c r="N38" s="88"/>
-      <c r="O38" s="88"/>
-      <c r="P38" s="88"/>
-      <c r="Q38" s="88"/>
-      <c r="R38" s="88"/>
-      <c r="S38" s="88"/>
-      <c r="T38" s="88"/>
-      <c r="U38" s="89"/>
+      <c r="G38" s="57"/>
+      <c r="H38" s="57"/>
+      <c r="I38" s="57"/>
+      <c r="J38" s="57"/>
+      <c r="K38" s="57"/>
+      <c r="L38" s="57"/>
+      <c r="M38" s="57"/>
+      <c r="N38" s="57"/>
+      <c r="O38" s="57"/>
+      <c r="P38" s="57"/>
+      <c r="Q38" s="57"/>
+      <c r="R38" s="57"/>
+      <c r="S38" s="57"/>
+      <c r="T38" s="57"/>
+      <c r="U38" s="58"/>
     </row>
     <row r="39" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F39" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="G39" s="72" t="s">
+      <c r="G39" s="59" t="s">
         <v>40</v>
       </c>
-      <c r="H39" s="72"/>
-      <c r="I39" s="72"/>
-      <c r="J39" s="72"/>
-      <c r="K39" s="72"/>
-      <c r="L39" s="72"/>
-      <c r="M39" s="72"/>
-      <c r="N39" s="72"/>
-      <c r="O39" s="72"/>
-      <c r="P39" s="72"/>
-      <c r="Q39" s="72"/>
-      <c r="R39" s="72"/>
-      <c r="S39" s="72"/>
-      <c r="T39" s="72"/>
-      <c r="U39" s="73"/>
+      <c r="H39" s="59"/>
+      <c r="I39" s="59"/>
+      <c r="J39" s="59"/>
+      <c r="K39" s="59"/>
+      <c r="L39" s="59"/>
+      <c r="M39" s="59"/>
+      <c r="N39" s="59"/>
+      <c r="O39" s="59"/>
+      <c r="P39" s="59"/>
+      <c r="Q39" s="59"/>
+      <c r="R39" s="59"/>
+      <c r="S39" s="59"/>
+      <c r="T39" s="59"/>
+      <c r="U39" s="60"/>
     </row>
     <row r="40" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F40" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="G40" s="72" t="s">
+      <c r="G40" s="59" t="s">
         <v>31</v>
       </c>
-      <c r="H40" s="72"/>
-      <c r="I40" s="72"/>
-      <c r="J40" s="72"/>
-      <c r="K40" s="72"/>
-      <c r="L40" s="72"/>
-      <c r="M40" s="72"/>
-      <c r="N40" s="72"/>
-      <c r="O40" s="72"/>
-      <c r="P40" s="72"/>
-      <c r="Q40" s="72"/>
-      <c r="R40" s="72"/>
-      <c r="S40" s="72"/>
-      <c r="T40" s="72"/>
-      <c r="U40" s="73"/>
+      <c r="H40" s="59"/>
+      <c r="I40" s="59"/>
+      <c r="J40" s="59"/>
+      <c r="K40" s="59"/>
+      <c r="L40" s="59"/>
+      <c r="M40" s="59"/>
+      <c r="N40" s="59"/>
+      <c r="O40" s="59"/>
+      <c r="P40" s="59"/>
+      <c r="Q40" s="59"/>
+      <c r="R40" s="59"/>
+      <c r="S40" s="59"/>
+      <c r="T40" s="59"/>
+      <c r="U40" s="60"/>
     </row>
     <row r="41" spans="6:21" x14ac:dyDescent="0.2">
       <c r="F41" s="41"/>
@@ -2764,189 +2764,216 @@
       <c r="F42" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="G42" s="72" t="s">
+      <c r="G42" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="H42" s="72"/>
-      <c r="I42" s="72"/>
-      <c r="J42" s="72"/>
-      <c r="K42" s="72"/>
-      <c r="L42" s="72"/>
-      <c r="M42" s="72"/>
-      <c r="N42" s="72"/>
-      <c r="O42" s="72"/>
-      <c r="P42" s="72"/>
-      <c r="Q42" s="72"/>
-      <c r="R42" s="72"/>
-      <c r="S42" s="72"/>
-      <c r="T42" s="72"/>
-      <c r="U42" s="73"/>
+      <c r="H42" s="59"/>
+      <c r="I42" s="59"/>
+      <c r="J42" s="59"/>
+      <c r="K42" s="59"/>
+      <c r="L42" s="59"/>
+      <c r="M42" s="59"/>
+      <c r="N42" s="59"/>
+      <c r="O42" s="59"/>
+      <c r="P42" s="59"/>
+      <c r="Q42" s="59"/>
+      <c r="R42" s="59"/>
+      <c r="S42" s="59"/>
+      <c r="T42" s="59"/>
+      <c r="U42" s="60"/>
     </row>
     <row r="43" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F43" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="G43" s="90" t="s">
+      <c r="G43" s="44" t="s">
         <v>42</v>
       </c>
-      <c r="H43" s="90"/>
-      <c r="I43" s="90"/>
-      <c r="J43" s="90"/>
-      <c r="K43" s="90"/>
-      <c r="L43" s="90"/>
-      <c r="M43" s="90"/>
-      <c r="N43" s="90"/>
-      <c r="O43" s="90"/>
-      <c r="P43" s="90"/>
-      <c r="Q43" s="90"/>
-      <c r="R43" s="90"/>
-      <c r="S43" s="90"/>
-      <c r="T43" s="90"/>
-      <c r="U43" s="91"/>
+      <c r="H43" s="44"/>
+      <c r="I43" s="44"/>
+      <c r="J43" s="44"/>
+      <c r="K43" s="44"/>
+      <c r="L43" s="44"/>
+      <c r="M43" s="44"/>
+      <c r="N43" s="44"/>
+      <c r="O43" s="44"/>
+      <c r="P43" s="44"/>
+      <c r="Q43" s="44"/>
+      <c r="R43" s="44"/>
+      <c r="S43" s="44"/>
+      <c r="T43" s="44"/>
+      <c r="U43" s="45"/>
     </row>
     <row r="49" spans="5:25" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="M49" s="65" t="s">
+      <c r="M49" s="93" t="s">
         <v>49</v>
       </c>
-      <c r="N49" s="65"/>
-      <c r="O49" s="65"/>
+      <c r="N49" s="93"/>
+      <c r="O49" s="93"/>
     </row>
     <row r="51" spans="5:25" x14ac:dyDescent="0.2">
-      <c r="G51" s="56" t="s">
+      <c r="G51" s="84" t="s">
         <v>50</v>
       </c>
-      <c r="H51" s="57"/>
-      <c r="I51" s="58"/>
-      <c r="K51" s="56" t="s">
+      <c r="H51" s="85"/>
+      <c r="I51" s="86"/>
+      <c r="K51" s="84" t="s">
         <v>51</v>
       </c>
-      <c r="L51" s="57"/>
-      <c r="M51" s="58"/>
-      <c r="O51" s="56" t="s">
+      <c r="L51" s="85"/>
+      <c r="M51" s="86"/>
+      <c r="O51" s="84" t="s">
         <v>52</v>
       </c>
-      <c r="P51" s="57"/>
-      <c r="Q51" s="58"/>
-      <c r="S51" s="56" t="s">
+      <c r="P51" s="85"/>
+      <c r="Q51" s="86"/>
+      <c r="S51" s="84" t="s">
         <v>53</v>
       </c>
-      <c r="T51" s="57"/>
-      <c r="U51" s="58"/>
+      <c r="T51" s="85"/>
+      <c r="U51" s="86"/>
     </row>
     <row r="52" spans="5:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G52" s="59"/>
-      <c r="H52" s="60"/>
-      <c r="I52" s="61"/>
-      <c r="K52" s="59"/>
-      <c r="L52" s="60"/>
-      <c r="M52" s="61"/>
-      <c r="O52" s="59"/>
-      <c r="P52" s="60"/>
-      <c r="Q52" s="61"/>
-      <c r="S52" s="59"/>
-      <c r="T52" s="60"/>
-      <c r="U52" s="61"/>
+      <c r="G52" s="87"/>
+      <c r="H52" s="88"/>
+      <c r="I52" s="89"/>
+      <c r="K52" s="87"/>
+      <c r="L52" s="88"/>
+      <c r="M52" s="89"/>
+      <c r="O52" s="87"/>
+      <c r="P52" s="88"/>
+      <c r="Q52" s="89"/>
+      <c r="S52" s="87"/>
+      <c r="T52" s="88"/>
+      <c r="U52" s="89"/>
     </row>
     <row r="53" spans="5:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G53" s="62"/>
-      <c r="H53" s="63"/>
-      <c r="I53" s="64"/>
-      <c r="K53" s="62"/>
-      <c r="L53" s="63"/>
-      <c r="M53" s="64"/>
-      <c r="O53" s="62"/>
-      <c r="P53" s="63"/>
-      <c r="Q53" s="64"/>
-      <c r="S53" s="62"/>
-      <c r="T53" s="63"/>
-      <c r="U53" s="64"/>
+      <c r="G53" s="90"/>
+      <c r="H53" s="91"/>
+      <c r="I53" s="92"/>
+      <c r="K53" s="90"/>
+      <c r="L53" s="91"/>
+      <c r="M53" s="92"/>
+      <c r="O53" s="90"/>
+      <c r="P53" s="91"/>
+      <c r="Q53" s="92"/>
+      <c r="S53" s="90"/>
+      <c r="T53" s="91"/>
+      <c r="U53" s="92"/>
     </row>
     <row r="62" spans="5:25" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E62" s="65" t="s">
+      <c r="E62" s="93" t="s">
         <v>60</v>
       </c>
-      <c r="F62" s="65"/>
-      <c r="G62" s="65"/>
-      <c r="H62" s="65"/>
-      <c r="P62" s="65" t="s">
+      <c r="F62" s="93"/>
+      <c r="G62" s="93"/>
+      <c r="H62" s="93"/>
+      <c r="P62" s="93" t="s">
         <v>61</v>
       </c>
-      <c r="Q62" s="65"/>
-      <c r="R62" s="65"/>
-      <c r="S62" s="65"/>
-      <c r="V62" s="65" t="s">
+      <c r="Q62" s="93"/>
+      <c r="R62" s="93"/>
+      <c r="S62" s="93"/>
+      <c r="V62" s="93" t="s">
         <v>62</v>
       </c>
-      <c r="W62" s="65"/>
-      <c r="X62" s="65"/>
-      <c r="Y62" s="65"/>
+      <c r="W62" s="93"/>
+      <c r="X62" s="93"/>
+      <c r="Y62" s="93"/>
     </row>
     <row r="63" spans="5:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="66" spans="3:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C66" s="66" t="s">
+      <c r="C66" s="94" t="s">
         <v>56</v>
       </c>
-      <c r="D66" s="67"/>
-      <c r="F66" s="66" t="s">
+      <c r="D66" s="95"/>
+      <c r="F66" s="94" t="s">
         <v>56</v>
       </c>
-      <c r="G66" s="67"/>
-      <c r="I66" s="66" t="s">
+      <c r="G66" s="95"/>
+      <c r="I66" s="94" t="s">
         <v>56</v>
       </c>
-      <c r="J66" s="67"/>
-      <c r="N66" s="44" t="s">
+      <c r="J66" s="95"/>
+      <c r="N66" s="72" t="s">
         <v>56</v>
       </c>
-      <c r="O66" s="45"/>
-      <c r="Q66" s="44" t="s">
+      <c r="O66" s="73"/>
+      <c r="Q66" s="72" t="s">
         <v>56</v>
       </c>
-      <c r="R66" s="45"/>
-      <c r="T66" s="44" t="s">
+      <c r="R66" s="73"/>
+      <c r="T66" s="72" t="s">
         <v>55</v>
       </c>
-      <c r="U66" s="45"/>
-      <c r="W66" s="50" t="s">
+      <c r="U66" s="73"/>
+      <c r="W66" s="78" t="s">
         <v>54</v>
       </c>
-      <c r="X66" s="51"/>
+      <c r="X66" s="79"/>
     </row>
     <row r="67" spans="3:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C67" s="68"/>
-      <c r="D67" s="69"/>
-      <c r="F67" s="68"/>
-      <c r="G67" s="69"/>
-      <c r="I67" s="68"/>
-      <c r="J67" s="69"/>
-      <c r="N67" s="46"/>
-      <c r="O67" s="47"/>
-      <c r="Q67" s="46"/>
-      <c r="R67" s="47"/>
-      <c r="T67" s="46"/>
-      <c r="U67" s="47"/>
-      <c r="W67" s="52"/>
-      <c r="X67" s="53"/>
+      <c r="C67" s="96"/>
+      <c r="D67" s="97"/>
+      <c r="F67" s="96"/>
+      <c r="G67" s="97"/>
+      <c r="I67" s="96"/>
+      <c r="J67" s="97"/>
+      <c r="N67" s="74"/>
+      <c r="O67" s="75"/>
+      <c r="Q67" s="74"/>
+      <c r="R67" s="75"/>
+      <c r="T67" s="74"/>
+      <c r="U67" s="75"/>
+      <c r="W67" s="80"/>
+      <c r="X67" s="81"/>
     </row>
     <row r="68" spans="3:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C68" s="70"/>
-      <c r="D68" s="71"/>
-      <c r="F68" s="70"/>
-      <c r="G68" s="71"/>
-      <c r="I68" s="70"/>
-      <c r="J68" s="71"/>
-      <c r="N68" s="48"/>
-      <c r="O68" s="49"/>
-      <c r="Q68" s="48"/>
-      <c r="R68" s="49"/>
-      <c r="T68" s="48"/>
-      <c r="U68" s="49"/>
-      <c r="W68" s="54"/>
-      <c r="X68" s="55"/>
+      <c r="C68" s="98"/>
+      <c r="D68" s="99"/>
+      <c r="F68" s="98"/>
+      <c r="G68" s="99"/>
+      <c r="I68" s="98"/>
+      <c r="J68" s="99"/>
+      <c r="N68" s="76"/>
+      <c r="O68" s="77"/>
+      <c r="Q68" s="76"/>
+      <c r="R68" s="77"/>
+      <c r="T68" s="76"/>
+      <c r="U68" s="77"/>
+      <c r="W68" s="82"/>
+      <c r="X68" s="83"/>
     </row>
     <row r="69" spans="3:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="43">
+    <mergeCell ref="T66:U68"/>
+    <mergeCell ref="W66:X68"/>
+    <mergeCell ref="S51:U53"/>
+    <mergeCell ref="M49:O49"/>
+    <mergeCell ref="C66:D68"/>
+    <mergeCell ref="F66:G68"/>
+    <mergeCell ref="I66:J68"/>
+    <mergeCell ref="N66:O68"/>
+    <mergeCell ref="Q66:R68"/>
+    <mergeCell ref="G51:I53"/>
+    <mergeCell ref="K51:M53"/>
+    <mergeCell ref="O51:Q53"/>
+    <mergeCell ref="E62:H62"/>
+    <mergeCell ref="P62:S62"/>
+    <mergeCell ref="V62:Y62"/>
+    <mergeCell ref="G39:U39"/>
+    <mergeCell ref="G40:U40"/>
+    <mergeCell ref="G30:U30"/>
+    <mergeCell ref="G31:U31"/>
+    <mergeCell ref="G32:U32"/>
+    <mergeCell ref="G33:U33"/>
+    <mergeCell ref="G34:U34"/>
+    <mergeCell ref="G24:U24"/>
+    <mergeCell ref="G35:U35"/>
+    <mergeCell ref="F17:U17"/>
+    <mergeCell ref="F28:U28"/>
+    <mergeCell ref="F38:U38"/>
     <mergeCell ref="G43:U43"/>
     <mergeCell ref="G29:U29"/>
     <mergeCell ref="F2:U2"/>
@@ -2963,33 +2990,6 @@
     <mergeCell ref="G15:U15"/>
     <mergeCell ref="G42:U42"/>
     <mergeCell ref="F23:U23"/>
-    <mergeCell ref="G24:U24"/>
-    <mergeCell ref="G35:U35"/>
-    <mergeCell ref="F17:U17"/>
-    <mergeCell ref="F28:U28"/>
-    <mergeCell ref="F38:U38"/>
-    <mergeCell ref="G39:U39"/>
-    <mergeCell ref="G40:U40"/>
-    <mergeCell ref="G30:U30"/>
-    <mergeCell ref="G31:U31"/>
-    <mergeCell ref="G32:U32"/>
-    <mergeCell ref="G33:U33"/>
-    <mergeCell ref="G34:U34"/>
-    <mergeCell ref="T66:U68"/>
-    <mergeCell ref="W66:X68"/>
-    <mergeCell ref="S51:U53"/>
-    <mergeCell ref="M49:O49"/>
-    <mergeCell ref="C66:D68"/>
-    <mergeCell ref="F66:G68"/>
-    <mergeCell ref="I66:J68"/>
-    <mergeCell ref="N66:O68"/>
-    <mergeCell ref="Q66:R68"/>
-    <mergeCell ref="G51:I53"/>
-    <mergeCell ref="K51:M53"/>
-    <mergeCell ref="O51:Q53"/>
-    <mergeCell ref="E62:H62"/>
-    <mergeCell ref="P62:S62"/>
-    <mergeCell ref="V62:Y62"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3932,6 +3932,14 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="F15:H15"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="F18:H18"/>
     <mergeCell ref="F12:H12"/>
     <mergeCell ref="E2:M2"/>
     <mergeCell ref="E4:E5"/>
@@ -3944,14 +3952,6 @@
     <mergeCell ref="F9:H9"/>
     <mergeCell ref="F10:H10"/>
     <mergeCell ref="F11:H11"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="F14:H14"/>
-    <mergeCell ref="F15:H15"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="F18:H18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="53" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
move to the new families sheet format
</commit_message>
<xml_diff>
--- a/cockpit_template.xlsx
+++ b/cockpit_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Roi.Dital/roid_playground/paamonim/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE3B73D5-58F7-1847-803C-B5B9DF2AC5D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32B18C83-3304-4445-A5C8-07106323E6B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="19440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="19440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="רציונל" sheetId="3" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="82">
   <si>
     <t>#</t>
   </si>
@@ -237,47 +237,81 @@
     <t xml:space="preserve">  משפחות שהסתיימו</t>
   </si>
   <si>
-    <t>מספר פגישות שהתקיימו (בוטלו)</t>
-  </si>
-  <si>
     <t>דוח משפחות פעילות</t>
   </si>
   <si>
-    <t>שיקוף/ביצוע אחרון</t>
+    <t>החזר חובות חודשי</t>
+  </si>
+  <si>
+    <t>חובות לא בהסדר</t>
+  </si>
+  <si>
+    <t>נושאים לבירור עם המלווה</t>
+  </si>
+  <si>
+    <t>פרטים אישיים</t>
+  </si>
+  <si>
+    <t>תאריכים ופגישות</t>
+  </si>
+  <si>
+    <t>תקציב אחרון</t>
+  </si>
+  <si>
+    <t>חובות</t>
+  </si>
+  <si>
+    <t>ביצוע אחרון</t>
+  </si>
+  <si>
+    <t>מזומן</t>
+  </si>
+  <si>
+    <t>ותק הליווי בימים</t>
+  </si>
+  <si>
+    <t>מספר פגישות שהתקיימו</t>
+  </si>
+  <si>
+    <t xml:space="preserve">מספר פגישות שבוטלו </t>
+  </si>
+  <si>
+    <t>הכנסות</t>
+  </si>
+  <si>
+    <t>הוצאות</t>
+  </si>
+  <si>
+    <t>הפרש</t>
+  </si>
+  <si>
+    <t>סך החובות</t>
   </si>
   <si>
     <t>רישום עו״ש אחרון</t>
   </si>
   <si>
-    <t>סה״כ חובות</t>
-  </si>
-  <si>
-    <t>תקציב</t>
-  </si>
-  <si>
-    <t>ותק ליווי</t>
-  </si>
-  <si>
-    <t>החזר חובות חודשי</t>
-  </si>
-  <si>
-    <t>חובות לא בהסדר</t>
-  </si>
-  <si>
-    <t>נושאים לבירור עם המלווה</t>
+    <t>יתרת עו״שׁ</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="177"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -417,6 +451,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="15">
     <fill>
@@ -503,7 +551,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -653,30 +701,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color indexed="64"/>
       </left>
       <right/>
@@ -693,106 +717,95 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="128">
+  <cellXfs count="138">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -804,290 +817,318 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1995,24 +2036,24 @@
   <sheetData>
     <row r="1" spans="6:21" ht="20" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F2" s="48" t="s">
+      <c r="F2" s="51" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="48"/>
-      <c r="H2" s="48"/>
-      <c r="I2" s="48"/>
-      <c r="J2" s="48"/>
-      <c r="K2" s="48"/>
-      <c r="L2" s="48"/>
-      <c r="M2" s="48"/>
-      <c r="N2" s="48"/>
-      <c r="O2" s="48"/>
-      <c r="P2" s="48"/>
-      <c r="Q2" s="48"/>
-      <c r="R2" s="48"/>
-      <c r="S2" s="48"/>
-      <c r="T2" s="48"/>
-      <c r="U2" s="48"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="51"/>
+      <c r="J2" s="51"/>
+      <c r="K2" s="51"/>
+      <c r="L2" s="51"/>
+      <c r="M2" s="51"/>
+      <c r="N2" s="51"/>
+      <c r="O2" s="51"/>
+      <c r="P2" s="51"/>
+      <c r="Q2" s="51"/>
+      <c r="R2" s="51"/>
+      <c r="S2" s="51"/>
+      <c r="T2" s="51"/>
+      <c r="U2" s="51"/>
     </row>
     <row r="3" spans="6:21" x14ac:dyDescent="0.2">
       <c r="F3" s="30"/>
@@ -2033,68 +2074,68 @@
       <c r="U3" s="30"/>
     </row>
     <row r="4" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F4" s="56" t="s">
+      <c r="F4" s="59" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="57"/>
-      <c r="H4" s="57"/>
-      <c r="I4" s="57"/>
-      <c r="J4" s="57"/>
-      <c r="K4" s="57"/>
-      <c r="L4" s="57"/>
-      <c r="M4" s="57"/>
-      <c r="N4" s="57"/>
-      <c r="O4" s="57"/>
-      <c r="P4" s="57"/>
-      <c r="Q4" s="57"/>
-      <c r="R4" s="57"/>
-      <c r="S4" s="57"/>
-      <c r="T4" s="57"/>
-      <c r="U4" s="58"/>
+      <c r="G4" s="60"/>
+      <c r="H4" s="60"/>
+      <c r="I4" s="60"/>
+      <c r="J4" s="60"/>
+      <c r="K4" s="60"/>
+      <c r="L4" s="60"/>
+      <c r="M4" s="60"/>
+      <c r="N4" s="60"/>
+      <c r="O4" s="60"/>
+      <c r="P4" s="60"/>
+      <c r="Q4" s="60"/>
+      <c r="R4" s="60"/>
+      <c r="S4" s="60"/>
+      <c r="T4" s="60"/>
+      <c r="U4" s="61"/>
     </row>
     <row r="5" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F5" s="35" t="s">
+      <c r="F5" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="59" t="s">
+      <c r="G5" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="H5" s="59"/>
-      <c r="I5" s="59"/>
-      <c r="J5" s="59"/>
-      <c r="K5" s="59"/>
-      <c r="L5" s="59"/>
-      <c r="M5" s="59"/>
-      <c r="N5" s="59"/>
-      <c r="O5" s="59"/>
-      <c r="P5" s="59"/>
-      <c r="Q5" s="59"/>
-      <c r="R5" s="59"/>
-      <c r="S5" s="59"/>
-      <c r="T5" s="59"/>
-      <c r="U5" s="60"/>
+      <c r="H5" s="62"/>
+      <c r="I5" s="62"/>
+      <c r="J5" s="62"/>
+      <c r="K5" s="62"/>
+      <c r="L5" s="62"/>
+      <c r="M5" s="62"/>
+      <c r="N5" s="62"/>
+      <c r="O5" s="62"/>
+      <c r="P5" s="62"/>
+      <c r="Q5" s="62"/>
+      <c r="R5" s="62"/>
+      <c r="S5" s="62"/>
+      <c r="T5" s="62"/>
+      <c r="U5" s="63"/>
     </row>
     <row r="6" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F6" s="38" t="s">
+      <c r="F6" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="44" t="s">
+      <c r="G6" s="47" t="s">
         <v>41</v>
       </c>
-      <c r="H6" s="44"/>
-      <c r="I6" s="44"/>
-      <c r="J6" s="44"/>
-      <c r="K6" s="44"/>
-      <c r="L6" s="44"/>
-      <c r="M6" s="44"/>
-      <c r="N6" s="44"/>
-      <c r="O6" s="44"/>
-      <c r="P6" s="44"/>
-      <c r="Q6" s="44"/>
-      <c r="R6" s="44"/>
-      <c r="S6" s="44"/>
-      <c r="T6" s="44"/>
-      <c r="U6" s="45"/>
+      <c r="H6" s="47"/>
+      <c r="I6" s="47"/>
+      <c r="J6" s="47"/>
+      <c r="K6" s="47"/>
+      <c r="L6" s="47"/>
+      <c r="M6" s="47"/>
+      <c r="N6" s="47"/>
+      <c r="O6" s="47"/>
+      <c r="P6" s="47"/>
+      <c r="Q6" s="47"/>
+      <c r="R6" s="47"/>
+      <c r="S6" s="47"/>
+      <c r="T6" s="47"/>
+      <c r="U6" s="48"/>
     </row>
     <row r="7" spans="6:21" x14ac:dyDescent="0.2">
       <c r="F7" s="31"/>
@@ -2115,46 +2156,46 @@
       <c r="U7" s="31"/>
     </row>
     <row r="8" spans="6:21" ht="26" x14ac:dyDescent="0.2">
-      <c r="F8" s="49" t="s">
+      <c r="F8" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="G8" s="50"/>
-      <c r="H8" s="50"/>
-      <c r="I8" s="50"/>
-      <c r="J8" s="50"/>
-      <c r="K8" s="50"/>
-      <c r="L8" s="50"/>
-      <c r="M8" s="50"/>
-      <c r="N8" s="50"/>
-      <c r="O8" s="50"/>
-      <c r="P8" s="50"/>
-      <c r="Q8" s="50"/>
-      <c r="R8" s="50"/>
-      <c r="S8" s="50"/>
-      <c r="T8" s="50"/>
-      <c r="U8" s="51"/>
+      <c r="G8" s="53"/>
+      <c r="H8" s="53"/>
+      <c r="I8" s="53"/>
+      <c r="J8" s="53"/>
+      <c r="K8" s="53"/>
+      <c r="L8" s="53"/>
+      <c r="M8" s="53"/>
+      <c r="N8" s="53"/>
+      <c r="O8" s="53"/>
+      <c r="P8" s="53"/>
+      <c r="Q8" s="53"/>
+      <c r="R8" s="53"/>
+      <c r="S8" s="53"/>
+      <c r="T8" s="53"/>
+      <c r="U8" s="54"/>
     </row>
     <row r="9" spans="6:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F9" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="G9" s="52" t="s">
+      <c r="G9" s="55" t="s">
         <v>59</v>
       </c>
-      <c r="H9" s="52"/>
-      <c r="I9" s="52"/>
-      <c r="J9" s="52"/>
-      <c r="K9" s="52"/>
-      <c r="L9" s="52"/>
-      <c r="M9" s="52"/>
-      <c r="N9" s="52"/>
-      <c r="O9" s="52"/>
-      <c r="P9" s="52"/>
-      <c r="Q9" s="52"/>
-      <c r="R9" s="52"/>
-      <c r="S9" s="52"/>
-      <c r="T9" s="52"/>
-      <c r="U9" s="53"/>
+      <c r="H9" s="55"/>
+      <c r="I9" s="55"/>
+      <c r="J9" s="55"/>
+      <c r="K9" s="55"/>
+      <c r="L9" s="55"/>
+      <c r="M9" s="55"/>
+      <c r="N9" s="55"/>
+      <c r="O9" s="55"/>
+      <c r="P9" s="55"/>
+      <c r="Q9" s="55"/>
+      <c r="R9" s="55"/>
+      <c r="S9" s="55"/>
+      <c r="T9" s="55"/>
+      <c r="U9" s="56"/>
     </row>
     <row r="10" spans="6:21" x14ac:dyDescent="0.2">
       <c r="F10" s="32"/>
@@ -2193,71 +2234,71 @@
       <c r="U12" s="32"/>
     </row>
     <row r="13" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F13" s="56" t="s">
+      <c r="F13" s="59" t="s">
         <v>57</v>
       </c>
-      <c r="G13" s="57"/>
-      <c r="H13" s="57"/>
-      <c r="I13" s="57"/>
-      <c r="J13" s="57"/>
-      <c r="K13" s="57"/>
-      <c r="L13" s="57"/>
-      <c r="M13" s="57"/>
-      <c r="N13" s="57"/>
-      <c r="O13" s="57"/>
-      <c r="P13" s="57"/>
-      <c r="Q13" s="57"/>
-      <c r="R13" s="57"/>
-      <c r="S13" s="57"/>
-      <c r="T13" s="57"/>
-      <c r="U13" s="58"/>
+      <c r="G13" s="60"/>
+      <c r="H13" s="60"/>
+      <c r="I13" s="60"/>
+      <c r="J13" s="60"/>
+      <c r="K13" s="60"/>
+      <c r="L13" s="60"/>
+      <c r="M13" s="60"/>
+      <c r="N13" s="60"/>
+      <c r="O13" s="60"/>
+      <c r="P13" s="60"/>
+      <c r="Q13" s="60"/>
+      <c r="R13" s="60"/>
+      <c r="S13" s="60"/>
+      <c r="T13" s="60"/>
+      <c r="U13" s="61"/>
     </row>
     <row r="14" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F14" s="35" t="s">
+      <c r="F14" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="G14" s="54" t="s">
+      <c r="G14" s="57" t="s">
         <v>43</v>
       </c>
-      <c r="H14" s="54"/>
-      <c r="I14" s="54"/>
-      <c r="J14" s="54"/>
-      <c r="K14" s="54"/>
-      <c r="L14" s="54"/>
-      <c r="M14" s="54"/>
-      <c r="N14" s="54"/>
-      <c r="O14" s="54"/>
-      <c r="P14" s="54"/>
-      <c r="Q14" s="54"/>
-      <c r="R14" s="54"/>
-      <c r="S14" s="54"/>
-      <c r="T14" s="54"/>
-      <c r="U14" s="55"/>
+      <c r="H14" s="57"/>
+      <c r="I14" s="57"/>
+      <c r="J14" s="57"/>
+      <c r="K14" s="57"/>
+      <c r="L14" s="57"/>
+      <c r="M14" s="57"/>
+      <c r="N14" s="57"/>
+      <c r="O14" s="57"/>
+      <c r="P14" s="57"/>
+      <c r="Q14" s="57"/>
+      <c r="R14" s="57"/>
+      <c r="S14" s="57"/>
+      <c r="T14" s="57"/>
+      <c r="U14" s="58"/>
     </row>
     <row r="15" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F15" s="35" t="s">
+      <c r="F15" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="G15" s="54" t="s">
+      <c r="G15" s="57" t="s">
         <v>48</v>
       </c>
-      <c r="H15" s="54"/>
-      <c r="I15" s="54"/>
-      <c r="J15" s="54"/>
-      <c r="K15" s="54"/>
-      <c r="L15" s="54"/>
-      <c r="M15" s="54"/>
-      <c r="N15" s="54"/>
-      <c r="O15" s="54"/>
-      <c r="P15" s="54"/>
-      <c r="Q15" s="54"/>
-      <c r="R15" s="54"/>
-      <c r="S15" s="54"/>
-      <c r="T15" s="54"/>
-      <c r="U15" s="55"/>
+      <c r="H15" s="57"/>
+      <c r="I15" s="57"/>
+      <c r="J15" s="57"/>
+      <c r="K15" s="57"/>
+      <c r="L15" s="57"/>
+      <c r="M15" s="57"/>
+      <c r="N15" s="57"/>
+      <c r="O15" s="57"/>
+      <c r="P15" s="57"/>
+      <c r="Q15" s="57"/>
+      <c r="R15" s="57"/>
+      <c r="S15" s="57"/>
+      <c r="T15" s="57"/>
+      <c r="U15" s="58"/>
     </row>
     <row r="16" spans="6:21" x14ac:dyDescent="0.2">
-      <c r="F16" s="36"/>
+      <c r="F16" s="35"/>
       <c r="G16" s="32"/>
       <c r="H16" s="32"/>
       <c r="I16" s="32"/>
@@ -2272,52 +2313,52 @@
       <c r="R16" s="32"/>
       <c r="S16" s="32"/>
       <c r="T16" s="32"/>
-      <c r="U16" s="37"/>
+      <c r="U16" s="36"/>
     </row>
     <row r="17" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F17" s="61" t="s">
+      <c r="F17" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="G17" s="62"/>
-      <c r="H17" s="62"/>
-      <c r="I17" s="62"/>
-      <c r="J17" s="62"/>
-      <c r="K17" s="62"/>
-      <c r="L17" s="62"/>
-      <c r="M17" s="62"/>
-      <c r="N17" s="62"/>
-      <c r="O17" s="62"/>
-      <c r="P17" s="62"/>
-      <c r="Q17" s="62"/>
-      <c r="R17" s="62"/>
-      <c r="S17" s="62"/>
-      <c r="T17" s="62"/>
-      <c r="U17" s="63"/>
+      <c r="G17" s="65"/>
+      <c r="H17" s="65"/>
+      <c r="I17" s="65"/>
+      <c r="J17" s="65"/>
+      <c r="K17" s="65"/>
+      <c r="L17" s="65"/>
+      <c r="M17" s="65"/>
+      <c r="N17" s="65"/>
+      <c r="O17" s="65"/>
+      <c r="P17" s="65"/>
+      <c r="Q17" s="65"/>
+      <c r="R17" s="65"/>
+      <c r="S17" s="65"/>
+      <c r="T17" s="65"/>
+      <c r="U17" s="66"/>
     </row>
     <row r="18" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F18" s="35" t="s">
+      <c r="F18" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="G18" s="54" t="s">
+      <c r="G18" s="57" t="s">
         <v>47</v>
       </c>
-      <c r="H18" s="54"/>
-      <c r="I18" s="54"/>
-      <c r="J18" s="54"/>
-      <c r="K18" s="54"/>
-      <c r="L18" s="54"/>
-      <c r="M18" s="54"/>
-      <c r="N18" s="54"/>
-      <c r="O18" s="54"/>
-      <c r="P18" s="54"/>
-      <c r="Q18" s="54"/>
-      <c r="R18" s="54"/>
-      <c r="S18" s="54"/>
-      <c r="T18" s="54"/>
-      <c r="U18" s="55"/>
+      <c r="H18" s="57"/>
+      <c r="I18" s="57"/>
+      <c r="J18" s="57"/>
+      <c r="K18" s="57"/>
+      <c r="L18" s="57"/>
+      <c r="M18" s="57"/>
+      <c r="N18" s="57"/>
+      <c r="O18" s="57"/>
+      <c r="P18" s="57"/>
+      <c r="Q18" s="57"/>
+      <c r="R18" s="57"/>
+      <c r="S18" s="57"/>
+      <c r="T18" s="57"/>
+      <c r="U18" s="58"/>
     </row>
     <row r="19" spans="6:21" x14ac:dyDescent="0.2">
-      <c r="F19" s="36"/>
+      <c r="F19" s="35"/>
       <c r="G19" s="32"/>
       <c r="H19" s="32"/>
       <c r="I19" s="32"/>
@@ -2332,52 +2373,52 @@
       <c r="R19" s="32"/>
       <c r="S19" s="32"/>
       <c r="T19" s="32"/>
-      <c r="U19" s="37"/>
+      <c r="U19" s="36"/>
     </row>
     <row r="20" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F20" s="61" t="s">
+      <c r="F20" s="64" t="s">
         <v>44</v>
       </c>
-      <c r="G20" s="62"/>
-      <c r="H20" s="62"/>
-      <c r="I20" s="62"/>
-      <c r="J20" s="62"/>
-      <c r="K20" s="62"/>
-      <c r="L20" s="62"/>
-      <c r="M20" s="62"/>
-      <c r="N20" s="62"/>
-      <c r="O20" s="62"/>
-      <c r="P20" s="62"/>
-      <c r="Q20" s="62"/>
-      <c r="R20" s="62"/>
-      <c r="S20" s="62"/>
-      <c r="T20" s="62"/>
-      <c r="U20" s="63"/>
+      <c r="G20" s="65"/>
+      <c r="H20" s="65"/>
+      <c r="I20" s="65"/>
+      <c r="J20" s="65"/>
+      <c r="K20" s="65"/>
+      <c r="L20" s="65"/>
+      <c r="M20" s="65"/>
+      <c r="N20" s="65"/>
+      <c r="O20" s="65"/>
+      <c r="P20" s="65"/>
+      <c r="Q20" s="65"/>
+      <c r="R20" s="65"/>
+      <c r="S20" s="65"/>
+      <c r="T20" s="65"/>
+      <c r="U20" s="66"/>
     </row>
     <row r="21" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F21" s="35" t="s">
+      <c r="F21" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="G21" s="54" t="s">
+      <c r="G21" s="57" t="s">
         <v>58</v>
       </c>
-      <c r="H21" s="54"/>
-      <c r="I21" s="54"/>
-      <c r="J21" s="54"/>
-      <c r="K21" s="54"/>
-      <c r="L21" s="54"/>
-      <c r="M21" s="54"/>
-      <c r="N21" s="54"/>
-      <c r="O21" s="54"/>
-      <c r="P21" s="54"/>
-      <c r="Q21" s="54"/>
-      <c r="R21" s="54"/>
-      <c r="S21" s="54"/>
-      <c r="T21" s="54"/>
-      <c r="U21" s="55"/>
+      <c r="H21" s="57"/>
+      <c r="I21" s="57"/>
+      <c r="J21" s="57"/>
+      <c r="K21" s="57"/>
+      <c r="L21" s="57"/>
+      <c r="M21" s="57"/>
+      <c r="N21" s="57"/>
+      <c r="O21" s="57"/>
+      <c r="P21" s="57"/>
+      <c r="Q21" s="57"/>
+      <c r="R21" s="57"/>
+      <c r="S21" s="57"/>
+      <c r="T21" s="57"/>
+      <c r="U21" s="58"/>
     </row>
     <row r="22" spans="6:21" x14ac:dyDescent="0.2">
-      <c r="F22" s="36"/>
+      <c r="F22" s="35"/>
       <c r="G22" s="32"/>
       <c r="H22" s="32"/>
       <c r="I22" s="32"/>
@@ -2392,49 +2433,49 @@
       <c r="R22" s="32"/>
       <c r="S22" s="32"/>
       <c r="T22" s="32"/>
-      <c r="U22" s="37"/>
+      <c r="U22" s="36"/>
     </row>
     <row r="23" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F23" s="61" t="s">
+      <c r="F23" s="64" t="s">
         <v>45</v>
       </c>
-      <c r="G23" s="62"/>
-      <c r="H23" s="62"/>
-      <c r="I23" s="62"/>
-      <c r="J23" s="62"/>
-      <c r="K23" s="62"/>
-      <c r="L23" s="62"/>
-      <c r="M23" s="62"/>
-      <c r="N23" s="62"/>
-      <c r="O23" s="62"/>
-      <c r="P23" s="62"/>
-      <c r="Q23" s="62"/>
-      <c r="R23" s="62"/>
-      <c r="S23" s="62"/>
-      <c r="T23" s="62"/>
-      <c r="U23" s="63"/>
+      <c r="G23" s="65"/>
+      <c r="H23" s="65"/>
+      <c r="I23" s="65"/>
+      <c r="J23" s="65"/>
+      <c r="K23" s="65"/>
+      <c r="L23" s="65"/>
+      <c r="M23" s="65"/>
+      <c r="N23" s="65"/>
+      <c r="O23" s="65"/>
+      <c r="P23" s="65"/>
+      <c r="Q23" s="65"/>
+      <c r="R23" s="65"/>
+      <c r="S23" s="65"/>
+      <c r="T23" s="65"/>
+      <c r="U23" s="66"/>
     </row>
     <row r="24" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F24" s="38" t="s">
+      <c r="F24" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="G24" s="64" t="s">
+      <c r="G24" s="67" t="s">
         <v>46</v>
       </c>
-      <c r="H24" s="64"/>
-      <c r="I24" s="64"/>
-      <c r="J24" s="64"/>
-      <c r="K24" s="64"/>
-      <c r="L24" s="64"/>
-      <c r="M24" s="64"/>
-      <c r="N24" s="64"/>
-      <c r="O24" s="64"/>
-      <c r="P24" s="64"/>
-      <c r="Q24" s="64"/>
-      <c r="R24" s="64"/>
-      <c r="S24" s="64"/>
-      <c r="T24" s="64"/>
-      <c r="U24" s="65"/>
+      <c r="H24" s="67"/>
+      <c r="I24" s="67"/>
+      <c r="J24" s="67"/>
+      <c r="K24" s="67"/>
+      <c r="L24" s="67"/>
+      <c r="M24" s="67"/>
+      <c r="N24" s="67"/>
+      <c r="O24" s="67"/>
+      <c r="P24" s="67"/>
+      <c r="Q24" s="67"/>
+      <c r="R24" s="67"/>
+      <c r="S24" s="67"/>
+      <c r="T24" s="67"/>
+      <c r="U24" s="68"/>
     </row>
     <row r="25" spans="6:21" x14ac:dyDescent="0.2">
       <c r="F25" s="32"/>
@@ -2491,174 +2532,174 @@
       <c r="U27" s="32"/>
     </row>
     <row r="28" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F28" s="67" t="s">
+      <c r="F28" s="70" t="s">
         <v>16</v>
       </c>
-      <c r="G28" s="68"/>
-      <c r="H28" s="68"/>
-      <c r="I28" s="68"/>
-      <c r="J28" s="68"/>
-      <c r="K28" s="68"/>
-      <c r="L28" s="68"/>
-      <c r="M28" s="68"/>
-      <c r="N28" s="68"/>
-      <c r="O28" s="68"/>
-      <c r="P28" s="68"/>
-      <c r="Q28" s="68"/>
-      <c r="R28" s="68"/>
-      <c r="S28" s="68"/>
-      <c r="T28" s="68"/>
-      <c r="U28" s="69"/>
+      <c r="G28" s="71"/>
+      <c r="H28" s="71"/>
+      <c r="I28" s="71"/>
+      <c r="J28" s="71"/>
+      <c r="K28" s="71"/>
+      <c r="L28" s="71"/>
+      <c r="M28" s="71"/>
+      <c r="N28" s="71"/>
+      <c r="O28" s="71"/>
+      <c r="P28" s="71"/>
+      <c r="Q28" s="71"/>
+      <c r="R28" s="71"/>
+      <c r="S28" s="71"/>
+      <c r="T28" s="71"/>
+      <c r="U28" s="72"/>
     </row>
     <row r="29" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F29" s="39" t="s">
+      <c r="F29" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="G29" s="46" t="s">
+      <c r="G29" s="49" t="s">
         <v>25</v>
       </c>
-      <c r="H29" s="46"/>
-      <c r="I29" s="46"/>
-      <c r="J29" s="46"/>
-      <c r="K29" s="46"/>
-      <c r="L29" s="46"/>
-      <c r="M29" s="46"/>
-      <c r="N29" s="46"/>
-      <c r="O29" s="46"/>
-      <c r="P29" s="46"/>
-      <c r="Q29" s="46"/>
-      <c r="R29" s="46"/>
-      <c r="S29" s="46"/>
-      <c r="T29" s="46"/>
-      <c r="U29" s="47"/>
+      <c r="H29" s="49"/>
+      <c r="I29" s="49"/>
+      <c r="J29" s="49"/>
+      <c r="K29" s="49"/>
+      <c r="L29" s="49"/>
+      <c r="M29" s="49"/>
+      <c r="N29" s="49"/>
+      <c r="O29" s="49"/>
+      <c r="P29" s="49"/>
+      <c r="Q29" s="49"/>
+      <c r="R29" s="49"/>
+      <c r="S29" s="49"/>
+      <c r="T29" s="49"/>
+      <c r="U29" s="50"/>
     </row>
     <row r="30" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F30" s="39" t="s">
+      <c r="F30" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="G30" s="46" t="s">
+      <c r="G30" s="49" t="s">
         <v>21</v>
       </c>
-      <c r="H30" s="46"/>
-      <c r="I30" s="46"/>
-      <c r="J30" s="46"/>
-      <c r="K30" s="46"/>
-      <c r="L30" s="46"/>
-      <c r="M30" s="46"/>
-      <c r="N30" s="46"/>
-      <c r="O30" s="46"/>
-      <c r="P30" s="46"/>
-      <c r="Q30" s="46"/>
-      <c r="R30" s="46"/>
-      <c r="S30" s="46"/>
-      <c r="T30" s="46"/>
-      <c r="U30" s="47"/>
+      <c r="H30" s="49"/>
+      <c r="I30" s="49"/>
+      <c r="J30" s="49"/>
+      <c r="K30" s="49"/>
+      <c r="L30" s="49"/>
+      <c r="M30" s="49"/>
+      <c r="N30" s="49"/>
+      <c r="O30" s="49"/>
+      <c r="P30" s="49"/>
+      <c r="Q30" s="49"/>
+      <c r="R30" s="49"/>
+      <c r="S30" s="49"/>
+      <c r="T30" s="49"/>
+      <c r="U30" s="50"/>
     </row>
     <row r="31" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F31" s="39" t="s">
+      <c r="F31" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="G31" s="46" t="s">
+      <c r="G31" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="H31" s="46"/>
-      <c r="I31" s="46"/>
-      <c r="J31" s="46"/>
-      <c r="K31" s="46"/>
-      <c r="L31" s="46"/>
-      <c r="M31" s="46"/>
-      <c r="N31" s="46"/>
-      <c r="O31" s="46"/>
-      <c r="P31" s="46"/>
-      <c r="Q31" s="46"/>
-      <c r="R31" s="46"/>
-      <c r="S31" s="46"/>
-      <c r="T31" s="46"/>
-      <c r="U31" s="47"/>
+      <c r="H31" s="49"/>
+      <c r="I31" s="49"/>
+      <c r="J31" s="49"/>
+      <c r="K31" s="49"/>
+      <c r="L31" s="49"/>
+      <c r="M31" s="49"/>
+      <c r="N31" s="49"/>
+      <c r="O31" s="49"/>
+      <c r="P31" s="49"/>
+      <c r="Q31" s="49"/>
+      <c r="R31" s="49"/>
+      <c r="S31" s="49"/>
+      <c r="T31" s="49"/>
+      <c r="U31" s="50"/>
     </row>
     <row r="32" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F32" s="39" t="s">
+      <c r="F32" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="G32" s="46" t="s">
+      <c r="G32" s="49" t="s">
         <v>28</v>
       </c>
-      <c r="H32" s="46"/>
-      <c r="I32" s="46"/>
-      <c r="J32" s="46"/>
-      <c r="K32" s="46"/>
-      <c r="L32" s="46"/>
-      <c r="M32" s="46"/>
-      <c r="N32" s="46"/>
-      <c r="O32" s="46"/>
-      <c r="P32" s="46"/>
-      <c r="Q32" s="46"/>
-      <c r="R32" s="46"/>
-      <c r="S32" s="46"/>
-      <c r="T32" s="46"/>
-      <c r="U32" s="47"/>
+      <c r="H32" s="49"/>
+      <c r="I32" s="49"/>
+      <c r="J32" s="49"/>
+      <c r="K32" s="49"/>
+      <c r="L32" s="49"/>
+      <c r="M32" s="49"/>
+      <c r="N32" s="49"/>
+      <c r="O32" s="49"/>
+      <c r="P32" s="49"/>
+      <c r="Q32" s="49"/>
+      <c r="R32" s="49"/>
+      <c r="S32" s="49"/>
+      <c r="T32" s="49"/>
+      <c r="U32" s="50"/>
     </row>
     <row r="33" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F33" s="39" t="s">
+      <c r="F33" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="G33" s="46" t="s">
+      <c r="G33" s="49" t="s">
         <v>27</v>
       </c>
-      <c r="H33" s="46"/>
-      <c r="I33" s="46"/>
-      <c r="J33" s="46"/>
-      <c r="K33" s="46"/>
-      <c r="L33" s="46"/>
-      <c r="M33" s="46"/>
-      <c r="N33" s="46"/>
-      <c r="O33" s="46"/>
-      <c r="P33" s="46"/>
-      <c r="Q33" s="46"/>
-      <c r="R33" s="46"/>
-      <c r="S33" s="46"/>
-      <c r="T33" s="46"/>
-      <c r="U33" s="47"/>
+      <c r="H33" s="49"/>
+      <c r="I33" s="49"/>
+      <c r="J33" s="49"/>
+      <c r="K33" s="49"/>
+      <c r="L33" s="49"/>
+      <c r="M33" s="49"/>
+      <c r="N33" s="49"/>
+      <c r="O33" s="49"/>
+      <c r="P33" s="49"/>
+      <c r="Q33" s="49"/>
+      <c r="R33" s="49"/>
+      <c r="S33" s="49"/>
+      <c r="T33" s="49"/>
+      <c r="U33" s="50"/>
     </row>
     <row r="34" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F34" s="40" t="s">
+      <c r="F34" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="G34" s="70" t="s">
+      <c r="G34" s="73" t="s">
         <v>30</v>
       </c>
-      <c r="H34" s="70"/>
-      <c r="I34" s="70"/>
-      <c r="J34" s="70"/>
-      <c r="K34" s="70"/>
-      <c r="L34" s="70"/>
-      <c r="M34" s="70"/>
-      <c r="N34" s="70"/>
-      <c r="O34" s="70"/>
-      <c r="P34" s="70"/>
-      <c r="Q34" s="70"/>
-      <c r="R34" s="70"/>
-      <c r="S34" s="70"/>
-      <c r="T34" s="70"/>
-      <c r="U34" s="71"/>
+      <c r="H34" s="73"/>
+      <c r="I34" s="73"/>
+      <c r="J34" s="73"/>
+      <c r="K34" s="73"/>
+      <c r="L34" s="73"/>
+      <c r="M34" s="73"/>
+      <c r="N34" s="73"/>
+      <c r="O34" s="73"/>
+      <c r="P34" s="73"/>
+      <c r="Q34" s="73"/>
+      <c r="R34" s="73"/>
+      <c r="S34" s="73"/>
+      <c r="T34" s="73"/>
+      <c r="U34" s="74"/>
     </row>
     <row r="35" spans="6:21" x14ac:dyDescent="0.2">
       <c r="F35" s="32"/>
-      <c r="G35" s="66"/>
-      <c r="H35" s="66"/>
-      <c r="I35" s="66"/>
-      <c r="J35" s="66"/>
-      <c r="K35" s="66"/>
-      <c r="L35" s="66"/>
-      <c r="M35" s="66"/>
-      <c r="N35" s="66"/>
-      <c r="O35" s="66"/>
-      <c r="P35" s="66"/>
-      <c r="Q35" s="66"/>
-      <c r="R35" s="66"/>
-      <c r="S35" s="66"/>
-      <c r="T35" s="66"/>
-      <c r="U35" s="66"/>
+      <c r="G35" s="69"/>
+      <c r="H35" s="69"/>
+      <c r="I35" s="69"/>
+      <c r="J35" s="69"/>
+      <c r="K35" s="69"/>
+      <c r="L35" s="69"/>
+      <c r="M35" s="69"/>
+      <c r="N35" s="69"/>
+      <c r="O35" s="69"/>
+      <c r="P35" s="69"/>
+      <c r="Q35" s="69"/>
+      <c r="R35" s="69"/>
+      <c r="S35" s="69"/>
+      <c r="T35" s="69"/>
+      <c r="U35" s="69"/>
     </row>
     <row r="37" spans="6:21" x14ac:dyDescent="0.2">
       <c r="F37" s="32"/>
@@ -2679,71 +2720,71 @@
       <c r="U37" s="32"/>
     </row>
     <row r="38" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F38" s="56" t="s">
+      <c r="F38" s="59" t="s">
         <v>20</v>
       </c>
-      <c r="G38" s="57"/>
-      <c r="H38" s="57"/>
-      <c r="I38" s="57"/>
-      <c r="J38" s="57"/>
-      <c r="K38" s="57"/>
-      <c r="L38" s="57"/>
-      <c r="M38" s="57"/>
-      <c r="N38" s="57"/>
-      <c r="O38" s="57"/>
-      <c r="P38" s="57"/>
-      <c r="Q38" s="57"/>
-      <c r="R38" s="57"/>
-      <c r="S38" s="57"/>
-      <c r="T38" s="57"/>
-      <c r="U38" s="58"/>
+      <c r="G38" s="60"/>
+      <c r="H38" s="60"/>
+      <c r="I38" s="60"/>
+      <c r="J38" s="60"/>
+      <c r="K38" s="60"/>
+      <c r="L38" s="60"/>
+      <c r="M38" s="60"/>
+      <c r="N38" s="60"/>
+      <c r="O38" s="60"/>
+      <c r="P38" s="60"/>
+      <c r="Q38" s="60"/>
+      <c r="R38" s="60"/>
+      <c r="S38" s="60"/>
+      <c r="T38" s="60"/>
+      <c r="U38" s="61"/>
     </row>
     <row r="39" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F39" s="35" t="s">
+      <c r="F39" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="G39" s="59" t="s">
+      <c r="G39" s="62" t="s">
         <v>40</v>
       </c>
-      <c r="H39" s="59"/>
-      <c r="I39" s="59"/>
-      <c r="J39" s="59"/>
-      <c r="K39" s="59"/>
-      <c r="L39" s="59"/>
-      <c r="M39" s="59"/>
-      <c r="N39" s="59"/>
-      <c r="O39" s="59"/>
-      <c r="P39" s="59"/>
-      <c r="Q39" s="59"/>
-      <c r="R39" s="59"/>
-      <c r="S39" s="59"/>
-      <c r="T39" s="59"/>
-      <c r="U39" s="60"/>
+      <c r="H39" s="62"/>
+      <c r="I39" s="62"/>
+      <c r="J39" s="62"/>
+      <c r="K39" s="62"/>
+      <c r="L39" s="62"/>
+      <c r="M39" s="62"/>
+      <c r="N39" s="62"/>
+      <c r="O39" s="62"/>
+      <c r="P39" s="62"/>
+      <c r="Q39" s="62"/>
+      <c r="R39" s="62"/>
+      <c r="S39" s="62"/>
+      <c r="T39" s="62"/>
+      <c r="U39" s="63"/>
     </row>
     <row r="40" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F40" s="35" t="s">
+      <c r="F40" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="G40" s="59" t="s">
+      <c r="G40" s="62" t="s">
         <v>31</v>
       </c>
-      <c r="H40" s="59"/>
-      <c r="I40" s="59"/>
-      <c r="J40" s="59"/>
-      <c r="K40" s="59"/>
-      <c r="L40" s="59"/>
-      <c r="M40" s="59"/>
-      <c r="N40" s="59"/>
-      <c r="O40" s="59"/>
-      <c r="P40" s="59"/>
-      <c r="Q40" s="59"/>
-      <c r="R40" s="59"/>
-      <c r="S40" s="59"/>
-      <c r="T40" s="59"/>
-      <c r="U40" s="60"/>
+      <c r="H40" s="62"/>
+      <c r="I40" s="62"/>
+      <c r="J40" s="62"/>
+      <c r="K40" s="62"/>
+      <c r="L40" s="62"/>
+      <c r="M40" s="62"/>
+      <c r="N40" s="62"/>
+      <c r="O40" s="62"/>
+      <c r="P40" s="62"/>
+      <c r="Q40" s="62"/>
+      <c r="R40" s="62"/>
+      <c r="S40" s="62"/>
+      <c r="T40" s="62"/>
+      <c r="U40" s="63"/>
     </row>
     <row r="41" spans="6:21" x14ac:dyDescent="0.2">
-      <c r="F41" s="41"/>
+      <c r="F41" s="40"/>
       <c r="G41" s="31"/>
       <c r="H41" s="31"/>
       <c r="I41" s="31"/>
@@ -2758,191 +2799,191 @@
       <c r="R41" s="31"/>
       <c r="S41" s="31"/>
       <c r="T41" s="31"/>
-      <c r="U41" s="42"/>
+      <c r="U41" s="41"/>
     </row>
     <row r="42" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F42" s="35" t="s">
+      <c r="F42" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="G42" s="59" t="s">
+      <c r="G42" s="62" t="s">
         <v>29</v>
       </c>
-      <c r="H42" s="59"/>
-      <c r="I42" s="59"/>
-      <c r="J42" s="59"/>
-      <c r="K42" s="59"/>
-      <c r="L42" s="59"/>
-      <c r="M42" s="59"/>
-      <c r="N42" s="59"/>
-      <c r="O42" s="59"/>
-      <c r="P42" s="59"/>
-      <c r="Q42" s="59"/>
-      <c r="R42" s="59"/>
-      <c r="S42" s="59"/>
-      <c r="T42" s="59"/>
-      <c r="U42" s="60"/>
+      <c r="H42" s="62"/>
+      <c r="I42" s="62"/>
+      <c r="J42" s="62"/>
+      <c r="K42" s="62"/>
+      <c r="L42" s="62"/>
+      <c r="M42" s="62"/>
+      <c r="N42" s="62"/>
+      <c r="O42" s="62"/>
+      <c r="P42" s="62"/>
+      <c r="Q42" s="62"/>
+      <c r="R42" s="62"/>
+      <c r="S42" s="62"/>
+      <c r="T42" s="62"/>
+      <c r="U42" s="63"/>
     </row>
     <row r="43" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F43" s="38" t="s">
+      <c r="F43" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="G43" s="44" t="s">
+      <c r="G43" s="47" t="s">
         <v>42</v>
       </c>
-      <c r="H43" s="44"/>
-      <c r="I43" s="44"/>
-      <c r="J43" s="44"/>
-      <c r="K43" s="44"/>
-      <c r="L43" s="44"/>
-      <c r="M43" s="44"/>
-      <c r="N43" s="44"/>
-      <c r="O43" s="44"/>
-      <c r="P43" s="44"/>
-      <c r="Q43" s="44"/>
-      <c r="R43" s="44"/>
-      <c r="S43" s="44"/>
-      <c r="T43" s="44"/>
-      <c r="U43" s="45"/>
+      <c r="H43" s="47"/>
+      <c r="I43" s="47"/>
+      <c r="J43" s="47"/>
+      <c r="K43" s="47"/>
+      <c r="L43" s="47"/>
+      <c r="M43" s="47"/>
+      <c r="N43" s="47"/>
+      <c r="O43" s="47"/>
+      <c r="P43" s="47"/>
+      <c r="Q43" s="47"/>
+      <c r="R43" s="47"/>
+      <c r="S43" s="47"/>
+      <c r="T43" s="47"/>
+      <c r="U43" s="48"/>
     </row>
     <row r="49" spans="5:25" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="M49" s="93" t="s">
+      <c r="M49" s="96" t="s">
         <v>49</v>
       </c>
-      <c r="N49" s="93"/>
-      <c r="O49" s="93"/>
+      <c r="N49" s="96"/>
+      <c r="O49" s="96"/>
     </row>
     <row r="51" spans="5:25" x14ac:dyDescent="0.2">
-      <c r="G51" s="84" t="s">
+      <c r="G51" s="87" t="s">
         <v>50</v>
       </c>
-      <c r="H51" s="85"/>
-      <c r="I51" s="86"/>
-      <c r="K51" s="84" t="s">
+      <c r="H51" s="88"/>
+      <c r="I51" s="89"/>
+      <c r="K51" s="87" t="s">
         <v>51</v>
       </c>
-      <c r="L51" s="85"/>
-      <c r="M51" s="86"/>
-      <c r="O51" s="84" t="s">
+      <c r="L51" s="88"/>
+      <c r="M51" s="89"/>
+      <c r="O51" s="87" t="s">
         <v>52</v>
       </c>
-      <c r="P51" s="85"/>
-      <c r="Q51" s="86"/>
-      <c r="S51" s="84" t="s">
+      <c r="P51" s="88"/>
+      <c r="Q51" s="89"/>
+      <c r="S51" s="87" t="s">
         <v>53</v>
       </c>
-      <c r="T51" s="85"/>
-      <c r="U51" s="86"/>
+      <c r="T51" s="88"/>
+      <c r="U51" s="89"/>
     </row>
     <row r="52" spans="5:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G52" s="87"/>
-      <c r="H52" s="88"/>
-      <c r="I52" s="89"/>
-      <c r="K52" s="87"/>
-      <c r="L52" s="88"/>
-      <c r="M52" s="89"/>
-      <c r="O52" s="87"/>
-      <c r="P52" s="88"/>
-      <c r="Q52" s="89"/>
-      <c r="S52" s="87"/>
-      <c r="T52" s="88"/>
-      <c r="U52" s="89"/>
+      <c r="G52" s="90"/>
+      <c r="H52" s="91"/>
+      <c r="I52" s="92"/>
+      <c r="K52" s="90"/>
+      <c r="L52" s="91"/>
+      <c r="M52" s="92"/>
+      <c r="O52" s="90"/>
+      <c r="P52" s="91"/>
+      <c r="Q52" s="92"/>
+      <c r="S52" s="90"/>
+      <c r="T52" s="91"/>
+      <c r="U52" s="92"/>
     </row>
     <row r="53" spans="5:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G53" s="90"/>
-      <c r="H53" s="91"/>
-      <c r="I53" s="92"/>
-      <c r="K53" s="90"/>
-      <c r="L53" s="91"/>
-      <c r="M53" s="92"/>
-      <c r="O53" s="90"/>
-      <c r="P53" s="91"/>
-      <c r="Q53" s="92"/>
-      <c r="S53" s="90"/>
-      <c r="T53" s="91"/>
-      <c r="U53" s="92"/>
+      <c r="G53" s="93"/>
+      <c r="H53" s="94"/>
+      <c r="I53" s="95"/>
+      <c r="K53" s="93"/>
+      <c r="L53" s="94"/>
+      <c r="M53" s="95"/>
+      <c r="O53" s="93"/>
+      <c r="P53" s="94"/>
+      <c r="Q53" s="95"/>
+      <c r="S53" s="93"/>
+      <c r="T53" s="94"/>
+      <c r="U53" s="95"/>
     </row>
     <row r="62" spans="5:25" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E62" s="93" t="s">
+      <c r="E62" s="96" t="s">
         <v>60</v>
       </c>
-      <c r="F62" s="93"/>
-      <c r="G62" s="93"/>
-      <c r="H62" s="93"/>
-      <c r="P62" s="93" t="s">
+      <c r="F62" s="96"/>
+      <c r="G62" s="96"/>
+      <c r="H62" s="96"/>
+      <c r="P62" s="96" t="s">
         <v>61</v>
       </c>
-      <c r="Q62" s="93"/>
-      <c r="R62" s="93"/>
-      <c r="S62" s="93"/>
-      <c r="V62" s="93" t="s">
+      <c r="Q62" s="96"/>
+      <c r="R62" s="96"/>
+      <c r="S62" s="96"/>
+      <c r="V62" s="96" t="s">
         <v>62</v>
       </c>
-      <c r="W62" s="93"/>
-      <c r="X62" s="93"/>
-      <c r="Y62" s="93"/>
+      <c r="W62" s="96"/>
+      <c r="X62" s="96"/>
+      <c r="Y62" s="96"/>
     </row>
     <row r="63" spans="5:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="66" spans="3:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C66" s="94" t="s">
+      <c r="C66" s="97" t="s">
         <v>56</v>
       </c>
-      <c r="D66" s="95"/>
-      <c r="F66" s="94" t="s">
+      <c r="D66" s="98"/>
+      <c r="F66" s="97" t="s">
         <v>56</v>
       </c>
-      <c r="G66" s="95"/>
-      <c r="I66" s="94" t="s">
+      <c r="G66" s="98"/>
+      <c r="I66" s="97" t="s">
         <v>56</v>
       </c>
-      <c r="J66" s="95"/>
-      <c r="N66" s="72" t="s">
+      <c r="J66" s="98"/>
+      <c r="N66" s="75" t="s">
         <v>56</v>
       </c>
-      <c r="O66" s="73"/>
-      <c r="Q66" s="72" t="s">
+      <c r="O66" s="76"/>
+      <c r="Q66" s="75" t="s">
         <v>56</v>
       </c>
-      <c r="R66" s="73"/>
-      <c r="T66" s="72" t="s">
+      <c r="R66" s="76"/>
+      <c r="T66" s="75" t="s">
         <v>55</v>
       </c>
-      <c r="U66" s="73"/>
-      <c r="W66" s="78" t="s">
+      <c r="U66" s="76"/>
+      <c r="W66" s="81" t="s">
         <v>54</v>
       </c>
-      <c r="X66" s="79"/>
+      <c r="X66" s="82"/>
     </row>
     <row r="67" spans="3:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C67" s="96"/>
-      <c r="D67" s="97"/>
-      <c r="F67" s="96"/>
-      <c r="G67" s="97"/>
-      <c r="I67" s="96"/>
-      <c r="J67" s="97"/>
-      <c r="N67" s="74"/>
-      <c r="O67" s="75"/>
-      <c r="Q67" s="74"/>
-      <c r="R67" s="75"/>
-      <c r="T67" s="74"/>
-      <c r="U67" s="75"/>
-      <c r="W67" s="80"/>
-      <c r="X67" s="81"/>
+      <c r="C67" s="99"/>
+      <c r="D67" s="100"/>
+      <c r="F67" s="99"/>
+      <c r="G67" s="100"/>
+      <c r="I67" s="99"/>
+      <c r="J67" s="100"/>
+      <c r="N67" s="77"/>
+      <c r="O67" s="78"/>
+      <c r="Q67" s="77"/>
+      <c r="R67" s="78"/>
+      <c r="T67" s="77"/>
+      <c r="U67" s="78"/>
+      <c r="W67" s="83"/>
+      <c r="X67" s="84"/>
     </row>
     <row r="68" spans="3:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C68" s="98"/>
-      <c r="D68" s="99"/>
-      <c r="F68" s="98"/>
-      <c r="G68" s="99"/>
-      <c r="I68" s="98"/>
-      <c r="J68" s="99"/>
-      <c r="N68" s="76"/>
-      <c r="O68" s="77"/>
-      <c r="Q68" s="76"/>
-      <c r="R68" s="77"/>
-      <c r="T68" s="76"/>
-      <c r="U68" s="77"/>
-      <c r="W68" s="82"/>
-      <c r="X68" s="83"/>
+      <c r="C68" s="101"/>
+      <c r="D68" s="102"/>
+      <c r="F68" s="101"/>
+      <c r="G68" s="102"/>
+      <c r="I68" s="101"/>
+      <c r="J68" s="102"/>
+      <c r="N68" s="79"/>
+      <c r="O68" s="80"/>
+      <c r="Q68" s="79"/>
+      <c r="R68" s="80"/>
+      <c r="T68" s="79"/>
+      <c r="U68" s="80"/>
+      <c r="W68" s="85"/>
+      <c r="X68" s="86"/>
     </row>
     <row r="69" spans="3:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
@@ -3001,7 +3042,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="E1:M48"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView rightToLeft="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="M8" sqref="M8"/>
     </sheetView>
@@ -3021,32 +3062,32 @@
       </c>
     </row>
     <row r="2" spans="5:13" ht="26" x14ac:dyDescent="0.2">
-      <c r="E2" s="102" t="s">
+      <c r="E2" s="105" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="102"/>
-      <c r="G2" s="102"/>
-      <c r="H2" s="102"/>
-      <c r="I2" s="102"/>
-      <c r="J2" s="102"/>
-      <c r="K2" s="102"/>
-      <c r="L2" s="102"/>
-      <c r="M2" s="102"/>
+      <c r="F2" s="105"/>
+      <c r="G2" s="105"/>
+      <c r="H2" s="105"/>
+      <c r="I2" s="105"/>
+      <c r="J2" s="105"/>
+      <c r="K2" s="105"/>
+      <c r="L2" s="105"/>
+      <c r="M2" s="105"/>
     </row>
     <row r="4" spans="5:13" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E4"/>
-      <c r="F4" s="104" t="s">
+      <c r="F4" s="107" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="105"/>
-      <c r="H4" s="106"/>
-      <c r="I4" s="103" t="s">
+      <c r="G4" s="108"/>
+      <c r="H4" s="109"/>
+      <c r="I4" s="106" t="s">
         <v>38</v>
       </c>
-      <c r="J4" s="103"/>
-      <c r="K4" s="103"/>
-      <c r="L4" s="103"/>
-      <c r="M4" s="100" t="s">
+      <c r="J4" s="106"/>
+      <c r="K4" s="106"/>
+      <c r="L4" s="106"/>
+      <c r="M4" s="103" t="s">
         <v>3</v>
       </c>
     </row>
@@ -3061,15 +3102,15 @@
       <c r="H5" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="I5" s="107" t="s">
+      <c r="I5" s="110" t="s">
         <v>4</v>
       </c>
-      <c r="J5" s="108"/>
-      <c r="K5" s="103" t="s">
+      <c r="J5" s="111"/>
+      <c r="K5" s="106" t="s">
         <v>1</v>
       </c>
-      <c r="L5" s="103"/>
-      <c r="M5" s="101"/>
+      <c r="L5" s="106"/>
+      <c r="M5" s="104"/>
     </row>
     <row r="6" spans="5:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E6"/>
@@ -3233,14 +3274,14 @@
   </cols>
   <sheetData>
     <row r="3" spans="4:9" s="13" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D3" s="109" t="s">
+      <c r="D3" s="112" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="109"/>
-      <c r="F3" s="109"/>
-      <c r="G3" s="109"/>
-      <c r="H3" s="109"/>
-      <c r="I3" s="109"/>
+      <c r="E3" s="112"/>
+      <c r="F3" s="112"/>
+      <c r="G3" s="112"/>
+      <c r="H3" s="112"/>
+      <c r="I3" s="112"/>
     </row>
     <row r="5" spans="4:9" s="8" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D5" s="27" t="s">
@@ -3577,11 +3618,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="F1:S21"/>
+  <dimension ref="B1:U21"/>
   <sheetViews>
-    <sheetView rightToLeft="1" topLeftCell="B1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S3" sqref="S3"/>
+    <sheetView rightToLeft="1" tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3590,85 +3631,195 @@
     <col min="2" max="2" width="18.1640625" customWidth="1"/>
     <col min="4" max="4" width="15.5" customWidth="1"/>
     <col min="5" max="6" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.1640625" customWidth="1"/>
-    <col min="12" max="12" width="11.83203125" customWidth="1"/>
-    <col min="13" max="14" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="9" bestFit="1" customWidth="1"/>
-    <col min="23" max="24" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="25" max="26" width="9" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.83203125" customWidth="1"/>
+    <col min="10" max="10" width="9.1640625" customWidth="1"/>
+    <col min="11" max="11" width="11.83203125" customWidth="1"/>
+    <col min="12" max="13" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="9" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="9" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="6:19" ht="21" x14ac:dyDescent="0.2">
-      <c r="F1" s="110" t="s">
+    <row r="1" spans="2:21" ht="21" x14ac:dyDescent="0.2">
+      <c r="B1" s="113" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" s="114"/>
+      <c r="D1" s="114"/>
+      <c r="E1" s="114"/>
+      <c r="F1" s="114"/>
+      <c r="G1" s="114"/>
+      <c r="H1" s="114"/>
+      <c r="I1" s="114"/>
+      <c r="J1" s="114"/>
+      <c r="K1" s="114"/>
+      <c r="L1" s="114"/>
+      <c r="M1" s="114"/>
+      <c r="N1" s="114"/>
+      <c r="O1" s="114"/>
+      <c r="P1" s="114"/>
+      <c r="Q1" s="114"/>
+      <c r="R1" s="114"/>
+      <c r="S1" s="114"/>
+      <c r="T1" s="114"/>
+      <c r="U1" s="114"/>
+    </row>
+    <row r="2" spans="2:21" ht="19" x14ac:dyDescent="0.25">
+      <c r="B2" s="115" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" s="116"/>
+      <c r="D2" s="116"/>
+      <c r="E2" s="116"/>
+      <c r="F2" s="115" t="s">
+        <v>68</v>
+      </c>
+      <c r="G2" s="116"/>
+      <c r="H2" s="116"/>
+      <c r="I2" s="116"/>
+      <c r="J2" s="117" t="s">
+        <v>69</v>
+      </c>
+      <c r="K2" s="118"/>
+      <c r="L2" s="118"/>
+      <c r="M2" s="117" t="s">
+        <v>70</v>
+      </c>
+      <c r="N2" s="118"/>
+      <c r="O2" s="118"/>
+      <c r="P2" s="117" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q2" s="118"/>
+      <c r="R2" s="118"/>
+      <c r="S2" s="117" t="s">
+        <v>72</v>
+      </c>
+      <c r="T2" s="118"/>
+      <c r="U2" s="42" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="2:21" ht="68" x14ac:dyDescent="0.2">
+      <c r="B3" s="43" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="43" t="s">
+        <v>73</v>
+      </c>
+      <c r="F3" s="43" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" s="43" t="s">
+        <v>36</v>
+      </c>
+      <c r="H3" s="43" t="s">
+        <v>74</v>
+      </c>
+      <c r="I3" s="136" t="s">
+        <v>75</v>
+      </c>
+      <c r="J3" s="43" t="s">
+        <v>76</v>
+      </c>
+      <c r="K3" s="43" t="s">
+        <v>77</v>
+      </c>
+      <c r="L3" s="43" t="s">
+        <v>78</v>
+      </c>
+      <c r="M3" s="43" t="s">
+        <v>79</v>
+      </c>
+      <c r="N3" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="G1" s="110"/>
-      <c r="H1" s="110"/>
-      <c r="I1" s="110"/>
-      <c r="J1" s="110"/>
-      <c r="K1" s="110"/>
-      <c r="L1" s="110"/>
-      <c r="M1" s="110"/>
-      <c r="N1" s="110"/>
-      <c r="O1" s="110"/>
-      <c r="P1" s="110"/>
-      <c r="Q1" s="110"/>
-      <c r="R1" s="110"/>
-      <c r="S1" s="110"/>
-    </row>
-    <row r="2" spans="6:19" ht="68" x14ac:dyDescent="0.2">
-      <c r="F2" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="G2" s="33" t="s">
-        <v>33</v>
-      </c>
-      <c r="H2" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="I2" s="33" t="s">
-        <v>35</v>
-      </c>
-      <c r="J2" s="33" t="s">
-        <v>36</v>
-      </c>
-      <c r="K2" s="33" t="s">
-        <v>63</v>
-      </c>
-      <c r="L2" s="33" t="s">
+      <c r="O3" s="43" t="s">
         <v>65</v>
       </c>
-      <c r="M2" s="33" t="s">
+      <c r="P3" s="43" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q3" s="43" t="s">
+        <v>77</v>
+      </c>
+      <c r="R3" s="43" t="s">
+        <v>78</v>
+      </c>
+      <c r="S3" s="43" t="s">
+        <v>80</v>
+      </c>
+      <c r="T3" s="43" t="s">
+        <v>81</v>
+      </c>
+      <c r="U3" s="43" t="s">
         <v>66</v>
       </c>
-      <c r="N2" s="33" t="s">
-        <v>67</v>
-      </c>
-      <c r="O2" s="33" t="s">
-        <v>70</v>
-      </c>
-      <c r="P2" s="33" t="s">
-        <v>71</v>
-      </c>
-      <c r="Q2" s="33" t="s">
-        <v>68</v>
-      </c>
-      <c r="R2" s="33" t="s">
-        <v>69</v>
-      </c>
-      <c r="S2" s="43" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="8" spans="6:19" s="34" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="17" s="34" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="21" s="34" customFormat="1" x14ac:dyDescent="0.2"/>
+    </row>
+    <row r="4" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B4" s="44"/>
+      <c r="C4" s="44"/>
+      <c r="D4" s="44"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="44"/>
+      <c r="G4" s="44"/>
+      <c r="H4" s="44"/>
+      <c r="I4" s="137"/>
+      <c r="J4" s="44"/>
+      <c r="K4" s="44"/>
+      <c r="L4" s="44"/>
+      <c r="M4" s="44"/>
+      <c r="N4" s="44"/>
+      <c r="O4" s="44"/>
+      <c r="P4" s="44"/>
+      <c r="Q4" s="44"/>
+      <c r="R4" s="44"/>
+      <c r="S4" s="44"/>
+      <c r="T4" s="44"/>
+      <c r="U4" s="44"/>
+    </row>
+    <row r="5" spans="2:21" ht="16" x14ac:dyDescent="0.2">
+      <c r="B5" s="45"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="45"/>
+      <c r="H5" s="45"/>
+      <c r="I5" s="137"/>
+      <c r="J5" s="45"/>
+      <c r="K5" s="45"/>
+      <c r="L5" s="45"/>
+      <c r="M5" s="45"/>
+      <c r="N5" s="45"/>
+      <c r="O5" s="45"/>
+      <c r="P5" s="45"/>
+      <c r="Q5" s="45"/>
+      <c r="R5" s="45"/>
+      <c r="S5" s="45"/>
+      <c r="T5" s="46"/>
+      <c r="U5" s="44"/>
+    </row>
+    <row r="8" spans="2:21" s="33" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="17" s="33" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="21" s="33" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="F1:S1"/>
+  <mergeCells count="7">
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="M2:O2"/>
+    <mergeCell ref="P2:R2"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="B1:U1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3693,55 +3844,55 @@
   </cols>
   <sheetData>
     <row r="2" spans="5:13" ht="26" x14ac:dyDescent="0.2">
-      <c r="E2" s="102" t="s">
+      <c r="E2" s="105" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="102"/>
-      <c r="G2" s="102"/>
-      <c r="H2" s="102"/>
-      <c r="I2" s="102"/>
-      <c r="J2" s="102"/>
-      <c r="K2" s="102"/>
-      <c r="L2" s="102"/>
-      <c r="M2" s="102"/>
+      <c r="F2" s="105"/>
+      <c r="G2" s="105"/>
+      <c r="H2" s="105"/>
+      <c r="I2" s="105"/>
+      <c r="J2" s="105"/>
+      <c r="K2" s="105"/>
+      <c r="L2" s="105"/>
+      <c r="M2" s="105"/>
     </row>
     <row r="4" spans="5:13" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E4" s="100" t="s">
+      <c r="E4" s="103" t="s">
         <v>0</v>
       </c>
-      <c r="F4" s="114" t="s">
+      <c r="F4" s="122" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="115"/>
-      <c r="H4" s="116"/>
-      <c r="I4" s="107" t="s">
+      <c r="G4" s="123"/>
+      <c r="H4" s="124"/>
+      <c r="I4" s="110" t="s">
         <v>8</v>
       </c>
-      <c r="J4" s="120"/>
-      <c r="K4" s="120"/>
-      <c r="L4" s="121"/>
-      <c r="M4" s="100" t="s">
+      <c r="J4" s="128"/>
+      <c r="K4" s="128"/>
+      <c r="L4" s="129"/>
+      <c r="M4" s="103" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="5:13" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E5" s="101"/>
-      <c r="F5" s="117"/>
-      <c r="G5" s="118"/>
-      <c r="H5" s="119"/>
+      <c r="E5" s="104"/>
+      <c r="F5" s="125"/>
+      <c r="G5" s="126"/>
+      <c r="H5" s="127"/>
       <c r="I5" s="4"/>
       <c r="J5" s="5"/>
       <c r="K5" s="6"/>
       <c r="L5" s="4"/>
-      <c r="M5" s="101"/>
+      <c r="M5" s="104"/>
     </row>
     <row r="6" spans="5:13" ht="167.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E6" s="2">
         <v>1</v>
       </c>
-      <c r="F6" s="122"/>
-      <c r="G6" s="123"/>
-      <c r="H6" s="124"/>
+      <c r="F6" s="130"/>
+      <c r="G6" s="131"/>
+      <c r="H6" s="132"/>
       <c r="I6" s="24"/>
       <c r="J6" s="24"/>
       <c r="K6" s="24"/>
@@ -3752,9 +3903,9 @@
       <c r="E7" s="2">
         <v>2</v>
       </c>
-      <c r="F7" s="122"/>
-      <c r="G7" s="123"/>
-      <c r="H7" s="124"/>
+      <c r="F7" s="130"/>
+      <c r="G7" s="131"/>
+      <c r="H7" s="132"/>
       <c r="I7" s="24"/>
       <c r="J7" s="24"/>
       <c r="K7" s="24"/>
@@ -3765,9 +3916,9 @@
       <c r="E8" s="2">
         <v>3</v>
       </c>
-      <c r="F8" s="125"/>
-      <c r="G8" s="126"/>
-      <c r="H8" s="127"/>
+      <c r="F8" s="133"/>
+      <c r="G8" s="134"/>
+      <c r="H8" s="135"/>
       <c r="I8" s="24"/>
       <c r="J8" s="24"/>
       <c r="K8" s="24"/>
@@ -3778,9 +3929,9 @@
       <c r="E9" s="2">
         <v>4</v>
       </c>
-      <c r="F9" s="125"/>
-      <c r="G9" s="126"/>
-      <c r="H9" s="127"/>
+      <c r="F9" s="133"/>
+      <c r="G9" s="134"/>
+      <c r="H9" s="135"/>
       <c r="I9" s="24"/>
       <c r="J9" s="24"/>
       <c r="K9" s="24"/>
@@ -3791,9 +3942,9 @@
       <c r="E10" s="2">
         <v>5</v>
       </c>
-      <c r="F10" s="111"/>
-      <c r="G10" s="112"/>
-      <c r="H10" s="113"/>
+      <c r="F10" s="119"/>
+      <c r="G10" s="120"/>
+      <c r="H10" s="121"/>
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
@@ -3804,9 +3955,9 @@
       <c r="E11" s="2">
         <v>6</v>
       </c>
-      <c r="F11" s="111"/>
-      <c r="G11" s="112"/>
-      <c r="H11" s="113"/>
+      <c r="F11" s="119"/>
+      <c r="G11" s="120"/>
+      <c r="H11" s="121"/>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
@@ -3817,9 +3968,9 @@
       <c r="E12" s="2">
         <v>7</v>
       </c>
-      <c r="F12" s="111"/>
-      <c r="G12" s="112"/>
-      <c r="H12" s="113"/>
+      <c r="F12" s="119"/>
+      <c r="G12" s="120"/>
+      <c r="H12" s="121"/>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
@@ -3830,9 +3981,9 @@
       <c r="E13" s="2">
         <v>8</v>
       </c>
-      <c r="F13" s="111"/>
-      <c r="G13" s="112"/>
-      <c r="H13" s="113"/>
+      <c r="F13" s="119"/>
+      <c r="G13" s="120"/>
+      <c r="H13" s="121"/>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
@@ -3843,9 +3994,9 @@
       <c r="E14" s="2">
         <v>9</v>
       </c>
-      <c r="F14" s="111"/>
-      <c r="G14" s="112"/>
-      <c r="H14" s="113"/>
+      <c r="F14" s="119"/>
+      <c r="G14" s="120"/>
+      <c r="H14" s="121"/>
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
@@ -3856,9 +4007,9 @@
       <c r="E15" s="2">
         <v>10</v>
       </c>
-      <c r="F15" s="111"/>
-      <c r="G15" s="112"/>
-      <c r="H15" s="113"/>
+      <c r="F15" s="119"/>
+      <c r="G15" s="120"/>
+      <c r="H15" s="121"/>
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
@@ -3869,9 +4020,9 @@
       <c r="E16" s="2">
         <v>11</v>
       </c>
-      <c r="F16" s="111"/>
-      <c r="G16" s="112"/>
-      <c r="H16" s="113"/>
+      <c r="F16" s="119"/>
+      <c r="G16" s="120"/>
+      <c r="H16" s="121"/>
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
@@ -3882,9 +4033,9 @@
       <c r="E17" s="2">
         <v>12</v>
       </c>
-      <c r="F17" s="111"/>
-      <c r="G17" s="112"/>
-      <c r="H17" s="113"/>
+      <c r="F17" s="119"/>
+      <c r="G17" s="120"/>
+      <c r="H17" s="121"/>
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
@@ -3895,9 +4046,9 @@
       <c r="E18" s="2">
         <v>13</v>
       </c>
-      <c r="F18" s="111"/>
-      <c r="G18" s="112"/>
-      <c r="H18" s="113"/>
+      <c r="F18" s="119"/>
+      <c r="G18" s="120"/>
+      <c r="H18" s="121"/>
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
@@ -3908,9 +4059,9 @@
       <c r="E19" s="2">
         <v>14</v>
       </c>
-      <c r="F19" s="111"/>
-      <c r="G19" s="112"/>
-      <c r="H19" s="113"/>
+      <c r="F19" s="119"/>
+      <c r="G19" s="120"/>
+      <c r="H19" s="121"/>
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
@@ -3921,9 +4072,9 @@
       <c r="E20" s="2">
         <v>15</v>
       </c>
-      <c r="F20" s="111"/>
-      <c r="G20" s="112"/>
-      <c r="H20" s="113"/>
+      <c r="F20" s="119"/>
+      <c r="G20" s="120"/>
+      <c r="H20" s="121"/>
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>

</xml_diff>

<commit_message>
move to the new families sheet format (#1)
Co-authored-by: Roi Dital <roi.dital@cyberark.com>
</commit_message>
<xml_diff>
--- a/cockpit_template.xlsx
+++ b/cockpit_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Roi.Dital/roid_playground/paamonim/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE3B73D5-58F7-1847-803C-B5B9DF2AC5D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32B18C83-3304-4445-A5C8-07106323E6B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="19440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="19440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="רציונל" sheetId="3" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="82">
   <si>
     <t>#</t>
   </si>
@@ -237,47 +237,81 @@
     <t xml:space="preserve">  משפחות שהסתיימו</t>
   </si>
   <si>
-    <t>מספר פגישות שהתקיימו (בוטלו)</t>
-  </si>
-  <si>
     <t>דוח משפחות פעילות</t>
   </si>
   <si>
-    <t>שיקוף/ביצוע אחרון</t>
+    <t>החזר חובות חודשי</t>
+  </si>
+  <si>
+    <t>חובות לא בהסדר</t>
+  </si>
+  <si>
+    <t>נושאים לבירור עם המלווה</t>
+  </si>
+  <si>
+    <t>פרטים אישיים</t>
+  </si>
+  <si>
+    <t>תאריכים ופגישות</t>
+  </si>
+  <si>
+    <t>תקציב אחרון</t>
+  </si>
+  <si>
+    <t>חובות</t>
+  </si>
+  <si>
+    <t>ביצוע אחרון</t>
+  </si>
+  <si>
+    <t>מזומן</t>
+  </si>
+  <si>
+    <t>ותק הליווי בימים</t>
+  </si>
+  <si>
+    <t>מספר פגישות שהתקיימו</t>
+  </si>
+  <si>
+    <t xml:space="preserve">מספר פגישות שבוטלו </t>
+  </si>
+  <si>
+    <t>הכנסות</t>
+  </si>
+  <si>
+    <t>הוצאות</t>
+  </si>
+  <si>
+    <t>הפרש</t>
+  </si>
+  <si>
+    <t>סך החובות</t>
   </si>
   <si>
     <t>רישום עו״ש אחרון</t>
   </si>
   <si>
-    <t>סה״כ חובות</t>
-  </si>
-  <si>
-    <t>תקציב</t>
-  </si>
-  <si>
-    <t>ותק ליווי</t>
-  </si>
-  <si>
-    <t>החזר חובות חודשי</t>
-  </si>
-  <si>
-    <t>חובות לא בהסדר</t>
-  </si>
-  <si>
-    <t>נושאים לבירור עם המלווה</t>
+    <t>יתרת עו״שׁ</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="177"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -417,6 +451,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="15">
     <fill>
@@ -503,7 +551,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -653,30 +701,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color indexed="64"/>
       </left>
       <right/>
@@ -693,106 +717,95 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="128">
+  <cellXfs count="138">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -804,290 +817,318 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1995,24 +2036,24 @@
   <sheetData>
     <row r="1" spans="6:21" ht="20" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F2" s="48" t="s">
+      <c r="F2" s="51" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="48"/>
-      <c r="H2" s="48"/>
-      <c r="I2" s="48"/>
-      <c r="J2" s="48"/>
-      <c r="K2" s="48"/>
-      <c r="L2" s="48"/>
-      <c r="M2" s="48"/>
-      <c r="N2" s="48"/>
-      <c r="O2" s="48"/>
-      <c r="P2" s="48"/>
-      <c r="Q2" s="48"/>
-      <c r="R2" s="48"/>
-      <c r="S2" s="48"/>
-      <c r="T2" s="48"/>
-      <c r="U2" s="48"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="51"/>
+      <c r="J2" s="51"/>
+      <c r="K2" s="51"/>
+      <c r="L2" s="51"/>
+      <c r="M2" s="51"/>
+      <c r="N2" s="51"/>
+      <c r="O2" s="51"/>
+      <c r="P2" s="51"/>
+      <c r="Q2" s="51"/>
+      <c r="R2" s="51"/>
+      <c r="S2" s="51"/>
+      <c r="T2" s="51"/>
+      <c r="U2" s="51"/>
     </row>
     <row r="3" spans="6:21" x14ac:dyDescent="0.2">
       <c r="F3" s="30"/>
@@ -2033,68 +2074,68 @@
       <c r="U3" s="30"/>
     </row>
     <row r="4" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F4" s="56" t="s">
+      <c r="F4" s="59" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="57"/>
-      <c r="H4" s="57"/>
-      <c r="I4" s="57"/>
-      <c r="J4" s="57"/>
-      <c r="K4" s="57"/>
-      <c r="L4" s="57"/>
-      <c r="M4" s="57"/>
-      <c r="N4" s="57"/>
-      <c r="O4" s="57"/>
-      <c r="P4" s="57"/>
-      <c r="Q4" s="57"/>
-      <c r="R4" s="57"/>
-      <c r="S4" s="57"/>
-      <c r="T4" s="57"/>
-      <c r="U4" s="58"/>
+      <c r="G4" s="60"/>
+      <c r="H4" s="60"/>
+      <c r="I4" s="60"/>
+      <c r="J4" s="60"/>
+      <c r="K4" s="60"/>
+      <c r="L4" s="60"/>
+      <c r="M4" s="60"/>
+      <c r="N4" s="60"/>
+      <c r="O4" s="60"/>
+      <c r="P4" s="60"/>
+      <c r="Q4" s="60"/>
+      <c r="R4" s="60"/>
+      <c r="S4" s="60"/>
+      <c r="T4" s="60"/>
+      <c r="U4" s="61"/>
     </row>
     <row r="5" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F5" s="35" t="s">
+      <c r="F5" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="59" t="s">
+      <c r="G5" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="H5" s="59"/>
-      <c r="I5" s="59"/>
-      <c r="J5" s="59"/>
-      <c r="K5" s="59"/>
-      <c r="L5" s="59"/>
-      <c r="M5" s="59"/>
-      <c r="N5" s="59"/>
-      <c r="O5" s="59"/>
-      <c r="P5" s="59"/>
-      <c r="Q5" s="59"/>
-      <c r="R5" s="59"/>
-      <c r="S5" s="59"/>
-      <c r="T5" s="59"/>
-      <c r="U5" s="60"/>
+      <c r="H5" s="62"/>
+      <c r="I5" s="62"/>
+      <c r="J5" s="62"/>
+      <c r="K5" s="62"/>
+      <c r="L5" s="62"/>
+      <c r="M5" s="62"/>
+      <c r="N5" s="62"/>
+      <c r="O5" s="62"/>
+      <c r="P5" s="62"/>
+      <c r="Q5" s="62"/>
+      <c r="R5" s="62"/>
+      <c r="S5" s="62"/>
+      <c r="T5" s="62"/>
+      <c r="U5" s="63"/>
     </row>
     <row r="6" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F6" s="38" t="s">
+      <c r="F6" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="44" t="s">
+      <c r="G6" s="47" t="s">
         <v>41</v>
       </c>
-      <c r="H6" s="44"/>
-      <c r="I6" s="44"/>
-      <c r="J6" s="44"/>
-      <c r="K6" s="44"/>
-      <c r="L6" s="44"/>
-      <c r="M6" s="44"/>
-      <c r="N6" s="44"/>
-      <c r="O6" s="44"/>
-      <c r="P6" s="44"/>
-      <c r="Q6" s="44"/>
-      <c r="R6" s="44"/>
-      <c r="S6" s="44"/>
-      <c r="T6" s="44"/>
-      <c r="U6" s="45"/>
+      <c r="H6" s="47"/>
+      <c r="I6" s="47"/>
+      <c r="J6" s="47"/>
+      <c r="K6" s="47"/>
+      <c r="L6" s="47"/>
+      <c r="M6" s="47"/>
+      <c r="N6" s="47"/>
+      <c r="O6" s="47"/>
+      <c r="P6" s="47"/>
+      <c r="Q6" s="47"/>
+      <c r="R6" s="47"/>
+      <c r="S6" s="47"/>
+      <c r="T6" s="47"/>
+      <c r="U6" s="48"/>
     </row>
     <row r="7" spans="6:21" x14ac:dyDescent="0.2">
       <c r="F7" s="31"/>
@@ -2115,46 +2156,46 @@
       <c r="U7" s="31"/>
     </row>
     <row r="8" spans="6:21" ht="26" x14ac:dyDescent="0.2">
-      <c r="F8" s="49" t="s">
+      <c r="F8" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="G8" s="50"/>
-      <c r="H8" s="50"/>
-      <c r="I8" s="50"/>
-      <c r="J8" s="50"/>
-      <c r="K8" s="50"/>
-      <c r="L8" s="50"/>
-      <c r="M8" s="50"/>
-      <c r="N8" s="50"/>
-      <c r="O8" s="50"/>
-      <c r="P8" s="50"/>
-      <c r="Q8" s="50"/>
-      <c r="R8" s="50"/>
-      <c r="S8" s="50"/>
-      <c r="T8" s="50"/>
-      <c r="U8" s="51"/>
+      <c r="G8" s="53"/>
+      <c r="H8" s="53"/>
+      <c r="I8" s="53"/>
+      <c r="J8" s="53"/>
+      <c r="K8" s="53"/>
+      <c r="L8" s="53"/>
+      <c r="M8" s="53"/>
+      <c r="N8" s="53"/>
+      <c r="O8" s="53"/>
+      <c r="P8" s="53"/>
+      <c r="Q8" s="53"/>
+      <c r="R8" s="53"/>
+      <c r="S8" s="53"/>
+      <c r="T8" s="53"/>
+      <c r="U8" s="54"/>
     </row>
     <row r="9" spans="6:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F9" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="G9" s="52" t="s">
+      <c r="G9" s="55" t="s">
         <v>59</v>
       </c>
-      <c r="H9" s="52"/>
-      <c r="I9" s="52"/>
-      <c r="J9" s="52"/>
-      <c r="K9" s="52"/>
-      <c r="L9" s="52"/>
-      <c r="M9" s="52"/>
-      <c r="N9" s="52"/>
-      <c r="O9" s="52"/>
-      <c r="P9" s="52"/>
-      <c r="Q9" s="52"/>
-      <c r="R9" s="52"/>
-      <c r="S9" s="52"/>
-      <c r="T9" s="52"/>
-      <c r="U9" s="53"/>
+      <c r="H9" s="55"/>
+      <c r="I9" s="55"/>
+      <c r="J9" s="55"/>
+      <c r="K9" s="55"/>
+      <c r="L9" s="55"/>
+      <c r="M9" s="55"/>
+      <c r="N9" s="55"/>
+      <c r="O9" s="55"/>
+      <c r="P9" s="55"/>
+      <c r="Q9" s="55"/>
+      <c r="R9" s="55"/>
+      <c r="S9" s="55"/>
+      <c r="T9" s="55"/>
+      <c r="U9" s="56"/>
     </row>
     <row r="10" spans="6:21" x14ac:dyDescent="0.2">
       <c r="F10" s="32"/>
@@ -2193,71 +2234,71 @@
       <c r="U12" s="32"/>
     </row>
     <row r="13" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F13" s="56" t="s">
+      <c r="F13" s="59" t="s">
         <v>57</v>
       </c>
-      <c r="G13" s="57"/>
-      <c r="H13" s="57"/>
-      <c r="I13" s="57"/>
-      <c r="J13" s="57"/>
-      <c r="K13" s="57"/>
-      <c r="L13" s="57"/>
-      <c r="M13" s="57"/>
-      <c r="N13" s="57"/>
-      <c r="O13" s="57"/>
-      <c r="P13" s="57"/>
-      <c r="Q13" s="57"/>
-      <c r="R13" s="57"/>
-      <c r="S13" s="57"/>
-      <c r="T13" s="57"/>
-      <c r="U13" s="58"/>
+      <c r="G13" s="60"/>
+      <c r="H13" s="60"/>
+      <c r="I13" s="60"/>
+      <c r="J13" s="60"/>
+      <c r="K13" s="60"/>
+      <c r="L13" s="60"/>
+      <c r="M13" s="60"/>
+      <c r="N13" s="60"/>
+      <c r="O13" s="60"/>
+      <c r="P13" s="60"/>
+      <c r="Q13" s="60"/>
+      <c r="R13" s="60"/>
+      <c r="S13" s="60"/>
+      <c r="T13" s="60"/>
+      <c r="U13" s="61"/>
     </row>
     <row r="14" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F14" s="35" t="s">
+      <c r="F14" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="G14" s="54" t="s">
+      <c r="G14" s="57" t="s">
         <v>43</v>
       </c>
-      <c r="H14" s="54"/>
-      <c r="I14" s="54"/>
-      <c r="J14" s="54"/>
-      <c r="K14" s="54"/>
-      <c r="L14" s="54"/>
-      <c r="M14" s="54"/>
-      <c r="N14" s="54"/>
-      <c r="O14" s="54"/>
-      <c r="P14" s="54"/>
-      <c r="Q14" s="54"/>
-      <c r="R14" s="54"/>
-      <c r="S14" s="54"/>
-      <c r="T14" s="54"/>
-      <c r="U14" s="55"/>
+      <c r="H14" s="57"/>
+      <c r="I14" s="57"/>
+      <c r="J14" s="57"/>
+      <c r="K14" s="57"/>
+      <c r="L14" s="57"/>
+      <c r="M14" s="57"/>
+      <c r="N14" s="57"/>
+      <c r="O14" s="57"/>
+      <c r="P14" s="57"/>
+      <c r="Q14" s="57"/>
+      <c r="R14" s="57"/>
+      <c r="S14" s="57"/>
+      <c r="T14" s="57"/>
+      <c r="U14" s="58"/>
     </row>
     <row r="15" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F15" s="35" t="s">
+      <c r="F15" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="G15" s="54" t="s">
+      <c r="G15" s="57" t="s">
         <v>48</v>
       </c>
-      <c r="H15" s="54"/>
-      <c r="I15" s="54"/>
-      <c r="J15" s="54"/>
-      <c r="K15" s="54"/>
-      <c r="L15" s="54"/>
-      <c r="M15" s="54"/>
-      <c r="N15" s="54"/>
-      <c r="O15" s="54"/>
-      <c r="P15" s="54"/>
-      <c r="Q15" s="54"/>
-      <c r="R15" s="54"/>
-      <c r="S15" s="54"/>
-      <c r="T15" s="54"/>
-      <c r="U15" s="55"/>
+      <c r="H15" s="57"/>
+      <c r="I15" s="57"/>
+      <c r="J15" s="57"/>
+      <c r="K15" s="57"/>
+      <c r="L15" s="57"/>
+      <c r="M15" s="57"/>
+      <c r="N15" s="57"/>
+      <c r="O15" s="57"/>
+      <c r="P15" s="57"/>
+      <c r="Q15" s="57"/>
+      <c r="R15" s="57"/>
+      <c r="S15" s="57"/>
+      <c r="T15" s="57"/>
+      <c r="U15" s="58"/>
     </row>
     <row r="16" spans="6:21" x14ac:dyDescent="0.2">
-      <c r="F16" s="36"/>
+      <c r="F16" s="35"/>
       <c r="G16" s="32"/>
       <c r="H16" s="32"/>
       <c r="I16" s="32"/>
@@ -2272,52 +2313,52 @@
       <c r="R16" s="32"/>
       <c r="S16" s="32"/>
       <c r="T16" s="32"/>
-      <c r="U16" s="37"/>
+      <c r="U16" s="36"/>
     </row>
     <row r="17" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F17" s="61" t="s">
+      <c r="F17" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="G17" s="62"/>
-      <c r="H17" s="62"/>
-      <c r="I17" s="62"/>
-      <c r="J17" s="62"/>
-      <c r="K17" s="62"/>
-      <c r="L17" s="62"/>
-      <c r="M17" s="62"/>
-      <c r="N17" s="62"/>
-      <c r="O17" s="62"/>
-      <c r="P17" s="62"/>
-      <c r="Q17" s="62"/>
-      <c r="R17" s="62"/>
-      <c r="S17" s="62"/>
-      <c r="T17" s="62"/>
-      <c r="U17" s="63"/>
+      <c r="G17" s="65"/>
+      <c r="H17" s="65"/>
+      <c r="I17" s="65"/>
+      <c r="J17" s="65"/>
+      <c r="K17" s="65"/>
+      <c r="L17" s="65"/>
+      <c r="M17" s="65"/>
+      <c r="N17" s="65"/>
+      <c r="O17" s="65"/>
+      <c r="P17" s="65"/>
+      <c r="Q17" s="65"/>
+      <c r="R17" s="65"/>
+      <c r="S17" s="65"/>
+      <c r="T17" s="65"/>
+      <c r="U17" s="66"/>
     </row>
     <row r="18" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F18" s="35" t="s">
+      <c r="F18" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="G18" s="54" t="s">
+      <c r="G18" s="57" t="s">
         <v>47</v>
       </c>
-      <c r="H18" s="54"/>
-      <c r="I18" s="54"/>
-      <c r="J18" s="54"/>
-      <c r="K18" s="54"/>
-      <c r="L18" s="54"/>
-      <c r="M18" s="54"/>
-      <c r="N18" s="54"/>
-      <c r="O18" s="54"/>
-      <c r="P18" s="54"/>
-      <c r="Q18" s="54"/>
-      <c r="R18" s="54"/>
-      <c r="S18" s="54"/>
-      <c r="T18" s="54"/>
-      <c r="U18" s="55"/>
+      <c r="H18" s="57"/>
+      <c r="I18" s="57"/>
+      <c r="J18" s="57"/>
+      <c r="K18" s="57"/>
+      <c r="L18" s="57"/>
+      <c r="M18" s="57"/>
+      <c r="N18" s="57"/>
+      <c r="O18" s="57"/>
+      <c r="P18" s="57"/>
+      <c r="Q18" s="57"/>
+      <c r="R18" s="57"/>
+      <c r="S18" s="57"/>
+      <c r="T18" s="57"/>
+      <c r="U18" s="58"/>
     </row>
     <row r="19" spans="6:21" x14ac:dyDescent="0.2">
-      <c r="F19" s="36"/>
+      <c r="F19" s="35"/>
       <c r="G19" s="32"/>
       <c r="H19" s="32"/>
       <c r="I19" s="32"/>
@@ -2332,52 +2373,52 @@
       <c r="R19" s="32"/>
       <c r="S19" s="32"/>
       <c r="T19" s="32"/>
-      <c r="U19" s="37"/>
+      <c r="U19" s="36"/>
     </row>
     <row r="20" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F20" s="61" t="s">
+      <c r="F20" s="64" t="s">
         <v>44</v>
       </c>
-      <c r="G20" s="62"/>
-      <c r="H20" s="62"/>
-      <c r="I20" s="62"/>
-      <c r="J20" s="62"/>
-      <c r="K20" s="62"/>
-      <c r="L20" s="62"/>
-      <c r="M20" s="62"/>
-      <c r="N20" s="62"/>
-      <c r="O20" s="62"/>
-      <c r="P20" s="62"/>
-      <c r="Q20" s="62"/>
-      <c r="R20" s="62"/>
-      <c r="S20" s="62"/>
-      <c r="T20" s="62"/>
-      <c r="U20" s="63"/>
+      <c r="G20" s="65"/>
+      <c r="H20" s="65"/>
+      <c r="I20" s="65"/>
+      <c r="J20" s="65"/>
+      <c r="K20" s="65"/>
+      <c r="L20" s="65"/>
+      <c r="M20" s="65"/>
+      <c r="N20" s="65"/>
+      <c r="O20" s="65"/>
+      <c r="P20" s="65"/>
+      <c r="Q20" s="65"/>
+      <c r="R20" s="65"/>
+      <c r="S20" s="65"/>
+      <c r="T20" s="65"/>
+      <c r="U20" s="66"/>
     </row>
     <row r="21" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F21" s="35" t="s">
+      <c r="F21" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="G21" s="54" t="s">
+      <c r="G21" s="57" t="s">
         <v>58</v>
       </c>
-      <c r="H21" s="54"/>
-      <c r="I21" s="54"/>
-      <c r="J21" s="54"/>
-      <c r="K21" s="54"/>
-      <c r="L21" s="54"/>
-      <c r="M21" s="54"/>
-      <c r="N21" s="54"/>
-      <c r="O21" s="54"/>
-      <c r="P21" s="54"/>
-      <c r="Q21" s="54"/>
-      <c r="R21" s="54"/>
-      <c r="S21" s="54"/>
-      <c r="T21" s="54"/>
-      <c r="U21" s="55"/>
+      <c r="H21" s="57"/>
+      <c r="I21" s="57"/>
+      <c r="J21" s="57"/>
+      <c r="K21" s="57"/>
+      <c r="L21" s="57"/>
+      <c r="M21" s="57"/>
+      <c r="N21" s="57"/>
+      <c r="O21" s="57"/>
+      <c r="P21" s="57"/>
+      <c r="Q21" s="57"/>
+      <c r="R21" s="57"/>
+      <c r="S21" s="57"/>
+      <c r="T21" s="57"/>
+      <c r="U21" s="58"/>
     </row>
     <row r="22" spans="6:21" x14ac:dyDescent="0.2">
-      <c r="F22" s="36"/>
+      <c r="F22" s="35"/>
       <c r="G22" s="32"/>
       <c r="H22" s="32"/>
       <c r="I22" s="32"/>
@@ -2392,49 +2433,49 @@
       <c r="R22" s="32"/>
       <c r="S22" s="32"/>
       <c r="T22" s="32"/>
-      <c r="U22" s="37"/>
+      <c r="U22" s="36"/>
     </row>
     <row r="23" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F23" s="61" t="s">
+      <c r="F23" s="64" t="s">
         <v>45</v>
       </c>
-      <c r="G23" s="62"/>
-      <c r="H23" s="62"/>
-      <c r="I23" s="62"/>
-      <c r="J23" s="62"/>
-      <c r="K23" s="62"/>
-      <c r="L23" s="62"/>
-      <c r="M23" s="62"/>
-      <c r="N23" s="62"/>
-      <c r="O23" s="62"/>
-      <c r="P23" s="62"/>
-      <c r="Q23" s="62"/>
-      <c r="R23" s="62"/>
-      <c r="S23" s="62"/>
-      <c r="T23" s="62"/>
-      <c r="U23" s="63"/>
+      <c r="G23" s="65"/>
+      <c r="H23" s="65"/>
+      <c r="I23" s="65"/>
+      <c r="J23" s="65"/>
+      <c r="K23" s="65"/>
+      <c r="L23" s="65"/>
+      <c r="M23" s="65"/>
+      <c r="N23" s="65"/>
+      <c r="O23" s="65"/>
+      <c r="P23" s="65"/>
+      <c r="Q23" s="65"/>
+      <c r="R23" s="65"/>
+      <c r="S23" s="65"/>
+      <c r="T23" s="65"/>
+      <c r="U23" s="66"/>
     </row>
     <row r="24" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F24" s="38" t="s">
+      <c r="F24" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="G24" s="64" t="s">
+      <c r="G24" s="67" t="s">
         <v>46</v>
       </c>
-      <c r="H24" s="64"/>
-      <c r="I24" s="64"/>
-      <c r="J24" s="64"/>
-      <c r="K24" s="64"/>
-      <c r="L24" s="64"/>
-      <c r="M24" s="64"/>
-      <c r="N24" s="64"/>
-      <c r="O24" s="64"/>
-      <c r="P24" s="64"/>
-      <c r="Q24" s="64"/>
-      <c r="R24" s="64"/>
-      <c r="S24" s="64"/>
-      <c r="T24" s="64"/>
-      <c r="U24" s="65"/>
+      <c r="H24" s="67"/>
+      <c r="I24" s="67"/>
+      <c r="J24" s="67"/>
+      <c r="K24" s="67"/>
+      <c r="L24" s="67"/>
+      <c r="M24" s="67"/>
+      <c r="N24" s="67"/>
+      <c r="O24" s="67"/>
+      <c r="P24" s="67"/>
+      <c r="Q24" s="67"/>
+      <c r="R24" s="67"/>
+      <c r="S24" s="67"/>
+      <c r="T24" s="67"/>
+      <c r="U24" s="68"/>
     </row>
     <row r="25" spans="6:21" x14ac:dyDescent="0.2">
       <c r="F25" s="32"/>
@@ -2491,174 +2532,174 @@
       <c r="U27" s="32"/>
     </row>
     <row r="28" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F28" s="67" t="s">
+      <c r="F28" s="70" t="s">
         <v>16</v>
       </c>
-      <c r="G28" s="68"/>
-      <c r="H28" s="68"/>
-      <c r="I28" s="68"/>
-      <c r="J28" s="68"/>
-      <c r="K28" s="68"/>
-      <c r="L28" s="68"/>
-      <c r="M28" s="68"/>
-      <c r="N28" s="68"/>
-      <c r="O28" s="68"/>
-      <c r="P28" s="68"/>
-      <c r="Q28" s="68"/>
-      <c r="R28" s="68"/>
-      <c r="S28" s="68"/>
-      <c r="T28" s="68"/>
-      <c r="U28" s="69"/>
+      <c r="G28" s="71"/>
+      <c r="H28" s="71"/>
+      <c r="I28" s="71"/>
+      <c r="J28" s="71"/>
+      <c r="K28" s="71"/>
+      <c r="L28" s="71"/>
+      <c r="M28" s="71"/>
+      <c r="N28" s="71"/>
+      <c r="O28" s="71"/>
+      <c r="P28" s="71"/>
+      <c r="Q28" s="71"/>
+      <c r="R28" s="71"/>
+      <c r="S28" s="71"/>
+      <c r="T28" s="71"/>
+      <c r="U28" s="72"/>
     </row>
     <row r="29" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F29" s="39" t="s">
+      <c r="F29" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="G29" s="46" t="s">
+      <c r="G29" s="49" t="s">
         <v>25</v>
       </c>
-      <c r="H29" s="46"/>
-      <c r="I29" s="46"/>
-      <c r="J29" s="46"/>
-      <c r="K29" s="46"/>
-      <c r="L29" s="46"/>
-      <c r="M29" s="46"/>
-      <c r="N29" s="46"/>
-      <c r="O29" s="46"/>
-      <c r="P29" s="46"/>
-      <c r="Q29" s="46"/>
-      <c r="R29" s="46"/>
-      <c r="S29" s="46"/>
-      <c r="T29" s="46"/>
-      <c r="U29" s="47"/>
+      <c r="H29" s="49"/>
+      <c r="I29" s="49"/>
+      <c r="J29" s="49"/>
+      <c r="K29" s="49"/>
+      <c r="L29" s="49"/>
+      <c r="M29" s="49"/>
+      <c r="N29" s="49"/>
+      <c r="O29" s="49"/>
+      <c r="P29" s="49"/>
+      <c r="Q29" s="49"/>
+      <c r="R29" s="49"/>
+      <c r="S29" s="49"/>
+      <c r="T29" s="49"/>
+      <c r="U29" s="50"/>
     </row>
     <row r="30" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F30" s="39" t="s">
+      <c r="F30" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="G30" s="46" t="s">
+      <c r="G30" s="49" t="s">
         <v>21</v>
       </c>
-      <c r="H30" s="46"/>
-      <c r="I30" s="46"/>
-      <c r="J30" s="46"/>
-      <c r="K30" s="46"/>
-      <c r="L30" s="46"/>
-      <c r="M30" s="46"/>
-      <c r="N30" s="46"/>
-      <c r="O30" s="46"/>
-      <c r="P30" s="46"/>
-      <c r="Q30" s="46"/>
-      <c r="R30" s="46"/>
-      <c r="S30" s="46"/>
-      <c r="T30" s="46"/>
-      <c r="U30" s="47"/>
+      <c r="H30" s="49"/>
+      <c r="I30" s="49"/>
+      <c r="J30" s="49"/>
+      <c r="K30" s="49"/>
+      <c r="L30" s="49"/>
+      <c r="M30" s="49"/>
+      <c r="N30" s="49"/>
+      <c r="O30" s="49"/>
+      <c r="P30" s="49"/>
+      <c r="Q30" s="49"/>
+      <c r="R30" s="49"/>
+      <c r="S30" s="49"/>
+      <c r="T30" s="49"/>
+      <c r="U30" s="50"/>
     </row>
     <row r="31" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F31" s="39" t="s">
+      <c r="F31" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="G31" s="46" t="s">
+      <c r="G31" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="H31" s="46"/>
-      <c r="I31" s="46"/>
-      <c r="J31" s="46"/>
-      <c r="K31" s="46"/>
-      <c r="L31" s="46"/>
-      <c r="M31" s="46"/>
-      <c r="N31" s="46"/>
-      <c r="O31" s="46"/>
-      <c r="P31" s="46"/>
-      <c r="Q31" s="46"/>
-      <c r="R31" s="46"/>
-      <c r="S31" s="46"/>
-      <c r="T31" s="46"/>
-      <c r="U31" s="47"/>
+      <c r="H31" s="49"/>
+      <c r="I31" s="49"/>
+      <c r="J31" s="49"/>
+      <c r="K31" s="49"/>
+      <c r="L31" s="49"/>
+      <c r="M31" s="49"/>
+      <c r="N31" s="49"/>
+      <c r="O31" s="49"/>
+      <c r="P31" s="49"/>
+      <c r="Q31" s="49"/>
+      <c r="R31" s="49"/>
+      <c r="S31" s="49"/>
+      <c r="T31" s="49"/>
+      <c r="U31" s="50"/>
     </row>
     <row r="32" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F32" s="39" t="s">
+      <c r="F32" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="G32" s="46" t="s">
+      <c r="G32" s="49" t="s">
         <v>28</v>
       </c>
-      <c r="H32" s="46"/>
-      <c r="I32" s="46"/>
-      <c r="J32" s="46"/>
-      <c r="K32" s="46"/>
-      <c r="L32" s="46"/>
-      <c r="M32" s="46"/>
-      <c r="N32" s="46"/>
-      <c r="O32" s="46"/>
-      <c r="P32" s="46"/>
-      <c r="Q32" s="46"/>
-      <c r="R32" s="46"/>
-      <c r="S32" s="46"/>
-      <c r="T32" s="46"/>
-      <c r="U32" s="47"/>
+      <c r="H32" s="49"/>
+      <c r="I32" s="49"/>
+      <c r="J32" s="49"/>
+      <c r="K32" s="49"/>
+      <c r="L32" s="49"/>
+      <c r="M32" s="49"/>
+      <c r="N32" s="49"/>
+      <c r="O32" s="49"/>
+      <c r="P32" s="49"/>
+      <c r="Q32" s="49"/>
+      <c r="R32" s="49"/>
+      <c r="S32" s="49"/>
+      <c r="T32" s="49"/>
+      <c r="U32" s="50"/>
     </row>
     <row r="33" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F33" s="39" t="s">
+      <c r="F33" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="G33" s="46" t="s">
+      <c r="G33" s="49" t="s">
         <v>27</v>
       </c>
-      <c r="H33" s="46"/>
-      <c r="I33" s="46"/>
-      <c r="J33" s="46"/>
-      <c r="K33" s="46"/>
-      <c r="L33" s="46"/>
-      <c r="M33" s="46"/>
-      <c r="N33" s="46"/>
-      <c r="O33" s="46"/>
-      <c r="P33" s="46"/>
-      <c r="Q33" s="46"/>
-      <c r="R33" s="46"/>
-      <c r="S33" s="46"/>
-      <c r="T33" s="46"/>
-      <c r="U33" s="47"/>
+      <c r="H33" s="49"/>
+      <c r="I33" s="49"/>
+      <c r="J33" s="49"/>
+      <c r="K33" s="49"/>
+      <c r="L33" s="49"/>
+      <c r="M33" s="49"/>
+      <c r="N33" s="49"/>
+      <c r="O33" s="49"/>
+      <c r="P33" s="49"/>
+      <c r="Q33" s="49"/>
+      <c r="R33" s="49"/>
+      <c r="S33" s="49"/>
+      <c r="T33" s="49"/>
+      <c r="U33" s="50"/>
     </row>
     <row r="34" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F34" s="40" t="s">
+      <c r="F34" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="G34" s="70" t="s">
+      <c r="G34" s="73" t="s">
         <v>30</v>
       </c>
-      <c r="H34" s="70"/>
-      <c r="I34" s="70"/>
-      <c r="J34" s="70"/>
-      <c r="K34" s="70"/>
-      <c r="L34" s="70"/>
-      <c r="M34" s="70"/>
-      <c r="N34" s="70"/>
-      <c r="O34" s="70"/>
-      <c r="P34" s="70"/>
-      <c r="Q34" s="70"/>
-      <c r="R34" s="70"/>
-      <c r="S34" s="70"/>
-      <c r="T34" s="70"/>
-      <c r="U34" s="71"/>
+      <c r="H34" s="73"/>
+      <c r="I34" s="73"/>
+      <c r="J34" s="73"/>
+      <c r="K34" s="73"/>
+      <c r="L34" s="73"/>
+      <c r="M34" s="73"/>
+      <c r="N34" s="73"/>
+      <c r="O34" s="73"/>
+      <c r="P34" s="73"/>
+      <c r="Q34" s="73"/>
+      <c r="R34" s="73"/>
+      <c r="S34" s="73"/>
+      <c r="T34" s="73"/>
+      <c r="U34" s="74"/>
     </row>
     <row r="35" spans="6:21" x14ac:dyDescent="0.2">
       <c r="F35" s="32"/>
-      <c r="G35" s="66"/>
-      <c r="H35" s="66"/>
-      <c r="I35" s="66"/>
-      <c r="J35" s="66"/>
-      <c r="K35" s="66"/>
-      <c r="L35" s="66"/>
-      <c r="M35" s="66"/>
-      <c r="N35" s="66"/>
-      <c r="O35" s="66"/>
-      <c r="P35" s="66"/>
-      <c r="Q35" s="66"/>
-      <c r="R35" s="66"/>
-      <c r="S35" s="66"/>
-      <c r="T35" s="66"/>
-      <c r="U35" s="66"/>
+      <c r="G35" s="69"/>
+      <c r="H35" s="69"/>
+      <c r="I35" s="69"/>
+      <c r="J35" s="69"/>
+      <c r="K35" s="69"/>
+      <c r="L35" s="69"/>
+      <c r="M35" s="69"/>
+      <c r="N35" s="69"/>
+      <c r="O35" s="69"/>
+      <c r="P35" s="69"/>
+      <c r="Q35" s="69"/>
+      <c r="R35" s="69"/>
+      <c r="S35" s="69"/>
+      <c r="T35" s="69"/>
+      <c r="U35" s="69"/>
     </row>
     <row r="37" spans="6:21" x14ac:dyDescent="0.2">
       <c r="F37" s="32"/>
@@ -2679,71 +2720,71 @@
       <c r="U37" s="32"/>
     </row>
     <row r="38" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F38" s="56" t="s">
+      <c r="F38" s="59" t="s">
         <v>20</v>
       </c>
-      <c r="G38" s="57"/>
-      <c r="H38" s="57"/>
-      <c r="I38" s="57"/>
-      <c r="J38" s="57"/>
-      <c r="K38" s="57"/>
-      <c r="L38" s="57"/>
-      <c r="M38" s="57"/>
-      <c r="N38" s="57"/>
-      <c r="O38" s="57"/>
-      <c r="P38" s="57"/>
-      <c r="Q38" s="57"/>
-      <c r="R38" s="57"/>
-      <c r="S38" s="57"/>
-      <c r="T38" s="57"/>
-      <c r="U38" s="58"/>
+      <c r="G38" s="60"/>
+      <c r="H38" s="60"/>
+      <c r="I38" s="60"/>
+      <c r="J38" s="60"/>
+      <c r="K38" s="60"/>
+      <c r="L38" s="60"/>
+      <c r="M38" s="60"/>
+      <c r="N38" s="60"/>
+      <c r="O38" s="60"/>
+      <c r="P38" s="60"/>
+      <c r="Q38" s="60"/>
+      <c r="R38" s="60"/>
+      <c r="S38" s="60"/>
+      <c r="T38" s="60"/>
+      <c r="U38" s="61"/>
     </row>
     <row r="39" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F39" s="35" t="s">
+      <c r="F39" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="G39" s="59" t="s">
+      <c r="G39" s="62" t="s">
         <v>40</v>
       </c>
-      <c r="H39" s="59"/>
-      <c r="I39" s="59"/>
-      <c r="J39" s="59"/>
-      <c r="K39" s="59"/>
-      <c r="L39" s="59"/>
-      <c r="M39" s="59"/>
-      <c r="N39" s="59"/>
-      <c r="O39" s="59"/>
-      <c r="P39" s="59"/>
-      <c r="Q39" s="59"/>
-      <c r="R39" s="59"/>
-      <c r="S39" s="59"/>
-      <c r="T39" s="59"/>
-      <c r="U39" s="60"/>
+      <c r="H39" s="62"/>
+      <c r="I39" s="62"/>
+      <c r="J39" s="62"/>
+      <c r="K39" s="62"/>
+      <c r="L39" s="62"/>
+      <c r="M39" s="62"/>
+      <c r="N39" s="62"/>
+      <c r="O39" s="62"/>
+      <c r="P39" s="62"/>
+      <c r="Q39" s="62"/>
+      <c r="R39" s="62"/>
+      <c r="S39" s="62"/>
+      <c r="T39" s="62"/>
+      <c r="U39" s="63"/>
     </row>
     <row r="40" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F40" s="35" t="s">
+      <c r="F40" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="G40" s="59" t="s">
+      <c r="G40" s="62" t="s">
         <v>31</v>
       </c>
-      <c r="H40" s="59"/>
-      <c r="I40" s="59"/>
-      <c r="J40" s="59"/>
-      <c r="K40" s="59"/>
-      <c r="L40" s="59"/>
-      <c r="M40" s="59"/>
-      <c r="N40" s="59"/>
-      <c r="O40" s="59"/>
-      <c r="P40" s="59"/>
-      <c r="Q40" s="59"/>
-      <c r="R40" s="59"/>
-      <c r="S40" s="59"/>
-      <c r="T40" s="59"/>
-      <c r="U40" s="60"/>
+      <c r="H40" s="62"/>
+      <c r="I40" s="62"/>
+      <c r="J40" s="62"/>
+      <c r="K40" s="62"/>
+      <c r="L40" s="62"/>
+      <c r="M40" s="62"/>
+      <c r="N40" s="62"/>
+      <c r="O40" s="62"/>
+      <c r="P40" s="62"/>
+      <c r="Q40" s="62"/>
+      <c r="R40" s="62"/>
+      <c r="S40" s="62"/>
+      <c r="T40" s="62"/>
+      <c r="U40" s="63"/>
     </row>
     <row r="41" spans="6:21" x14ac:dyDescent="0.2">
-      <c r="F41" s="41"/>
+      <c r="F41" s="40"/>
       <c r="G41" s="31"/>
       <c r="H41" s="31"/>
       <c r="I41" s="31"/>
@@ -2758,191 +2799,191 @@
       <c r="R41" s="31"/>
       <c r="S41" s="31"/>
       <c r="T41" s="31"/>
-      <c r="U41" s="42"/>
+      <c r="U41" s="41"/>
     </row>
     <row r="42" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F42" s="35" t="s">
+      <c r="F42" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="G42" s="59" t="s">
+      <c r="G42" s="62" t="s">
         <v>29</v>
       </c>
-      <c r="H42" s="59"/>
-      <c r="I42" s="59"/>
-      <c r="J42" s="59"/>
-      <c r="K42" s="59"/>
-      <c r="L42" s="59"/>
-      <c r="M42" s="59"/>
-      <c r="N42" s="59"/>
-      <c r="O42" s="59"/>
-      <c r="P42" s="59"/>
-      <c r="Q42" s="59"/>
-      <c r="R42" s="59"/>
-      <c r="S42" s="59"/>
-      <c r="T42" s="59"/>
-      <c r="U42" s="60"/>
+      <c r="H42" s="62"/>
+      <c r="I42" s="62"/>
+      <c r="J42" s="62"/>
+      <c r="K42" s="62"/>
+      <c r="L42" s="62"/>
+      <c r="M42" s="62"/>
+      <c r="N42" s="62"/>
+      <c r="O42" s="62"/>
+      <c r="P42" s="62"/>
+      <c r="Q42" s="62"/>
+      <c r="R42" s="62"/>
+      <c r="S42" s="62"/>
+      <c r="T42" s="62"/>
+      <c r="U42" s="63"/>
     </row>
     <row r="43" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F43" s="38" t="s">
+      <c r="F43" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="G43" s="44" t="s">
+      <c r="G43" s="47" t="s">
         <v>42</v>
       </c>
-      <c r="H43" s="44"/>
-      <c r="I43" s="44"/>
-      <c r="J43" s="44"/>
-      <c r="K43" s="44"/>
-      <c r="L43" s="44"/>
-      <c r="M43" s="44"/>
-      <c r="N43" s="44"/>
-      <c r="O43" s="44"/>
-      <c r="P43" s="44"/>
-      <c r="Q43" s="44"/>
-      <c r="R43" s="44"/>
-      <c r="S43" s="44"/>
-      <c r="T43" s="44"/>
-      <c r="U43" s="45"/>
+      <c r="H43" s="47"/>
+      <c r="I43" s="47"/>
+      <c r="J43" s="47"/>
+      <c r="K43" s="47"/>
+      <c r="L43" s="47"/>
+      <c r="M43" s="47"/>
+      <c r="N43" s="47"/>
+      <c r="O43" s="47"/>
+      <c r="P43" s="47"/>
+      <c r="Q43" s="47"/>
+      <c r="R43" s="47"/>
+      <c r="S43" s="47"/>
+      <c r="T43" s="47"/>
+      <c r="U43" s="48"/>
     </row>
     <row r="49" spans="5:25" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="M49" s="93" t="s">
+      <c r="M49" s="96" t="s">
         <v>49</v>
       </c>
-      <c r="N49" s="93"/>
-      <c r="O49" s="93"/>
+      <c r="N49" s="96"/>
+      <c r="O49" s="96"/>
     </row>
     <row r="51" spans="5:25" x14ac:dyDescent="0.2">
-      <c r="G51" s="84" t="s">
+      <c r="G51" s="87" t="s">
         <v>50</v>
       </c>
-      <c r="H51" s="85"/>
-      <c r="I51" s="86"/>
-      <c r="K51" s="84" t="s">
+      <c r="H51" s="88"/>
+      <c r="I51" s="89"/>
+      <c r="K51" s="87" t="s">
         <v>51</v>
       </c>
-      <c r="L51" s="85"/>
-      <c r="M51" s="86"/>
-      <c r="O51" s="84" t="s">
+      <c r="L51" s="88"/>
+      <c r="M51" s="89"/>
+      <c r="O51" s="87" t="s">
         <v>52</v>
       </c>
-      <c r="P51" s="85"/>
-      <c r="Q51" s="86"/>
-      <c r="S51" s="84" t="s">
+      <c r="P51" s="88"/>
+      <c r="Q51" s="89"/>
+      <c r="S51" s="87" t="s">
         <v>53</v>
       </c>
-      <c r="T51" s="85"/>
-      <c r="U51" s="86"/>
+      <c r="T51" s="88"/>
+      <c r="U51" s="89"/>
     </row>
     <row r="52" spans="5:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G52" s="87"/>
-      <c r="H52" s="88"/>
-      <c r="I52" s="89"/>
-      <c r="K52" s="87"/>
-      <c r="L52" s="88"/>
-      <c r="M52" s="89"/>
-      <c r="O52" s="87"/>
-      <c r="P52" s="88"/>
-      <c r="Q52" s="89"/>
-      <c r="S52" s="87"/>
-      <c r="T52" s="88"/>
-      <c r="U52" s="89"/>
+      <c r="G52" s="90"/>
+      <c r="H52" s="91"/>
+      <c r="I52" s="92"/>
+      <c r="K52" s="90"/>
+      <c r="L52" s="91"/>
+      <c r="M52" s="92"/>
+      <c r="O52" s="90"/>
+      <c r="P52" s="91"/>
+      <c r="Q52" s="92"/>
+      <c r="S52" s="90"/>
+      <c r="T52" s="91"/>
+      <c r="U52" s="92"/>
     </row>
     <row r="53" spans="5:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G53" s="90"/>
-      <c r="H53" s="91"/>
-      <c r="I53" s="92"/>
-      <c r="K53" s="90"/>
-      <c r="L53" s="91"/>
-      <c r="M53" s="92"/>
-      <c r="O53" s="90"/>
-      <c r="P53" s="91"/>
-      <c r="Q53" s="92"/>
-      <c r="S53" s="90"/>
-      <c r="T53" s="91"/>
-      <c r="U53" s="92"/>
+      <c r="G53" s="93"/>
+      <c r="H53" s="94"/>
+      <c r="I53" s="95"/>
+      <c r="K53" s="93"/>
+      <c r="L53" s="94"/>
+      <c r="M53" s="95"/>
+      <c r="O53" s="93"/>
+      <c r="P53" s="94"/>
+      <c r="Q53" s="95"/>
+      <c r="S53" s="93"/>
+      <c r="T53" s="94"/>
+      <c r="U53" s="95"/>
     </row>
     <row r="62" spans="5:25" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E62" s="93" t="s">
+      <c r="E62" s="96" t="s">
         <v>60</v>
       </c>
-      <c r="F62" s="93"/>
-      <c r="G62" s="93"/>
-      <c r="H62" s="93"/>
-      <c r="P62" s="93" t="s">
+      <c r="F62" s="96"/>
+      <c r="G62" s="96"/>
+      <c r="H62" s="96"/>
+      <c r="P62" s="96" t="s">
         <v>61</v>
       </c>
-      <c r="Q62" s="93"/>
-      <c r="R62" s="93"/>
-      <c r="S62" s="93"/>
-      <c r="V62" s="93" t="s">
+      <c r="Q62" s="96"/>
+      <c r="R62" s="96"/>
+      <c r="S62" s="96"/>
+      <c r="V62" s="96" t="s">
         <v>62</v>
       </c>
-      <c r="W62" s="93"/>
-      <c r="X62" s="93"/>
-      <c r="Y62" s="93"/>
+      <c r="W62" s="96"/>
+      <c r="X62" s="96"/>
+      <c r="Y62" s="96"/>
     </row>
     <row r="63" spans="5:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="66" spans="3:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C66" s="94" t="s">
+      <c r="C66" s="97" t="s">
         <v>56</v>
       </c>
-      <c r="D66" s="95"/>
-      <c r="F66" s="94" t="s">
+      <c r="D66" s="98"/>
+      <c r="F66" s="97" t="s">
         <v>56</v>
       </c>
-      <c r="G66" s="95"/>
-      <c r="I66" s="94" t="s">
+      <c r="G66" s="98"/>
+      <c r="I66" s="97" t="s">
         <v>56</v>
       </c>
-      <c r="J66" s="95"/>
-      <c r="N66" s="72" t="s">
+      <c r="J66" s="98"/>
+      <c r="N66" s="75" t="s">
         <v>56</v>
       </c>
-      <c r="O66" s="73"/>
-      <c r="Q66" s="72" t="s">
+      <c r="O66" s="76"/>
+      <c r="Q66" s="75" t="s">
         <v>56</v>
       </c>
-      <c r="R66" s="73"/>
-      <c r="T66" s="72" t="s">
+      <c r="R66" s="76"/>
+      <c r="T66" s="75" t="s">
         <v>55</v>
       </c>
-      <c r="U66" s="73"/>
-      <c r="W66" s="78" t="s">
+      <c r="U66" s="76"/>
+      <c r="W66" s="81" t="s">
         <v>54</v>
       </c>
-      <c r="X66" s="79"/>
+      <c r="X66" s="82"/>
     </row>
     <row r="67" spans="3:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C67" s="96"/>
-      <c r="D67" s="97"/>
-      <c r="F67" s="96"/>
-      <c r="G67" s="97"/>
-      <c r="I67" s="96"/>
-      <c r="J67" s="97"/>
-      <c r="N67" s="74"/>
-      <c r="O67" s="75"/>
-      <c r="Q67" s="74"/>
-      <c r="R67" s="75"/>
-      <c r="T67" s="74"/>
-      <c r="U67" s="75"/>
-      <c r="W67" s="80"/>
-      <c r="X67" s="81"/>
+      <c r="C67" s="99"/>
+      <c r="D67" s="100"/>
+      <c r="F67" s="99"/>
+      <c r="G67" s="100"/>
+      <c r="I67" s="99"/>
+      <c r="J67" s="100"/>
+      <c r="N67" s="77"/>
+      <c r="O67" s="78"/>
+      <c r="Q67" s="77"/>
+      <c r="R67" s="78"/>
+      <c r="T67" s="77"/>
+      <c r="U67" s="78"/>
+      <c r="W67" s="83"/>
+      <c r="X67" s="84"/>
     </row>
     <row r="68" spans="3:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C68" s="98"/>
-      <c r="D68" s="99"/>
-      <c r="F68" s="98"/>
-      <c r="G68" s="99"/>
-      <c r="I68" s="98"/>
-      <c r="J68" s="99"/>
-      <c r="N68" s="76"/>
-      <c r="O68" s="77"/>
-      <c r="Q68" s="76"/>
-      <c r="R68" s="77"/>
-      <c r="T68" s="76"/>
-      <c r="U68" s="77"/>
-      <c r="W68" s="82"/>
-      <c r="X68" s="83"/>
+      <c r="C68" s="101"/>
+      <c r="D68" s="102"/>
+      <c r="F68" s="101"/>
+      <c r="G68" s="102"/>
+      <c r="I68" s="101"/>
+      <c r="J68" s="102"/>
+      <c r="N68" s="79"/>
+      <c r="O68" s="80"/>
+      <c r="Q68" s="79"/>
+      <c r="R68" s="80"/>
+      <c r="T68" s="79"/>
+      <c r="U68" s="80"/>
+      <c r="W68" s="85"/>
+      <c r="X68" s="86"/>
     </row>
     <row r="69" spans="3:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
@@ -3001,7 +3042,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="E1:M48"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView rightToLeft="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="M8" sqref="M8"/>
     </sheetView>
@@ -3021,32 +3062,32 @@
       </c>
     </row>
     <row r="2" spans="5:13" ht="26" x14ac:dyDescent="0.2">
-      <c r="E2" s="102" t="s">
+      <c r="E2" s="105" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="102"/>
-      <c r="G2" s="102"/>
-      <c r="H2" s="102"/>
-      <c r="I2" s="102"/>
-      <c r="J2" s="102"/>
-      <c r="K2" s="102"/>
-      <c r="L2" s="102"/>
-      <c r="M2" s="102"/>
+      <c r="F2" s="105"/>
+      <c r="G2" s="105"/>
+      <c r="H2" s="105"/>
+      <c r="I2" s="105"/>
+      <c r="J2" s="105"/>
+      <c r="K2" s="105"/>
+      <c r="L2" s="105"/>
+      <c r="M2" s="105"/>
     </row>
     <row r="4" spans="5:13" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E4"/>
-      <c r="F4" s="104" t="s">
+      <c r="F4" s="107" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="105"/>
-      <c r="H4" s="106"/>
-      <c r="I4" s="103" t="s">
+      <c r="G4" s="108"/>
+      <c r="H4" s="109"/>
+      <c r="I4" s="106" t="s">
         <v>38</v>
       </c>
-      <c r="J4" s="103"/>
-      <c r="K4" s="103"/>
-      <c r="L4" s="103"/>
-      <c r="M4" s="100" t="s">
+      <c r="J4" s="106"/>
+      <c r="K4" s="106"/>
+      <c r="L4" s="106"/>
+      <c r="M4" s="103" t="s">
         <v>3</v>
       </c>
     </row>
@@ -3061,15 +3102,15 @@
       <c r="H5" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="I5" s="107" t="s">
+      <c r="I5" s="110" t="s">
         <v>4</v>
       </c>
-      <c r="J5" s="108"/>
-      <c r="K5" s="103" t="s">
+      <c r="J5" s="111"/>
+      <c r="K5" s="106" t="s">
         <v>1</v>
       </c>
-      <c r="L5" s="103"/>
-      <c r="M5" s="101"/>
+      <c r="L5" s="106"/>
+      <c r="M5" s="104"/>
     </row>
     <row r="6" spans="5:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E6"/>
@@ -3233,14 +3274,14 @@
   </cols>
   <sheetData>
     <row r="3" spans="4:9" s="13" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D3" s="109" t="s">
+      <c r="D3" s="112" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="109"/>
-      <c r="F3" s="109"/>
-      <c r="G3" s="109"/>
-      <c r="H3" s="109"/>
-      <c r="I3" s="109"/>
+      <c r="E3" s="112"/>
+      <c r="F3" s="112"/>
+      <c r="G3" s="112"/>
+      <c r="H3" s="112"/>
+      <c r="I3" s="112"/>
     </row>
     <row r="5" spans="4:9" s="8" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D5" s="27" t="s">
@@ -3577,11 +3618,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="F1:S21"/>
+  <dimension ref="B1:U21"/>
   <sheetViews>
-    <sheetView rightToLeft="1" topLeftCell="B1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S3" sqref="S3"/>
+    <sheetView rightToLeft="1" tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3590,85 +3631,195 @@
     <col min="2" max="2" width="18.1640625" customWidth="1"/>
     <col min="4" max="4" width="15.5" customWidth="1"/>
     <col min="5" max="6" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.1640625" customWidth="1"/>
-    <col min="12" max="12" width="11.83203125" customWidth="1"/>
-    <col min="13" max="14" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="9" bestFit="1" customWidth="1"/>
-    <col min="23" max="24" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="25" max="26" width="9" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.83203125" customWidth="1"/>
+    <col min="10" max="10" width="9.1640625" customWidth="1"/>
+    <col min="11" max="11" width="11.83203125" customWidth="1"/>
+    <col min="12" max="13" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="9" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="9" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="6:19" ht="21" x14ac:dyDescent="0.2">
-      <c r="F1" s="110" t="s">
+    <row r="1" spans="2:21" ht="21" x14ac:dyDescent="0.2">
+      <c r="B1" s="113" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" s="114"/>
+      <c r="D1" s="114"/>
+      <c r="E1" s="114"/>
+      <c r="F1" s="114"/>
+      <c r="G1" s="114"/>
+      <c r="H1" s="114"/>
+      <c r="I1" s="114"/>
+      <c r="J1" s="114"/>
+      <c r="K1" s="114"/>
+      <c r="L1" s="114"/>
+      <c r="M1" s="114"/>
+      <c r="N1" s="114"/>
+      <c r="O1" s="114"/>
+      <c r="P1" s="114"/>
+      <c r="Q1" s="114"/>
+      <c r="R1" s="114"/>
+      <c r="S1" s="114"/>
+      <c r="T1" s="114"/>
+      <c r="U1" s="114"/>
+    </row>
+    <row r="2" spans="2:21" ht="19" x14ac:dyDescent="0.25">
+      <c r="B2" s="115" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" s="116"/>
+      <c r="D2" s="116"/>
+      <c r="E2" s="116"/>
+      <c r="F2" s="115" t="s">
+        <v>68</v>
+      </c>
+      <c r="G2" s="116"/>
+      <c r="H2" s="116"/>
+      <c r="I2" s="116"/>
+      <c r="J2" s="117" t="s">
+        <v>69</v>
+      </c>
+      <c r="K2" s="118"/>
+      <c r="L2" s="118"/>
+      <c r="M2" s="117" t="s">
+        <v>70</v>
+      </c>
+      <c r="N2" s="118"/>
+      <c r="O2" s="118"/>
+      <c r="P2" s="117" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q2" s="118"/>
+      <c r="R2" s="118"/>
+      <c r="S2" s="117" t="s">
+        <v>72</v>
+      </c>
+      <c r="T2" s="118"/>
+      <c r="U2" s="42" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="2:21" ht="68" x14ac:dyDescent="0.2">
+      <c r="B3" s="43" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="43" t="s">
+        <v>73</v>
+      </c>
+      <c r="F3" s="43" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" s="43" t="s">
+        <v>36</v>
+      </c>
+      <c r="H3" s="43" t="s">
+        <v>74</v>
+      </c>
+      <c r="I3" s="136" t="s">
+        <v>75</v>
+      </c>
+      <c r="J3" s="43" t="s">
+        <v>76</v>
+      </c>
+      <c r="K3" s="43" t="s">
+        <v>77</v>
+      </c>
+      <c r="L3" s="43" t="s">
+        <v>78</v>
+      </c>
+      <c r="M3" s="43" t="s">
+        <v>79</v>
+      </c>
+      <c r="N3" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="G1" s="110"/>
-      <c r="H1" s="110"/>
-      <c r="I1" s="110"/>
-      <c r="J1" s="110"/>
-      <c r="K1" s="110"/>
-      <c r="L1" s="110"/>
-      <c r="M1" s="110"/>
-      <c r="N1" s="110"/>
-      <c r="O1" s="110"/>
-      <c r="P1" s="110"/>
-      <c r="Q1" s="110"/>
-      <c r="R1" s="110"/>
-      <c r="S1" s="110"/>
-    </row>
-    <row r="2" spans="6:19" ht="68" x14ac:dyDescent="0.2">
-      <c r="F2" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="G2" s="33" t="s">
-        <v>33</v>
-      </c>
-      <c r="H2" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="I2" s="33" t="s">
-        <v>35</v>
-      </c>
-      <c r="J2" s="33" t="s">
-        <v>36</v>
-      </c>
-      <c r="K2" s="33" t="s">
-        <v>63</v>
-      </c>
-      <c r="L2" s="33" t="s">
+      <c r="O3" s="43" t="s">
         <v>65</v>
       </c>
-      <c r="M2" s="33" t="s">
+      <c r="P3" s="43" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q3" s="43" t="s">
+        <v>77</v>
+      </c>
+      <c r="R3" s="43" t="s">
+        <v>78</v>
+      </c>
+      <c r="S3" s="43" t="s">
+        <v>80</v>
+      </c>
+      <c r="T3" s="43" t="s">
+        <v>81</v>
+      </c>
+      <c r="U3" s="43" t="s">
         <v>66</v>
       </c>
-      <c r="N2" s="33" t="s">
-        <v>67</v>
-      </c>
-      <c r="O2" s="33" t="s">
-        <v>70</v>
-      </c>
-      <c r="P2" s="33" t="s">
-        <v>71</v>
-      </c>
-      <c r="Q2" s="33" t="s">
-        <v>68</v>
-      </c>
-      <c r="R2" s="33" t="s">
-        <v>69</v>
-      </c>
-      <c r="S2" s="43" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="8" spans="6:19" s="34" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="17" s="34" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="21" s="34" customFormat="1" x14ac:dyDescent="0.2"/>
+    </row>
+    <row r="4" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B4" s="44"/>
+      <c r="C4" s="44"/>
+      <c r="D4" s="44"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="44"/>
+      <c r="G4" s="44"/>
+      <c r="H4" s="44"/>
+      <c r="I4" s="137"/>
+      <c r="J4" s="44"/>
+      <c r="K4" s="44"/>
+      <c r="L4" s="44"/>
+      <c r="M4" s="44"/>
+      <c r="N4" s="44"/>
+      <c r="O4" s="44"/>
+      <c r="P4" s="44"/>
+      <c r="Q4" s="44"/>
+      <c r="R4" s="44"/>
+      <c r="S4" s="44"/>
+      <c r="T4" s="44"/>
+      <c r="U4" s="44"/>
+    </row>
+    <row r="5" spans="2:21" ht="16" x14ac:dyDescent="0.2">
+      <c r="B5" s="45"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="45"/>
+      <c r="H5" s="45"/>
+      <c r="I5" s="137"/>
+      <c r="J5" s="45"/>
+      <c r="K5" s="45"/>
+      <c r="L5" s="45"/>
+      <c r="M5" s="45"/>
+      <c r="N5" s="45"/>
+      <c r="O5" s="45"/>
+      <c r="P5" s="45"/>
+      <c r="Q5" s="45"/>
+      <c r="R5" s="45"/>
+      <c r="S5" s="45"/>
+      <c r="T5" s="46"/>
+      <c r="U5" s="44"/>
+    </row>
+    <row r="8" spans="2:21" s="33" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="17" s="33" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="21" s="33" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="F1:S1"/>
+  <mergeCells count="7">
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="M2:O2"/>
+    <mergeCell ref="P2:R2"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="B1:U1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3693,55 +3844,55 @@
   </cols>
   <sheetData>
     <row r="2" spans="5:13" ht="26" x14ac:dyDescent="0.2">
-      <c r="E2" s="102" t="s">
+      <c r="E2" s="105" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="102"/>
-      <c r="G2" s="102"/>
-      <c r="H2" s="102"/>
-      <c r="I2" s="102"/>
-      <c r="J2" s="102"/>
-      <c r="K2" s="102"/>
-      <c r="L2" s="102"/>
-      <c r="M2" s="102"/>
+      <c r="F2" s="105"/>
+      <c r="G2" s="105"/>
+      <c r="H2" s="105"/>
+      <c r="I2" s="105"/>
+      <c r="J2" s="105"/>
+      <c r="K2" s="105"/>
+      <c r="L2" s="105"/>
+      <c r="M2" s="105"/>
     </row>
     <row r="4" spans="5:13" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E4" s="100" t="s">
+      <c r="E4" s="103" t="s">
         <v>0</v>
       </c>
-      <c r="F4" s="114" t="s">
+      <c r="F4" s="122" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="115"/>
-      <c r="H4" s="116"/>
-      <c r="I4" s="107" t="s">
+      <c r="G4" s="123"/>
+      <c r="H4" s="124"/>
+      <c r="I4" s="110" t="s">
         <v>8</v>
       </c>
-      <c r="J4" s="120"/>
-      <c r="K4" s="120"/>
-      <c r="L4" s="121"/>
-      <c r="M4" s="100" t="s">
+      <c r="J4" s="128"/>
+      <c r="K4" s="128"/>
+      <c r="L4" s="129"/>
+      <c r="M4" s="103" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="5:13" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E5" s="101"/>
-      <c r="F5" s="117"/>
-      <c r="G5" s="118"/>
-      <c r="H5" s="119"/>
+      <c r="E5" s="104"/>
+      <c r="F5" s="125"/>
+      <c r="G5" s="126"/>
+      <c r="H5" s="127"/>
       <c r="I5" s="4"/>
       <c r="J5" s="5"/>
       <c r="K5" s="6"/>
       <c r="L5" s="4"/>
-      <c r="M5" s="101"/>
+      <c r="M5" s="104"/>
     </row>
     <row r="6" spans="5:13" ht="167.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E6" s="2">
         <v>1</v>
       </c>
-      <c r="F6" s="122"/>
-      <c r="G6" s="123"/>
-      <c r="H6" s="124"/>
+      <c r="F6" s="130"/>
+      <c r="G6" s="131"/>
+      <c r="H6" s="132"/>
       <c r="I6" s="24"/>
       <c r="J6" s="24"/>
       <c r="K6" s="24"/>
@@ -3752,9 +3903,9 @@
       <c r="E7" s="2">
         <v>2</v>
       </c>
-      <c r="F7" s="122"/>
-      <c r="G7" s="123"/>
-      <c r="H7" s="124"/>
+      <c r="F7" s="130"/>
+      <c r="G7" s="131"/>
+      <c r="H7" s="132"/>
       <c r="I7" s="24"/>
       <c r="J7" s="24"/>
       <c r="K7" s="24"/>
@@ -3765,9 +3916,9 @@
       <c r="E8" s="2">
         <v>3</v>
       </c>
-      <c r="F8" s="125"/>
-      <c r="G8" s="126"/>
-      <c r="H8" s="127"/>
+      <c r="F8" s="133"/>
+      <c r="G8" s="134"/>
+      <c r="H8" s="135"/>
       <c r="I8" s="24"/>
       <c r="J8" s="24"/>
       <c r="K8" s="24"/>
@@ -3778,9 +3929,9 @@
       <c r="E9" s="2">
         <v>4</v>
       </c>
-      <c r="F9" s="125"/>
-      <c r="G9" s="126"/>
-      <c r="H9" s="127"/>
+      <c r="F9" s="133"/>
+      <c r="G9" s="134"/>
+      <c r="H9" s="135"/>
       <c r="I9" s="24"/>
       <c r="J9" s="24"/>
       <c r="K9" s="24"/>
@@ -3791,9 +3942,9 @@
       <c r="E10" s="2">
         <v>5</v>
       </c>
-      <c r="F10" s="111"/>
-      <c r="G10" s="112"/>
-      <c r="H10" s="113"/>
+      <c r="F10" s="119"/>
+      <c r="G10" s="120"/>
+      <c r="H10" s="121"/>
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
@@ -3804,9 +3955,9 @@
       <c r="E11" s="2">
         <v>6</v>
       </c>
-      <c r="F11" s="111"/>
-      <c r="G11" s="112"/>
-      <c r="H11" s="113"/>
+      <c r="F11" s="119"/>
+      <c r="G11" s="120"/>
+      <c r="H11" s="121"/>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
@@ -3817,9 +3968,9 @@
       <c r="E12" s="2">
         <v>7</v>
       </c>
-      <c r="F12" s="111"/>
-      <c r="G12" s="112"/>
-      <c r="H12" s="113"/>
+      <c r="F12" s="119"/>
+      <c r="G12" s="120"/>
+      <c r="H12" s="121"/>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
@@ -3830,9 +3981,9 @@
       <c r="E13" s="2">
         <v>8</v>
       </c>
-      <c r="F13" s="111"/>
-      <c r="G13" s="112"/>
-      <c r="H13" s="113"/>
+      <c r="F13" s="119"/>
+      <c r="G13" s="120"/>
+      <c r="H13" s="121"/>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
@@ -3843,9 +3994,9 @@
       <c r="E14" s="2">
         <v>9</v>
       </c>
-      <c r="F14" s="111"/>
-      <c r="G14" s="112"/>
-      <c r="H14" s="113"/>
+      <c r="F14" s="119"/>
+      <c r="G14" s="120"/>
+      <c r="H14" s="121"/>
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
@@ -3856,9 +4007,9 @@
       <c r="E15" s="2">
         <v>10</v>
       </c>
-      <c r="F15" s="111"/>
-      <c r="G15" s="112"/>
-      <c r="H15" s="113"/>
+      <c r="F15" s="119"/>
+      <c r="G15" s="120"/>
+      <c r="H15" s="121"/>
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
@@ -3869,9 +4020,9 @@
       <c r="E16" s="2">
         <v>11</v>
       </c>
-      <c r="F16" s="111"/>
-      <c r="G16" s="112"/>
-      <c r="H16" s="113"/>
+      <c r="F16" s="119"/>
+      <c r="G16" s="120"/>
+      <c r="H16" s="121"/>
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
@@ -3882,9 +4033,9 @@
       <c r="E17" s="2">
         <v>12</v>
       </c>
-      <c r="F17" s="111"/>
-      <c r="G17" s="112"/>
-      <c r="H17" s="113"/>
+      <c r="F17" s="119"/>
+      <c r="G17" s="120"/>
+      <c r="H17" s="121"/>
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
@@ -3895,9 +4046,9 @@
       <c r="E18" s="2">
         <v>13</v>
       </c>
-      <c r="F18" s="111"/>
-      <c r="G18" s="112"/>
-      <c r="H18" s="113"/>
+      <c r="F18" s="119"/>
+      <c r="G18" s="120"/>
+      <c r="H18" s="121"/>
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
@@ -3908,9 +4059,9 @@
       <c r="E19" s="2">
         <v>14</v>
       </c>
-      <c r="F19" s="111"/>
-      <c r="G19" s="112"/>
-      <c r="H19" s="113"/>
+      <c r="F19" s="119"/>
+      <c r="G19" s="120"/>
+      <c r="H19" s="121"/>
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
@@ -3921,9 +4072,9 @@
       <c r="E20" s="2">
         <v>15</v>
       </c>
-      <c r="F20" s="111"/>
-      <c r="G20" s="112"/>
-      <c r="H20" s="113"/>
+      <c r="F20" s="119"/>
+      <c r="G20" s="120"/>
+      <c r="H20" s="121"/>
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>

</xml_diff>

<commit_message>
improve code quality and some bug fixes
</commit_message>
<xml_diff>
--- a/cockpit_template.xlsx
+++ b/cockpit_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Roi.Dital/roid_playground/paamonim/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32B18C83-3304-4445-A5C8-07106323E6B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{511B55F8-FF7D-234F-8E97-859F74FB0EE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="19440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="83">
   <si>
     <t>#</t>
   </si>
@@ -265,6 +265,9 @@
   </si>
   <si>
     <t>מזומן</t>
+  </si>
+  <si>
+    <t>שם המלווה</t>
   </si>
   <si>
     <t>ותק הליווי בימים</t>
@@ -298,20 +301,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="177"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -458,12 +454,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="15">
@@ -721,91 +711,91 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="138">
+  <cellXfs count="136">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -820,7 +810,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
@@ -829,13 +819,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
@@ -844,47 +834,64 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -893,242 +900,221 @@
     <xf numFmtId="0" fontId="13" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2036,24 +2022,24 @@
   <sheetData>
     <row r="1" spans="6:21" ht="20" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F2" s="51" t="s">
+      <c r="F2" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="51"/>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51"/>
-      <c r="J2" s="51"/>
-      <c r="K2" s="51"/>
-      <c r="L2" s="51"/>
-      <c r="M2" s="51"/>
-      <c r="N2" s="51"/>
-      <c r="O2" s="51"/>
-      <c r="P2" s="51"/>
-      <c r="Q2" s="51"/>
-      <c r="R2" s="51"/>
-      <c r="S2" s="51"/>
-      <c r="T2" s="51"/>
-      <c r="U2" s="51"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="48"/>
+      <c r="J2" s="48"/>
+      <c r="K2" s="48"/>
+      <c r="L2" s="48"/>
+      <c r="M2" s="48"/>
+      <c r="N2" s="48"/>
+      <c r="O2" s="48"/>
+      <c r="P2" s="48"/>
+      <c r="Q2" s="48"/>
+      <c r="R2" s="48"/>
+      <c r="S2" s="48"/>
+      <c r="T2" s="48"/>
+      <c r="U2" s="48"/>
     </row>
     <row r="3" spans="6:21" x14ac:dyDescent="0.2">
       <c r="F3" s="30"/>
@@ -2074,68 +2060,68 @@
       <c r="U3" s="30"/>
     </row>
     <row r="4" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F4" s="59" t="s">
+      <c r="F4" s="56" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="60"/>
-      <c r="H4" s="60"/>
-      <c r="I4" s="60"/>
-      <c r="J4" s="60"/>
-      <c r="K4" s="60"/>
-      <c r="L4" s="60"/>
-      <c r="M4" s="60"/>
-      <c r="N4" s="60"/>
-      <c r="O4" s="60"/>
-      <c r="P4" s="60"/>
-      <c r="Q4" s="60"/>
-      <c r="R4" s="60"/>
-      <c r="S4" s="60"/>
-      <c r="T4" s="60"/>
-      <c r="U4" s="61"/>
+      <c r="G4" s="57"/>
+      <c r="H4" s="57"/>
+      <c r="I4" s="57"/>
+      <c r="J4" s="57"/>
+      <c r="K4" s="57"/>
+      <c r="L4" s="57"/>
+      <c r="M4" s="57"/>
+      <c r="N4" s="57"/>
+      <c r="O4" s="57"/>
+      <c r="P4" s="57"/>
+      <c r="Q4" s="57"/>
+      <c r="R4" s="57"/>
+      <c r="S4" s="57"/>
+      <c r="T4" s="57"/>
+      <c r="U4" s="58"/>
     </row>
     <row r="5" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F5" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="62" t="s">
+      <c r="G5" s="59" t="s">
         <v>39</v>
       </c>
-      <c r="H5" s="62"/>
-      <c r="I5" s="62"/>
-      <c r="J5" s="62"/>
-      <c r="K5" s="62"/>
-      <c r="L5" s="62"/>
-      <c r="M5" s="62"/>
-      <c r="N5" s="62"/>
-      <c r="O5" s="62"/>
-      <c r="P5" s="62"/>
-      <c r="Q5" s="62"/>
-      <c r="R5" s="62"/>
-      <c r="S5" s="62"/>
-      <c r="T5" s="62"/>
-      <c r="U5" s="63"/>
+      <c r="H5" s="59"/>
+      <c r="I5" s="59"/>
+      <c r="J5" s="59"/>
+      <c r="K5" s="59"/>
+      <c r="L5" s="59"/>
+      <c r="M5" s="59"/>
+      <c r="N5" s="59"/>
+      <c r="O5" s="59"/>
+      <c r="P5" s="59"/>
+      <c r="Q5" s="59"/>
+      <c r="R5" s="59"/>
+      <c r="S5" s="59"/>
+      <c r="T5" s="59"/>
+      <c r="U5" s="60"/>
     </row>
     <row r="6" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F6" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="47" t="s">
+      <c r="G6" s="44" t="s">
         <v>41</v>
       </c>
-      <c r="H6" s="47"/>
-      <c r="I6" s="47"/>
-      <c r="J6" s="47"/>
-      <c r="K6" s="47"/>
-      <c r="L6" s="47"/>
-      <c r="M6" s="47"/>
-      <c r="N6" s="47"/>
-      <c r="O6" s="47"/>
-      <c r="P6" s="47"/>
-      <c r="Q6" s="47"/>
-      <c r="R6" s="47"/>
-      <c r="S6" s="47"/>
-      <c r="T6" s="47"/>
-      <c r="U6" s="48"/>
+      <c r="H6" s="44"/>
+      <c r="I6" s="44"/>
+      <c r="J6" s="44"/>
+      <c r="K6" s="44"/>
+      <c r="L6" s="44"/>
+      <c r="M6" s="44"/>
+      <c r="N6" s="44"/>
+      <c r="O6" s="44"/>
+      <c r="P6" s="44"/>
+      <c r="Q6" s="44"/>
+      <c r="R6" s="44"/>
+      <c r="S6" s="44"/>
+      <c r="T6" s="44"/>
+      <c r="U6" s="45"/>
     </row>
     <row r="7" spans="6:21" x14ac:dyDescent="0.2">
       <c r="F7" s="31"/>
@@ -2156,46 +2142,46 @@
       <c r="U7" s="31"/>
     </row>
     <row r="8" spans="6:21" ht="26" x14ac:dyDescent="0.2">
-      <c r="F8" s="52" t="s">
+      <c r="F8" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="G8" s="53"/>
-      <c r="H8" s="53"/>
-      <c r="I8" s="53"/>
-      <c r="J8" s="53"/>
-      <c r="K8" s="53"/>
-      <c r="L8" s="53"/>
-      <c r="M8" s="53"/>
-      <c r="N8" s="53"/>
-      <c r="O8" s="53"/>
-      <c r="P8" s="53"/>
-      <c r="Q8" s="53"/>
-      <c r="R8" s="53"/>
-      <c r="S8" s="53"/>
-      <c r="T8" s="53"/>
-      <c r="U8" s="54"/>
+      <c r="G8" s="50"/>
+      <c r="H8" s="50"/>
+      <c r="I8" s="50"/>
+      <c r="J8" s="50"/>
+      <c r="K8" s="50"/>
+      <c r="L8" s="50"/>
+      <c r="M8" s="50"/>
+      <c r="N8" s="50"/>
+      <c r="O8" s="50"/>
+      <c r="P8" s="50"/>
+      <c r="Q8" s="50"/>
+      <c r="R8" s="50"/>
+      <c r="S8" s="50"/>
+      <c r="T8" s="50"/>
+      <c r="U8" s="51"/>
     </row>
     <row r="9" spans="6:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F9" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="G9" s="55" t="s">
+      <c r="G9" s="52" t="s">
         <v>59</v>
       </c>
-      <c r="H9" s="55"/>
-      <c r="I9" s="55"/>
-      <c r="J9" s="55"/>
-      <c r="K9" s="55"/>
-      <c r="L9" s="55"/>
-      <c r="M9" s="55"/>
-      <c r="N9" s="55"/>
-      <c r="O9" s="55"/>
-      <c r="P9" s="55"/>
-      <c r="Q9" s="55"/>
-      <c r="R9" s="55"/>
-      <c r="S9" s="55"/>
-      <c r="T9" s="55"/>
-      <c r="U9" s="56"/>
+      <c r="H9" s="52"/>
+      <c r="I9" s="52"/>
+      <c r="J9" s="52"/>
+      <c r="K9" s="52"/>
+      <c r="L9" s="52"/>
+      <c r="M9" s="52"/>
+      <c r="N9" s="52"/>
+      <c r="O9" s="52"/>
+      <c r="P9" s="52"/>
+      <c r="Q9" s="52"/>
+      <c r="R9" s="52"/>
+      <c r="S9" s="52"/>
+      <c r="T9" s="52"/>
+      <c r="U9" s="53"/>
     </row>
     <row r="10" spans="6:21" x14ac:dyDescent="0.2">
       <c r="F10" s="32"/>
@@ -2234,68 +2220,68 @@
       <c r="U12" s="32"/>
     </row>
     <row r="13" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F13" s="59" t="s">
+      <c r="F13" s="56" t="s">
         <v>57</v>
       </c>
-      <c r="G13" s="60"/>
-      <c r="H13" s="60"/>
-      <c r="I13" s="60"/>
-      <c r="J13" s="60"/>
-      <c r="K13" s="60"/>
-      <c r="L13" s="60"/>
-      <c r="M13" s="60"/>
-      <c r="N13" s="60"/>
-      <c r="O13" s="60"/>
-      <c r="P13" s="60"/>
-      <c r="Q13" s="60"/>
-      <c r="R13" s="60"/>
-      <c r="S13" s="60"/>
-      <c r="T13" s="60"/>
-      <c r="U13" s="61"/>
+      <c r="G13" s="57"/>
+      <c r="H13" s="57"/>
+      <c r="I13" s="57"/>
+      <c r="J13" s="57"/>
+      <c r="K13" s="57"/>
+      <c r="L13" s="57"/>
+      <c r="M13" s="57"/>
+      <c r="N13" s="57"/>
+      <c r="O13" s="57"/>
+      <c r="P13" s="57"/>
+      <c r="Q13" s="57"/>
+      <c r="R13" s="57"/>
+      <c r="S13" s="57"/>
+      <c r="T13" s="57"/>
+      <c r="U13" s="58"/>
     </row>
     <row r="14" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F14" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="G14" s="57" t="s">
+      <c r="G14" s="54" t="s">
         <v>43</v>
       </c>
-      <c r="H14" s="57"/>
-      <c r="I14" s="57"/>
-      <c r="J14" s="57"/>
-      <c r="K14" s="57"/>
-      <c r="L14" s="57"/>
-      <c r="M14" s="57"/>
-      <c r="N14" s="57"/>
-      <c r="O14" s="57"/>
-      <c r="P14" s="57"/>
-      <c r="Q14" s="57"/>
-      <c r="R14" s="57"/>
-      <c r="S14" s="57"/>
-      <c r="T14" s="57"/>
-      <c r="U14" s="58"/>
+      <c r="H14" s="54"/>
+      <c r="I14" s="54"/>
+      <c r="J14" s="54"/>
+      <c r="K14" s="54"/>
+      <c r="L14" s="54"/>
+      <c r="M14" s="54"/>
+      <c r="N14" s="54"/>
+      <c r="O14" s="54"/>
+      <c r="P14" s="54"/>
+      <c r="Q14" s="54"/>
+      <c r="R14" s="54"/>
+      <c r="S14" s="54"/>
+      <c r="T14" s="54"/>
+      <c r="U14" s="55"/>
     </row>
     <row r="15" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F15" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="G15" s="57" t="s">
+      <c r="G15" s="54" t="s">
         <v>48</v>
       </c>
-      <c r="H15" s="57"/>
-      <c r="I15" s="57"/>
-      <c r="J15" s="57"/>
-      <c r="K15" s="57"/>
-      <c r="L15" s="57"/>
-      <c r="M15" s="57"/>
-      <c r="N15" s="57"/>
-      <c r="O15" s="57"/>
-      <c r="P15" s="57"/>
-      <c r="Q15" s="57"/>
-      <c r="R15" s="57"/>
-      <c r="S15" s="57"/>
-      <c r="T15" s="57"/>
-      <c r="U15" s="58"/>
+      <c r="H15" s="54"/>
+      <c r="I15" s="54"/>
+      <c r="J15" s="54"/>
+      <c r="K15" s="54"/>
+      <c r="L15" s="54"/>
+      <c r="M15" s="54"/>
+      <c r="N15" s="54"/>
+      <c r="O15" s="54"/>
+      <c r="P15" s="54"/>
+      <c r="Q15" s="54"/>
+      <c r="R15" s="54"/>
+      <c r="S15" s="54"/>
+      <c r="T15" s="54"/>
+      <c r="U15" s="55"/>
     </row>
     <row r="16" spans="6:21" x14ac:dyDescent="0.2">
       <c r="F16" s="35"/>
@@ -2316,46 +2302,46 @@
       <c r="U16" s="36"/>
     </row>
     <row r="17" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F17" s="64" t="s">
+      <c r="F17" s="61" t="s">
         <v>15</v>
       </c>
-      <c r="G17" s="65"/>
-      <c r="H17" s="65"/>
-      <c r="I17" s="65"/>
-      <c r="J17" s="65"/>
-      <c r="K17" s="65"/>
-      <c r="L17" s="65"/>
-      <c r="M17" s="65"/>
-      <c r="N17" s="65"/>
-      <c r="O17" s="65"/>
-      <c r="P17" s="65"/>
-      <c r="Q17" s="65"/>
-      <c r="R17" s="65"/>
-      <c r="S17" s="65"/>
-      <c r="T17" s="65"/>
-      <c r="U17" s="66"/>
+      <c r="G17" s="62"/>
+      <c r="H17" s="62"/>
+      <c r="I17" s="62"/>
+      <c r="J17" s="62"/>
+      <c r="K17" s="62"/>
+      <c r="L17" s="62"/>
+      <c r="M17" s="62"/>
+      <c r="N17" s="62"/>
+      <c r="O17" s="62"/>
+      <c r="P17" s="62"/>
+      <c r="Q17" s="62"/>
+      <c r="R17" s="62"/>
+      <c r="S17" s="62"/>
+      <c r="T17" s="62"/>
+      <c r="U17" s="63"/>
     </row>
     <row r="18" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F18" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="G18" s="57" t="s">
+      <c r="G18" s="54" t="s">
         <v>47</v>
       </c>
-      <c r="H18" s="57"/>
-      <c r="I18" s="57"/>
-      <c r="J18" s="57"/>
-      <c r="K18" s="57"/>
-      <c r="L18" s="57"/>
-      <c r="M18" s="57"/>
-      <c r="N18" s="57"/>
-      <c r="O18" s="57"/>
-      <c r="P18" s="57"/>
-      <c r="Q18" s="57"/>
-      <c r="R18" s="57"/>
-      <c r="S18" s="57"/>
-      <c r="T18" s="57"/>
-      <c r="U18" s="58"/>
+      <c r="H18" s="54"/>
+      <c r="I18" s="54"/>
+      <c r="J18" s="54"/>
+      <c r="K18" s="54"/>
+      <c r="L18" s="54"/>
+      <c r="M18" s="54"/>
+      <c r="N18" s="54"/>
+      <c r="O18" s="54"/>
+      <c r="P18" s="54"/>
+      <c r="Q18" s="54"/>
+      <c r="R18" s="54"/>
+      <c r="S18" s="54"/>
+      <c r="T18" s="54"/>
+      <c r="U18" s="55"/>
     </row>
     <row r="19" spans="6:21" x14ac:dyDescent="0.2">
       <c r="F19" s="35"/>
@@ -2376,46 +2362,46 @@
       <c r="U19" s="36"/>
     </row>
     <row r="20" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F20" s="64" t="s">
+      <c r="F20" s="61" t="s">
         <v>44</v>
       </c>
-      <c r="G20" s="65"/>
-      <c r="H20" s="65"/>
-      <c r="I20" s="65"/>
-      <c r="J20" s="65"/>
-      <c r="K20" s="65"/>
-      <c r="L20" s="65"/>
-      <c r="M20" s="65"/>
-      <c r="N20" s="65"/>
-      <c r="O20" s="65"/>
-      <c r="P20" s="65"/>
-      <c r="Q20" s="65"/>
-      <c r="R20" s="65"/>
-      <c r="S20" s="65"/>
-      <c r="T20" s="65"/>
-      <c r="U20" s="66"/>
+      <c r="G20" s="62"/>
+      <c r="H20" s="62"/>
+      <c r="I20" s="62"/>
+      <c r="J20" s="62"/>
+      <c r="K20" s="62"/>
+      <c r="L20" s="62"/>
+      <c r="M20" s="62"/>
+      <c r="N20" s="62"/>
+      <c r="O20" s="62"/>
+      <c r="P20" s="62"/>
+      <c r="Q20" s="62"/>
+      <c r="R20" s="62"/>
+      <c r="S20" s="62"/>
+      <c r="T20" s="62"/>
+      <c r="U20" s="63"/>
     </row>
     <row r="21" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F21" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="G21" s="57" t="s">
+      <c r="G21" s="54" t="s">
         <v>58</v>
       </c>
-      <c r="H21" s="57"/>
-      <c r="I21" s="57"/>
-      <c r="J21" s="57"/>
-      <c r="K21" s="57"/>
-      <c r="L21" s="57"/>
-      <c r="M21" s="57"/>
-      <c r="N21" s="57"/>
-      <c r="O21" s="57"/>
-      <c r="P21" s="57"/>
-      <c r="Q21" s="57"/>
-      <c r="R21" s="57"/>
-      <c r="S21" s="57"/>
-      <c r="T21" s="57"/>
-      <c r="U21" s="58"/>
+      <c r="H21" s="54"/>
+      <c r="I21" s="54"/>
+      <c r="J21" s="54"/>
+      <c r="K21" s="54"/>
+      <c r="L21" s="54"/>
+      <c r="M21" s="54"/>
+      <c r="N21" s="54"/>
+      <c r="O21" s="54"/>
+      <c r="P21" s="54"/>
+      <c r="Q21" s="54"/>
+      <c r="R21" s="54"/>
+      <c r="S21" s="54"/>
+      <c r="T21" s="54"/>
+      <c r="U21" s="55"/>
     </row>
     <row r="22" spans="6:21" x14ac:dyDescent="0.2">
       <c r="F22" s="35"/>
@@ -2436,46 +2422,46 @@
       <c r="U22" s="36"/>
     </row>
     <row r="23" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F23" s="64" t="s">
+      <c r="F23" s="61" t="s">
         <v>45</v>
       </c>
-      <c r="G23" s="65"/>
-      <c r="H23" s="65"/>
-      <c r="I23" s="65"/>
-      <c r="J23" s="65"/>
-      <c r="K23" s="65"/>
-      <c r="L23" s="65"/>
-      <c r="M23" s="65"/>
-      <c r="N23" s="65"/>
-      <c r="O23" s="65"/>
-      <c r="P23" s="65"/>
-      <c r="Q23" s="65"/>
-      <c r="R23" s="65"/>
-      <c r="S23" s="65"/>
-      <c r="T23" s="65"/>
-      <c r="U23" s="66"/>
+      <c r="G23" s="62"/>
+      <c r="H23" s="62"/>
+      <c r="I23" s="62"/>
+      <c r="J23" s="62"/>
+      <c r="K23" s="62"/>
+      <c r="L23" s="62"/>
+      <c r="M23" s="62"/>
+      <c r="N23" s="62"/>
+      <c r="O23" s="62"/>
+      <c r="P23" s="62"/>
+      <c r="Q23" s="62"/>
+      <c r="R23" s="62"/>
+      <c r="S23" s="62"/>
+      <c r="T23" s="62"/>
+      <c r="U23" s="63"/>
     </row>
     <row r="24" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F24" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="G24" s="67" t="s">
+      <c r="G24" s="64" t="s">
         <v>46</v>
       </c>
-      <c r="H24" s="67"/>
-      <c r="I24" s="67"/>
-      <c r="J24" s="67"/>
-      <c r="K24" s="67"/>
-      <c r="L24" s="67"/>
-      <c r="M24" s="67"/>
-      <c r="N24" s="67"/>
-      <c r="O24" s="67"/>
-      <c r="P24" s="67"/>
-      <c r="Q24" s="67"/>
-      <c r="R24" s="67"/>
-      <c r="S24" s="67"/>
-      <c r="T24" s="67"/>
-      <c r="U24" s="68"/>
+      <c r="H24" s="64"/>
+      <c r="I24" s="64"/>
+      <c r="J24" s="64"/>
+      <c r="K24" s="64"/>
+      <c r="L24" s="64"/>
+      <c r="M24" s="64"/>
+      <c r="N24" s="64"/>
+      <c r="O24" s="64"/>
+      <c r="P24" s="64"/>
+      <c r="Q24" s="64"/>
+      <c r="R24" s="64"/>
+      <c r="S24" s="64"/>
+      <c r="T24" s="64"/>
+      <c r="U24" s="65"/>
     </row>
     <row r="25" spans="6:21" x14ac:dyDescent="0.2">
       <c r="F25" s="32"/>
@@ -2532,174 +2518,174 @@
       <c r="U27" s="32"/>
     </row>
     <row r="28" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F28" s="70" t="s">
+      <c r="F28" s="67" t="s">
         <v>16</v>
       </c>
-      <c r="G28" s="71"/>
-      <c r="H28" s="71"/>
-      <c r="I28" s="71"/>
-      <c r="J28" s="71"/>
-      <c r="K28" s="71"/>
-      <c r="L28" s="71"/>
-      <c r="M28" s="71"/>
-      <c r="N28" s="71"/>
-      <c r="O28" s="71"/>
-      <c r="P28" s="71"/>
-      <c r="Q28" s="71"/>
-      <c r="R28" s="71"/>
-      <c r="S28" s="71"/>
-      <c r="T28" s="71"/>
-      <c r="U28" s="72"/>
+      <c r="G28" s="68"/>
+      <c r="H28" s="68"/>
+      <c r="I28" s="68"/>
+      <c r="J28" s="68"/>
+      <c r="K28" s="68"/>
+      <c r="L28" s="68"/>
+      <c r="M28" s="68"/>
+      <c r="N28" s="68"/>
+      <c r="O28" s="68"/>
+      <c r="P28" s="68"/>
+      <c r="Q28" s="68"/>
+      <c r="R28" s="68"/>
+      <c r="S28" s="68"/>
+      <c r="T28" s="68"/>
+      <c r="U28" s="69"/>
     </row>
     <row r="29" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F29" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="G29" s="49" t="s">
+      <c r="G29" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="H29" s="49"/>
-      <c r="I29" s="49"/>
-      <c r="J29" s="49"/>
-      <c r="K29" s="49"/>
-      <c r="L29" s="49"/>
-      <c r="M29" s="49"/>
-      <c r="N29" s="49"/>
-      <c r="O29" s="49"/>
-      <c r="P29" s="49"/>
-      <c r="Q29" s="49"/>
-      <c r="R29" s="49"/>
-      <c r="S29" s="49"/>
-      <c r="T29" s="49"/>
-      <c r="U29" s="50"/>
+      <c r="H29" s="46"/>
+      <c r="I29" s="46"/>
+      <c r="J29" s="46"/>
+      <c r="K29" s="46"/>
+      <c r="L29" s="46"/>
+      <c r="M29" s="46"/>
+      <c r="N29" s="46"/>
+      <c r="O29" s="46"/>
+      <c r="P29" s="46"/>
+      <c r="Q29" s="46"/>
+      <c r="R29" s="46"/>
+      <c r="S29" s="46"/>
+      <c r="T29" s="46"/>
+      <c r="U29" s="47"/>
     </row>
     <row r="30" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F30" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="G30" s="49" t="s">
+      <c r="G30" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="H30" s="49"/>
-      <c r="I30" s="49"/>
-      <c r="J30" s="49"/>
-      <c r="K30" s="49"/>
-      <c r="L30" s="49"/>
-      <c r="M30" s="49"/>
-      <c r="N30" s="49"/>
-      <c r="O30" s="49"/>
-      <c r="P30" s="49"/>
-      <c r="Q30" s="49"/>
-      <c r="R30" s="49"/>
-      <c r="S30" s="49"/>
-      <c r="T30" s="49"/>
-      <c r="U30" s="50"/>
+      <c r="H30" s="46"/>
+      <c r="I30" s="46"/>
+      <c r="J30" s="46"/>
+      <c r="K30" s="46"/>
+      <c r="L30" s="46"/>
+      <c r="M30" s="46"/>
+      <c r="N30" s="46"/>
+      <c r="O30" s="46"/>
+      <c r="P30" s="46"/>
+      <c r="Q30" s="46"/>
+      <c r="R30" s="46"/>
+      <c r="S30" s="46"/>
+      <c r="T30" s="46"/>
+      <c r="U30" s="47"/>
     </row>
     <row r="31" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F31" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="G31" s="49" t="s">
+      <c r="G31" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="H31" s="49"/>
-      <c r="I31" s="49"/>
-      <c r="J31" s="49"/>
-      <c r="K31" s="49"/>
-      <c r="L31" s="49"/>
-      <c r="M31" s="49"/>
-      <c r="N31" s="49"/>
-      <c r="O31" s="49"/>
-      <c r="P31" s="49"/>
-      <c r="Q31" s="49"/>
-      <c r="R31" s="49"/>
-      <c r="S31" s="49"/>
-      <c r="T31" s="49"/>
-      <c r="U31" s="50"/>
+      <c r="H31" s="46"/>
+      <c r="I31" s="46"/>
+      <c r="J31" s="46"/>
+      <c r="K31" s="46"/>
+      <c r="L31" s="46"/>
+      <c r="M31" s="46"/>
+      <c r="N31" s="46"/>
+      <c r="O31" s="46"/>
+      <c r="P31" s="46"/>
+      <c r="Q31" s="46"/>
+      <c r="R31" s="46"/>
+      <c r="S31" s="46"/>
+      <c r="T31" s="46"/>
+      <c r="U31" s="47"/>
     </row>
     <row r="32" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F32" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="G32" s="49" t="s">
+      <c r="G32" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="H32" s="49"/>
-      <c r="I32" s="49"/>
-      <c r="J32" s="49"/>
-      <c r="K32" s="49"/>
-      <c r="L32" s="49"/>
-      <c r="M32" s="49"/>
-      <c r="N32" s="49"/>
-      <c r="O32" s="49"/>
-      <c r="P32" s="49"/>
-      <c r="Q32" s="49"/>
-      <c r="R32" s="49"/>
-      <c r="S32" s="49"/>
-      <c r="T32" s="49"/>
-      <c r="U32" s="50"/>
+      <c r="H32" s="46"/>
+      <c r="I32" s="46"/>
+      <c r="J32" s="46"/>
+      <c r="K32" s="46"/>
+      <c r="L32" s="46"/>
+      <c r="M32" s="46"/>
+      <c r="N32" s="46"/>
+      <c r="O32" s="46"/>
+      <c r="P32" s="46"/>
+      <c r="Q32" s="46"/>
+      <c r="R32" s="46"/>
+      <c r="S32" s="46"/>
+      <c r="T32" s="46"/>
+      <c r="U32" s="47"/>
     </row>
     <row r="33" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F33" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="G33" s="49" t="s">
+      <c r="G33" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="H33" s="49"/>
-      <c r="I33" s="49"/>
-      <c r="J33" s="49"/>
-      <c r="K33" s="49"/>
-      <c r="L33" s="49"/>
-      <c r="M33" s="49"/>
-      <c r="N33" s="49"/>
-      <c r="O33" s="49"/>
-      <c r="P33" s="49"/>
-      <c r="Q33" s="49"/>
-      <c r="R33" s="49"/>
-      <c r="S33" s="49"/>
-      <c r="T33" s="49"/>
-      <c r="U33" s="50"/>
+      <c r="H33" s="46"/>
+      <c r="I33" s="46"/>
+      <c r="J33" s="46"/>
+      <c r="K33" s="46"/>
+      <c r="L33" s="46"/>
+      <c r="M33" s="46"/>
+      <c r="N33" s="46"/>
+      <c r="O33" s="46"/>
+      <c r="P33" s="46"/>
+      <c r="Q33" s="46"/>
+      <c r="R33" s="46"/>
+      <c r="S33" s="46"/>
+      <c r="T33" s="46"/>
+      <c r="U33" s="47"/>
     </row>
     <row r="34" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F34" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="G34" s="73" t="s">
+      <c r="G34" s="70" t="s">
         <v>30</v>
       </c>
-      <c r="H34" s="73"/>
-      <c r="I34" s="73"/>
-      <c r="J34" s="73"/>
-      <c r="K34" s="73"/>
-      <c r="L34" s="73"/>
-      <c r="M34" s="73"/>
-      <c r="N34" s="73"/>
-      <c r="O34" s="73"/>
-      <c r="P34" s="73"/>
-      <c r="Q34" s="73"/>
-      <c r="R34" s="73"/>
-      <c r="S34" s="73"/>
-      <c r="T34" s="73"/>
-      <c r="U34" s="74"/>
+      <c r="H34" s="70"/>
+      <c r="I34" s="70"/>
+      <c r="J34" s="70"/>
+      <c r="K34" s="70"/>
+      <c r="L34" s="70"/>
+      <c r="M34" s="70"/>
+      <c r="N34" s="70"/>
+      <c r="O34" s="70"/>
+      <c r="P34" s="70"/>
+      <c r="Q34" s="70"/>
+      <c r="R34" s="70"/>
+      <c r="S34" s="70"/>
+      <c r="T34" s="70"/>
+      <c r="U34" s="71"/>
     </row>
     <row r="35" spans="6:21" x14ac:dyDescent="0.2">
       <c r="F35" s="32"/>
-      <c r="G35" s="69"/>
-      <c r="H35" s="69"/>
-      <c r="I35" s="69"/>
-      <c r="J35" s="69"/>
-      <c r="K35" s="69"/>
-      <c r="L35" s="69"/>
-      <c r="M35" s="69"/>
-      <c r="N35" s="69"/>
-      <c r="O35" s="69"/>
-      <c r="P35" s="69"/>
-      <c r="Q35" s="69"/>
-      <c r="R35" s="69"/>
-      <c r="S35" s="69"/>
-      <c r="T35" s="69"/>
-      <c r="U35" s="69"/>
+      <c r="G35" s="66"/>
+      <c r="H35" s="66"/>
+      <c r="I35" s="66"/>
+      <c r="J35" s="66"/>
+      <c r="K35" s="66"/>
+      <c r="L35" s="66"/>
+      <c r="M35" s="66"/>
+      <c r="N35" s="66"/>
+      <c r="O35" s="66"/>
+      <c r="P35" s="66"/>
+      <c r="Q35" s="66"/>
+      <c r="R35" s="66"/>
+      <c r="S35" s="66"/>
+      <c r="T35" s="66"/>
+      <c r="U35" s="66"/>
     </row>
     <row r="37" spans="6:21" x14ac:dyDescent="0.2">
       <c r="F37" s="32"/>
@@ -2720,68 +2706,68 @@
       <c r="U37" s="32"/>
     </row>
     <row r="38" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F38" s="59" t="s">
+      <c r="F38" s="56" t="s">
         <v>20</v>
       </c>
-      <c r="G38" s="60"/>
-      <c r="H38" s="60"/>
-      <c r="I38" s="60"/>
-      <c r="J38" s="60"/>
-      <c r="K38" s="60"/>
-      <c r="L38" s="60"/>
-      <c r="M38" s="60"/>
-      <c r="N38" s="60"/>
-      <c r="O38" s="60"/>
-      <c r="P38" s="60"/>
-      <c r="Q38" s="60"/>
-      <c r="R38" s="60"/>
-      <c r="S38" s="60"/>
-      <c r="T38" s="60"/>
-      <c r="U38" s="61"/>
+      <c r="G38" s="57"/>
+      <c r="H38" s="57"/>
+      <c r="I38" s="57"/>
+      <c r="J38" s="57"/>
+      <c r="K38" s="57"/>
+      <c r="L38" s="57"/>
+      <c r="M38" s="57"/>
+      <c r="N38" s="57"/>
+      <c r="O38" s="57"/>
+      <c r="P38" s="57"/>
+      <c r="Q38" s="57"/>
+      <c r="R38" s="57"/>
+      <c r="S38" s="57"/>
+      <c r="T38" s="57"/>
+      <c r="U38" s="58"/>
     </row>
     <row r="39" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F39" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="G39" s="62" t="s">
+      <c r="G39" s="59" t="s">
         <v>40</v>
       </c>
-      <c r="H39" s="62"/>
-      <c r="I39" s="62"/>
-      <c r="J39" s="62"/>
-      <c r="K39" s="62"/>
-      <c r="L39" s="62"/>
-      <c r="M39" s="62"/>
-      <c r="N39" s="62"/>
-      <c r="O39" s="62"/>
-      <c r="P39" s="62"/>
-      <c r="Q39" s="62"/>
-      <c r="R39" s="62"/>
-      <c r="S39" s="62"/>
-      <c r="T39" s="62"/>
-      <c r="U39" s="63"/>
+      <c r="H39" s="59"/>
+      <c r="I39" s="59"/>
+      <c r="J39" s="59"/>
+      <c r="K39" s="59"/>
+      <c r="L39" s="59"/>
+      <c r="M39" s="59"/>
+      <c r="N39" s="59"/>
+      <c r="O39" s="59"/>
+      <c r="P39" s="59"/>
+      <c r="Q39" s="59"/>
+      <c r="R39" s="59"/>
+      <c r="S39" s="59"/>
+      <c r="T39" s="59"/>
+      <c r="U39" s="60"/>
     </row>
     <row r="40" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F40" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="G40" s="62" t="s">
+      <c r="G40" s="59" t="s">
         <v>31</v>
       </c>
-      <c r="H40" s="62"/>
-      <c r="I40" s="62"/>
-      <c r="J40" s="62"/>
-      <c r="K40" s="62"/>
-      <c r="L40" s="62"/>
-      <c r="M40" s="62"/>
-      <c r="N40" s="62"/>
-      <c r="O40" s="62"/>
-      <c r="P40" s="62"/>
-      <c r="Q40" s="62"/>
-      <c r="R40" s="62"/>
-      <c r="S40" s="62"/>
-      <c r="T40" s="62"/>
-      <c r="U40" s="63"/>
+      <c r="H40" s="59"/>
+      <c r="I40" s="59"/>
+      <c r="J40" s="59"/>
+      <c r="K40" s="59"/>
+      <c r="L40" s="59"/>
+      <c r="M40" s="59"/>
+      <c r="N40" s="59"/>
+      <c r="O40" s="59"/>
+      <c r="P40" s="59"/>
+      <c r="Q40" s="59"/>
+      <c r="R40" s="59"/>
+      <c r="S40" s="59"/>
+      <c r="T40" s="59"/>
+      <c r="U40" s="60"/>
     </row>
     <row r="41" spans="6:21" x14ac:dyDescent="0.2">
       <c r="F41" s="40"/>
@@ -2805,185 +2791,185 @@
       <c r="F42" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="G42" s="62" t="s">
+      <c r="G42" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="H42" s="62"/>
-      <c r="I42" s="62"/>
-      <c r="J42" s="62"/>
-      <c r="K42" s="62"/>
-      <c r="L42" s="62"/>
-      <c r="M42" s="62"/>
-      <c r="N42" s="62"/>
-      <c r="O42" s="62"/>
-      <c r="P42" s="62"/>
-      <c r="Q42" s="62"/>
-      <c r="R42" s="62"/>
-      <c r="S42" s="62"/>
-      <c r="T42" s="62"/>
-      <c r="U42" s="63"/>
+      <c r="H42" s="59"/>
+      <c r="I42" s="59"/>
+      <c r="J42" s="59"/>
+      <c r="K42" s="59"/>
+      <c r="L42" s="59"/>
+      <c r="M42" s="59"/>
+      <c r="N42" s="59"/>
+      <c r="O42" s="59"/>
+      <c r="P42" s="59"/>
+      <c r="Q42" s="59"/>
+      <c r="R42" s="59"/>
+      <c r="S42" s="59"/>
+      <c r="T42" s="59"/>
+      <c r="U42" s="60"/>
     </row>
     <row r="43" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F43" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="G43" s="47" t="s">
+      <c r="G43" s="44" t="s">
         <v>42</v>
       </c>
-      <c r="H43" s="47"/>
-      <c r="I43" s="47"/>
-      <c r="J43" s="47"/>
-      <c r="K43" s="47"/>
-      <c r="L43" s="47"/>
-      <c r="M43" s="47"/>
-      <c r="N43" s="47"/>
-      <c r="O43" s="47"/>
-      <c r="P43" s="47"/>
-      <c r="Q43" s="47"/>
-      <c r="R43" s="47"/>
-      <c r="S43" s="47"/>
-      <c r="T43" s="47"/>
-      <c r="U43" s="48"/>
+      <c r="H43" s="44"/>
+      <c r="I43" s="44"/>
+      <c r="J43" s="44"/>
+      <c r="K43" s="44"/>
+      <c r="L43" s="44"/>
+      <c r="M43" s="44"/>
+      <c r="N43" s="44"/>
+      <c r="O43" s="44"/>
+      <c r="P43" s="44"/>
+      <c r="Q43" s="44"/>
+      <c r="R43" s="44"/>
+      <c r="S43" s="44"/>
+      <c r="T43" s="44"/>
+      <c r="U43" s="45"/>
     </row>
     <row r="49" spans="5:25" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="M49" s="96" t="s">
+      <c r="M49" s="93" t="s">
         <v>49</v>
       </c>
-      <c r="N49" s="96"/>
-      <c r="O49" s="96"/>
+      <c r="N49" s="93"/>
+      <c r="O49" s="93"/>
     </row>
     <row r="51" spans="5:25" x14ac:dyDescent="0.2">
-      <c r="G51" s="87" t="s">
+      <c r="G51" s="84" t="s">
         <v>50</v>
       </c>
-      <c r="H51" s="88"/>
-      <c r="I51" s="89"/>
-      <c r="K51" s="87" t="s">
+      <c r="H51" s="85"/>
+      <c r="I51" s="86"/>
+      <c r="K51" s="84" t="s">
         <v>51</v>
       </c>
-      <c r="L51" s="88"/>
-      <c r="M51" s="89"/>
-      <c r="O51" s="87" t="s">
+      <c r="L51" s="85"/>
+      <c r="M51" s="86"/>
+      <c r="O51" s="84" t="s">
         <v>52</v>
       </c>
-      <c r="P51" s="88"/>
-      <c r="Q51" s="89"/>
-      <c r="S51" s="87" t="s">
+      <c r="P51" s="85"/>
+      <c r="Q51" s="86"/>
+      <c r="S51" s="84" t="s">
         <v>53</v>
       </c>
-      <c r="T51" s="88"/>
-      <c r="U51" s="89"/>
+      <c r="T51" s="85"/>
+      <c r="U51" s="86"/>
     </row>
     <row r="52" spans="5:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G52" s="90"/>
-      <c r="H52" s="91"/>
-      <c r="I52" s="92"/>
-      <c r="K52" s="90"/>
-      <c r="L52" s="91"/>
-      <c r="M52" s="92"/>
-      <c r="O52" s="90"/>
-      <c r="P52" s="91"/>
-      <c r="Q52" s="92"/>
-      <c r="S52" s="90"/>
-      <c r="T52" s="91"/>
-      <c r="U52" s="92"/>
+      <c r="G52" s="87"/>
+      <c r="H52" s="88"/>
+      <c r="I52" s="89"/>
+      <c r="K52" s="87"/>
+      <c r="L52" s="88"/>
+      <c r="M52" s="89"/>
+      <c r="O52" s="87"/>
+      <c r="P52" s="88"/>
+      <c r="Q52" s="89"/>
+      <c r="S52" s="87"/>
+      <c r="T52" s="88"/>
+      <c r="U52" s="89"/>
     </row>
     <row r="53" spans="5:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G53" s="93"/>
-      <c r="H53" s="94"/>
-      <c r="I53" s="95"/>
-      <c r="K53" s="93"/>
-      <c r="L53" s="94"/>
-      <c r="M53" s="95"/>
-      <c r="O53" s="93"/>
-      <c r="P53" s="94"/>
-      <c r="Q53" s="95"/>
-      <c r="S53" s="93"/>
-      <c r="T53" s="94"/>
-      <c r="U53" s="95"/>
+      <c r="G53" s="90"/>
+      <c r="H53" s="91"/>
+      <c r="I53" s="92"/>
+      <c r="K53" s="90"/>
+      <c r="L53" s="91"/>
+      <c r="M53" s="92"/>
+      <c r="O53" s="90"/>
+      <c r="P53" s="91"/>
+      <c r="Q53" s="92"/>
+      <c r="S53" s="90"/>
+      <c r="T53" s="91"/>
+      <c r="U53" s="92"/>
     </row>
     <row r="62" spans="5:25" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E62" s="96" t="s">
+      <c r="E62" s="93" t="s">
         <v>60</v>
       </c>
-      <c r="F62" s="96"/>
-      <c r="G62" s="96"/>
-      <c r="H62" s="96"/>
-      <c r="P62" s="96" t="s">
+      <c r="F62" s="93"/>
+      <c r="G62" s="93"/>
+      <c r="H62" s="93"/>
+      <c r="P62" s="93" t="s">
         <v>61</v>
       </c>
-      <c r="Q62" s="96"/>
-      <c r="R62" s="96"/>
-      <c r="S62" s="96"/>
-      <c r="V62" s="96" t="s">
+      <c r="Q62" s="93"/>
+      <c r="R62" s="93"/>
+      <c r="S62" s="93"/>
+      <c r="V62" s="93" t="s">
         <v>62</v>
       </c>
-      <c r="W62" s="96"/>
-      <c r="X62" s="96"/>
-      <c r="Y62" s="96"/>
+      <c r="W62" s="93"/>
+      <c r="X62" s="93"/>
+      <c r="Y62" s="93"/>
     </row>
     <row r="63" spans="5:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="66" spans="3:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C66" s="97" t="s">
+      <c r="C66" s="94" t="s">
         <v>56</v>
       </c>
-      <c r="D66" s="98"/>
-      <c r="F66" s="97" t="s">
+      <c r="D66" s="95"/>
+      <c r="F66" s="94" t="s">
         <v>56</v>
       </c>
-      <c r="G66" s="98"/>
-      <c r="I66" s="97" t="s">
+      <c r="G66" s="95"/>
+      <c r="I66" s="94" t="s">
         <v>56</v>
       </c>
-      <c r="J66" s="98"/>
-      <c r="N66" s="75" t="s">
+      <c r="J66" s="95"/>
+      <c r="N66" s="72" t="s">
         <v>56</v>
       </c>
-      <c r="O66" s="76"/>
-      <c r="Q66" s="75" t="s">
+      <c r="O66" s="73"/>
+      <c r="Q66" s="72" t="s">
         <v>56</v>
       </c>
-      <c r="R66" s="76"/>
-      <c r="T66" s="75" t="s">
+      <c r="R66" s="73"/>
+      <c r="T66" s="72" t="s">
         <v>55</v>
       </c>
-      <c r="U66" s="76"/>
-      <c r="W66" s="81" t="s">
+      <c r="U66" s="73"/>
+      <c r="W66" s="78" t="s">
         <v>54</v>
       </c>
-      <c r="X66" s="82"/>
+      <c r="X66" s="79"/>
     </row>
     <row r="67" spans="3:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C67" s="99"/>
-      <c r="D67" s="100"/>
-      <c r="F67" s="99"/>
-      <c r="G67" s="100"/>
-      <c r="I67" s="99"/>
-      <c r="J67" s="100"/>
-      <c r="N67" s="77"/>
-      <c r="O67" s="78"/>
-      <c r="Q67" s="77"/>
-      <c r="R67" s="78"/>
-      <c r="T67" s="77"/>
-      <c r="U67" s="78"/>
-      <c r="W67" s="83"/>
-      <c r="X67" s="84"/>
+      <c r="C67" s="96"/>
+      <c r="D67" s="97"/>
+      <c r="F67" s="96"/>
+      <c r="G67" s="97"/>
+      <c r="I67" s="96"/>
+      <c r="J67" s="97"/>
+      <c r="N67" s="74"/>
+      <c r="O67" s="75"/>
+      <c r="Q67" s="74"/>
+      <c r="R67" s="75"/>
+      <c r="T67" s="74"/>
+      <c r="U67" s="75"/>
+      <c r="W67" s="80"/>
+      <c r="X67" s="81"/>
     </row>
     <row r="68" spans="3:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C68" s="101"/>
-      <c r="D68" s="102"/>
-      <c r="F68" s="101"/>
-      <c r="G68" s="102"/>
-      <c r="I68" s="101"/>
-      <c r="J68" s="102"/>
-      <c r="N68" s="79"/>
-      <c r="O68" s="80"/>
-      <c r="Q68" s="79"/>
-      <c r="R68" s="80"/>
-      <c r="T68" s="79"/>
-      <c r="U68" s="80"/>
-      <c r="W68" s="85"/>
-      <c r="X68" s="86"/>
+      <c r="C68" s="98"/>
+      <c r="D68" s="99"/>
+      <c r="F68" s="98"/>
+      <c r="G68" s="99"/>
+      <c r="I68" s="98"/>
+      <c r="J68" s="99"/>
+      <c r="N68" s="76"/>
+      <c r="O68" s="77"/>
+      <c r="Q68" s="76"/>
+      <c r="R68" s="77"/>
+      <c r="T68" s="76"/>
+      <c r="U68" s="77"/>
+      <c r="W68" s="82"/>
+      <c r="X68" s="83"/>
     </row>
     <row r="69" spans="3:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
@@ -3062,32 +3048,32 @@
       </c>
     </row>
     <row r="2" spans="5:13" ht="26" x14ac:dyDescent="0.2">
-      <c r="E2" s="105" t="s">
+      <c r="E2" s="102" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="105"/>
-      <c r="G2" s="105"/>
-      <c r="H2" s="105"/>
-      <c r="I2" s="105"/>
-      <c r="J2" s="105"/>
-      <c r="K2" s="105"/>
-      <c r="L2" s="105"/>
-      <c r="M2" s="105"/>
+      <c r="F2" s="102"/>
+      <c r="G2" s="102"/>
+      <c r="H2" s="102"/>
+      <c r="I2" s="102"/>
+      <c r="J2" s="102"/>
+      <c r="K2" s="102"/>
+      <c r="L2" s="102"/>
+      <c r="M2" s="102"/>
     </row>
     <row r="4" spans="5:13" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E4"/>
-      <c r="F4" s="107" t="s">
+      <c r="F4" s="104" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="108"/>
-      <c r="H4" s="109"/>
-      <c r="I4" s="106" t="s">
+      <c r="G4" s="105"/>
+      <c r="H4" s="106"/>
+      <c r="I4" s="103" t="s">
         <v>38</v>
       </c>
-      <c r="J4" s="106"/>
-      <c r="K4" s="106"/>
-      <c r="L4" s="106"/>
-      <c r="M4" s="103" t="s">
+      <c r="J4" s="103"/>
+      <c r="K4" s="103"/>
+      <c r="L4" s="103"/>
+      <c r="M4" s="100" t="s">
         <v>3</v>
       </c>
     </row>
@@ -3102,15 +3088,15 @@
       <c r="H5" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="I5" s="110" t="s">
+      <c r="I5" s="107" t="s">
         <v>4</v>
       </c>
-      <c r="J5" s="111"/>
-      <c r="K5" s="106" t="s">
+      <c r="J5" s="108"/>
+      <c r="K5" s="103" t="s">
         <v>1</v>
       </c>
-      <c r="L5" s="106"/>
-      <c r="M5" s="104"/>
+      <c r="L5" s="103"/>
+      <c r="M5" s="101"/>
     </row>
     <row r="6" spans="5:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E6"/>
@@ -3274,14 +3260,14 @@
   </cols>
   <sheetData>
     <row r="3" spans="4:9" s="13" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D3" s="112" t="s">
+      <c r="D3" s="109" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="112"/>
-      <c r="F3" s="112"/>
-      <c r="G3" s="112"/>
-      <c r="H3" s="112"/>
-      <c r="I3" s="112"/>
+      <c r="E3" s="109"/>
+      <c r="F3" s="109"/>
+      <c r="G3" s="109"/>
+      <c r="H3" s="109"/>
+      <c r="I3" s="109"/>
     </row>
     <row r="5" spans="4:9" s="8" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D5" s="27" t="s">
@@ -3618,11 +3604,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="B1:U21"/>
+  <dimension ref="B1:V21"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
+      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3642,92 +3628,94 @@
     <col min="25" max="26" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:21" ht="21" x14ac:dyDescent="0.2">
-      <c r="B1" s="113" t="s">
+    <row r="1" spans="2:22" ht="21" x14ac:dyDescent="0.2">
+      <c r="B1" s="134" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="114"/>
-      <c r="D1" s="114"/>
-      <c r="E1" s="114"/>
-      <c r="F1" s="114"/>
-      <c r="G1" s="114"/>
-      <c r="H1" s="114"/>
-      <c r="I1" s="114"/>
-      <c r="J1" s="114"/>
-      <c r="K1" s="114"/>
-      <c r="L1" s="114"/>
-      <c r="M1" s="114"/>
-      <c r="N1" s="114"/>
-      <c r="O1" s="114"/>
-      <c r="P1" s="114"/>
-      <c r="Q1" s="114"/>
-      <c r="R1" s="114"/>
-      <c r="S1" s="114"/>
-      <c r="T1" s="114"/>
-      <c r="U1" s="114"/>
-    </row>
-    <row r="2" spans="2:21" ht="19" x14ac:dyDescent="0.25">
-      <c r="B2" s="115" t="s">
+      <c r="C1" s="135"/>
+      <c r="D1" s="135"/>
+      <c r="E1" s="135"/>
+      <c r="F1" s="135"/>
+      <c r="G1" s="135"/>
+      <c r="H1" s="135"/>
+      <c r="I1" s="135"/>
+      <c r="J1" s="135"/>
+      <c r="K1" s="135"/>
+      <c r="L1" s="135"/>
+      <c r="M1" s="135"/>
+      <c r="N1" s="135"/>
+      <c r="O1" s="135"/>
+      <c r="P1" s="135"/>
+      <c r="Q1" s="135"/>
+      <c r="R1" s="135"/>
+      <c r="S1" s="135"/>
+      <c r="T1" s="135"/>
+      <c r="U1" s="135"/>
+      <c r="V1" s="135"/>
+    </row>
+    <row r="2" spans="2:22" ht="19" x14ac:dyDescent="0.25">
+      <c r="B2" s="110" t="s">
         <v>67</v>
       </c>
-      <c r="C2" s="116"/>
-      <c r="D2" s="116"/>
-      <c r="E2" s="116"/>
-      <c r="F2" s="115" t="s">
+      <c r="C2" s="111"/>
+      <c r="D2" s="111"/>
+      <c r="E2" s="111"/>
+      <c r="F2" s="112"/>
+      <c r="G2" s="110" t="s">
         <v>68</v>
       </c>
-      <c r="G2" s="116"/>
-      <c r="H2" s="116"/>
-      <c r="I2" s="116"/>
-      <c r="J2" s="117" t="s">
+      <c r="H2" s="111"/>
+      <c r="I2" s="111"/>
+      <c r="J2" s="112"/>
+      <c r="K2" s="113" t="s">
         <v>69</v>
       </c>
-      <c r="K2" s="118"/>
-      <c r="L2" s="118"/>
-      <c r="M2" s="117" t="s">
+      <c r="L2" s="114"/>
+      <c r="M2" s="115"/>
+      <c r="N2" s="113" t="s">
         <v>70</v>
       </c>
-      <c r="N2" s="118"/>
-      <c r="O2" s="118"/>
-      <c r="P2" s="117" t="s">
+      <c r="O2" s="114"/>
+      <c r="P2" s="115"/>
+      <c r="Q2" s="113" t="s">
         <v>71</v>
       </c>
-      <c r="Q2" s="118"/>
-      <c r="R2" s="118"/>
-      <c r="S2" s="117" t="s">
+      <c r="R2" s="114"/>
+      <c r="S2" s="115"/>
+      <c r="T2" s="113" t="s">
         <v>72</v>
       </c>
-      <c r="T2" s="118"/>
-      <c r="U2" s="42" t="s">
+      <c r="U2" s="115"/>
+      <c r="V2" s="42" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="2:21" ht="68" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:22" ht="51" x14ac:dyDescent="0.2">
       <c r="B3" s="43" t="s">
         <v>33</v>
       </c>
       <c r="C3" s="43" t="s">
+        <v>73</v>
+      </c>
+      <c r="D3" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="43" t="s">
+      <c r="E3" s="43" t="s">
         <v>34</v>
       </c>
-      <c r="E3" s="43" t="s">
-        <v>73</v>
-      </c>
       <c r="F3" s="43" t="s">
+        <v>74</v>
+      </c>
+      <c r="G3" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="G3" s="43" t="s">
+      <c r="H3" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="H3" s="43" t="s">
-        <v>74</v>
-      </c>
-      <c r="I3" s="136" t="s">
+      <c r="I3" s="43" t="s">
         <v>75</v>
       </c>
-      <c r="J3" s="43" t="s">
+      <c r="J3" s="133" t="s">
         <v>76</v>
       </c>
       <c r="K3" s="43" t="s">
@@ -3740,13 +3728,13 @@
         <v>79</v>
       </c>
       <c r="N3" s="43" t="s">
+        <v>80</v>
+      </c>
+      <c r="O3" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="O3" s="43" t="s">
+      <c r="P3" s="43" t="s">
         <v>65</v>
-      </c>
-      <c r="P3" s="43" t="s">
-        <v>76</v>
       </c>
       <c r="Q3" s="43" t="s">
         <v>77</v>
@@ -3755,71 +3743,30 @@
         <v>78</v>
       </c>
       <c r="S3" s="43" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="T3" s="43" t="s">
         <v>81</v>
       </c>
       <c r="U3" s="43" t="s">
+        <v>82</v>
+      </c>
+      <c r="V3" s="43" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B4" s="44"/>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44"/>
-      <c r="E4" s="44"/>
-      <c r="F4" s="44"/>
-      <c r="G4" s="44"/>
-      <c r="H4" s="44"/>
-      <c r="I4" s="137"/>
-      <c r="J4" s="44"/>
-      <c r="K4" s="44"/>
-      <c r="L4" s="44"/>
-      <c r="M4" s="44"/>
-      <c r="N4" s="44"/>
-      <c r="O4" s="44"/>
-      <c r="P4" s="44"/>
-      <c r="Q4" s="44"/>
-      <c r="R4" s="44"/>
-      <c r="S4" s="44"/>
-      <c r="T4" s="44"/>
-      <c r="U4" s="44"/>
-    </row>
-    <row r="5" spans="2:21" ht="16" x14ac:dyDescent="0.2">
-      <c r="B5" s="45"/>
-      <c r="C5" s="45"/>
-      <c r="D5" s="45"/>
-      <c r="E5" s="45"/>
-      <c r="F5" s="45"/>
-      <c r="G5" s="45"/>
-      <c r="H5" s="45"/>
-      <c r="I5" s="137"/>
-      <c r="J5" s="45"/>
-      <c r="K5" s="45"/>
-      <c r="L5" s="45"/>
-      <c r="M5" s="45"/>
-      <c r="N5" s="45"/>
-      <c r="O5" s="45"/>
-      <c r="P5" s="45"/>
-      <c r="Q5" s="45"/>
-      <c r="R5" s="45"/>
-      <c r="S5" s="45"/>
-      <c r="T5" s="46"/>
-      <c r="U5" s="44"/>
-    </row>
-    <row r="8" spans="2:21" s="33" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="2:22" s="33" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="17" s="33" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="21" s="33" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="M2:O2"/>
-    <mergeCell ref="P2:R2"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="S2:T2"/>
-    <mergeCell ref="B1:U1"/>
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="K2:M2"/>
+    <mergeCell ref="Q2:S2"/>
+    <mergeCell ref="N2:P2"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="B1:V1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3844,55 +3791,55 @@
   </cols>
   <sheetData>
     <row r="2" spans="5:13" ht="26" x14ac:dyDescent="0.2">
-      <c r="E2" s="105" t="s">
+      <c r="E2" s="102" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="105"/>
-      <c r="G2" s="105"/>
-      <c r="H2" s="105"/>
-      <c r="I2" s="105"/>
-      <c r="J2" s="105"/>
-      <c r="K2" s="105"/>
-      <c r="L2" s="105"/>
-      <c r="M2" s="105"/>
+      <c r="F2" s="102"/>
+      <c r="G2" s="102"/>
+      <c r="H2" s="102"/>
+      <c r="I2" s="102"/>
+      <c r="J2" s="102"/>
+      <c r="K2" s="102"/>
+      <c r="L2" s="102"/>
+      <c r="M2" s="102"/>
     </row>
     <row r="4" spans="5:13" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E4" s="103" t="s">
+      <c r="E4" s="100" t="s">
         <v>0</v>
       </c>
-      <c r="F4" s="122" t="s">
+      <c r="F4" s="119" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="123"/>
-      <c r="H4" s="124"/>
-      <c r="I4" s="110" t="s">
+      <c r="G4" s="120"/>
+      <c r="H4" s="121"/>
+      <c r="I4" s="107" t="s">
         <v>8</v>
       </c>
-      <c r="J4" s="128"/>
-      <c r="K4" s="128"/>
-      <c r="L4" s="129"/>
-      <c r="M4" s="103" t="s">
+      <c r="J4" s="125"/>
+      <c r="K4" s="125"/>
+      <c r="L4" s="126"/>
+      <c r="M4" s="100" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="5:13" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E5" s="104"/>
-      <c r="F5" s="125"/>
-      <c r="G5" s="126"/>
-      <c r="H5" s="127"/>
+      <c r="E5" s="101"/>
+      <c r="F5" s="122"/>
+      <c r="G5" s="123"/>
+      <c r="H5" s="124"/>
       <c r="I5" s="4"/>
       <c r="J5" s="5"/>
       <c r="K5" s="6"/>
       <c r="L5" s="4"/>
-      <c r="M5" s="104"/>
+      <c r="M5" s="101"/>
     </row>
     <row r="6" spans="5:13" ht="167.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E6" s="2">
         <v>1</v>
       </c>
-      <c r="F6" s="130"/>
-      <c r="G6" s="131"/>
-      <c r="H6" s="132"/>
+      <c r="F6" s="127"/>
+      <c r="G6" s="128"/>
+      <c r="H6" s="129"/>
       <c r="I6" s="24"/>
       <c r="J6" s="24"/>
       <c r="K6" s="24"/>
@@ -3903,9 +3850,9 @@
       <c r="E7" s="2">
         <v>2</v>
       </c>
-      <c r="F7" s="130"/>
-      <c r="G7" s="131"/>
-      <c r="H7" s="132"/>
+      <c r="F7" s="127"/>
+      <c r="G7" s="128"/>
+      <c r="H7" s="129"/>
       <c r="I7" s="24"/>
       <c r="J7" s="24"/>
       <c r="K7" s="24"/>
@@ -3916,9 +3863,9 @@
       <c r="E8" s="2">
         <v>3</v>
       </c>
-      <c r="F8" s="133"/>
-      <c r="G8" s="134"/>
-      <c r="H8" s="135"/>
+      <c r="F8" s="130"/>
+      <c r="G8" s="131"/>
+      <c r="H8" s="132"/>
       <c r="I8" s="24"/>
       <c r="J8" s="24"/>
       <c r="K8" s="24"/>
@@ -3929,9 +3876,9 @@
       <c r="E9" s="2">
         <v>4</v>
       </c>
-      <c r="F9" s="133"/>
-      <c r="G9" s="134"/>
-      <c r="H9" s="135"/>
+      <c r="F9" s="130"/>
+      <c r="G9" s="131"/>
+      <c r="H9" s="132"/>
       <c r="I9" s="24"/>
       <c r="J9" s="24"/>
       <c r="K9" s="24"/>
@@ -3942,9 +3889,9 @@
       <c r="E10" s="2">
         <v>5</v>
       </c>
-      <c r="F10" s="119"/>
-      <c r="G10" s="120"/>
-      <c r="H10" s="121"/>
+      <c r="F10" s="116"/>
+      <c r="G10" s="117"/>
+      <c r="H10" s="118"/>
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
@@ -3955,9 +3902,9 @@
       <c r="E11" s="2">
         <v>6</v>
       </c>
-      <c r="F11" s="119"/>
-      <c r="G11" s="120"/>
-      <c r="H11" s="121"/>
+      <c r="F11" s="116"/>
+      <c r="G11" s="117"/>
+      <c r="H11" s="118"/>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
@@ -3968,9 +3915,9 @@
       <c r="E12" s="2">
         <v>7</v>
       </c>
-      <c r="F12" s="119"/>
-      <c r="G12" s="120"/>
-      <c r="H12" s="121"/>
+      <c r="F12" s="116"/>
+      <c r="G12" s="117"/>
+      <c r="H12" s="118"/>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
@@ -3981,9 +3928,9 @@
       <c r="E13" s="2">
         <v>8</v>
       </c>
-      <c r="F13" s="119"/>
-      <c r="G13" s="120"/>
-      <c r="H13" s="121"/>
+      <c r="F13" s="116"/>
+      <c r="G13" s="117"/>
+      <c r="H13" s="118"/>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
@@ -3994,9 +3941,9 @@
       <c r="E14" s="2">
         <v>9</v>
       </c>
-      <c r="F14" s="119"/>
-      <c r="G14" s="120"/>
-      <c r="H14" s="121"/>
+      <c r="F14" s="116"/>
+      <c r="G14" s="117"/>
+      <c r="H14" s="118"/>
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
@@ -4007,9 +3954,9 @@
       <c r="E15" s="2">
         <v>10</v>
       </c>
-      <c r="F15" s="119"/>
-      <c r="G15" s="120"/>
-      <c r="H15" s="121"/>
+      <c r="F15" s="116"/>
+      <c r="G15" s="117"/>
+      <c r="H15" s="118"/>
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
@@ -4020,9 +3967,9 @@
       <c r="E16" s="2">
         <v>11</v>
       </c>
-      <c r="F16" s="119"/>
-      <c r="G16" s="120"/>
-      <c r="H16" s="121"/>
+      <c r="F16" s="116"/>
+      <c r="G16" s="117"/>
+      <c r="H16" s="118"/>
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
@@ -4033,9 +3980,9 @@
       <c r="E17" s="2">
         <v>12</v>
       </c>
-      <c r="F17" s="119"/>
-      <c r="G17" s="120"/>
-      <c r="H17" s="121"/>
+      <c r="F17" s="116"/>
+      <c r="G17" s="117"/>
+      <c r="H17" s="118"/>
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
@@ -4046,9 +3993,9 @@
       <c r="E18" s="2">
         <v>13</v>
       </c>
-      <c r="F18" s="119"/>
-      <c r="G18" s="120"/>
-      <c r="H18" s="121"/>
+      <c r="F18" s="116"/>
+      <c r="G18" s="117"/>
+      <c r="H18" s="118"/>
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
@@ -4059,9 +4006,9 @@
       <c r="E19" s="2">
         <v>14</v>
       </c>
-      <c r="F19" s="119"/>
-      <c r="G19" s="120"/>
-      <c r="H19" s="121"/>
+      <c r="F19" s="116"/>
+      <c r="G19" s="117"/>
+      <c r="H19" s="118"/>
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
@@ -4072,9 +4019,9 @@
       <c r="E20" s="2">
         <v>15</v>
       </c>
-      <c r="F20" s="119"/>
-      <c r="G20" s="120"/>
-      <c r="H20" s="121"/>
+      <c r="F20" s="116"/>
+      <c r="G20" s="117"/>
+      <c r="H20" s="118"/>
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>

</xml_diff>

<commit_message>
add osh data and columns and fix some performance bug
</commit_message>
<xml_diff>
--- a/cockpit_template.xlsx
+++ b/cockpit_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Roi.Dital/roid_playground/paamonim/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{511B55F8-FF7D-234F-8E97-859F74FB0EE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FCACDA2-4AD7-2F4E-ADA5-A27F0E4DA648}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="19440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="85">
   <si>
     <t>#</t>
   </si>
@@ -294,7 +294,13 @@
     <t>רישום עו״ש אחרון</t>
   </si>
   <si>
-    <t>יתרת עו״שׁ</t>
+    <t>עו״ש חודש קודם</t>
+  </si>
+  <si>
+    <t>שינוי בעו״ש מחודש קודם</t>
+  </si>
+  <si>
+    <t>עו״ש חודש נוכחי</t>
   </si>
 </sst>
 </file>
@@ -541,7 +547,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -707,11 +713,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="136">
+  <cellXfs count="137">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -840,18 +857,153 @@
     <xf numFmtId="0" fontId="15" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="2"/>
     </xf>
@@ -876,138 +1028,6 @@
     <xf numFmtId="0" fontId="12" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1056,6 +1076,12 @@
     <xf numFmtId="0" fontId="19" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
@@ -1107,14 +1133,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2022,24 +2042,24 @@
   <sheetData>
     <row r="1" spans="6:21" ht="20" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F2" s="48" t="s">
+      <c r="F2" s="93" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="48"/>
-      <c r="H2" s="48"/>
-      <c r="I2" s="48"/>
-      <c r="J2" s="48"/>
-      <c r="K2" s="48"/>
-      <c r="L2" s="48"/>
-      <c r="M2" s="48"/>
-      <c r="N2" s="48"/>
-      <c r="O2" s="48"/>
-      <c r="P2" s="48"/>
-      <c r="Q2" s="48"/>
-      <c r="R2" s="48"/>
-      <c r="S2" s="48"/>
-      <c r="T2" s="48"/>
-      <c r="U2" s="48"/>
+      <c r="G2" s="93"/>
+      <c r="H2" s="93"/>
+      <c r="I2" s="93"/>
+      <c r="J2" s="93"/>
+      <c r="K2" s="93"/>
+      <c r="L2" s="93"/>
+      <c r="M2" s="93"/>
+      <c r="N2" s="93"/>
+      <c r="O2" s="93"/>
+      <c r="P2" s="93"/>
+      <c r="Q2" s="93"/>
+      <c r="R2" s="93"/>
+      <c r="S2" s="93"/>
+      <c r="T2" s="93"/>
+      <c r="U2" s="93"/>
     </row>
     <row r="3" spans="6:21" x14ac:dyDescent="0.2">
       <c r="F3" s="30"/>
@@ -2060,68 +2080,68 @@
       <c r="U3" s="30"/>
     </row>
     <row r="4" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F4" s="56" t="s">
+      <c r="F4" s="88" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="57"/>
-      <c r="H4" s="57"/>
-      <c r="I4" s="57"/>
-      <c r="J4" s="57"/>
-      <c r="K4" s="57"/>
-      <c r="L4" s="57"/>
-      <c r="M4" s="57"/>
-      <c r="N4" s="57"/>
-      <c r="O4" s="57"/>
-      <c r="P4" s="57"/>
-      <c r="Q4" s="57"/>
-      <c r="R4" s="57"/>
-      <c r="S4" s="57"/>
-      <c r="T4" s="57"/>
-      <c r="U4" s="58"/>
+      <c r="G4" s="89"/>
+      <c r="H4" s="89"/>
+      <c r="I4" s="89"/>
+      <c r="J4" s="89"/>
+      <c r="K4" s="89"/>
+      <c r="L4" s="89"/>
+      <c r="M4" s="89"/>
+      <c r="N4" s="89"/>
+      <c r="O4" s="89"/>
+      <c r="P4" s="89"/>
+      <c r="Q4" s="89"/>
+      <c r="R4" s="89"/>
+      <c r="S4" s="89"/>
+      <c r="T4" s="89"/>
+      <c r="U4" s="90"/>
     </row>
     <row r="5" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F5" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="59" t="s">
+      <c r="G5" s="73" t="s">
         <v>39</v>
       </c>
-      <c r="H5" s="59"/>
-      <c r="I5" s="59"/>
-      <c r="J5" s="59"/>
-      <c r="K5" s="59"/>
-      <c r="L5" s="59"/>
-      <c r="M5" s="59"/>
-      <c r="N5" s="59"/>
-      <c r="O5" s="59"/>
-      <c r="P5" s="59"/>
-      <c r="Q5" s="59"/>
-      <c r="R5" s="59"/>
-      <c r="S5" s="59"/>
-      <c r="T5" s="59"/>
-      <c r="U5" s="60"/>
+      <c r="H5" s="73"/>
+      <c r="I5" s="73"/>
+      <c r="J5" s="73"/>
+      <c r="K5" s="73"/>
+      <c r="L5" s="73"/>
+      <c r="M5" s="73"/>
+      <c r="N5" s="73"/>
+      <c r="O5" s="73"/>
+      <c r="P5" s="73"/>
+      <c r="Q5" s="73"/>
+      <c r="R5" s="73"/>
+      <c r="S5" s="73"/>
+      <c r="T5" s="73"/>
+      <c r="U5" s="74"/>
     </row>
     <row r="6" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F6" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="44" t="s">
+      <c r="G6" s="91" t="s">
         <v>41</v>
       </c>
-      <c r="H6" s="44"/>
-      <c r="I6" s="44"/>
-      <c r="J6" s="44"/>
-      <c r="K6" s="44"/>
-      <c r="L6" s="44"/>
-      <c r="M6" s="44"/>
-      <c r="N6" s="44"/>
-      <c r="O6" s="44"/>
-      <c r="P6" s="44"/>
-      <c r="Q6" s="44"/>
-      <c r="R6" s="44"/>
-      <c r="S6" s="44"/>
-      <c r="T6" s="44"/>
-      <c r="U6" s="45"/>
+      <c r="H6" s="91"/>
+      <c r="I6" s="91"/>
+      <c r="J6" s="91"/>
+      <c r="K6" s="91"/>
+      <c r="L6" s="91"/>
+      <c r="M6" s="91"/>
+      <c r="N6" s="91"/>
+      <c r="O6" s="91"/>
+      <c r="P6" s="91"/>
+      <c r="Q6" s="91"/>
+      <c r="R6" s="91"/>
+      <c r="S6" s="91"/>
+      <c r="T6" s="91"/>
+      <c r="U6" s="92"/>
     </row>
     <row r="7" spans="6:21" x14ac:dyDescent="0.2">
       <c r="F7" s="31"/>
@@ -2142,46 +2162,46 @@
       <c r="U7" s="31"/>
     </row>
     <row r="8" spans="6:21" ht="26" x14ac:dyDescent="0.2">
-      <c r="F8" s="49" t="s">
+      <c r="F8" s="94" t="s">
         <v>18</v>
       </c>
-      <c r="G8" s="50"/>
-      <c r="H8" s="50"/>
-      <c r="I8" s="50"/>
-      <c r="J8" s="50"/>
-      <c r="K8" s="50"/>
-      <c r="L8" s="50"/>
-      <c r="M8" s="50"/>
-      <c r="N8" s="50"/>
-      <c r="O8" s="50"/>
-      <c r="P8" s="50"/>
-      <c r="Q8" s="50"/>
-      <c r="R8" s="50"/>
-      <c r="S8" s="50"/>
-      <c r="T8" s="50"/>
-      <c r="U8" s="51"/>
+      <c r="G8" s="95"/>
+      <c r="H8" s="95"/>
+      <c r="I8" s="95"/>
+      <c r="J8" s="95"/>
+      <c r="K8" s="95"/>
+      <c r="L8" s="95"/>
+      <c r="M8" s="95"/>
+      <c r="N8" s="95"/>
+      <c r="O8" s="95"/>
+      <c r="P8" s="95"/>
+      <c r="Q8" s="95"/>
+      <c r="R8" s="95"/>
+      <c r="S8" s="95"/>
+      <c r="T8" s="95"/>
+      <c r="U8" s="96"/>
     </row>
     <row r="9" spans="6:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F9" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="G9" s="52" t="s">
+      <c r="G9" s="97" t="s">
         <v>59</v>
       </c>
-      <c r="H9" s="52"/>
-      <c r="I9" s="52"/>
-      <c r="J9" s="52"/>
-      <c r="K9" s="52"/>
-      <c r="L9" s="52"/>
-      <c r="M9" s="52"/>
-      <c r="N9" s="52"/>
-      <c r="O9" s="52"/>
-      <c r="P9" s="52"/>
-      <c r="Q9" s="52"/>
-      <c r="R9" s="52"/>
-      <c r="S9" s="52"/>
-      <c r="T9" s="52"/>
-      <c r="U9" s="53"/>
+      <c r="H9" s="97"/>
+      <c r="I9" s="97"/>
+      <c r="J9" s="97"/>
+      <c r="K9" s="97"/>
+      <c r="L9" s="97"/>
+      <c r="M9" s="97"/>
+      <c r="N9" s="97"/>
+      <c r="O9" s="97"/>
+      <c r="P9" s="97"/>
+      <c r="Q9" s="97"/>
+      <c r="R9" s="97"/>
+      <c r="S9" s="97"/>
+      <c r="T9" s="97"/>
+      <c r="U9" s="98"/>
     </row>
     <row r="10" spans="6:21" x14ac:dyDescent="0.2">
       <c r="F10" s="32"/>
@@ -2220,68 +2240,68 @@
       <c r="U12" s="32"/>
     </row>
     <row r="13" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F13" s="56" t="s">
+      <c r="F13" s="88" t="s">
         <v>57</v>
       </c>
-      <c r="G13" s="57"/>
-      <c r="H13" s="57"/>
-      <c r="I13" s="57"/>
-      <c r="J13" s="57"/>
-      <c r="K13" s="57"/>
-      <c r="L13" s="57"/>
-      <c r="M13" s="57"/>
-      <c r="N13" s="57"/>
-      <c r="O13" s="57"/>
-      <c r="P13" s="57"/>
-      <c r="Q13" s="57"/>
-      <c r="R13" s="57"/>
-      <c r="S13" s="57"/>
-      <c r="T13" s="57"/>
-      <c r="U13" s="58"/>
+      <c r="G13" s="89"/>
+      <c r="H13" s="89"/>
+      <c r="I13" s="89"/>
+      <c r="J13" s="89"/>
+      <c r="K13" s="89"/>
+      <c r="L13" s="89"/>
+      <c r="M13" s="89"/>
+      <c r="N13" s="89"/>
+      <c r="O13" s="89"/>
+      <c r="P13" s="89"/>
+      <c r="Q13" s="89"/>
+      <c r="R13" s="89"/>
+      <c r="S13" s="89"/>
+      <c r="T13" s="89"/>
+      <c r="U13" s="90"/>
     </row>
     <row r="14" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F14" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="G14" s="54" t="s">
+      <c r="G14" s="99" t="s">
         <v>43</v>
       </c>
-      <c r="H14" s="54"/>
-      <c r="I14" s="54"/>
-      <c r="J14" s="54"/>
-      <c r="K14" s="54"/>
-      <c r="L14" s="54"/>
-      <c r="M14" s="54"/>
-      <c r="N14" s="54"/>
-      <c r="O14" s="54"/>
-      <c r="P14" s="54"/>
-      <c r="Q14" s="54"/>
-      <c r="R14" s="54"/>
-      <c r="S14" s="54"/>
-      <c r="T14" s="54"/>
-      <c r="U14" s="55"/>
+      <c r="H14" s="99"/>
+      <c r="I14" s="99"/>
+      <c r="J14" s="99"/>
+      <c r="K14" s="99"/>
+      <c r="L14" s="99"/>
+      <c r="M14" s="99"/>
+      <c r="N14" s="99"/>
+      <c r="O14" s="99"/>
+      <c r="P14" s="99"/>
+      <c r="Q14" s="99"/>
+      <c r="R14" s="99"/>
+      <c r="S14" s="99"/>
+      <c r="T14" s="99"/>
+      <c r="U14" s="100"/>
     </row>
     <row r="15" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F15" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="G15" s="54" t="s">
+      <c r="G15" s="99" t="s">
         <v>48</v>
       </c>
-      <c r="H15" s="54"/>
-      <c r="I15" s="54"/>
-      <c r="J15" s="54"/>
-      <c r="K15" s="54"/>
-      <c r="L15" s="54"/>
-      <c r="M15" s="54"/>
-      <c r="N15" s="54"/>
-      <c r="O15" s="54"/>
-      <c r="P15" s="54"/>
-      <c r="Q15" s="54"/>
-      <c r="R15" s="54"/>
-      <c r="S15" s="54"/>
-      <c r="T15" s="54"/>
-      <c r="U15" s="55"/>
+      <c r="H15" s="99"/>
+      <c r="I15" s="99"/>
+      <c r="J15" s="99"/>
+      <c r="K15" s="99"/>
+      <c r="L15" s="99"/>
+      <c r="M15" s="99"/>
+      <c r="N15" s="99"/>
+      <c r="O15" s="99"/>
+      <c r="P15" s="99"/>
+      <c r="Q15" s="99"/>
+      <c r="R15" s="99"/>
+      <c r="S15" s="99"/>
+      <c r="T15" s="99"/>
+      <c r="U15" s="100"/>
     </row>
     <row r="16" spans="6:21" x14ac:dyDescent="0.2">
       <c r="F16" s="35"/>
@@ -2302,46 +2322,46 @@
       <c r="U16" s="36"/>
     </row>
     <row r="17" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F17" s="61" t="s">
+      <c r="F17" s="82" t="s">
         <v>15</v>
       </c>
-      <c r="G17" s="62"/>
-      <c r="H17" s="62"/>
-      <c r="I17" s="62"/>
-      <c r="J17" s="62"/>
-      <c r="K17" s="62"/>
-      <c r="L17" s="62"/>
-      <c r="M17" s="62"/>
-      <c r="N17" s="62"/>
-      <c r="O17" s="62"/>
-      <c r="P17" s="62"/>
-      <c r="Q17" s="62"/>
-      <c r="R17" s="62"/>
-      <c r="S17" s="62"/>
-      <c r="T17" s="62"/>
-      <c r="U17" s="63"/>
+      <c r="G17" s="83"/>
+      <c r="H17" s="83"/>
+      <c r="I17" s="83"/>
+      <c r="J17" s="83"/>
+      <c r="K17" s="83"/>
+      <c r="L17" s="83"/>
+      <c r="M17" s="83"/>
+      <c r="N17" s="83"/>
+      <c r="O17" s="83"/>
+      <c r="P17" s="83"/>
+      <c r="Q17" s="83"/>
+      <c r="R17" s="83"/>
+      <c r="S17" s="83"/>
+      <c r="T17" s="83"/>
+      <c r="U17" s="84"/>
     </row>
     <row r="18" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F18" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="G18" s="54" t="s">
+      <c r="G18" s="99" t="s">
         <v>47</v>
       </c>
-      <c r="H18" s="54"/>
-      <c r="I18" s="54"/>
-      <c r="J18" s="54"/>
-      <c r="K18" s="54"/>
-      <c r="L18" s="54"/>
-      <c r="M18" s="54"/>
-      <c r="N18" s="54"/>
-      <c r="O18" s="54"/>
-      <c r="P18" s="54"/>
-      <c r="Q18" s="54"/>
-      <c r="R18" s="54"/>
-      <c r="S18" s="54"/>
-      <c r="T18" s="54"/>
-      <c r="U18" s="55"/>
+      <c r="H18" s="99"/>
+      <c r="I18" s="99"/>
+      <c r="J18" s="99"/>
+      <c r="K18" s="99"/>
+      <c r="L18" s="99"/>
+      <c r="M18" s="99"/>
+      <c r="N18" s="99"/>
+      <c r="O18" s="99"/>
+      <c r="P18" s="99"/>
+      <c r="Q18" s="99"/>
+      <c r="R18" s="99"/>
+      <c r="S18" s="99"/>
+      <c r="T18" s="99"/>
+      <c r="U18" s="100"/>
     </row>
     <row r="19" spans="6:21" x14ac:dyDescent="0.2">
       <c r="F19" s="35"/>
@@ -2362,46 +2382,46 @@
       <c r="U19" s="36"/>
     </row>
     <row r="20" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F20" s="61" t="s">
+      <c r="F20" s="82" t="s">
         <v>44</v>
       </c>
-      <c r="G20" s="62"/>
-      <c r="H20" s="62"/>
-      <c r="I20" s="62"/>
-      <c r="J20" s="62"/>
-      <c r="K20" s="62"/>
-      <c r="L20" s="62"/>
-      <c r="M20" s="62"/>
-      <c r="N20" s="62"/>
-      <c r="O20" s="62"/>
-      <c r="P20" s="62"/>
-      <c r="Q20" s="62"/>
-      <c r="R20" s="62"/>
-      <c r="S20" s="62"/>
-      <c r="T20" s="62"/>
-      <c r="U20" s="63"/>
+      <c r="G20" s="83"/>
+      <c r="H20" s="83"/>
+      <c r="I20" s="83"/>
+      <c r="J20" s="83"/>
+      <c r="K20" s="83"/>
+      <c r="L20" s="83"/>
+      <c r="M20" s="83"/>
+      <c r="N20" s="83"/>
+      <c r="O20" s="83"/>
+      <c r="P20" s="83"/>
+      <c r="Q20" s="83"/>
+      <c r="R20" s="83"/>
+      <c r="S20" s="83"/>
+      <c r="T20" s="83"/>
+      <c r="U20" s="84"/>
     </row>
     <row r="21" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F21" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="G21" s="54" t="s">
+      <c r="G21" s="99" t="s">
         <v>58</v>
       </c>
-      <c r="H21" s="54"/>
-      <c r="I21" s="54"/>
-      <c r="J21" s="54"/>
-      <c r="K21" s="54"/>
-      <c r="L21" s="54"/>
-      <c r="M21" s="54"/>
-      <c r="N21" s="54"/>
-      <c r="O21" s="54"/>
-      <c r="P21" s="54"/>
-      <c r="Q21" s="54"/>
-      <c r="R21" s="54"/>
-      <c r="S21" s="54"/>
-      <c r="T21" s="54"/>
-      <c r="U21" s="55"/>
+      <c r="H21" s="99"/>
+      <c r="I21" s="99"/>
+      <c r="J21" s="99"/>
+      <c r="K21" s="99"/>
+      <c r="L21" s="99"/>
+      <c r="M21" s="99"/>
+      <c r="N21" s="99"/>
+      <c r="O21" s="99"/>
+      <c r="P21" s="99"/>
+      <c r="Q21" s="99"/>
+      <c r="R21" s="99"/>
+      <c r="S21" s="99"/>
+      <c r="T21" s="99"/>
+      <c r="U21" s="100"/>
     </row>
     <row r="22" spans="6:21" x14ac:dyDescent="0.2">
       <c r="F22" s="35"/>
@@ -2422,46 +2442,46 @@
       <c r="U22" s="36"/>
     </row>
     <row r="23" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F23" s="61" t="s">
+      <c r="F23" s="82" t="s">
         <v>45</v>
       </c>
-      <c r="G23" s="62"/>
-      <c r="H23" s="62"/>
-      <c r="I23" s="62"/>
-      <c r="J23" s="62"/>
-      <c r="K23" s="62"/>
-      <c r="L23" s="62"/>
-      <c r="M23" s="62"/>
-      <c r="N23" s="62"/>
-      <c r="O23" s="62"/>
-      <c r="P23" s="62"/>
-      <c r="Q23" s="62"/>
-      <c r="R23" s="62"/>
-      <c r="S23" s="62"/>
-      <c r="T23" s="62"/>
-      <c r="U23" s="63"/>
+      <c r="G23" s="83"/>
+      <c r="H23" s="83"/>
+      <c r="I23" s="83"/>
+      <c r="J23" s="83"/>
+      <c r="K23" s="83"/>
+      <c r="L23" s="83"/>
+      <c r="M23" s="83"/>
+      <c r="N23" s="83"/>
+      <c r="O23" s="83"/>
+      <c r="P23" s="83"/>
+      <c r="Q23" s="83"/>
+      <c r="R23" s="83"/>
+      <c r="S23" s="83"/>
+      <c r="T23" s="83"/>
+      <c r="U23" s="84"/>
     </row>
     <row r="24" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F24" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="G24" s="64" t="s">
+      <c r="G24" s="79" t="s">
         <v>46</v>
       </c>
-      <c r="H24" s="64"/>
-      <c r="I24" s="64"/>
-      <c r="J24" s="64"/>
-      <c r="K24" s="64"/>
-      <c r="L24" s="64"/>
-      <c r="M24" s="64"/>
-      <c r="N24" s="64"/>
-      <c r="O24" s="64"/>
-      <c r="P24" s="64"/>
-      <c r="Q24" s="64"/>
-      <c r="R24" s="64"/>
-      <c r="S24" s="64"/>
-      <c r="T24" s="64"/>
-      <c r="U24" s="65"/>
+      <c r="H24" s="79"/>
+      <c r="I24" s="79"/>
+      <c r="J24" s="79"/>
+      <c r="K24" s="79"/>
+      <c r="L24" s="79"/>
+      <c r="M24" s="79"/>
+      <c r="N24" s="79"/>
+      <c r="O24" s="79"/>
+      <c r="P24" s="79"/>
+      <c r="Q24" s="79"/>
+      <c r="R24" s="79"/>
+      <c r="S24" s="79"/>
+      <c r="T24" s="79"/>
+      <c r="U24" s="80"/>
     </row>
     <row r="25" spans="6:21" x14ac:dyDescent="0.2">
       <c r="F25" s="32"/>
@@ -2518,174 +2538,174 @@
       <c r="U27" s="32"/>
     </row>
     <row r="28" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F28" s="67" t="s">
+      <c r="F28" s="85" t="s">
         <v>16</v>
       </c>
-      <c r="G28" s="68"/>
-      <c r="H28" s="68"/>
-      <c r="I28" s="68"/>
-      <c r="J28" s="68"/>
-      <c r="K28" s="68"/>
-      <c r="L28" s="68"/>
-      <c r="M28" s="68"/>
-      <c r="N28" s="68"/>
-      <c r="O28" s="68"/>
-      <c r="P28" s="68"/>
-      <c r="Q28" s="68"/>
-      <c r="R28" s="68"/>
-      <c r="S28" s="68"/>
-      <c r="T28" s="68"/>
-      <c r="U28" s="69"/>
+      <c r="G28" s="86"/>
+      <c r="H28" s="86"/>
+      <c r="I28" s="86"/>
+      <c r="J28" s="86"/>
+      <c r="K28" s="86"/>
+      <c r="L28" s="86"/>
+      <c r="M28" s="86"/>
+      <c r="N28" s="86"/>
+      <c r="O28" s="86"/>
+      <c r="P28" s="86"/>
+      <c r="Q28" s="86"/>
+      <c r="R28" s="86"/>
+      <c r="S28" s="86"/>
+      <c r="T28" s="86"/>
+      <c r="U28" s="87"/>
     </row>
     <row r="29" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F29" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="G29" s="46" t="s">
+      <c r="G29" s="75" t="s">
         <v>25</v>
       </c>
-      <c r="H29" s="46"/>
-      <c r="I29" s="46"/>
-      <c r="J29" s="46"/>
-      <c r="K29" s="46"/>
-      <c r="L29" s="46"/>
-      <c r="M29" s="46"/>
-      <c r="N29" s="46"/>
-      <c r="O29" s="46"/>
-      <c r="P29" s="46"/>
-      <c r="Q29" s="46"/>
-      <c r="R29" s="46"/>
-      <c r="S29" s="46"/>
-      <c r="T29" s="46"/>
-      <c r="U29" s="47"/>
+      <c r="H29" s="75"/>
+      <c r="I29" s="75"/>
+      <c r="J29" s="75"/>
+      <c r="K29" s="75"/>
+      <c r="L29" s="75"/>
+      <c r="M29" s="75"/>
+      <c r="N29" s="75"/>
+      <c r="O29" s="75"/>
+      <c r="P29" s="75"/>
+      <c r="Q29" s="75"/>
+      <c r="R29" s="75"/>
+      <c r="S29" s="75"/>
+      <c r="T29" s="75"/>
+      <c r="U29" s="76"/>
     </row>
     <row r="30" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F30" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="G30" s="46" t="s">
+      <c r="G30" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="H30" s="46"/>
-      <c r="I30" s="46"/>
-      <c r="J30" s="46"/>
-      <c r="K30" s="46"/>
-      <c r="L30" s="46"/>
-      <c r="M30" s="46"/>
-      <c r="N30" s="46"/>
-      <c r="O30" s="46"/>
-      <c r="P30" s="46"/>
-      <c r="Q30" s="46"/>
-      <c r="R30" s="46"/>
-      <c r="S30" s="46"/>
-      <c r="T30" s="46"/>
-      <c r="U30" s="47"/>
+      <c r="H30" s="75"/>
+      <c r="I30" s="75"/>
+      <c r="J30" s="75"/>
+      <c r="K30" s="75"/>
+      <c r="L30" s="75"/>
+      <c r="M30" s="75"/>
+      <c r="N30" s="75"/>
+      <c r="O30" s="75"/>
+      <c r="P30" s="75"/>
+      <c r="Q30" s="75"/>
+      <c r="R30" s="75"/>
+      <c r="S30" s="75"/>
+      <c r="T30" s="75"/>
+      <c r="U30" s="76"/>
     </row>
     <row r="31" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F31" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="G31" s="46" t="s">
+      <c r="G31" s="75" t="s">
         <v>26</v>
       </c>
-      <c r="H31" s="46"/>
-      <c r="I31" s="46"/>
-      <c r="J31" s="46"/>
-      <c r="K31" s="46"/>
-      <c r="L31" s="46"/>
-      <c r="M31" s="46"/>
-      <c r="N31" s="46"/>
-      <c r="O31" s="46"/>
-      <c r="P31" s="46"/>
-      <c r="Q31" s="46"/>
-      <c r="R31" s="46"/>
-      <c r="S31" s="46"/>
-      <c r="T31" s="46"/>
-      <c r="U31" s="47"/>
+      <c r="H31" s="75"/>
+      <c r="I31" s="75"/>
+      <c r="J31" s="75"/>
+      <c r="K31" s="75"/>
+      <c r="L31" s="75"/>
+      <c r="M31" s="75"/>
+      <c r="N31" s="75"/>
+      <c r="O31" s="75"/>
+      <c r="P31" s="75"/>
+      <c r="Q31" s="75"/>
+      <c r="R31" s="75"/>
+      <c r="S31" s="75"/>
+      <c r="T31" s="75"/>
+      <c r="U31" s="76"/>
     </row>
     <row r="32" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F32" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="G32" s="46" t="s">
+      <c r="G32" s="75" t="s">
         <v>28</v>
       </c>
-      <c r="H32" s="46"/>
-      <c r="I32" s="46"/>
-      <c r="J32" s="46"/>
-      <c r="K32" s="46"/>
-      <c r="L32" s="46"/>
-      <c r="M32" s="46"/>
-      <c r="N32" s="46"/>
-      <c r="O32" s="46"/>
-      <c r="P32" s="46"/>
-      <c r="Q32" s="46"/>
-      <c r="R32" s="46"/>
-      <c r="S32" s="46"/>
-      <c r="T32" s="46"/>
-      <c r="U32" s="47"/>
+      <c r="H32" s="75"/>
+      <c r="I32" s="75"/>
+      <c r="J32" s="75"/>
+      <c r="K32" s="75"/>
+      <c r="L32" s="75"/>
+      <c r="M32" s="75"/>
+      <c r="N32" s="75"/>
+      <c r="O32" s="75"/>
+      <c r="P32" s="75"/>
+      <c r="Q32" s="75"/>
+      <c r="R32" s="75"/>
+      <c r="S32" s="75"/>
+      <c r="T32" s="75"/>
+      <c r="U32" s="76"/>
     </row>
     <row r="33" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F33" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="G33" s="46" t="s">
+      <c r="G33" s="75" t="s">
         <v>27</v>
       </c>
-      <c r="H33" s="46"/>
-      <c r="I33" s="46"/>
-      <c r="J33" s="46"/>
-      <c r="K33" s="46"/>
-      <c r="L33" s="46"/>
-      <c r="M33" s="46"/>
-      <c r="N33" s="46"/>
-      <c r="O33" s="46"/>
-      <c r="P33" s="46"/>
-      <c r="Q33" s="46"/>
-      <c r="R33" s="46"/>
-      <c r="S33" s="46"/>
-      <c r="T33" s="46"/>
-      <c r="U33" s="47"/>
+      <c r="H33" s="75"/>
+      <c r="I33" s="75"/>
+      <c r="J33" s="75"/>
+      <c r="K33" s="75"/>
+      <c r="L33" s="75"/>
+      <c r="M33" s="75"/>
+      <c r="N33" s="75"/>
+      <c r="O33" s="75"/>
+      <c r="P33" s="75"/>
+      <c r="Q33" s="75"/>
+      <c r="R33" s="75"/>
+      <c r="S33" s="75"/>
+      <c r="T33" s="75"/>
+      <c r="U33" s="76"/>
     </row>
     <row r="34" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F34" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="G34" s="70" t="s">
+      <c r="G34" s="77" t="s">
         <v>30</v>
       </c>
-      <c r="H34" s="70"/>
-      <c r="I34" s="70"/>
-      <c r="J34" s="70"/>
-      <c r="K34" s="70"/>
-      <c r="L34" s="70"/>
-      <c r="M34" s="70"/>
-      <c r="N34" s="70"/>
-      <c r="O34" s="70"/>
-      <c r="P34" s="70"/>
-      <c r="Q34" s="70"/>
-      <c r="R34" s="70"/>
-      <c r="S34" s="70"/>
-      <c r="T34" s="70"/>
-      <c r="U34" s="71"/>
+      <c r="H34" s="77"/>
+      <c r="I34" s="77"/>
+      <c r="J34" s="77"/>
+      <c r="K34" s="77"/>
+      <c r="L34" s="77"/>
+      <c r="M34" s="77"/>
+      <c r="N34" s="77"/>
+      <c r="O34" s="77"/>
+      <c r="P34" s="77"/>
+      <c r="Q34" s="77"/>
+      <c r="R34" s="77"/>
+      <c r="S34" s="77"/>
+      <c r="T34" s="77"/>
+      <c r="U34" s="78"/>
     </row>
     <row r="35" spans="6:21" x14ac:dyDescent="0.2">
       <c r="F35" s="32"/>
-      <c r="G35" s="66"/>
-      <c r="H35" s="66"/>
-      <c r="I35" s="66"/>
-      <c r="J35" s="66"/>
-      <c r="K35" s="66"/>
-      <c r="L35" s="66"/>
-      <c r="M35" s="66"/>
-      <c r="N35" s="66"/>
-      <c r="O35" s="66"/>
-      <c r="P35" s="66"/>
-      <c r="Q35" s="66"/>
-      <c r="R35" s="66"/>
-      <c r="S35" s="66"/>
-      <c r="T35" s="66"/>
-      <c r="U35" s="66"/>
+      <c r="G35" s="81"/>
+      <c r="H35" s="81"/>
+      <c r="I35" s="81"/>
+      <c r="J35" s="81"/>
+      <c r="K35" s="81"/>
+      <c r="L35" s="81"/>
+      <c r="M35" s="81"/>
+      <c r="N35" s="81"/>
+      <c r="O35" s="81"/>
+      <c r="P35" s="81"/>
+      <c r="Q35" s="81"/>
+      <c r="R35" s="81"/>
+      <c r="S35" s="81"/>
+      <c r="T35" s="81"/>
+      <c r="U35" s="81"/>
     </row>
     <row r="37" spans="6:21" x14ac:dyDescent="0.2">
       <c r="F37" s="32"/>
@@ -2706,68 +2726,68 @@
       <c r="U37" s="32"/>
     </row>
     <row r="38" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F38" s="56" t="s">
+      <c r="F38" s="88" t="s">
         <v>20</v>
       </c>
-      <c r="G38" s="57"/>
-      <c r="H38" s="57"/>
-      <c r="I38" s="57"/>
-      <c r="J38" s="57"/>
-      <c r="K38" s="57"/>
-      <c r="L38" s="57"/>
-      <c r="M38" s="57"/>
-      <c r="N38" s="57"/>
-      <c r="O38" s="57"/>
-      <c r="P38" s="57"/>
-      <c r="Q38" s="57"/>
-      <c r="R38" s="57"/>
-      <c r="S38" s="57"/>
-      <c r="T38" s="57"/>
-      <c r="U38" s="58"/>
+      <c r="G38" s="89"/>
+      <c r="H38" s="89"/>
+      <c r="I38" s="89"/>
+      <c r="J38" s="89"/>
+      <c r="K38" s="89"/>
+      <c r="L38" s="89"/>
+      <c r="M38" s="89"/>
+      <c r="N38" s="89"/>
+      <c r="O38" s="89"/>
+      <c r="P38" s="89"/>
+      <c r="Q38" s="89"/>
+      <c r="R38" s="89"/>
+      <c r="S38" s="89"/>
+      <c r="T38" s="89"/>
+      <c r="U38" s="90"/>
     </row>
     <row r="39" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F39" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="G39" s="59" t="s">
+      <c r="G39" s="73" t="s">
         <v>40</v>
       </c>
-      <c r="H39" s="59"/>
-      <c r="I39" s="59"/>
-      <c r="J39" s="59"/>
-      <c r="K39" s="59"/>
-      <c r="L39" s="59"/>
-      <c r="M39" s="59"/>
-      <c r="N39" s="59"/>
-      <c r="O39" s="59"/>
-      <c r="P39" s="59"/>
-      <c r="Q39" s="59"/>
-      <c r="R39" s="59"/>
-      <c r="S39" s="59"/>
-      <c r="T39" s="59"/>
-      <c r="U39" s="60"/>
+      <c r="H39" s="73"/>
+      <c r="I39" s="73"/>
+      <c r="J39" s="73"/>
+      <c r="K39" s="73"/>
+      <c r="L39" s="73"/>
+      <c r="M39" s="73"/>
+      <c r="N39" s="73"/>
+      <c r="O39" s="73"/>
+      <c r="P39" s="73"/>
+      <c r="Q39" s="73"/>
+      <c r="R39" s="73"/>
+      <c r="S39" s="73"/>
+      <c r="T39" s="73"/>
+      <c r="U39" s="74"/>
     </row>
     <row r="40" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F40" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="G40" s="59" t="s">
+      <c r="G40" s="73" t="s">
         <v>31</v>
       </c>
-      <c r="H40" s="59"/>
-      <c r="I40" s="59"/>
-      <c r="J40" s="59"/>
-      <c r="K40" s="59"/>
-      <c r="L40" s="59"/>
-      <c r="M40" s="59"/>
-      <c r="N40" s="59"/>
-      <c r="O40" s="59"/>
-      <c r="P40" s="59"/>
-      <c r="Q40" s="59"/>
-      <c r="R40" s="59"/>
-      <c r="S40" s="59"/>
-      <c r="T40" s="59"/>
-      <c r="U40" s="60"/>
+      <c r="H40" s="73"/>
+      <c r="I40" s="73"/>
+      <c r="J40" s="73"/>
+      <c r="K40" s="73"/>
+      <c r="L40" s="73"/>
+      <c r="M40" s="73"/>
+      <c r="N40" s="73"/>
+      <c r="O40" s="73"/>
+      <c r="P40" s="73"/>
+      <c r="Q40" s="73"/>
+      <c r="R40" s="73"/>
+      <c r="S40" s="73"/>
+      <c r="T40" s="73"/>
+      <c r="U40" s="74"/>
     </row>
     <row r="41" spans="6:21" x14ac:dyDescent="0.2">
       <c r="F41" s="40"/>
@@ -2791,216 +2811,189 @@
       <c r="F42" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="G42" s="59" t="s">
+      <c r="G42" s="73" t="s">
         <v>29</v>
       </c>
-      <c r="H42" s="59"/>
-      <c r="I42" s="59"/>
-      <c r="J42" s="59"/>
-      <c r="K42" s="59"/>
-      <c r="L42" s="59"/>
-      <c r="M42" s="59"/>
-      <c r="N42" s="59"/>
-      <c r="O42" s="59"/>
-      <c r="P42" s="59"/>
-      <c r="Q42" s="59"/>
-      <c r="R42" s="59"/>
-      <c r="S42" s="59"/>
-      <c r="T42" s="59"/>
-      <c r="U42" s="60"/>
+      <c r="H42" s="73"/>
+      <c r="I42" s="73"/>
+      <c r="J42" s="73"/>
+      <c r="K42" s="73"/>
+      <c r="L42" s="73"/>
+      <c r="M42" s="73"/>
+      <c r="N42" s="73"/>
+      <c r="O42" s="73"/>
+      <c r="P42" s="73"/>
+      <c r="Q42" s="73"/>
+      <c r="R42" s="73"/>
+      <c r="S42" s="73"/>
+      <c r="T42" s="73"/>
+      <c r="U42" s="74"/>
     </row>
     <row r="43" spans="6:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F43" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="G43" s="44" t="s">
+      <c r="G43" s="91" t="s">
         <v>42</v>
       </c>
-      <c r="H43" s="44"/>
-      <c r="I43" s="44"/>
-      <c r="J43" s="44"/>
-      <c r="K43" s="44"/>
-      <c r="L43" s="44"/>
-      <c r="M43" s="44"/>
-      <c r="N43" s="44"/>
-      <c r="O43" s="44"/>
-      <c r="P43" s="44"/>
-      <c r="Q43" s="44"/>
-      <c r="R43" s="44"/>
-      <c r="S43" s="44"/>
-      <c r="T43" s="44"/>
-      <c r="U43" s="45"/>
+      <c r="H43" s="91"/>
+      <c r="I43" s="91"/>
+      <c r="J43" s="91"/>
+      <c r="K43" s="91"/>
+      <c r="L43" s="91"/>
+      <c r="M43" s="91"/>
+      <c r="N43" s="91"/>
+      <c r="O43" s="91"/>
+      <c r="P43" s="91"/>
+      <c r="Q43" s="91"/>
+      <c r="R43" s="91"/>
+      <c r="S43" s="91"/>
+      <c r="T43" s="91"/>
+      <c r="U43" s="92"/>
     </row>
     <row r="49" spans="5:25" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="M49" s="93" t="s">
+      <c r="M49" s="66" t="s">
         <v>49</v>
       </c>
-      <c r="N49" s="93"/>
-      <c r="O49" s="93"/>
+      <c r="N49" s="66"/>
+      <c r="O49" s="66"/>
     </row>
     <row r="51" spans="5:25" x14ac:dyDescent="0.2">
-      <c r="G51" s="84" t="s">
+      <c r="G51" s="57" t="s">
         <v>50</v>
       </c>
-      <c r="H51" s="85"/>
-      <c r="I51" s="86"/>
-      <c r="K51" s="84" t="s">
+      <c r="H51" s="58"/>
+      <c r="I51" s="59"/>
+      <c r="K51" s="57" t="s">
         <v>51</v>
       </c>
-      <c r="L51" s="85"/>
-      <c r="M51" s="86"/>
-      <c r="O51" s="84" t="s">
+      <c r="L51" s="58"/>
+      <c r="M51" s="59"/>
+      <c r="O51" s="57" t="s">
         <v>52</v>
       </c>
-      <c r="P51" s="85"/>
-      <c r="Q51" s="86"/>
-      <c r="S51" s="84" t="s">
+      <c r="P51" s="58"/>
+      <c r="Q51" s="59"/>
+      <c r="S51" s="57" t="s">
         <v>53</v>
       </c>
-      <c r="T51" s="85"/>
-      <c r="U51" s="86"/>
+      <c r="T51" s="58"/>
+      <c r="U51" s="59"/>
     </row>
     <row r="52" spans="5:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G52" s="87"/>
-      <c r="H52" s="88"/>
-      <c r="I52" s="89"/>
-      <c r="K52" s="87"/>
-      <c r="L52" s="88"/>
-      <c r="M52" s="89"/>
-      <c r="O52" s="87"/>
-      <c r="P52" s="88"/>
-      <c r="Q52" s="89"/>
-      <c r="S52" s="87"/>
-      <c r="T52" s="88"/>
-      <c r="U52" s="89"/>
+      <c r="G52" s="60"/>
+      <c r="H52" s="61"/>
+      <c r="I52" s="62"/>
+      <c r="K52" s="60"/>
+      <c r="L52" s="61"/>
+      <c r="M52" s="62"/>
+      <c r="O52" s="60"/>
+      <c r="P52" s="61"/>
+      <c r="Q52" s="62"/>
+      <c r="S52" s="60"/>
+      <c r="T52" s="61"/>
+      <c r="U52" s="62"/>
     </row>
     <row r="53" spans="5:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G53" s="90"/>
-      <c r="H53" s="91"/>
-      <c r="I53" s="92"/>
-      <c r="K53" s="90"/>
-      <c r="L53" s="91"/>
-      <c r="M53" s="92"/>
-      <c r="O53" s="90"/>
-      <c r="P53" s="91"/>
-      <c r="Q53" s="92"/>
-      <c r="S53" s="90"/>
-      <c r="T53" s="91"/>
-      <c r="U53" s="92"/>
+      <c r="G53" s="63"/>
+      <c r="H53" s="64"/>
+      <c r="I53" s="65"/>
+      <c r="K53" s="63"/>
+      <c r="L53" s="64"/>
+      <c r="M53" s="65"/>
+      <c r="O53" s="63"/>
+      <c r="P53" s="64"/>
+      <c r="Q53" s="65"/>
+      <c r="S53" s="63"/>
+      <c r="T53" s="64"/>
+      <c r="U53" s="65"/>
     </row>
     <row r="62" spans="5:25" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E62" s="93" t="s">
+      <c r="E62" s="66" t="s">
         <v>60</v>
       </c>
-      <c r="F62" s="93"/>
-      <c r="G62" s="93"/>
-      <c r="H62" s="93"/>
-      <c r="P62" s="93" t="s">
+      <c r="F62" s="66"/>
+      <c r="G62" s="66"/>
+      <c r="H62" s="66"/>
+      <c r="P62" s="66" t="s">
         <v>61</v>
       </c>
-      <c r="Q62" s="93"/>
-      <c r="R62" s="93"/>
-      <c r="S62" s="93"/>
-      <c r="V62" s="93" t="s">
+      <c r="Q62" s="66"/>
+      <c r="R62" s="66"/>
+      <c r="S62" s="66"/>
+      <c r="V62" s="66" t="s">
         <v>62</v>
       </c>
-      <c r="W62" s="93"/>
-      <c r="X62" s="93"/>
-      <c r="Y62" s="93"/>
+      <c r="W62" s="66"/>
+      <c r="X62" s="66"/>
+      <c r="Y62" s="66"/>
     </row>
     <row r="63" spans="5:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="66" spans="3:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C66" s="94" t="s">
+      <c r="C66" s="67" t="s">
         <v>56</v>
       </c>
-      <c r="D66" s="95"/>
-      <c r="F66" s="94" t="s">
+      <c r="D66" s="68"/>
+      <c r="F66" s="67" t="s">
         <v>56</v>
       </c>
-      <c r="G66" s="95"/>
-      <c r="I66" s="94" t="s">
+      <c r="G66" s="68"/>
+      <c r="I66" s="67" t="s">
         <v>56</v>
       </c>
-      <c r="J66" s="95"/>
-      <c r="N66" s="72" t="s">
+      <c r="J66" s="68"/>
+      <c r="N66" s="45" t="s">
         <v>56</v>
       </c>
-      <c r="O66" s="73"/>
-      <c r="Q66" s="72" t="s">
+      <c r="O66" s="46"/>
+      <c r="Q66" s="45" t="s">
         <v>56</v>
       </c>
-      <c r="R66" s="73"/>
-      <c r="T66" s="72" t="s">
+      <c r="R66" s="46"/>
+      <c r="T66" s="45" t="s">
         <v>55</v>
       </c>
-      <c r="U66" s="73"/>
-      <c r="W66" s="78" t="s">
+      <c r="U66" s="46"/>
+      <c r="W66" s="51" t="s">
         <v>54</v>
       </c>
-      <c r="X66" s="79"/>
+      <c r="X66" s="52"/>
     </row>
     <row r="67" spans="3:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C67" s="96"/>
-      <c r="D67" s="97"/>
-      <c r="F67" s="96"/>
-      <c r="G67" s="97"/>
-      <c r="I67" s="96"/>
-      <c r="J67" s="97"/>
-      <c r="N67" s="74"/>
-      <c r="O67" s="75"/>
-      <c r="Q67" s="74"/>
-      <c r="R67" s="75"/>
-      <c r="T67" s="74"/>
-      <c r="U67" s="75"/>
-      <c r="W67" s="80"/>
-      <c r="X67" s="81"/>
+      <c r="C67" s="69"/>
+      <c r="D67" s="70"/>
+      <c r="F67" s="69"/>
+      <c r="G67" s="70"/>
+      <c r="I67" s="69"/>
+      <c r="J67" s="70"/>
+      <c r="N67" s="47"/>
+      <c r="O67" s="48"/>
+      <c r="Q67" s="47"/>
+      <c r="R67" s="48"/>
+      <c r="T67" s="47"/>
+      <c r="U67" s="48"/>
+      <c r="W67" s="53"/>
+      <c r="X67" s="54"/>
     </row>
     <row r="68" spans="3:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C68" s="98"/>
-      <c r="D68" s="99"/>
-      <c r="F68" s="98"/>
-      <c r="G68" s="99"/>
-      <c r="I68" s="98"/>
-      <c r="J68" s="99"/>
-      <c r="N68" s="76"/>
-      <c r="O68" s="77"/>
-      <c r="Q68" s="76"/>
-      <c r="R68" s="77"/>
-      <c r="T68" s="76"/>
-      <c r="U68" s="77"/>
-      <c r="W68" s="82"/>
-      <c r="X68" s="83"/>
+      <c r="C68" s="71"/>
+      <c r="D68" s="72"/>
+      <c r="F68" s="71"/>
+      <c r="G68" s="72"/>
+      <c r="I68" s="71"/>
+      <c r="J68" s="72"/>
+      <c r="N68" s="49"/>
+      <c r="O68" s="50"/>
+      <c r="Q68" s="49"/>
+      <c r="R68" s="50"/>
+      <c r="T68" s="49"/>
+      <c r="U68" s="50"/>
+      <c r="W68" s="55"/>
+      <c r="X68" s="56"/>
     </row>
     <row r="69" spans="3:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="43">
-    <mergeCell ref="T66:U68"/>
-    <mergeCell ref="W66:X68"/>
-    <mergeCell ref="S51:U53"/>
-    <mergeCell ref="M49:O49"/>
-    <mergeCell ref="C66:D68"/>
-    <mergeCell ref="F66:G68"/>
-    <mergeCell ref="I66:J68"/>
-    <mergeCell ref="N66:O68"/>
-    <mergeCell ref="Q66:R68"/>
-    <mergeCell ref="G51:I53"/>
-    <mergeCell ref="K51:M53"/>
-    <mergeCell ref="O51:Q53"/>
-    <mergeCell ref="E62:H62"/>
-    <mergeCell ref="P62:S62"/>
-    <mergeCell ref="V62:Y62"/>
-    <mergeCell ref="G39:U39"/>
-    <mergeCell ref="G40:U40"/>
-    <mergeCell ref="G30:U30"/>
-    <mergeCell ref="G31:U31"/>
-    <mergeCell ref="G32:U32"/>
-    <mergeCell ref="G33:U33"/>
-    <mergeCell ref="G34:U34"/>
-    <mergeCell ref="G24:U24"/>
-    <mergeCell ref="G35:U35"/>
-    <mergeCell ref="F17:U17"/>
-    <mergeCell ref="F28:U28"/>
-    <mergeCell ref="F38:U38"/>
     <mergeCell ref="G43:U43"/>
     <mergeCell ref="G29:U29"/>
     <mergeCell ref="F2:U2"/>
@@ -3017,6 +3010,33 @@
     <mergeCell ref="G15:U15"/>
     <mergeCell ref="G42:U42"/>
     <mergeCell ref="F23:U23"/>
+    <mergeCell ref="G24:U24"/>
+    <mergeCell ref="G35:U35"/>
+    <mergeCell ref="F17:U17"/>
+    <mergeCell ref="F28:U28"/>
+    <mergeCell ref="F38:U38"/>
+    <mergeCell ref="G39:U39"/>
+    <mergeCell ref="G40:U40"/>
+    <mergeCell ref="G30:U30"/>
+    <mergeCell ref="G31:U31"/>
+    <mergeCell ref="G32:U32"/>
+    <mergeCell ref="G33:U33"/>
+    <mergeCell ref="G34:U34"/>
+    <mergeCell ref="T66:U68"/>
+    <mergeCell ref="W66:X68"/>
+    <mergeCell ref="S51:U53"/>
+    <mergeCell ref="M49:O49"/>
+    <mergeCell ref="C66:D68"/>
+    <mergeCell ref="F66:G68"/>
+    <mergeCell ref="I66:J68"/>
+    <mergeCell ref="N66:O68"/>
+    <mergeCell ref="Q66:R68"/>
+    <mergeCell ref="G51:I53"/>
+    <mergeCell ref="K51:M53"/>
+    <mergeCell ref="O51:Q53"/>
+    <mergeCell ref="E62:H62"/>
+    <mergeCell ref="P62:S62"/>
+    <mergeCell ref="V62:Y62"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3048,32 +3068,32 @@
       </c>
     </row>
     <row r="2" spans="5:13" ht="26" x14ac:dyDescent="0.2">
-      <c r="E2" s="102" t="s">
+      <c r="E2" s="103" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="102"/>
-      <c r="G2" s="102"/>
-      <c r="H2" s="102"/>
-      <c r="I2" s="102"/>
-      <c r="J2" s="102"/>
-      <c r="K2" s="102"/>
-      <c r="L2" s="102"/>
-      <c r="M2" s="102"/>
+      <c r="F2" s="103"/>
+      <c r="G2" s="103"/>
+      <c r="H2" s="103"/>
+      <c r="I2" s="103"/>
+      <c r="J2" s="103"/>
+      <c r="K2" s="103"/>
+      <c r="L2" s="103"/>
+      <c r="M2" s="103"/>
     </row>
     <row r="4" spans="5:13" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E4"/>
-      <c r="F4" s="104" t="s">
+      <c r="F4" s="105" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="105"/>
-      <c r="H4" s="106"/>
-      <c r="I4" s="103" t="s">
+      <c r="G4" s="106"/>
+      <c r="H4" s="107"/>
+      <c r="I4" s="104" t="s">
         <v>38</v>
       </c>
-      <c r="J4" s="103"/>
-      <c r="K4" s="103"/>
-      <c r="L4" s="103"/>
-      <c r="M4" s="100" t="s">
+      <c r="J4" s="104"/>
+      <c r="K4" s="104"/>
+      <c r="L4" s="104"/>
+      <c r="M4" s="101" t="s">
         <v>3</v>
       </c>
     </row>
@@ -3088,15 +3108,15 @@
       <c r="H5" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="I5" s="107" t="s">
+      <c r="I5" s="108" t="s">
         <v>4</v>
       </c>
-      <c r="J5" s="108"/>
-      <c r="K5" s="103" t="s">
+      <c r="J5" s="109"/>
+      <c r="K5" s="104" t="s">
         <v>1</v>
       </c>
-      <c r="L5" s="103"/>
-      <c r="M5" s="101"/>
+      <c r="L5" s="104"/>
+      <c r="M5" s="102"/>
     </row>
     <row r="6" spans="5:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E6"/>
@@ -3260,14 +3280,14 @@
   </cols>
   <sheetData>
     <row r="3" spans="4:9" s="13" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D3" s="109" t="s">
+      <c r="D3" s="110" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="109"/>
-      <c r="F3" s="109"/>
-      <c r="G3" s="109"/>
-      <c r="H3" s="109"/>
-      <c r="I3" s="109"/>
+      <c r="E3" s="110"/>
+      <c r="F3" s="110"/>
+      <c r="G3" s="110"/>
+      <c r="H3" s="110"/>
+      <c r="I3" s="110"/>
     </row>
     <row r="5" spans="4:9" s="8" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D5" s="27" t="s">
@@ -3604,11 +3624,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="B1:V21"/>
+  <dimension ref="B1:X21"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="C1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomLeft" activeCell="W3" sqref="W3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3623,74 +3643,80 @@
     <col min="12" max="13" width="10.5" bestFit="1" customWidth="1"/>
     <col min="17" max="18" width="10.5" bestFit="1" customWidth="1"/>
     <col min="19" max="20" width="9" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="23" max="24" width="9" bestFit="1" customWidth="1"/>
-    <col min="25" max="26" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="9" customWidth="1"/>
+    <col min="23" max="23" width="13.5" customWidth="1"/>
+    <col min="24" max="24" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="9" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:22" ht="21" x14ac:dyDescent="0.2">
-      <c r="B1" s="134" t="s">
+    <row r="1" spans="2:24" ht="21" x14ac:dyDescent="0.2">
+      <c r="B1" s="117" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="135"/>
-      <c r="D1" s="135"/>
-      <c r="E1" s="135"/>
-      <c r="F1" s="135"/>
-      <c r="G1" s="135"/>
-      <c r="H1" s="135"/>
-      <c r="I1" s="135"/>
-      <c r="J1" s="135"/>
-      <c r="K1" s="135"/>
-      <c r="L1" s="135"/>
-      <c r="M1" s="135"/>
-      <c r="N1" s="135"/>
-      <c r="O1" s="135"/>
-      <c r="P1" s="135"/>
-      <c r="Q1" s="135"/>
-      <c r="R1" s="135"/>
-      <c r="S1" s="135"/>
-      <c r="T1" s="135"/>
-      <c r="U1" s="135"/>
-      <c r="V1" s="135"/>
-    </row>
-    <row r="2" spans="2:22" ht="19" x14ac:dyDescent="0.25">
-      <c r="B2" s="110" t="s">
+      <c r="C1" s="118"/>
+      <c r="D1" s="118"/>
+      <c r="E1" s="118"/>
+      <c r="F1" s="118"/>
+      <c r="G1" s="118"/>
+      <c r="H1" s="118"/>
+      <c r="I1" s="118"/>
+      <c r="J1" s="118"/>
+      <c r="K1" s="118"/>
+      <c r="L1" s="118"/>
+      <c r="M1" s="118"/>
+      <c r="N1" s="118"/>
+      <c r="O1" s="118"/>
+      <c r="P1" s="118"/>
+      <c r="Q1" s="118"/>
+      <c r="R1" s="118"/>
+      <c r="S1" s="118"/>
+      <c r="T1" s="118"/>
+      <c r="U1" s="118"/>
+      <c r="V1" s="118"/>
+      <c r="W1" s="118"/>
+      <c r="X1" s="118"/>
+    </row>
+    <row r="2" spans="2:24" ht="19" x14ac:dyDescent="0.25">
+      <c r="B2" s="111" t="s">
         <v>67</v>
       </c>
-      <c r="C2" s="111"/>
-      <c r="D2" s="111"/>
-      <c r="E2" s="111"/>
-      <c r="F2" s="112"/>
-      <c r="G2" s="110" t="s">
+      <c r="C2" s="112"/>
+      <c r="D2" s="112"/>
+      <c r="E2" s="112"/>
+      <c r="F2" s="113"/>
+      <c r="G2" s="111" t="s">
         <v>68</v>
       </c>
-      <c r="H2" s="111"/>
-      <c r="I2" s="111"/>
-      <c r="J2" s="112"/>
-      <c r="K2" s="113" t="s">
+      <c r="H2" s="112"/>
+      <c r="I2" s="112"/>
+      <c r="J2" s="113"/>
+      <c r="K2" s="114" t="s">
         <v>69</v>
       </c>
-      <c r="L2" s="114"/>
-      <c r="M2" s="115"/>
-      <c r="N2" s="113" t="s">
+      <c r="L2" s="115"/>
+      <c r="M2" s="116"/>
+      <c r="N2" s="114" t="s">
         <v>70</v>
       </c>
-      <c r="O2" s="114"/>
-      <c r="P2" s="115"/>
-      <c r="Q2" s="113" t="s">
+      <c r="O2" s="115"/>
+      <c r="P2" s="116"/>
+      <c r="Q2" s="114" t="s">
         <v>71</v>
       </c>
-      <c r="R2" s="114"/>
-      <c r="S2" s="115"/>
-      <c r="T2" s="113" t="s">
+      <c r="R2" s="115"/>
+      <c r="S2" s="116"/>
+      <c r="T2" s="114" t="s">
         <v>72</v>
       </c>
       <c r="U2" s="115"/>
-      <c r="V2" s="42" t="s">
+      <c r="V2" s="115"/>
+      <c r="W2" s="116"/>
+      <c r="X2" s="42" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="2:22" ht="51" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:24" ht="51" x14ac:dyDescent="0.2">
       <c r="B3" s="43" t="s">
         <v>33</v>
       </c>
@@ -3715,7 +3741,7 @@
       <c r="I3" s="43" t="s">
         <v>75</v>
       </c>
-      <c r="J3" s="133" t="s">
+      <c r="J3" s="44" t="s">
         <v>76</v>
       </c>
       <c r="K3" s="43" t="s">
@@ -3749,24 +3775,30 @@
         <v>81</v>
       </c>
       <c r="U3" s="43" t="s">
+        <v>84</v>
+      </c>
+      <c r="V3" s="43" t="s">
         <v>82</v>
       </c>
-      <c r="V3" s="43" t="s">
+      <c r="W3" s="136" t="s">
+        <v>83</v>
+      </c>
+      <c r="X3" s="43" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="8" spans="2:22" s="33" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="2:24" s="33" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="17" s="33" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="21" s="33" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="T2:W2"/>
+    <mergeCell ref="B1:X1"/>
     <mergeCell ref="G2:J2"/>
     <mergeCell ref="K2:M2"/>
     <mergeCell ref="Q2:S2"/>
     <mergeCell ref="N2:P2"/>
     <mergeCell ref="B2:F2"/>
-    <mergeCell ref="T2:U2"/>
-    <mergeCell ref="B1:V1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3791,55 +3823,55 @@
   </cols>
   <sheetData>
     <row r="2" spans="5:13" ht="26" x14ac:dyDescent="0.2">
-      <c r="E2" s="102" t="s">
+      <c r="E2" s="103" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="102"/>
-      <c r="G2" s="102"/>
-      <c r="H2" s="102"/>
-      <c r="I2" s="102"/>
-      <c r="J2" s="102"/>
-      <c r="K2" s="102"/>
-      <c r="L2" s="102"/>
-      <c r="M2" s="102"/>
+      <c r="F2" s="103"/>
+      <c r="G2" s="103"/>
+      <c r="H2" s="103"/>
+      <c r="I2" s="103"/>
+      <c r="J2" s="103"/>
+      <c r="K2" s="103"/>
+      <c r="L2" s="103"/>
+      <c r="M2" s="103"/>
     </row>
     <row r="4" spans="5:13" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E4" s="100" t="s">
+      <c r="E4" s="101" t="s">
         <v>0</v>
       </c>
-      <c r="F4" s="119" t="s">
+      <c r="F4" s="122" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="120"/>
-      <c r="H4" s="121"/>
-      <c r="I4" s="107" t="s">
+      <c r="G4" s="123"/>
+      <c r="H4" s="124"/>
+      <c r="I4" s="108" t="s">
         <v>8</v>
       </c>
-      <c r="J4" s="125"/>
-      <c r="K4" s="125"/>
-      <c r="L4" s="126"/>
-      <c r="M4" s="100" t="s">
+      <c r="J4" s="128"/>
+      <c r="K4" s="128"/>
+      <c r="L4" s="129"/>
+      <c r="M4" s="101" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="5:13" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E5" s="101"/>
-      <c r="F5" s="122"/>
-      <c r="G5" s="123"/>
-      <c r="H5" s="124"/>
+      <c r="E5" s="102"/>
+      <c r="F5" s="125"/>
+      <c r="G5" s="126"/>
+      <c r="H5" s="127"/>
       <c r="I5" s="4"/>
       <c r="J5" s="5"/>
       <c r="K5" s="6"/>
       <c r="L5" s="4"/>
-      <c r="M5" s="101"/>
+      <c r="M5" s="102"/>
     </row>
     <row r="6" spans="5:13" ht="167.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E6" s="2">
         <v>1</v>
       </c>
-      <c r="F6" s="127"/>
-      <c r="G6" s="128"/>
-      <c r="H6" s="129"/>
+      <c r="F6" s="130"/>
+      <c r="G6" s="131"/>
+      <c r="H6" s="132"/>
       <c r="I6" s="24"/>
       <c r="J6" s="24"/>
       <c r="K6" s="24"/>
@@ -3850,9 +3882,9 @@
       <c r="E7" s="2">
         <v>2</v>
       </c>
-      <c r="F7" s="127"/>
-      <c r="G7" s="128"/>
-      <c r="H7" s="129"/>
+      <c r="F7" s="130"/>
+      <c r="G7" s="131"/>
+      <c r="H7" s="132"/>
       <c r="I7" s="24"/>
       <c r="J7" s="24"/>
       <c r="K7" s="24"/>
@@ -3863,9 +3895,9 @@
       <c r="E8" s="2">
         <v>3</v>
       </c>
-      <c r="F8" s="130"/>
-      <c r="G8" s="131"/>
-      <c r="H8" s="132"/>
+      <c r="F8" s="133"/>
+      <c r="G8" s="134"/>
+      <c r="H8" s="135"/>
       <c r="I8" s="24"/>
       <c r="J8" s="24"/>
       <c r="K8" s="24"/>
@@ -3876,9 +3908,9 @@
       <c r="E9" s="2">
         <v>4</v>
       </c>
-      <c r="F9" s="130"/>
-      <c r="G9" s="131"/>
-      <c r="H9" s="132"/>
+      <c r="F9" s="133"/>
+      <c r="G9" s="134"/>
+      <c r="H9" s="135"/>
       <c r="I9" s="24"/>
       <c r="J9" s="24"/>
       <c r="K9" s="24"/>
@@ -3889,9 +3921,9 @@
       <c r="E10" s="2">
         <v>5</v>
       </c>
-      <c r="F10" s="116"/>
-      <c r="G10" s="117"/>
-      <c r="H10" s="118"/>
+      <c r="F10" s="119"/>
+      <c r="G10" s="120"/>
+      <c r="H10" s="121"/>
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
@@ -3902,9 +3934,9 @@
       <c r="E11" s="2">
         <v>6</v>
       </c>
-      <c r="F11" s="116"/>
-      <c r="G11" s="117"/>
-      <c r="H11" s="118"/>
+      <c r="F11" s="119"/>
+      <c r="G11" s="120"/>
+      <c r="H11" s="121"/>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
@@ -3915,9 +3947,9 @@
       <c r="E12" s="2">
         <v>7</v>
       </c>
-      <c r="F12" s="116"/>
-      <c r="G12" s="117"/>
-      <c r="H12" s="118"/>
+      <c r="F12" s="119"/>
+      <c r="G12" s="120"/>
+      <c r="H12" s="121"/>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
@@ -3928,9 +3960,9 @@
       <c r="E13" s="2">
         <v>8</v>
       </c>
-      <c r="F13" s="116"/>
-      <c r="G13" s="117"/>
-      <c r="H13" s="118"/>
+      <c r="F13" s="119"/>
+      <c r="G13" s="120"/>
+      <c r="H13" s="121"/>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
@@ -3941,9 +3973,9 @@
       <c r="E14" s="2">
         <v>9</v>
       </c>
-      <c r="F14" s="116"/>
-      <c r="G14" s="117"/>
-      <c r="H14" s="118"/>
+      <c r="F14" s="119"/>
+      <c r="G14" s="120"/>
+      <c r="H14" s="121"/>
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
@@ -3954,9 +3986,9 @@
       <c r="E15" s="2">
         <v>10</v>
       </c>
-      <c r="F15" s="116"/>
-      <c r="G15" s="117"/>
-      <c r="H15" s="118"/>
+      <c r="F15" s="119"/>
+      <c r="G15" s="120"/>
+      <c r="H15" s="121"/>
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
@@ -3967,9 +3999,9 @@
       <c r="E16" s="2">
         <v>11</v>
       </c>
-      <c r="F16" s="116"/>
-      <c r="G16" s="117"/>
-      <c r="H16" s="118"/>
+      <c r="F16" s="119"/>
+      <c r="G16" s="120"/>
+      <c r="H16" s="121"/>
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
@@ -3980,9 +4012,9 @@
       <c r="E17" s="2">
         <v>12</v>
       </c>
-      <c r="F17" s="116"/>
-      <c r="G17" s="117"/>
-      <c r="H17" s="118"/>
+      <c r="F17" s="119"/>
+      <c r="G17" s="120"/>
+      <c r="H17" s="121"/>
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
@@ -3993,9 +4025,9 @@
       <c r="E18" s="2">
         <v>13</v>
       </c>
-      <c r="F18" s="116"/>
-      <c r="G18" s="117"/>
-      <c r="H18" s="118"/>
+      <c r="F18" s="119"/>
+      <c r="G18" s="120"/>
+      <c r="H18" s="121"/>
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
@@ -4006,9 +4038,9 @@
       <c r="E19" s="2">
         <v>14</v>
       </c>
-      <c r="F19" s="116"/>
-      <c r="G19" s="117"/>
-      <c r="H19" s="118"/>
+      <c r="F19" s="119"/>
+      <c r="G19" s="120"/>
+      <c r="H19" s="121"/>
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
@@ -4019,9 +4051,9 @@
       <c r="E20" s="2">
         <v>15</v>
       </c>
-      <c r="F20" s="116"/>
-      <c r="G20" s="117"/>
-      <c r="H20" s="118"/>
+      <c r="F20" s="119"/>
+      <c r="G20" s="120"/>
+      <c r="H20" s="121"/>
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
@@ -4030,14 +4062,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="F14:H14"/>
-    <mergeCell ref="F15:H15"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="F18:H18"/>
     <mergeCell ref="F12:H12"/>
     <mergeCell ref="E2:M2"/>
     <mergeCell ref="E4:E5"/>
@@ -4050,6 +4074,14 @@
     <mergeCell ref="F9:H9"/>
     <mergeCell ref="F10:H10"/>
     <mergeCell ref="F11:H11"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="F15:H15"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="F18:H18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="53" orientation="portrait" r:id="rId1"/>

</xml_diff>